<commit_message>
Add the test case of calculate the file or folder size on xlsx file
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="8.根据文件已有字段被替换为新名称" sheetId="13" r:id="rId8"/>
     <sheet name="9.特殊字符测试" sheetId="15" r:id="rId9"/>
     <sheet name="10.主界面基本功能检测" sheetId="16" r:id="rId10"/>
+    <sheet name="11.计算文件或文件夹大小" sheetId="17" r:id="rId11"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="302">
   <si>
     <t>删除文件夹</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4241,10 +4242,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>在"Please choose :"中输入1-9以外的任何数值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>在"Please choose :"中输入非数字字符</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -5515,93 +5512,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>文件夹名</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What file or folder you want to find on this folder?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入文件名或扩展名，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.txt，456.txt,20170614</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -5965,14 +5875,6 @@
       </rPr>
       <t>）</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10.11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在"Please choose :"中输入9</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -7962,6 +7864,517 @@
       </rPr>
       <t xml:space="preserve">的文件路径         
 </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算文件或文件夹大小</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9. Calculate the file or folder size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What file or folder you want to find on this folder?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入文件名或扩展名，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.txt，456.txt,20170614</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示该文件夹不存在的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1\123.txt is NOT exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示该文件夹不存在的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1 is NOT exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1\123.txt</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示出计算后，该文件夹容量信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The size of D:\Test1 are 10.122 MB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示出计算后，该文件容量信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The size of D:\Test1\123.txt are 10.112 MB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在"Please choose :"中输入10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在"Please choose :"中输入1-10以外的任何数值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在"Please choose :"中输入9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>进入"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>计算文件或文件夹大小</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"模块，并输出</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calculate the file or folder size</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7973,7 +8386,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8076,6 +8489,14 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF0070C0"/>
       <name val="宋体"/>
@@ -8188,7 +8609,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -8336,6 +8757,15 @@
     <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -8386,6 +8816,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8711,14 +9144,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="49"/>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
+      <c r="A1" s="52"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -8750,20 +9183,20 @@
       <c r="A3" s="22">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="56" t="s">
         <v>112</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="53" t="s">
         <v>103</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>26</v>
@@ -8774,12 +9207,12 @@
       <c r="A4" s="22">
         <v>1.2</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="51"/>
+      <c r="E4" s="54"/>
       <c r="F4" s="2" t="s">
         <v>101</v>
       </c>
@@ -8792,12 +9225,12 @@
       <c r="A5" s="22">
         <v>1.3</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="E5" s="51"/>
+        <v>262</v>
+      </c>
+      <c r="E5" s="54"/>
       <c r="F5" s="2" t="s">
         <v>80</v>
       </c>
@@ -8810,12 +9243,12 @@
       <c r="A6" s="22">
         <v>1.4</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="52"/>
+      <c r="E6" s="55"/>
       <c r="F6" s="2" t="s">
         <v>79</v>
       </c>
@@ -8828,8 +9261,8 @@
       <c r="A7" s="27">
         <v>1.5</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
       <c r="D7" s="20" t="s">
         <v>151</v>
       </c>
@@ -8863,7 +9296,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -8882,14 +9315,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="58"/>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
+      <c r="A1" s="61"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="45" t="s">
@@ -8921,23 +9354,23 @@
       <c r="A3" s="46">
         <v>10.1</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="68" t="s">
         <v>167</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="68" t="s">
         <v>168</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="68" t="s">
         <v>169</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>170</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -8945,14 +9378,14 @@
       <c r="A4" s="46">
         <v>10.199999999999999</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
       <c r="E4" s="2" t="s">
         <v>171</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>153</v>
@@ -8963,14 +9396,14 @@
       <c r="A5" s="46">
         <v>10.3</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
       <c r="E5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>153</v>
@@ -8981,14 +9414,14 @@
       <c r="A6" s="46">
         <v>10.4</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
       <c r="E6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>153</v>
@@ -8999,14 +9432,14 @@
       <c r="A7" s="46">
         <v>10.5</v>
       </c>
-      <c r="B7" s="65"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
       <c r="E7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>153</v>
@@ -9017,14 +9450,14 @@
       <c r="A8" s="46">
         <v>10.6</v>
       </c>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
       <c r="E8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>153</v>
@@ -9035,14 +9468,14 @@
       <c r="A9" s="46">
         <v>10.7</v>
       </c>
-      <c r="B9" s="65"/>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
       <c r="E9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>153</v>
@@ -9053,80 +9486,266 @@
       <c r="A10" s="46">
         <v>10.8</v>
       </c>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
       <c r="E10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>153</v>
       </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="46">
         <v>10.9</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
       <c r="E11" s="2" t="s">
-        <v>242</v>
+        <v>300</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="G11" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A12" s="69" t="s">
+        <v>297</v>
+      </c>
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A12" s="48">
-        <v>10.1</v>
-      </c>
-      <c r="B12" s="65"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>153</v>
-      </c>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A13" s="46" t="s">
-        <v>241</v>
-      </c>
-      <c r="B13" s="65"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
+      <c r="A13" s="48">
+        <v>10.11</v>
+      </c>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
       <c r="E13" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>153</v>
       </c>
       <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A14" s="46">
+        <v>10.119999999999999</v>
+      </c>
+      <c r="B14" s="68"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H14" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:B13"/>
-    <mergeCell ref="C3:C13"/>
-    <mergeCell ref="D3:D13"/>
+    <mergeCell ref="B3:B14"/>
+    <mergeCell ref="C3:C14"/>
+    <mergeCell ref="D3:D14"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" customWidth="1"/>
+    <col min="4" max="4" width="28.75" customWidth="1"/>
+    <col min="5" max="5" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.25" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="10.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A1" s="61"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="57" x14ac:dyDescent="0.15">
+      <c r="A3" s="22">
+        <v>11.1</v>
+      </c>
+      <c r="B3" s="56" t="s">
+        <v>284</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>285</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>293</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="57" x14ac:dyDescent="0.15">
+      <c r="A4" s="49">
+        <v>11.2</v>
+      </c>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E4" s="55"/>
+      <c r="F4" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.15">
+      <c r="A5" s="49">
+        <v>11.3</v>
+      </c>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E5" s="53" t="s">
+        <v>294</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" ht="57" x14ac:dyDescent="0.15">
+      <c r="A6" s="50">
+        <v>11.4</v>
+      </c>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="E6" s="55"/>
+      <c r="F6" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A7" s="51">
+        <v>11.5</v>
+      </c>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9138,7 +9757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C7" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -9156,14 +9775,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="49"/>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
+      <c r="A1" s="52"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -9195,10 +9814,10 @@
       <c r="A3" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="56" t="s">
         <v>113</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -9208,7 +9827,7 @@
         <v>73</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>30</v>
@@ -9219,16 +9838,16 @@
       <c r="A4" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>25</v>
@@ -9239,10 +9858,10 @@
       <c r="A5" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>73</v>
@@ -9259,8 +9878,8 @@
       <c r="A6" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
       <c r="D6" s="20" t="s">
         <v>151</v>
       </c>
@@ -9317,10 +9936,10 @@
       <c r="A9" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="56" t="s">
         <v>113</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -9330,7 +9949,7 @@
         <v>107</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>25</v>
@@ -9342,8 +9961,8 @@
       <c r="A10" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B10" s="54"/>
-      <c r="C10" s="54"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
       <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
@@ -9351,7 +9970,7 @@
         <v>94</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>72</v>
@@ -9365,10 +9984,10 @@
       <c r="A11" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
       <c r="D11" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>93</v>
@@ -9386,8 +10005,8 @@
       <c r="A12" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="B12" s="55"/>
-      <c r="C12" s="55"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58"/>
       <c r="D12" s="20" t="s">
         <v>151</v>
       </c>
@@ -9404,7 +10023,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
-      <c r="B13" s="56"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -9415,7 +10034,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
-      <c r="B14" s="56"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="4"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -9426,7 +10045,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
-      <c r="B15" s="56"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -9437,7 +10056,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
-      <c r="B16" s="56"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -9448,7 +10067,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
-      <c r="B17" s="56"/>
+      <c r="B17" s="59"/>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -9524,14 +10143,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A1" s="57"/>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
+      <c r="A1" s="60"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -9563,20 +10182,20 @@
       <c r="A3" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="56" t="s">
         <v>115</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E3" s="50" t="s">
+        <v>269</v>
+      </c>
+      <c r="E3" s="53" t="s">
         <v>95</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -9587,14 +10206,14 @@
       <c r="A4" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E4" s="51"/>
+        <v>270</v>
+      </c>
+      <c r="E4" s="54"/>
       <c r="F4" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>25</v>
@@ -9605,12 +10224,12 @@
       <c r="A5" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="E5" s="51"/>
+        <v>271</v>
+      </c>
+      <c r="E5" s="54"/>
       <c r="F5" s="2" t="s">
         <v>83</v>
       </c>
@@ -9623,14 +10242,14 @@
       <c r="A6" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E6" s="51"/>
+      <c r="E6" s="54"/>
       <c r="F6" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>25</v>
@@ -9641,14 +10260,14 @@
       <c r="A7" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
       <c r="D7" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="E7" s="51"/>
+        <v>272</v>
+      </c>
+      <c r="E7" s="54"/>
       <c r="F7" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>32</v>
@@ -9659,14 +10278,14 @@
       <c r="A8" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
       <c r="D8" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="E8" s="51"/>
+      <c r="E8" s="54"/>
       <c r="F8" s="19" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>37</v>
@@ -9677,14 +10296,14 @@
       <c r="A9" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="B9" s="54"/>
-      <c r="C9" s="54"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
       <c r="D9" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="E9" s="51"/>
+        <v>210</v>
+      </c>
+      <c r="E9" s="54"/>
       <c r="F9" s="19" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>25</v>
@@ -9693,28 +10312,28 @@
     </row>
     <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A10" s="35" t="s">
-        <v>215</v>
-      </c>
-      <c r="B10" s="54"/>
-      <c r="C10" s="54"/>
+        <v>214</v>
+      </c>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
       <c r="D10" s="35" t="s">
-        <v>219</v>
-      </c>
-      <c r="E10" s="52"/>
+        <v>218</v>
+      </c>
+      <c r="E10" s="55"/>
       <c r="F10" s="36" t="s">
+        <v>212</v>
+      </c>
+      <c r="G10" s="37" t="s">
         <v>213</v>
-      </c>
-      <c r="G10" s="37" t="s">
-        <v>214</v>
       </c>
       <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="20" t="s">
-        <v>216</v>
-      </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
+        <v>215</v>
+      </c>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
       <c r="D11" s="20" t="s">
         <v>151</v>
       </c>
@@ -9731,10 +10350,10 @@
     </row>
     <row r="12" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="B12" s="55"/>
-      <c r="C12" s="55"/>
+        <v>216</v>
+      </c>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58"/>
       <c r="D12" s="20" t="s">
         <v>152</v>
       </c>
@@ -9779,20 +10398,20 @@
       <c r="A16" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="56" t="s">
         <v>114</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="E16" s="50" t="s">
+      <c r="E16" s="53" t="s">
         <v>96</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G16" s="14" t="s">
         <v>25</v>
@@ -9803,12 +10422,12 @@
       <c r="A17" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="54"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
       <c r="D17" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="E17" s="51"/>
+        <v>273</v>
+      </c>
+      <c r="E17" s="54"/>
       <c r="F17" s="14" t="s">
         <v>82</v>
       </c>
@@ -9821,14 +10440,14 @@
       <c r="A18" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
       <c r="D18" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="51"/>
+      <c r="E18" s="54"/>
       <c r="F18" s="14" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>25</v>
@@ -9839,12 +10458,12 @@
       <c r="A19" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
       <c r="D19" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="E19" s="51"/>
+        <v>274</v>
+      </c>
+      <c r="E19" s="54"/>
       <c r="F19" s="14" t="s">
         <v>81</v>
       </c>
@@ -9857,14 +10476,14 @@
       <c r="A20" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B20" s="54"/>
-      <c r="C20" s="54"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
       <c r="D20" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="E20" s="51"/>
+      <c r="E20" s="54"/>
       <c r="F20" s="11" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>25</v>
@@ -9873,19 +10492,19 @@
     </row>
     <row r="21" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A21" s="35" t="s">
-        <v>220</v>
-      </c>
-      <c r="B21" s="54"/>
-      <c r="C21" s="54"/>
+        <v>219</v>
+      </c>
+      <c r="B21" s="57"/>
+      <c r="C21" s="57"/>
       <c r="D21" s="35" t="s">
-        <v>218</v>
-      </c>
-      <c r="E21" s="52"/>
+        <v>217</v>
+      </c>
+      <c r="E21" s="55"/>
       <c r="F21" s="36" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H21" s="37"/>
     </row>
@@ -9893,8 +10512,8 @@
       <c r="A22" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="B22" s="54"/>
-      <c r="C22" s="54"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="57"/>
       <c r="D22" s="20" t="s">
         <v>102</v>
       </c>
@@ -9911,10 +10530,10 @@
     </row>
     <row r="23" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A23" s="20" t="s">
-        <v>221</v>
-      </c>
-      <c r="B23" s="55"/>
-      <c r="C23" s="55"/>
+        <v>220</v>
+      </c>
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
       <c r="D23" s="20" t="s">
         <v>152</v>
       </c>
@@ -9966,14 +10585,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="58"/>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
+      <c r="A1" s="61"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10003,22 +10622,22 @@
     </row>
     <row r="3" spans="1:8" s="23" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="B3" s="59" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="59" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="62" t="s">
         <v>116</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="E3" s="62" t="s">
+        <v>275</v>
+      </c>
+      <c r="E3" s="65" t="s">
         <v>123</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>35</v>
@@ -10027,14 +10646,14 @@
     </row>
     <row r="4" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
+        <v>197</v>
+      </c>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
       <c r="D4" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="E4" s="63"/>
+        <v>276</v>
+      </c>
+      <c r="E4" s="66"/>
       <c r="F4" s="6" t="s">
         <v>84</v>
       </c>
@@ -10045,16 +10664,16 @@
     </row>
     <row r="5" spans="1:8" s="23" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
+        <v>198</v>
+      </c>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
       <c r="D5" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="63"/>
+      <c r="E5" s="66"/>
       <c r="F5" s="6" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>34</v>
@@ -10063,14 +10682,14 @@
     </row>
     <row r="6" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
+        <v>199</v>
+      </c>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
       <c r="D6" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="E6" s="63"/>
+        <v>277</v>
+      </c>
+      <c r="E6" s="66"/>
       <c r="F6" s="6" t="s">
         <v>84</v>
       </c>
@@ -10081,16 +10700,16 @@
     </row>
     <row r="7" spans="1:8" s="23" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
+        <v>200</v>
+      </c>
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
       <c r="D7" s="29" t="s">
-        <v>194</v>
-      </c>
-      <c r="E7" s="63"/>
+        <v>193</v>
+      </c>
+      <c r="E7" s="66"/>
       <c r="F7" s="29" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="G7" s="30" t="s">
         <v>61</v>
@@ -10099,28 +10718,28 @@
     </row>
     <row r="8" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A8" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
+        <v>224</v>
+      </c>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
       <c r="D8" s="35" t="s">
-        <v>228</v>
-      </c>
-      <c r="E8" s="64"/>
+        <v>227</v>
+      </c>
+      <c r="E8" s="67"/>
       <c r="F8" s="36" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H8" s="40"/>
     </row>
     <row r="9" spans="1:8" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A9" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
+        <v>201</v>
+      </c>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
       <c r="D9" s="20" t="s">
         <v>151</v>
       </c>
@@ -10137,10 +10756,10 @@
     </row>
     <row r="10" spans="1:8" s="33" customFormat="1" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A10" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="B10" s="61"/>
-      <c r="C10" s="61"/>
+        <v>223</v>
+      </c>
+      <c r="B10" s="64"/>
+      <c r="C10" s="64"/>
       <c r="D10" s="20" t="s">
         <v>152</v>
       </c>
@@ -10192,22 +10811,22 @@
     </row>
     <row r="13" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B13" s="53" t="s">
+        <v>202</v>
+      </c>
+      <c r="B13" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" s="62" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C13" s="59" t="s">
-        <v>116</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E13" s="50" t="s">
+      <c r="E13" s="53" t="s">
         <v>109</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>25</v>
@@ -10216,16 +10835,16 @@
     </row>
     <row r="14" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B14" s="54"/>
-      <c r="C14" s="60"/>
+        <v>203</v>
+      </c>
+      <c r="B14" s="57"/>
+      <c r="C14" s="63"/>
       <c r="D14" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="E14" s="51"/>
+        <v>192</v>
+      </c>
+      <c r="E14" s="54"/>
       <c r="F14" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>25</v>
@@ -10234,14 +10853,14 @@
     </row>
     <row r="15" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B15" s="54"/>
-      <c r="C15" s="60"/>
+        <v>204</v>
+      </c>
+      <c r="B15" s="57"/>
+      <c r="C15" s="63"/>
       <c r="D15" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="E15" s="51"/>
+        <v>278</v>
+      </c>
+      <c r="E15" s="54"/>
       <c r="F15" s="2" t="s">
         <v>86</v>
       </c>
@@ -10252,16 +10871,16 @@
     </row>
     <row r="16" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B16" s="54"/>
-      <c r="C16" s="60"/>
+        <v>205</v>
+      </c>
+      <c r="B16" s="57"/>
+      <c r="C16" s="63"/>
       <c r="D16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="51"/>
+      <c r="E16" s="54"/>
       <c r="F16" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>25</v>
@@ -10270,14 +10889,14 @@
     </row>
     <row r="17" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="60"/>
+        <v>206</v>
+      </c>
+      <c r="B17" s="57"/>
+      <c r="C17" s="63"/>
       <c r="D17" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="E17" s="51"/>
+        <v>279</v>
+      </c>
+      <c r="E17" s="54"/>
       <c r="F17" s="2" t="s">
         <v>85</v>
       </c>
@@ -10288,14 +10907,14 @@
     </row>
     <row r="18" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="60"/>
+        <v>207</v>
+      </c>
+      <c r="B18" s="57"/>
+      <c r="C18" s="63"/>
       <c r="D18" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="E18" s="51"/>
+        <v>195</v>
+      </c>
+      <c r="E18" s="54"/>
       <c r="F18" s="11" t="s">
         <v>76</v>
       </c>
@@ -10306,14 +10925,14 @@
     </row>
     <row r="19" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="60"/>
+        <v>208</v>
+      </c>
+      <c r="B19" s="57"/>
+      <c r="C19" s="63"/>
       <c r="D19" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="E19" s="51"/>
+        <v>194</v>
+      </c>
+      <c r="E19" s="54"/>
       <c r="F19" s="11" t="s">
         <v>76</v>
       </c>
@@ -10324,28 +10943,28 @@
     </row>
     <row r="20" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A20" s="35" t="s">
-        <v>227</v>
-      </c>
-      <c r="B20" s="54"/>
-      <c r="C20" s="60"/>
+        <v>226</v>
+      </c>
+      <c r="B20" s="57"/>
+      <c r="C20" s="63"/>
       <c r="D20" s="35" t="s">
-        <v>229</v>
-      </c>
-      <c r="E20" s="52"/>
+        <v>228</v>
+      </c>
+      <c r="E20" s="55"/>
       <c r="F20" s="36" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G20" s="41" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H20" s="42"/>
     </row>
     <row r="21" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A21" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="B21" s="54"/>
-      <c r="C21" s="60"/>
+        <v>209</v>
+      </c>
+      <c r="B21" s="57"/>
+      <c r="C21" s="63"/>
       <c r="D21" s="20" t="s">
         <v>151</v>
       </c>
@@ -10362,10 +10981,10 @@
     </row>
     <row r="22" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="B22" s="55"/>
-      <c r="C22" s="61"/>
+        <v>222</v>
+      </c>
+      <c r="B22" s="58"/>
+      <c r="C22" s="64"/>
       <c r="D22" s="20" t="s">
         <v>152</v>
       </c>
@@ -10401,7 +11020,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="D7" sqref="D7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -10417,14 +11036,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="58"/>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
+      <c r="A1" s="61"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10456,17 +11075,17 @@
       <c r="A3" s="22">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="56" t="s">
         <v>117</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="50" t="s">
-        <v>239</v>
+      <c r="E3" s="53" t="s">
+        <v>237</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>100</v>
@@ -10480,12 +11099,12 @@
       <c r="A4" s="22">
         <v>5.2</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="E4" s="51"/>
+        <v>263</v>
+      </c>
+      <c r="E4" s="54"/>
       <c r="F4" s="2" t="s">
         <v>99</v>
       </c>
@@ -10498,12 +11117,12 @@
       <c r="A5" s="22">
         <v>5.3</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="E5" s="51"/>
+        <v>280</v>
+      </c>
+      <c r="E5" s="54"/>
       <c r="F5" s="2" t="s">
         <v>87</v>
       </c>
@@ -10516,14 +11135,14 @@
       <c r="A6" s="22">
         <v>5.4</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E6" s="55"/>
+      <c r="F6" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="E6" s="52"/>
-      <c r="F6" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>31</v>
@@ -10534,8 +11153,8 @@
       <c r="A7" s="27">
         <v>5.5</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
       <c r="D7" s="20" t="s">
         <v>151</v>
       </c>
@@ -10574,7 +11193,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -10589,14 +11208,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="58"/>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
+      <c r="A1" s="61"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10635,13 +11254,13 @@
         <v>118</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="E3" s="50" t="s">
+        <v>230</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>286</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>235</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -10657,9 +11276,9 @@
       <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="51"/>
+      <c r="E4" s="54"/>
       <c r="F4" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>31</v>
@@ -10673,9 +11292,9 @@
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="D5" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="E5" s="52"/>
+        <v>264</v>
+      </c>
+      <c r="E5" s="55"/>
       <c r="F5" s="2" t="s">
         <v>88</v>
       </c>
@@ -10691,13 +11310,13 @@
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="D6" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="E6" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="F6" s="6" t="s">
         <v>234</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>236</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>153</v>
@@ -10743,7 +11362,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -10759,14 +11378,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="58"/>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
+      <c r="A1" s="61"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10798,20 +11417,20 @@
       <c r="A3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="56" t="s">
         <v>119</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="53" t="s">
         <v>97</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>29</v>
@@ -10822,12 +11441,12 @@
       <c r="A4" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="E4" s="51"/>
+        <v>265</v>
+      </c>
+      <c r="E4" s="54"/>
       <c r="F4" s="2" t="s">
         <v>62</v>
       </c>
@@ -10840,12 +11459,12 @@
       <c r="A5" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="E5" s="51"/>
+        <v>264</v>
+      </c>
+      <c r="E5" s="54"/>
       <c r="F5" s="2" t="s">
         <v>89</v>
       </c>
@@ -10858,12 +11477,12 @@
       <c r="A6" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="52"/>
+      <c r="E6" s="55"/>
       <c r="F6" s="6" t="s">
         <v>63</v>
       </c>
@@ -10876,8 +11495,8 @@
       <c r="A7" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
       <c r="D7" s="20" t="s">
         <v>151</v>
       </c>
@@ -10922,20 +11541,20 @@
       <c r="A10" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="56" t="s">
         <v>75</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="50" t="s">
+      <c r="E10" s="53" t="s">
         <v>98</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>25</v>
@@ -10946,12 +11565,12 @@
       <c r="A11" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
       <c r="D11" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="E11" s="51"/>
+        <v>266</v>
+      </c>
+      <c r="E11" s="54"/>
       <c r="F11" s="2" t="s">
         <v>154</v>
       </c>
@@ -10964,12 +11583,12 @@
       <c r="A12" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
       <c r="D12" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="E12" s="51"/>
+        <v>267</v>
+      </c>
+      <c r="E12" s="54"/>
       <c r="F12" s="2" t="s">
         <v>67</v>
       </c>
@@ -10982,12 +11601,12 @@
       <c r="A13" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="B13" s="54"/>
-      <c r="C13" s="54"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
       <c r="D13" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="52"/>
+      <c r="E13" s="55"/>
       <c r="F13" s="6" t="s">
         <v>70</v>
       </c>
@@ -11000,8 +11619,8 @@
       <c r="A14" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="B14" s="55"/>
-      <c r="C14" s="55"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
       <c r="D14" s="20" t="s">
         <v>151</v>
       </c>
@@ -11052,14 +11671,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="58"/>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
+      <c r="A1" s="61"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11091,20 +11710,20 @@
       <c r="A3" s="22">
         <v>8.1</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="56" t="s">
         <v>120</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="53" t="s">
         <v>111</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -11117,12 +11736,12 @@
       <c r="A4" s="22">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="51"/>
+      <c r="E4" s="54"/>
       <c r="F4" s="2" t="s">
         <v>52</v>
       </c>
@@ -11135,12 +11754,12 @@
       <c r="A5" s="22">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="E5" s="52"/>
+        <v>268</v>
+      </c>
+      <c r="E5" s="55"/>
       <c r="F5" s="2" t="s">
         <v>90</v>
       </c>
@@ -11153,8 +11772,8 @@
       <c r="A6" s="27">
         <v>8.4</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
       <c r="D6" s="20" t="s">
         <v>151</v>
       </c>
@@ -11207,14 +11826,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="58"/>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
+      <c r="A1" s="61"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11246,10 +11865,10 @@
       <c r="A3" s="22">
         <v>9.1</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="56" t="s">
         <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -11258,7 +11877,7 @@
       <c r="E3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="56" t="s">
         <v>45</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -11270,15 +11889,15 @@
       <c r="A4" s="22">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="54"/>
+      <c r="F4" s="57"/>
       <c r="G4" s="2" t="s">
         <v>47</v>
       </c>
@@ -11288,15 +11907,15 @@
       <c r="A5" s="22">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="54"/>
+      <c r="F5" s="57"/>
       <c r="G5" s="2" t="s">
         <v>47</v>
       </c>
@@ -11306,15 +11925,15 @@
       <c r="A6" s="22">
         <v>9.4</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="54"/>
+      <c r="F6" s="57"/>
       <c r="G6" s="5" t="s">
         <v>47</v>
       </c>
@@ -11324,15 +11943,15 @@
       <c r="A7" s="22">
         <v>9.5</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
       <c r="D7" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="55"/>
+      <c r="F7" s="58"/>
       <c r="G7" s="5" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Update the test cases file of FileOperation as bug found by #24 and #25
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="306">
   <si>
     <t>删除文件夹</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -8376,6 +8376,136 @@
       </rPr>
       <t>Calculate the file or folder size</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>任意文件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">路径
+2.输入任何内容进行查询
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\123.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 能够出现提示输入的信息
+2. 提示输入的路径为文件路径，并非文件夹路径 (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\123.txt is a file path , please input a folder path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">)
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -8609,7 +8739,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -8766,6 +8896,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -8816,9 +8952,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9125,9 +9258,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -9144,14 +9277,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="52"/>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="A1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -9183,16 +9316,16 @@
       <c r="A3" s="22">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="58" t="s">
         <v>112</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="55" t="s">
         <v>103</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -9207,12 +9340,12 @@
       <c r="A4" s="22">
         <v>1.2</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="54"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="2" t="s">
         <v>101</v>
       </c>
@@ -9225,12 +9358,12 @@
       <c r="A5" s="22">
         <v>1.3</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="E5" s="54"/>
+      <c r="E5" s="56"/>
       <c r="F5" s="2" t="s">
         <v>80</v>
       </c>
@@ -9243,12 +9376,12 @@
       <c r="A6" s="22">
         <v>1.4</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="55"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="2" t="s">
         <v>79</v>
       </c>
@@ -9257,36 +9390,54 @@
       </c>
       <c r="H6" s="18"/>
     </row>
-    <row r="7" spans="1:8" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A7" s="27">
+    <row r="7" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+      <c r="A7" s="22">
         <v>1.5</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="20" t="s">
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>303</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" spans="1:8" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A8" s="27">
+        <v>1.6</v>
+      </c>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E8" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F8" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G8" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="H7" s="21"/>
-    </row>
-    <row r="9" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A9" s="9"/>
-      <c r="B9" s="8"/>
+      <c r="H8" s="21"/>
+    </row>
+    <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A10" s="9"/>
+      <c r="B10" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E6"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="C3:C8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9315,14 +9466,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="61"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="45" t="s">
@@ -9354,13 +9505,13 @@
       <c r="A3" s="46">
         <v>10.1</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="70" t="s">
         <v>167</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="70" t="s">
         <v>168</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="70" t="s">
         <v>169</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -9378,9 +9529,9 @@
       <c r="A4" s="46">
         <v>10.199999999999999</v>
       </c>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
       <c r="E4" s="2" t="s">
         <v>171</v>
       </c>
@@ -9396,9 +9547,9 @@
       <c r="A5" s="46">
         <v>10.3</v>
       </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
       <c r="E5" s="2" t="s">
         <v>172</v>
       </c>
@@ -9414,9 +9565,9 @@
       <c r="A6" s="46">
         <v>10.4</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
       <c r="E6" s="2" t="s">
         <v>173</v>
       </c>
@@ -9432,9 +9583,9 @@
       <c r="A7" s="46">
         <v>10.5</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
       <c r="E7" s="2" t="s">
         <v>174</v>
       </c>
@@ -9450,9 +9601,9 @@
       <c r="A8" s="46">
         <v>10.6</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
       <c r="E8" s="2" t="s">
         <v>175</v>
       </c>
@@ -9468,9 +9619,9 @@
       <c r="A9" s="46">
         <v>10.7</v>
       </c>
-      <c r="B9" s="68"/>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
       <c r="E9" s="2" t="s">
         <v>176</v>
       </c>
@@ -9486,9 +9637,9 @@
       <c r="A10" s="46">
         <v>10.8</v>
       </c>
-      <c r="B10" s="68"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
       <c r="E10" s="2" t="s">
         <v>177</v>
       </c>
@@ -9504,9 +9655,9 @@
       <c r="A11" s="46">
         <v>10.9</v>
       </c>
-      <c r="B11" s="68"/>
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
       <c r="E11" s="2" t="s">
         <v>300</v>
       </c>
@@ -9517,12 +9668,12 @@
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A12" s="69" t="s">
+      <c r="A12" s="53" t="s">
         <v>297</v>
       </c>
-      <c r="B12" s="68"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
       <c r="E12" s="2" t="s">
         <v>298</v>
       </c>
@@ -9538,9 +9689,9 @@
       <c r="A13" s="48">
         <v>10.11</v>
       </c>
-      <c r="B13" s="68"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
       <c r="E13" s="2" t="s">
         <v>299</v>
       </c>
@@ -9556,9 +9707,9 @@
       <c r="A14" s="46">
         <v>10.119999999999999</v>
       </c>
-      <c r="B14" s="68"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
       <c r="E14" s="2" t="s">
         <v>178</v>
       </c>
@@ -9587,8 +9738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9604,14 +9755,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="61"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -9643,16 +9794,16 @@
       <c r="A3" s="22">
         <v>11.1</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="58" t="s">
         <v>284</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="58" t="s">
         <v>285</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="55" t="s">
         <v>293</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -9667,12 +9818,12 @@
       <c r="A4" s="49">
         <v>11.2</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="E4" s="55"/>
+      <c r="E4" s="57"/>
       <c r="F4" s="2" t="s">
         <v>292</v>
       </c>
@@ -9685,12 +9836,12 @@
       <c r="A5" s="49">
         <v>11.3</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="55" t="s">
         <v>294</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -9705,12 +9856,12 @@
       <c r="A6" s="50">
         <v>11.4</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="E6" s="55"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="2" t="s">
         <v>291</v>
       </c>
@@ -9723,8 +9874,8 @@
       <c r="A7" s="51">
         <v>11.5</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="20" t="s">
         <v>151</v>
       </c>
@@ -9775,14 +9926,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="52"/>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="A1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -9814,10 +9965,10 @@
       <c r="A3" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="58" t="s">
         <v>113</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -9838,8 +9989,8 @@
       <c r="A4" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
         <v>281</v>
       </c>
@@ -9858,8 +10009,8 @@
       <c r="A5" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
         <v>282</v>
       </c>
@@ -9878,8 +10029,8 @@
       <c r="A6" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="B6" s="58"/>
-      <c r="C6" s="58"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
       <c r="D6" s="20" t="s">
         <v>151</v>
       </c>
@@ -9936,10 +10087,10 @@
       <c r="A9" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="C9" s="58" t="s">
         <v>113</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -9961,8 +10112,8 @@
       <c r="A10" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
       <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
@@ -9984,8 +10135,8 @@
       <c r="A11" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
       <c r="D11" s="2" t="s">
         <v>283</v>
       </c>
@@ -10005,8 +10156,8 @@
       <c r="A12" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="B12" s="58"/>
-      <c r="C12" s="58"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
       <c r="D12" s="20" t="s">
         <v>151</v>
       </c>
@@ -10023,7 +10174,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
-      <c r="B13" s="59"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -10034,7 +10185,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
-      <c r="B14" s="59"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="4"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -10045,7 +10196,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
-      <c r="B15" s="59"/>
+      <c r="B15" s="61"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -10056,7 +10207,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
-      <c r="B16" s="59"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -10067,7 +10218,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
-      <c r="B17" s="59"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -10143,14 +10294,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A1" s="60"/>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
+      <c r="A1" s="62"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10182,16 +10333,16 @@
       <c r="A3" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="58" t="s">
         <v>115</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="55" t="s">
         <v>95</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -10206,12 +10357,12 @@
       <c r="A4" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="E4" s="54"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="2" t="s">
         <v>246</v>
       </c>
@@ -10224,12 +10375,12 @@
       <c r="A5" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="E5" s="54"/>
+      <c r="E5" s="56"/>
       <c r="F5" s="2" t="s">
         <v>83</v>
       </c>
@@ -10242,12 +10393,12 @@
       <c r="A6" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E6" s="54"/>
+      <c r="E6" s="56"/>
       <c r="F6" s="2" t="s">
         <v>247</v>
       </c>
@@ -10260,12 +10411,12 @@
       <c r="A7" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="E7" s="54"/>
+      <c r="E7" s="56"/>
       <c r="F7" s="2" t="s">
         <v>211</v>
       </c>
@@ -10278,12 +10429,12 @@
       <c r="A8" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
       <c r="D8" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="E8" s="54"/>
+      <c r="E8" s="56"/>
       <c r="F8" s="19" t="s">
         <v>248</v>
       </c>
@@ -10296,12 +10447,12 @@
       <c r="A9" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
       <c r="D9" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="E9" s="54"/>
+      <c r="E9" s="56"/>
       <c r="F9" s="19" t="s">
         <v>249</v>
       </c>
@@ -10314,12 +10465,12 @@
       <c r="A10" s="35" t="s">
         <v>214</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
       <c r="D10" s="35" t="s">
         <v>218</v>
       </c>
-      <c r="E10" s="55"/>
+      <c r="E10" s="57"/>
       <c r="F10" s="36" t="s">
         <v>212</v>
       </c>
@@ -10332,8 +10483,8 @@
       <c r="A11" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
       <c r="D11" s="20" t="s">
         <v>151</v>
       </c>
@@ -10352,8 +10503,8 @@
       <c r="A12" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="B12" s="58"/>
-      <c r="C12" s="58"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
       <c r="D12" s="20" t="s">
         <v>152</v>
       </c>
@@ -10398,16 +10549,16 @@
       <c r="A16" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="58" t="s">
         <v>114</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="E16" s="53" t="s">
+      <c r="E16" s="55" t="s">
         <v>96</v>
       </c>
       <c r="F16" s="14" t="s">
@@ -10422,12 +10573,12 @@
       <c r="A17" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
       <c r="D17" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="E17" s="54"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="14" t="s">
         <v>82</v>
       </c>
@@ -10440,12 +10591,12 @@
       <c r="A18" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
       <c r="D18" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="54"/>
+      <c r="E18" s="56"/>
       <c r="F18" s="14" t="s">
         <v>251</v>
       </c>
@@ -10458,12 +10609,12 @@
       <c r="A19" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
       <c r="D19" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="E19" s="54"/>
+      <c r="E19" s="56"/>
       <c r="F19" s="14" t="s">
         <v>81</v>
       </c>
@@ -10476,12 +10627,12 @@
       <c r="A20" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B20" s="57"/>
-      <c r="C20" s="57"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
       <c r="D20" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="E20" s="54"/>
+      <c r="E20" s="56"/>
       <c r="F20" s="11" t="s">
         <v>252</v>
       </c>
@@ -10494,12 +10645,12 @@
       <c r="A21" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="B21" s="57"/>
-      <c r="C21" s="57"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
       <c r="D21" s="35" t="s">
         <v>217</v>
       </c>
-      <c r="E21" s="55"/>
+      <c r="E21" s="57"/>
       <c r="F21" s="36" t="s">
         <v>221</v>
       </c>
@@ -10512,8 +10663,8 @@
       <c r="A22" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
       <c r="D22" s="20" t="s">
         <v>102</v>
       </c>
@@ -10532,8 +10683,8 @@
       <c r="A23" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="B23" s="58"/>
-      <c r="C23" s="58"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
       <c r="D23" s="20" t="s">
         <v>152</v>
       </c>
@@ -10585,14 +10736,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="61"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10624,16 +10775,16 @@
       <c r="A3" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="64" t="s">
         <v>189</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="64" t="s">
         <v>116</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="67" t="s">
         <v>123</v>
       </c>
       <c r="F3" s="6" t="s">
@@ -10648,12 +10799,12 @@
       <c r="A4" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="63"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="E4" s="66"/>
+      <c r="E4" s="68"/>
       <c r="F4" s="6" t="s">
         <v>84</v>
       </c>
@@ -10666,12 +10817,12 @@
       <c r="A5" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
       <c r="D5" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="66"/>
+      <c r="E5" s="68"/>
       <c r="F5" s="6" t="s">
         <v>254</v>
       </c>
@@ -10684,12 +10835,12 @@
       <c r="A6" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
       <c r="D6" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="E6" s="66"/>
+      <c r="E6" s="68"/>
       <c r="F6" s="6" t="s">
         <v>84</v>
       </c>
@@ -10702,12 +10853,12 @@
       <c r="A7" s="29" t="s">
         <v>200</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
       <c r="D7" s="29" t="s">
         <v>193</v>
       </c>
-      <c r="E7" s="66"/>
+      <c r="E7" s="68"/>
       <c r="F7" s="29" t="s">
         <v>255</v>
       </c>
@@ -10720,12 +10871,12 @@
       <c r="A8" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
       <c r="D8" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="E8" s="67"/>
+      <c r="E8" s="69"/>
       <c r="F8" s="36" t="s">
         <v>229</v>
       </c>
@@ -10738,8 +10889,8 @@
       <c r="A9" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
       <c r="D9" s="20" t="s">
         <v>151</v>
       </c>
@@ -10758,8 +10909,8 @@
       <c r="A10" s="20" t="s">
         <v>223</v>
       </c>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="20" t="s">
         <v>152</v>
       </c>
@@ -10813,16 +10964,16 @@
       <c r="A13" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="58" t="s">
         <v>190</v>
       </c>
-      <c r="C13" s="62" t="s">
+      <c r="C13" s="64" t="s">
         <v>116</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="E13" s="53" t="s">
+      <c r="E13" s="55" t="s">
         <v>109</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -10837,12 +10988,12 @@
       <c r="A14" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="63"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="65"/>
       <c r="D14" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E14" s="54"/>
+      <c r="E14" s="56"/>
       <c r="F14" s="2" t="s">
         <v>257</v>
       </c>
@@ -10855,12 +11006,12 @@
       <c r="A15" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B15" s="57"/>
-      <c r="C15" s="63"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="65"/>
       <c r="D15" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="E15" s="54"/>
+      <c r="E15" s="56"/>
       <c r="F15" s="2" t="s">
         <v>86</v>
       </c>
@@ -10873,12 +11024,12 @@
       <c r="A16" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="63"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="65"/>
       <c r="D16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="54"/>
+      <c r="E16" s="56"/>
       <c r="F16" s="2" t="s">
         <v>258</v>
       </c>
@@ -10891,12 +11042,12 @@
       <c r="A17" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="63"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="65"/>
       <c r="D17" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="E17" s="54"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="2" t="s">
         <v>85</v>
       </c>
@@ -10909,12 +11060,12 @@
       <c r="A18" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="63"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="65"/>
       <c r="D18" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="E18" s="54"/>
+      <c r="E18" s="56"/>
       <c r="F18" s="11" t="s">
         <v>76</v>
       </c>
@@ -10927,12 +11078,12 @@
       <c r="A19" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B19" s="57"/>
-      <c r="C19" s="63"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="65"/>
       <c r="D19" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="E19" s="54"/>
+      <c r="E19" s="56"/>
       <c r="F19" s="11" t="s">
         <v>76</v>
       </c>
@@ -10945,12 +11096,12 @@
       <c r="A20" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="B20" s="57"/>
-      <c r="C20" s="63"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="65"/>
       <c r="D20" s="35" t="s">
         <v>228</v>
       </c>
-      <c r="E20" s="55"/>
+      <c r="E20" s="57"/>
       <c r="F20" s="36" t="s">
         <v>225</v>
       </c>
@@ -10963,8 +11114,8 @@
       <c r="A21" s="20" t="s">
         <v>209</v>
       </c>
-      <c r="B21" s="57"/>
-      <c r="C21" s="63"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="65"/>
       <c r="D21" s="20" t="s">
         <v>151</v>
       </c>
@@ -10983,8 +11134,8 @@
       <c r="A22" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="B22" s="58"/>
-      <c r="C22" s="64"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="66"/>
       <c r="D22" s="20" t="s">
         <v>152</v>
       </c>
@@ -11017,10 +11168,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:F7"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -11036,14 +11187,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="61"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11075,16 +11226,16 @@
       <c r="A3" s="22">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="58" t="s">
         <v>117</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="55" t="s">
         <v>237</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -11099,12 +11250,12 @@
       <c r="A4" s="22">
         <v>5.2</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="E4" s="54"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="2" t="s">
         <v>99</v>
       </c>
@@ -11117,12 +11268,12 @@
       <c r="A5" s="22">
         <v>5.3</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="E5" s="54"/>
+      <c r="E5" s="56"/>
       <c r="F5" s="2" t="s">
         <v>87</v>
       </c>
@@ -11135,12 +11286,12 @@
       <c r="A6" s="22">
         <v>5.4</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="E6" s="55"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="2" t="s">
         <v>238</v>
       </c>
@@ -11149,38 +11300,58 @@
       </c>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A7" s="27">
+    <row r="7" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
+      <c r="A7" s="22">
         <v>5.5</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="20" t="s">
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>303</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A8" s="27">
+        <v>5.6</v>
+      </c>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E8" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F8" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G8" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="H7" s="21"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B8" s="8"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="8"/>
+      <c r="H8" s="21"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B9" s="8"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E6"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="C3:C8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11208,14 +11379,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="61"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11256,7 +11427,7 @@
       <c r="D3" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="55" t="s">
         <v>286</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -11276,7 +11447,7 @@
       <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="54"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="2" t="s">
         <v>235</v>
       </c>
@@ -11294,7 +11465,7 @@
       <c r="D5" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="E5" s="55"/>
+      <c r="E5" s="57"/>
       <c r="F5" s="2" t="s">
         <v>88</v>
       </c>
@@ -11378,14 +11549,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="61"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11417,16 +11588,16 @@
       <c r="A3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="58" t="s">
         <v>119</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="55" t="s">
         <v>97</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -11441,12 +11612,12 @@
       <c r="A4" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="E4" s="54"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="2" t="s">
         <v>62</v>
       </c>
@@ -11459,12 +11630,12 @@
       <c r="A5" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="E5" s="54"/>
+      <c r="E5" s="56"/>
       <c r="F5" s="2" t="s">
         <v>89</v>
       </c>
@@ -11477,12 +11648,12 @@
       <c r="A6" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="55"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="6" t="s">
         <v>63</v>
       </c>
@@ -11495,8 +11666,8 @@
       <c r="A7" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="20" t="s">
         <v>151</v>
       </c>
@@ -11541,16 +11712,16 @@
       <c r="A10" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="58" t="s">
         <v>75</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="53" t="s">
+      <c r="E10" s="55" t="s">
         <v>98</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -11565,12 +11736,12 @@
       <c r="A11" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
       <c r="D11" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="E11" s="54"/>
+      <c r="E11" s="56"/>
       <c r="F11" s="2" t="s">
         <v>154</v>
       </c>
@@ -11583,12 +11754,12 @@
       <c r="A12" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
       <c r="D12" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="E12" s="54"/>
+      <c r="E12" s="56"/>
       <c r="F12" s="2" t="s">
         <v>67</v>
       </c>
@@ -11601,12 +11772,12 @@
       <c r="A13" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
       <c r="D13" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="55"/>
+      <c r="E13" s="57"/>
       <c r="F13" s="6" t="s">
         <v>70</v>
       </c>
@@ -11619,8 +11790,8 @@
       <c r="A14" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="B14" s="58"/>
-      <c r="C14" s="58"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
       <c r="D14" s="20" t="s">
         <v>151</v>
       </c>
@@ -11671,14 +11842,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="61"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11710,16 +11881,16 @@
       <c r="A3" s="22">
         <v>8.1</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="58" t="s">
         <v>120</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="55" t="s">
         <v>111</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -11736,12 +11907,12 @@
       <c r="A4" s="22">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="54"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="2" t="s">
         <v>52</v>
       </c>
@@ -11754,12 +11925,12 @@
       <c r="A5" s="22">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="E5" s="55"/>
+      <c r="E5" s="57"/>
       <c r="F5" s="2" t="s">
         <v>90</v>
       </c>
@@ -11772,8 +11943,8 @@
       <c r="A6" s="27">
         <v>8.4</v>
       </c>
-      <c r="B6" s="58"/>
-      <c r="C6" s="58"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
       <c r="D6" s="20" t="s">
         <v>151</v>
       </c>
@@ -11826,14 +11997,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="61"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11865,10 +12036,10 @@
       <c r="A3" s="22">
         <v>9.1</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="58" t="s">
         <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -11877,7 +12048,7 @@
       <c r="E3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="58" t="s">
         <v>45</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -11889,15 +12060,15 @@
       <c r="A4" s="22">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="57"/>
+      <c r="F4" s="59"/>
       <c r="G4" s="2" t="s">
         <v>47</v>
       </c>
@@ -11907,15 +12078,15 @@
       <c r="A5" s="22">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="57"/>
+      <c r="F5" s="59"/>
       <c r="G5" s="2" t="s">
         <v>47</v>
       </c>
@@ -11925,15 +12096,15 @@
       <c r="A6" s="22">
         <v>9.4</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="57"/>
+      <c r="F6" s="59"/>
       <c r="G6" s="5" t="s">
         <v>47</v>
       </c>
@@ -11943,15 +12114,15 @@
       <c r="A7" s="22">
         <v>9.5</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="58"/>
+      <c r="F7" s="60"/>
       <c r="G7" s="5" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Add the test case of FileOperation as added the new function
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="314">
   <si>
     <t>删除文件夹</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3139,141 +3139,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>"出现时，输入一串空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What word do you want find?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alonso</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What word do you want replace?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Button</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -8501,6 +8366,555 @@
       </rPr>
       <t xml:space="preserve">)
 </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">文件路径
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件路径
+2. 根据</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件中的某一字段，输入想要被替换的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>已有字段</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3. 输入想要被替换的新名称
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件路径
+2. 根据</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件中的某一字段，输入想要被替换的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>未有字段</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3. 输入想要被替换的新名称</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the file or folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want find?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alonso</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want replace?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Button</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the file or folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want find?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alonso</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want replace?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Button</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 显示指定的文件夹路径不存在 （</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso1.jpg is NOT exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2. 重命名失败</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 显示成功的将相同字段的文件被替换为指定的新名称
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\alonso.txt has been replaced as D:\Test\Button.txt successfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+2.可以在本地计算机中查到新名称文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 显示查找的文件不包含指定字段 （</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Didn't found file named with alonso on file D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2. 重命名失败</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -9260,7 +9674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -9320,7 +9734,7 @@
         <v>21</v>
       </c>
       <c r="C3" s="58" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>23</v>
@@ -9329,7 +9743,7 @@
         <v>103</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>26</v>
@@ -9361,7 +9775,7 @@
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E5" s="56"/>
       <c r="F5" s="2" t="s">
@@ -9397,13 +9811,13 @@
       <c r="B7" s="59"/>
       <c r="C7" s="59"/>
       <c r="D7" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E7" s="52" t="s">
         <v>302</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="F7" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>304</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="18"/>
@@ -9415,7 +9829,7 @@
       <c r="B8" s="60"/>
       <c r="C8" s="60"/>
       <c r="D8" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>104</v>
@@ -9506,22 +9920,22 @@
         <v>10.1</v>
       </c>
       <c r="B3" s="70" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="70" t="s">
         <v>167</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="D3" s="70" t="s">
         <v>168</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="E3" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>170</v>
-      </c>
       <c r="F3" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -9533,13 +9947,13 @@
       <c r="C4" s="70"/>
       <c r="D4" s="70"/>
       <c r="E4" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -9551,13 +9965,13 @@
       <c r="C5" s="70"/>
       <c r="D5" s="70"/>
       <c r="E5" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -9569,13 +9983,13 @@
       <c r="C6" s="70"/>
       <c r="D6" s="70"/>
       <c r="E6" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H6" s="5"/>
     </row>
@@ -9587,13 +10001,13 @@
       <c r="C7" s="70"/>
       <c r="D7" s="70"/>
       <c r="E7" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H7" s="5"/>
     </row>
@@ -9605,13 +10019,13 @@
       <c r="C8" s="70"/>
       <c r="D8" s="70"/>
       <c r="E8" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H8" s="5"/>
     </row>
@@ -9623,13 +10037,13 @@
       <c r="C9" s="70"/>
       <c r="D9" s="70"/>
       <c r="E9" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H9" s="5"/>
     </row>
@@ -9641,13 +10055,13 @@
       <c r="C10" s="70"/>
       <c r="D10" s="70"/>
       <c r="E10" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H10" s="5"/>
     </row>
@@ -9659,26 +10073,26 @@
       <c r="C11" s="70"/>
       <c r="D11" s="70"/>
       <c r="E11" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>301</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A12" s="53" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B12" s="70"/>
       <c r="C12" s="70"/>
       <c r="D12" s="70"/>
       <c r="E12" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>25</v>
@@ -9693,13 +10107,13 @@
       <c r="C13" s="70"/>
       <c r="D13" s="70"/>
       <c r="E13" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H13" s="5"/>
     </row>
@@ -9711,13 +10125,13 @@
       <c r="C14" s="70"/>
       <c r="D14" s="70"/>
       <c r="E14" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>179</v>
-      </c>
       <c r="G14" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H14" s="5"/>
     </row>
@@ -9795,19 +10209,19 @@
         <v>11.1</v>
       </c>
       <c r="B3" s="58" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="58" t="s">
         <v>284</v>
       </c>
-      <c r="C3" s="58" t="s">
-        <v>285</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E3" s="55" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -9821,11 +10235,11 @@
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E4" s="57"/>
       <c r="F4" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>25</v>
@@ -9839,13 +10253,13 @@
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E5" s="55" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>25</v>
@@ -9859,11 +10273,11 @@
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
       <c r="D6" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E6" s="57"/>
       <c r="F6" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>25</v>
@@ -9877,7 +10291,7 @@
       <c r="B7" s="60"/>
       <c r="C7" s="60"/>
       <c r="D7" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>104</v>
@@ -9963,13 +10377,13 @@
     </row>
     <row r="3" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B3" s="58" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -9978,7 +10392,7 @@
         <v>73</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>30</v>
@@ -9987,18 +10401,18 @@
     </row>
     <row r="4" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>25</v>
@@ -10007,12 +10421,12 @@
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>73</v>
@@ -10027,12 +10441,12 @@
     </row>
     <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A6" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
       <c r="D6" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>108</v>
@@ -10085,13 +10499,13 @@
     </row>
     <row r="9" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B9" s="58" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
@@ -10100,7 +10514,7 @@
         <v>107</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>25</v>
@@ -10110,7 +10524,7 @@
     </row>
     <row r="10" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B10" s="59"/>
       <c r="C10" s="59"/>
@@ -10121,7 +10535,7 @@
         <v>94</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>72</v>
@@ -10133,12 +10547,12 @@
     </row>
     <row r="11" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11" s="59"/>
       <c r="C11" s="59"/>
       <c r="D11" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>93</v>
@@ -10154,12 +10568,12 @@
     </row>
     <row r="12" spans="1:9" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B12" s="60"/>
       <c r="C12" s="60"/>
       <c r="D12" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>108</v>
@@ -10331,22 +10745,22 @@
     </row>
     <row r="3" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B3" s="58" t="s">
         <v>91</v>
       </c>
       <c r="C3" s="58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E3" s="55" t="s">
         <v>95</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -10355,16 +10769,16 @@
     </row>
     <row r="4" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E4" s="56"/>
       <c r="F4" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>25</v>
@@ -10373,12 +10787,12 @@
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E5" s="56"/>
       <c r="F5" s="2" t="s">
@@ -10391,16 +10805,16 @@
     </row>
     <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
       <c r="D6" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E6" s="56"/>
       <c r="F6" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>25</v>
@@ -10409,16 +10823,16 @@
     </row>
     <row r="7" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B7" s="59"/>
       <c r="C7" s="59"/>
       <c r="D7" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E7" s="56"/>
       <c r="F7" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>32</v>
@@ -10427,16 +10841,16 @@
     </row>
     <row r="8" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
       <c r="D8" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E8" s="56"/>
       <c r="F8" s="19" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>37</v>
@@ -10445,16 +10859,16 @@
     </row>
     <row r="9" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B9" s="59"/>
       <c r="C9" s="59"/>
       <c r="D9" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E9" s="56"/>
       <c r="F9" s="19" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>25</v>
@@ -10463,30 +10877,30 @@
     </row>
     <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A10" s="35" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B10" s="59"/>
       <c r="C10" s="59"/>
       <c r="D10" s="35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E10" s="57"/>
       <c r="F10" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="G10" s="37" t="s">
         <v>212</v>
-      </c>
-      <c r="G10" s="37" t="s">
-        <v>213</v>
       </c>
       <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B11" s="59"/>
       <c r="C11" s="59"/>
       <c r="D11" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>108</v>
@@ -10501,18 +10915,18 @@
     </row>
     <row r="12" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B12" s="60"/>
       <c r="C12" s="60"/>
       <c r="D12" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G12" s="21" t="s">
         <v>25</v>
@@ -10547,22 +10961,22 @@
     </row>
     <row r="16" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A16" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B16" s="58" t="s">
         <v>92</v>
       </c>
       <c r="C16" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E16" s="55" t="s">
         <v>96</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G16" s="14" t="s">
         <v>25</v>
@@ -10571,12 +10985,12 @@
     </row>
     <row r="17" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A17" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B17" s="59"/>
       <c r="C17" s="59"/>
       <c r="D17" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E17" s="56"/>
       <c r="F17" s="14" t="s">
@@ -10589,7 +11003,7 @@
     </row>
     <row r="18" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A18" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B18" s="59"/>
       <c r="C18" s="59"/>
@@ -10598,7 +11012,7 @@
       </c>
       <c r="E18" s="56"/>
       <c r="F18" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>25</v>
@@ -10607,12 +11021,12 @@
     </row>
     <row r="19" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A19" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B19" s="59"/>
       <c r="C19" s="59"/>
       <c r="D19" s="14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E19" s="56"/>
       <c r="F19" s="14" t="s">
@@ -10625,16 +11039,16 @@
     </row>
     <row r="20" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A20" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B20" s="59"/>
       <c r="C20" s="59"/>
       <c r="D20" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E20" s="56"/>
       <c r="F20" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>25</v>
@@ -10643,25 +11057,25 @@
     </row>
     <row r="21" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A21" s="35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B21" s="59"/>
       <c r="C21" s="59"/>
       <c r="D21" s="35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E21" s="57"/>
       <c r="F21" s="36" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H21" s="37"/>
     </row>
     <row r="22" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B22" s="59"/>
       <c r="C22" s="59"/>
@@ -10681,18 +11095,18 @@
     </row>
     <row r="23" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A23" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B23" s="60"/>
       <c r="C23" s="60"/>
       <c r="D23" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G23" s="21" t="s">
         <v>25</v>
@@ -10773,22 +11187,22 @@
     </row>
     <row r="3" spans="1:8" s="23" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B3" s="64" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3" s="64" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E3" s="67" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>35</v>
@@ -10797,12 +11211,12 @@
     </row>
     <row r="4" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B4" s="65"/>
       <c r="C4" s="65"/>
       <c r="D4" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E4" s="68"/>
       <c r="F4" s="6" t="s">
@@ -10815,7 +11229,7 @@
     </row>
     <row r="5" spans="1:8" s="23" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B5" s="65"/>
       <c r="C5" s="65"/>
@@ -10824,7 +11238,7 @@
       </c>
       <c r="E5" s="68"/>
       <c r="F5" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>34</v>
@@ -10833,12 +11247,12 @@
     </row>
     <row r="6" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B6" s="65"/>
       <c r="C6" s="65"/>
       <c r="D6" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E6" s="68"/>
       <c r="F6" s="6" t="s">
@@ -10851,16 +11265,16 @@
     </row>
     <row r="7" spans="1:8" s="23" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="29" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B7" s="65"/>
       <c r="C7" s="65"/>
       <c r="D7" s="29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E7" s="68"/>
       <c r="F7" s="29" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G7" s="30" t="s">
         <v>61</v>
@@ -10869,30 +11283,30 @@
     </row>
     <row r="8" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A8" s="38" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B8" s="65"/>
       <c r="C8" s="65"/>
       <c r="D8" s="35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E8" s="69"/>
       <c r="F8" s="36" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H8" s="40"/>
     </row>
     <row r="9" spans="1:8" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A9" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B9" s="65"/>
       <c r="C9" s="65"/>
       <c r="D9" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>110</v>
@@ -10907,18 +11321,18 @@
     </row>
     <row r="10" spans="1:8" s="33" customFormat="1" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A10" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B10" s="66"/>
       <c r="C10" s="66"/>
       <c r="D10" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>25</v>
@@ -10962,22 +11376,22 @@
     </row>
     <row r="13" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B13" s="58" t="s">
+        <v>189</v>
+      </c>
+      <c r="C13" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="C13" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="E13" s="55" t="s">
         <v>109</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>25</v>
@@ -10986,16 +11400,16 @@
     </row>
     <row r="14" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B14" s="59"/>
       <c r="C14" s="65"/>
       <c r="D14" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E14" s="56"/>
       <c r="F14" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>25</v>
@@ -11004,12 +11418,12 @@
     </row>
     <row r="15" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B15" s="59"/>
       <c r="C15" s="65"/>
       <c r="D15" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E15" s="56"/>
       <c r="F15" s="2" t="s">
@@ -11022,7 +11436,7 @@
     </row>
     <row r="16" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B16" s="59"/>
       <c r="C16" s="65"/>
@@ -11031,7 +11445,7 @@
       </c>
       <c r="E16" s="56"/>
       <c r="F16" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>25</v>
@@ -11040,12 +11454,12 @@
     </row>
     <row r="17" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B17" s="59"/>
       <c r="C17" s="65"/>
       <c r="D17" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E17" s="56"/>
       <c r="F17" s="2" t="s">
@@ -11058,12 +11472,12 @@
     </row>
     <row r="18" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B18" s="59"/>
       <c r="C18" s="65"/>
       <c r="D18" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E18" s="56"/>
       <c r="F18" s="11" t="s">
@@ -11076,12 +11490,12 @@
     </row>
     <row r="19" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B19" s="59"/>
       <c r="C19" s="65"/>
       <c r="D19" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E19" s="56"/>
       <c r="F19" s="11" t="s">
@@ -11094,30 +11508,30 @@
     </row>
     <row r="20" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A20" s="35" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B20" s="59"/>
       <c r="C20" s="65"/>
       <c r="D20" s="35" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E20" s="57"/>
       <c r="F20" s="36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G20" s="41" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H20" s="42"/>
     </row>
     <row r="21" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A21" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B21" s="59"/>
       <c r="C21" s="65"/>
       <c r="D21" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>110</v>
@@ -11132,18 +11546,18 @@
     </row>
     <row r="22" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B22" s="60"/>
       <c r="C22" s="66"/>
       <c r="D22" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E22" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="F22" s="20" t="s">
         <v>125</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>126</v>
       </c>
       <c r="G22" s="21" t="s">
         <v>25</v>
@@ -11230,13 +11644,13 @@
         <v>12</v>
       </c>
       <c r="C3" s="58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="55" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>100</v>
@@ -11253,7 +11667,7 @@
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E4" s="56"/>
       <c r="F4" s="2" t="s">
@@ -11271,7 +11685,7 @@
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E5" s="56"/>
       <c r="F5" s="2" t="s">
@@ -11289,11 +11703,11 @@
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
       <c r="D6" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E6" s="57"/>
       <c r="F6" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>31</v>
@@ -11307,16 +11721,16 @@
       <c r="B7" s="59"/>
       <c r="C7" s="59"/>
       <c r="D7" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E7" s="52" t="s">
         <v>302</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="F7" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>305</v>
       </c>
       <c r="H7" s="13"/>
     </row>
@@ -11327,7 +11741,7 @@
       <c r="B8" s="60"/>
       <c r="C8" s="60"/>
       <c r="D8" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>104</v>
@@ -11422,16 +11836,16 @@
         <v>15</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E3" s="55" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -11449,7 +11863,7 @@
       </c>
       <c r="E4" s="56"/>
       <c r="F4" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>31</v>
@@ -11463,7 +11877,7 @@
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="D5" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E5" s="57"/>
       <c r="F5" s="2" t="s">
@@ -11481,16 +11895,16 @@
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="D6" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E6" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="E6" s="28" t="s">
-        <v>232</v>
-      </c>
       <c r="F6" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H6" s="6"/>
     </row>
@@ -11501,7 +11915,7 @@
       <c r="B7" s="44"/>
       <c r="C7" s="44"/>
       <c r="D7" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>104</v>
@@ -11586,13 +12000,13 @@
     </row>
     <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B3" s="58" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>65</v>
@@ -11601,7 +12015,7 @@
         <v>97</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>29</v>
@@ -11610,12 +12024,12 @@
     </row>
     <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E4" s="56"/>
       <c r="F4" s="2" t="s">
@@ -11628,12 +12042,12 @@
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E5" s="56"/>
       <c r="F5" s="2" t="s">
@@ -11646,7 +12060,7 @@
     </row>
     <row r="6" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -11664,12 +12078,12 @@
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60"/>
       <c r="D7" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>108</v>
@@ -11710,7 +12124,7 @@
     </row>
     <row r="10" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B10" s="58" t="s">
         <v>18</v>
@@ -11725,7 +12139,7 @@
         <v>98</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>25</v>
@@ -11734,16 +12148,16 @@
     </row>
     <row r="11" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B11" s="59"/>
       <c r="C11" s="59"/>
       <c r="D11" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E11" s="56"/>
       <c r="F11" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>25</v>
@@ -11752,12 +12166,12 @@
     </row>
     <row r="12" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B12" s="59"/>
       <c r="C12" s="59"/>
       <c r="D12" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E12" s="56"/>
       <c r="F12" s="2" t="s">
@@ -11770,7 +12184,7 @@
     </row>
     <row r="13" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B13" s="59"/>
       <c r="C13" s="59"/>
@@ -11788,12 +12202,12 @@
     </row>
     <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A14" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B14" s="60"/>
       <c r="C14" s="60"/>
       <c r="D14" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>108</v>
@@ -11824,9 +12238,9 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -11885,22 +12299,22 @@
         <v>19</v>
       </c>
       <c r="C3" s="58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E3" s="55" t="s">
-        <v>111</v>
+        <v>308</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
@@ -11928,7 +12342,7 @@
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E5" s="57"/>
       <c r="F5" s="2" t="s">
@@ -11939,36 +12353,93 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A6" s="27">
+    <row r="6" spans="1:8" ht="114" x14ac:dyDescent="0.15">
+      <c r="A6" s="22">
         <v>8.4</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="E6" s="20" t="s">
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E6" s="55" t="s">
+        <v>309</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+      <c r="A7" s="22">
+        <v>8.5</v>
+      </c>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E7" s="56"/>
+      <c r="F7" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" ht="57" x14ac:dyDescent="0.15">
+      <c r="A8" s="22">
+        <v>8.6</v>
+      </c>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="E8" s="57"/>
+      <c r="F8" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A9" s="27">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E9" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F9" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G9" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="H6" s="21"/>
-    </row>
-    <row r="8" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A8" s="9"/>
-      <c r="B8" s="8"/>
+      <c r="H9" s="21"/>
+    </row>
+    <row r="11" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A11" s="9"/>
+      <c r="B11" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E5"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="C3:C9"/>
+    <mergeCell ref="E6:E8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update the test cases file of FileOperation as #27 fixed
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="316">
   <si>
     <t>删除文件夹</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -5377,94 +5377,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>文件夹名</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What file or folder you want to find on this folder?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入文件夹名，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>McLaren</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -8920,6 +8832,165 @@
   </si>
   <si>
     <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">文件路径
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What file or folder you want to find on this folder?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入文件夹名，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>McLaren</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test9\123.txt</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -9153,7 +9224,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -9314,6 +9385,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -9674,7 +9748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -9691,14 +9765,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="54"/>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -9730,20 +9804,20 @@
       <c r="A3" s="22">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="59" t="s">
         <v>111</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="56" t="s">
         <v>103</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>26</v>
@@ -9754,12 +9828,12 @@
       <c r="A4" s="22">
         <v>1.2</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
       <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="56"/>
+      <c r="E4" s="57"/>
       <c r="F4" s="2" t="s">
         <v>101</v>
       </c>
@@ -9772,12 +9846,12 @@
       <c r="A5" s="22">
         <v>1.3</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
       <c r="D5" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="E5" s="56"/>
+        <v>260</v>
+      </c>
+      <c r="E5" s="57"/>
       <c r="F5" s="2" t="s">
         <v>80</v>
       </c>
@@ -9790,12 +9864,12 @@
       <c r="A6" s="22">
         <v>1.4</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
       <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="57"/>
+      <c r="E6" s="58"/>
       <c r="F6" s="2" t="s">
         <v>79</v>
       </c>
@@ -9808,16 +9882,16 @@
       <c r="A7" s="22">
         <v>1.5</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E7" s="52" t="s">
         <v>301</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="F7" s="2" t="s">
         <v>302</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>303</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="18"/>
@@ -9826,8 +9900,8 @@
       <c r="A8" s="27">
         <v>1.6</v>
       </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
       <c r="D8" s="20" t="s">
         <v>150</v>
       </c>
@@ -9880,14 +9954,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="63"/>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="45" t="s">
@@ -9919,13 +9993,13 @@
       <c r="A3" s="46">
         <v>10.1</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="71" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="71" t="s">
         <v>167</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="71" t="s">
         <v>168</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -9943,9 +10017,9 @@
       <c r="A4" s="46">
         <v>10.199999999999999</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
       <c r="E4" s="2" t="s">
         <v>170</v>
       </c>
@@ -9961,9 +10035,9 @@
       <c r="A5" s="46">
         <v>10.3</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
       <c r="E5" s="2" t="s">
         <v>171</v>
       </c>
@@ -9979,9 +10053,9 @@
       <c r="A6" s="46">
         <v>10.4</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
       <c r="E6" s="2" t="s">
         <v>172</v>
       </c>
@@ -9997,9 +10071,9 @@
       <c r="A7" s="46">
         <v>10.5</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="70"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
       <c r="E7" s="2" t="s">
         <v>173</v>
       </c>
@@ -10015,9 +10089,9 @@
       <c r="A8" s="46">
         <v>10.6</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
       <c r="E8" s="2" t="s">
         <v>174</v>
       </c>
@@ -10033,9 +10107,9 @@
       <c r="A9" s="46">
         <v>10.7</v>
       </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="70"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
       <c r="E9" s="2" t="s">
         <v>175</v>
       </c>
@@ -10051,9 +10125,9 @@
       <c r="A10" s="46">
         <v>10.8</v>
       </c>
-      <c r="B10" s="70"/>
-      <c r="C10" s="70"/>
-      <c r="D10" s="70"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
       <c r="E10" s="2" t="s">
         <v>176</v>
       </c>
@@ -10069,30 +10143,30 @@
       <c r="A11" s="46">
         <v>10.9</v>
       </c>
-      <c r="B11" s="70"/>
-      <c r="C11" s="70"/>
-      <c r="D11" s="70"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
       <c r="E11" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>300</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A12" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="B12" s="71"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B12" s="70"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="2" t="s">
-        <v>297</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>25</v>
@@ -10103,11 +10177,11 @@
       <c r="A13" s="48">
         <v>10.11</v>
       </c>
-      <c r="B13" s="70"/>
-      <c r="C13" s="70"/>
-      <c r="D13" s="70"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
       <c r="E13" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>178</v>
@@ -10121,9 +10195,9 @@
       <c r="A14" s="46">
         <v>10.119999999999999</v>
       </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="70"/>
-      <c r="D14" s="70"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
       <c r="E14" s="2" t="s">
         <v>177</v>
       </c>
@@ -10153,7 +10227,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -10169,14 +10243,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="63"/>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10208,20 +10282,20 @@
       <c r="A3" s="22">
         <v>11.1</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="59" t="s">
+        <v>282</v>
+      </c>
+      <c r="C3" s="59" t="s">
         <v>283</v>
       </c>
-      <c r="C3" s="58" t="s">
-        <v>284</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E3" s="55" t="s">
-        <v>292</v>
+        <v>287</v>
+      </c>
+      <c r="E3" s="56" t="s">
+        <v>291</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -10232,14 +10306,14 @@
       <c r="A4" s="49">
         <v>11.2</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
       <c r="D4" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="E4" s="57"/>
+        <v>288</v>
+      </c>
+      <c r="E4" s="58"/>
       <c r="F4" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>25</v>
@@ -10250,16 +10324,16 @@
       <c r="A5" s="49">
         <v>11.3</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
       <c r="D5" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="E5" s="55" t="s">
-        <v>293</v>
+        <v>285</v>
+      </c>
+      <c r="E5" s="56" t="s">
+        <v>292</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>25</v>
@@ -10270,14 +10344,14 @@
       <c r="A6" s="50">
         <v>11.4</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
       <c r="D6" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="E6" s="57"/>
+        <v>286</v>
+      </c>
+      <c r="E6" s="58"/>
       <c r="F6" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>25</v>
@@ -10288,8 +10362,8 @@
       <c r="A7" s="51">
         <v>11.5</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="20" t="s">
         <v>150</v>
       </c>
@@ -10322,7 +10396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -10340,14 +10414,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="54"/>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10379,10 +10453,10 @@
       <c r="A3" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="59" t="s">
         <v>112</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -10392,7 +10466,7 @@
         <v>73</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>30</v>
@@ -10403,16 +10477,16 @@
       <c r="A4" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
       <c r="D4" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>25</v>
@@ -10423,10 +10497,10 @@
       <c r="A5" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
       <c r="D5" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>73</v>
@@ -10443,8 +10517,8 @@
       <c r="A6" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="20" t="s">
         <v>150</v>
       </c>
@@ -10501,10 +10575,10 @@
       <c r="A9" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="59" t="s">
         <v>112</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -10514,7 +10588,7 @@
         <v>107</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>25</v>
@@ -10526,8 +10600,8 @@
       <c r="A10" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
       <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
@@ -10535,7 +10609,7 @@
         <v>94</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>72</v>
@@ -10549,10 +10623,10 @@
       <c r="A11" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
       <c r="D11" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>93</v>
@@ -10570,8 +10644,8 @@
       <c r="A12" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
       <c r="D12" s="20" t="s">
         <v>150</v>
       </c>
@@ -10588,7 +10662,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
-      <c r="B13" s="61"/>
+      <c r="B13" s="62"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -10599,7 +10673,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
-      <c r="B14" s="61"/>
+      <c r="B14" s="62"/>
       <c r="C14" s="4"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -10610,7 +10684,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
-      <c r="B15" s="61"/>
+      <c r="B15" s="62"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -10621,7 +10695,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
-      <c r="B16" s="61"/>
+      <c r="B16" s="62"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -10632,7 +10706,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
-      <c r="B17" s="61"/>
+      <c r="B17" s="62"/>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -10708,14 +10782,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A1" s="62"/>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10747,20 +10821,20 @@
       <c r="A3" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="59" t="s">
         <v>114</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="E3" s="55" t="s">
+        <v>267</v>
+      </c>
+      <c r="E3" s="56" t="s">
         <v>95</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -10771,14 +10845,14 @@
       <c r="A4" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
       <c r="D4" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="E4" s="56"/>
+        <v>268</v>
+      </c>
+      <c r="E4" s="57"/>
       <c r="F4" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>25</v>
@@ -10789,12 +10863,12 @@
       <c r="A5" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
       <c r="D5" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="E5" s="56"/>
+        <v>269</v>
+      </c>
+      <c r="E5" s="57"/>
       <c r="F5" s="2" t="s">
         <v>83</v>
       </c>
@@ -10807,14 +10881,14 @@
       <c r="A6" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
       <c r="D6" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E6" s="56"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>25</v>
@@ -10825,12 +10899,12 @@
       <c r="A7" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="E7" s="56"/>
+        <v>270</v>
+      </c>
+      <c r="E7" s="57"/>
       <c r="F7" s="2" t="s">
         <v>210</v>
       </c>
@@ -10843,14 +10917,14 @@
       <c r="A8" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
       <c r="D8" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E8" s="56"/>
+      <c r="E8" s="57"/>
       <c r="F8" s="19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>37</v>
@@ -10861,14 +10935,14 @@
       <c r="A9" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
       <c r="D9" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="E9" s="56"/>
+      <c r="E9" s="57"/>
       <c r="F9" s="19" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>25</v>
@@ -10879,12 +10953,12 @@
       <c r="A10" s="35" t="s">
         <v>213</v>
       </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
       <c r="D10" s="35" t="s">
         <v>217</v>
       </c>
-      <c r="E10" s="57"/>
+      <c r="E10" s="58"/>
       <c r="F10" s="36" t="s">
         <v>211</v>
       </c>
@@ -10897,8 +10971,8 @@
       <c r="A11" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
       <c r="D11" s="20" t="s">
         <v>150</v>
       </c>
@@ -10917,8 +10991,8 @@
       <c r="A12" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
       <c r="D12" s="20" t="s">
         <v>151</v>
       </c>
@@ -10963,20 +11037,20 @@
       <c r="A16" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="58" t="s">
+      <c r="C16" s="59" t="s">
         <v>113</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="E16" s="55" t="s">
+      <c r="E16" s="56" t="s">
         <v>96</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G16" s="14" t="s">
         <v>25</v>
@@ -10987,12 +11061,12 @@
       <c r="A17" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="B17" s="59"/>
-      <c r="C17" s="59"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="60"/>
       <c r="D17" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="E17" s="56"/>
+        <v>271</v>
+      </c>
+      <c r="E17" s="57"/>
       <c r="F17" s="14" t="s">
         <v>82</v>
       </c>
@@ -11005,14 +11079,14 @@
       <c r="A18" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
       <c r="D18" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="56"/>
+      <c r="E18" s="57"/>
       <c r="F18" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>25</v>
@@ -11023,12 +11097,12 @@
       <c r="A19" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="60"/>
       <c r="D19" s="14" t="s">
-        <v>273</v>
-      </c>
-      <c r="E19" s="56"/>
+        <v>272</v>
+      </c>
+      <c r="E19" s="57"/>
       <c r="F19" s="14" t="s">
         <v>81</v>
       </c>
@@ -11041,14 +11115,14 @@
       <c r="A20" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="B20" s="59"/>
-      <c r="C20" s="59"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="60"/>
       <c r="D20" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="E20" s="56"/>
+      <c r="E20" s="57"/>
       <c r="F20" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>25</v>
@@ -11059,12 +11133,12 @@
       <c r="A21" s="35" t="s">
         <v>218</v>
       </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="59"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="60"/>
       <c r="D21" s="35" t="s">
         <v>216</v>
       </c>
-      <c r="E21" s="57"/>
+      <c r="E21" s="58"/>
       <c r="F21" s="36" t="s">
         <v>220</v>
       </c>
@@ -11077,8 +11151,8 @@
       <c r="A22" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="B22" s="59"/>
-      <c r="C22" s="59"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="60"/>
       <c r="D22" s="20" t="s">
         <v>102</v>
       </c>
@@ -11097,8 +11171,8 @@
       <c r="A23" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
       <c r="D23" s="20" t="s">
         <v>151</v>
       </c>
@@ -11150,14 +11224,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="63"/>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11189,20 +11263,20 @@
       <c r="A3" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="65" t="s">
         <v>188</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="65" t="s">
         <v>115</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="E3" s="67" t="s">
+        <v>273</v>
+      </c>
+      <c r="E3" s="68" t="s">
         <v>122</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>35</v>
@@ -11213,12 +11287,12 @@
       <c r="A4" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
       <c r="D4" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="E4" s="68"/>
+        <v>274</v>
+      </c>
+      <c r="E4" s="69"/>
       <c r="F4" s="6" t="s">
         <v>84</v>
       </c>
@@ -11231,14 +11305,14 @@
       <c r="A5" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
       <c r="D5" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="68"/>
+      <c r="E5" s="69"/>
       <c r="F5" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>34</v>
@@ -11249,12 +11323,12 @@
       <c r="A6" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="E6" s="68"/>
+        <v>275</v>
+      </c>
+      <c r="E6" s="69"/>
       <c r="F6" s="6" t="s">
         <v>84</v>
       </c>
@@ -11267,14 +11341,14 @@
       <c r="A7" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="B7" s="65"/>
-      <c r="C7" s="65"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
       <c r="D7" s="29" t="s">
         <v>192</v>
       </c>
-      <c r="E7" s="68"/>
+      <c r="E7" s="69"/>
       <c r="F7" s="29" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G7" s="30" t="s">
         <v>61</v>
@@ -11285,12 +11359,12 @@
       <c r="A8" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="66"/>
       <c r="D8" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="E8" s="69"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="36" t="s">
         <v>228</v>
       </c>
@@ -11303,8 +11377,8 @@
       <c r="A9" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="B9" s="65"/>
-      <c r="C9" s="65"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="66"/>
       <c r="D9" s="20" t="s">
         <v>150</v>
       </c>
@@ -11323,8 +11397,8 @@
       <c r="A10" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="66"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
       <c r="D10" s="20" t="s">
         <v>151</v>
       </c>
@@ -11378,20 +11452,20 @@
       <c r="A13" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="59" t="s">
         <v>189</v>
       </c>
-      <c r="C13" s="64" t="s">
+      <c r="C13" s="65" t="s">
         <v>115</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E13" s="55" t="s">
+      <c r="E13" s="56" t="s">
         <v>109</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>25</v>
@@ -11402,14 +11476,14 @@
       <c r="A14" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="65"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="66"/>
       <c r="D14" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="E14" s="56"/>
+      <c r="E14" s="57"/>
       <c r="F14" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>25</v>
@@ -11420,12 +11494,12 @@
       <c r="A15" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="65"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="66"/>
       <c r="D15" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="E15" s="56"/>
+        <v>276</v>
+      </c>
+      <c r="E15" s="57"/>
       <c r="F15" s="2" t="s">
         <v>86</v>
       </c>
@@ -11438,14 +11512,14 @@
       <c r="A16" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B16" s="59"/>
-      <c r="C16" s="65"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="66"/>
       <c r="D16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="56"/>
+      <c r="E16" s="57"/>
       <c r="F16" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>25</v>
@@ -11456,12 +11530,12 @@
       <c r="A17" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="B17" s="59"/>
-      <c r="C17" s="65"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="66"/>
       <c r="D17" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E17" s="56"/>
+        <v>277</v>
+      </c>
+      <c r="E17" s="57"/>
       <c r="F17" s="2" t="s">
         <v>85</v>
       </c>
@@ -11474,12 +11548,12 @@
       <c r="A18" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="65"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="66"/>
       <c r="D18" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="E18" s="56"/>
+      <c r="E18" s="57"/>
       <c r="F18" s="11" t="s">
         <v>76</v>
       </c>
@@ -11492,12 +11566,12 @@
       <c r="A19" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="B19" s="59"/>
-      <c r="C19" s="65"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="66"/>
       <c r="D19" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="E19" s="56"/>
+      <c r="E19" s="57"/>
       <c r="F19" s="11" t="s">
         <v>76</v>
       </c>
@@ -11510,12 +11584,12 @@
       <c r="A20" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="B20" s="59"/>
-      <c r="C20" s="65"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="66"/>
       <c r="D20" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="E20" s="57"/>
+      <c r="E20" s="58"/>
       <c r="F20" s="36" t="s">
         <v>224</v>
       </c>
@@ -11528,8 +11602,8 @@
       <c r="A21" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="65"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="66"/>
       <c r="D21" s="20" t="s">
         <v>150</v>
       </c>
@@ -11548,8 +11622,8 @@
       <c r="A22" s="20" t="s">
         <v>221</v>
       </c>
-      <c r="B22" s="60"/>
-      <c r="C22" s="66"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="67"/>
       <c r="D22" s="20" t="s">
         <v>151</v>
       </c>
@@ -11601,14 +11675,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="63"/>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11640,17 +11714,17 @@
       <c r="A3" s="22">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="59" t="s">
         <v>116</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="55" t="s">
-        <v>236</v>
+      <c r="E3" s="56" t="s">
+        <v>235</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>100</v>
@@ -11664,12 +11738,12 @@
       <c r="A4" s="22">
         <v>5.2</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
       <c r="D4" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="E4" s="56"/>
+        <v>261</v>
+      </c>
+      <c r="E4" s="57"/>
       <c r="F4" s="2" t="s">
         <v>99</v>
       </c>
@@ -11682,12 +11756,12 @@
       <c r="A5" s="22">
         <v>5.3</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
       <c r="D5" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E5" s="56"/>
+        <v>278</v>
+      </c>
+      <c r="E5" s="57"/>
       <c r="F5" s="2" t="s">
         <v>87</v>
       </c>
@@ -11700,14 +11774,14 @@
       <c r="A6" s="22">
         <v>5.4</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
       <c r="D6" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="E6" s="57"/>
+        <v>234</v>
+      </c>
+      <c r="E6" s="58"/>
       <c r="F6" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>31</v>
@@ -11718,19 +11792,19 @@
       <c r="A7" s="22">
         <v>5.5</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E7" s="52" t="s">
         <v>301</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="F7" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>304</v>
       </c>
       <c r="H7" s="13"/>
     </row>
@@ -11738,8 +11812,8 @@
       <c r="A8" s="27">
         <v>5.6</v>
       </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
       <c r="D8" s="20" t="s">
         <v>150</v>
       </c>
@@ -11775,10 +11849,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -11787,20 +11861,20 @@
     <col min="2" max="3" width="12.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.375" customWidth="1"/>
     <col min="5" max="5" width="30.125" customWidth="1"/>
-    <col min="6" max="6" width="28.875" customWidth="1"/>
+    <col min="6" max="6" width="31.125" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="63"/>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11841,11 +11915,11 @@
       <c r="D3" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="E3" s="55" t="s">
-        <v>285</v>
+      <c r="E3" s="56" t="s">
+        <v>284</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -11861,9 +11935,9 @@
       <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="56"/>
+      <c r="E4" s="57"/>
       <c r="F4" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>31</v>
@@ -11877,9 +11951,9 @@
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="D5" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="E5" s="57"/>
+        <v>262</v>
+      </c>
+      <c r="E5" s="58"/>
       <c r="F5" s="2" t="s">
         <v>88</v>
       </c>
@@ -11898,38 +11972,56 @@
         <v>230</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>231</v>
+        <v>314</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>152</v>
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A7" s="27">
+    <row r="7" spans="1:8" ht="114" x14ac:dyDescent="0.15">
+      <c r="A7" s="24">
         <v>6.5</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="20" t="s">
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>315</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A8" s="27">
+        <v>6.6</v>
+      </c>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E8" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F8" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G8" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="H7" s="21"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B10" s="8"/>
+      <c r="H8" s="21"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B11" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -11947,7 +12039,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -11963,14 +12055,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="63"/>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -12002,20 +12094,20 @@
       <c r="A3" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="59" t="s">
         <v>118</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="56" t="s">
         <v>97</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>29</v>
@@ -12026,12 +12118,12 @@
       <c r="A4" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
       <c r="D4" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E4" s="56"/>
+        <v>263</v>
+      </c>
+      <c r="E4" s="57"/>
       <c r="F4" s="2" t="s">
         <v>62</v>
       </c>
@@ -12044,12 +12136,12 @@
       <c r="A5" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
       <c r="D5" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="E5" s="56"/>
+        <v>262</v>
+      </c>
+      <c r="E5" s="57"/>
       <c r="F5" s="2" t="s">
         <v>89</v>
       </c>
@@ -12062,12 +12154,12 @@
       <c r="A6" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
       <c r="D6" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="57"/>
+      <c r="E6" s="58"/>
       <c r="F6" s="6" t="s">
         <v>63</v>
       </c>
@@ -12080,8 +12172,8 @@
       <c r="A7" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="20" t="s">
         <v>150</v>
       </c>
@@ -12126,20 +12218,20 @@
       <c r="A10" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="59" t="s">
         <v>75</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="55" t="s">
+      <c r="E10" s="56" t="s">
         <v>98</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>25</v>
@@ -12150,12 +12242,12 @@
       <c r="A11" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
       <c r="D11" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="E11" s="56"/>
+        <v>264</v>
+      </c>
+      <c r="E11" s="57"/>
       <c r="F11" s="2" t="s">
         <v>153</v>
       </c>
@@ -12168,12 +12260,12 @@
       <c r="A12" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
       <c r="D12" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="E12" s="56"/>
+        <v>265</v>
+      </c>
+      <c r="E12" s="57"/>
       <c r="F12" s="2" t="s">
         <v>67</v>
       </c>
@@ -12186,12 +12278,12 @@
       <c r="A13" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="60"/>
       <c r="D13" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="57"/>
+      <c r="E13" s="58"/>
       <c r="F13" s="6" t="s">
         <v>70</v>
       </c>
@@ -12204,8 +12296,8 @@
       <c r="A14" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
       <c r="D14" s="20" t="s">
         <v>150</v>
       </c>
@@ -12240,7 +12332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -12256,14 +12348,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="63"/>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -12295,20 +12387,20 @@
       <c r="A3" s="22">
         <v>8.1</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="59" t="s">
         <v>119</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E3" s="55" t="s">
-        <v>308</v>
+      <c r="E3" s="56" t="s">
+        <v>307</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -12321,12 +12413,12 @@
       <c r="A4" s="22">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
       <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="56"/>
+      <c r="E4" s="57"/>
       <c r="F4" s="2" t="s">
         <v>52</v>
       </c>
@@ -12339,12 +12431,12 @@
       <c r="A5" s="22">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
       <c r="D5" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="E5" s="57"/>
+        <v>266</v>
+      </c>
+      <c r="E5" s="58"/>
       <c r="F5" s="2" t="s">
         <v>90</v>
       </c>
@@ -12357,19 +12449,19 @@
       <c r="A6" s="22">
         <v>8.4</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
       <c r="D6" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="E6" s="55" t="s">
-        <v>309</v>
+        <v>305</v>
+      </c>
+      <c r="E6" s="56" t="s">
+        <v>308</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -12377,17 +12469,17 @@
       <c r="A7" s="22">
         <v>8.5</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="E7" s="56"/>
+        <v>306</v>
+      </c>
+      <c r="E7" s="57"/>
       <c r="F7" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>312</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>313</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -12395,17 +12487,17 @@
       <c r="A8" s="22">
         <v>8.6</v>
       </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
       <c r="D8" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E8" s="57"/>
+        <v>304</v>
+      </c>
+      <c r="E8" s="58"/>
       <c r="F8" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -12413,8 +12505,8 @@
       <c r="A9" s="27">
         <v>8.6999999999999993</v>
       </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
       <c r="D9" s="20" t="s">
         <v>150</v>
       </c>
@@ -12468,14 +12560,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="63"/>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -12507,10 +12599,10 @@
       <c r="A3" s="22">
         <v>9.1</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="59" t="s">
         <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -12519,7 +12611,7 @@
       <c r="E3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="F3" s="59" t="s">
         <v>45</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -12531,15 +12623,15 @@
       <c r="A4" s="22">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
       <c r="D4" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="59"/>
+      <c r="F4" s="60"/>
       <c r="G4" s="2" t="s">
         <v>47</v>
       </c>
@@ -12549,15 +12641,15 @@
       <c r="A5" s="22">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
       <c r="D5" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="59"/>
+      <c r="F5" s="60"/>
       <c r="G5" s="2" t="s">
         <v>47</v>
       </c>
@@ -12567,15 +12659,15 @@
       <c r="A6" s="22">
         <v>9.4</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
       <c r="D6" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="59"/>
+      <c r="F6" s="60"/>
       <c r="G6" s="5" t="s">
         <v>47</v>
       </c>
@@ -12585,15 +12677,15 @@
       <c r="A7" s="22">
         <v>9.5</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="60"/>
+      <c r="F7" s="61"/>
       <c r="G7" s="5" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Update the test case file as judge path function added
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="328">
   <si>
     <t>删除文件夹</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3403,82 +3403,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>E:\Program Files\Test</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入被复制文件夹的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input target folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入空字符串</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -8991,6 +8915,159 @@
       </rPr>
       <t>D:\Test9\123.txt</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示输入需要被复制文件夹或者文件路径时，输入存在路径不带'\'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在提示信息"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"出现时，输入存在路径不带'\'</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.1.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在提示信息"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"出现时，输入一串空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在提示信息"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"出现时，输入存在路径不带'\'</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The format of " D:Test Folder " is incorrect! Should with '\'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.2.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.1.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.2.9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.1.9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.2.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.2.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.1.6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -9224,7 +9301,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -9421,15 +9498,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -9440,6 +9508,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9804,10 +9878,10 @@
       <c r="A3" s="22">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="17" t="s">
         <v>111</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -9817,7 +9891,7 @@
         <v>103</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>26</v>
@@ -9828,8 +9902,8 @@
       <c r="A4" s="22">
         <v>1.2</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
@@ -9846,10 +9920,10 @@
       <c r="A5" s="22">
         <v>1.3</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E5" s="57"/>
       <c r="F5" s="2" t="s">
@@ -9864,8 +9938,8 @@
       <c r="A6" s="22">
         <v>1.4</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
@@ -9882,16 +9956,16 @@
       <c r="A7" s="22">
         <v>1.5</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
       <c r="D7" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E7" s="52" t="s">
         <v>300</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="F7" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>302</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="18"/>
@@ -9900,10 +9974,10 @@
       <c r="A8" s="27">
         <v>1.6</v>
       </c>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
       <c r="D8" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>104</v>
@@ -9915,17 +9989,35 @@
         <v>106</v>
       </c>
       <c r="H8" s="21"/>
+    </row>
+    <row r="9" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A9" s="27">
+        <v>1.7</v>
+      </c>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A10" s="9"/>
       <c r="B10" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E6"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="C3:C8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9993,23 +10085,23 @@
       <c r="A3" s="46">
         <v>10.1</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="68" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" s="68" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="D3" s="68" t="s">
         <v>167</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="E3" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="F3" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -10017,17 +10109,17 @@
       <c r="A4" s="46">
         <v>10.199999999999999</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
       <c r="E4" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -10035,17 +10127,17 @@
       <c r="A5" s="46">
         <v>10.3</v>
       </c>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
       <c r="E5" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -10053,17 +10145,17 @@
       <c r="A6" s="46">
         <v>10.4</v>
       </c>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
       <c r="E6" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H6" s="5"/>
     </row>
@@ -10071,17 +10163,17 @@
       <c r="A7" s="46">
         <v>10.5</v>
       </c>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
       <c r="E7" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H7" s="5"/>
     </row>
@@ -10089,17 +10181,17 @@
       <c r="A8" s="46">
         <v>10.6</v>
       </c>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
       <c r="E8" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H8" s="5"/>
     </row>
@@ -10107,17 +10199,17 @@
       <c r="A9" s="46">
         <v>10.7</v>
       </c>
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
       <c r="E9" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H9" s="5"/>
     </row>
@@ -10125,17 +10217,17 @@
       <c r="A10" s="46">
         <v>10.8</v>
       </c>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
       <c r="E10" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H10" s="5"/>
     </row>
@@ -10143,30 +10235,30 @@
       <c r="A11" s="46">
         <v>10.9</v>
       </c>
-      <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
       <c r="E11" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>299</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A12" s="53" t="s">
+        <v>294</v>
+      </c>
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B12" s="71"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="2" t="s">
-        <v>296</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>25</v>
@@ -10177,17 +10269,17 @@
       <c r="A13" s="48">
         <v>10.11</v>
       </c>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
       <c r="E13" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H13" s="5"/>
     </row>
@@ -10195,17 +10287,17 @@
       <c r="A14" s="46">
         <v>10.119999999999999</v>
       </c>
-      <c r="B14" s="71"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
       <c r="E14" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>178</v>
-      </c>
       <c r="G14" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H14" s="5"/>
     </row>
@@ -10283,19 +10375,19 @@
         <v>11.1</v>
       </c>
       <c r="B3" s="59" t="s">
+        <v>281</v>
+      </c>
+      <c r="C3" s="59" t="s">
         <v>282</v>
       </c>
-      <c r="C3" s="59" t="s">
-        <v>283</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -10309,11 +10401,11 @@
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
       <c r="D4" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E4" s="58"/>
       <c r="F4" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>25</v>
@@ -10327,13 +10419,13 @@
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
       <c r="D5" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E5" s="56" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>25</v>
@@ -10347,11 +10439,11 @@
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
       <c r="D6" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E6" s="58"/>
       <c r="F6" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>25</v>
@@ -10365,7 +10457,7 @@
       <c r="B7" s="61"/>
       <c r="C7" s="61"/>
       <c r="D7" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>104</v>
@@ -10394,7 +10486,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -10451,12 +10543,12 @@
     </row>
     <row r="3" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B3" s="59" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="17" t="s">
         <v>112</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -10466,7 +10558,7 @@
         <v>73</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>30</v>
@@ -10475,18 +10567,18 @@
     </row>
     <row r="4" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
+        <v>126</v>
+      </c>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>25</v>
@@ -10495,12 +10587,12 @@
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
+        <v>127</v>
+      </c>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>73</v>
@@ -10515,15 +10607,15 @@
     </row>
     <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A6" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
+        <v>132</v>
+      </c>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>108</v>
+        <v>318</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>105</v>
@@ -10533,154 +10625,172 @@
       </c>
       <c r="H6" s="21"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+    <row r="7" spans="1:9" ht="57" x14ac:dyDescent="0.15">
+      <c r="A7" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B9" s="59" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="59" t="s">
-        <v>112</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="2"/>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
+        <v>128</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>112</v>
+      </c>
       <c r="D10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>71</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="H10" s="2"/>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A13" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G11" s="2" t="s">
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="H13" s="21"/>
+    </row>
+    <row r="14" spans="1:9" s="23" customFormat="1" ht="57" x14ac:dyDescent="0.15">
+      <c r="A14" s="27" t="s">
+        <v>321</v>
+      </c>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="G14" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A12" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="B12" s="61"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="H12" s="21"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A13" s="3"/>
-      <c r="B13" s="62"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A14" s="3"/>
-      <c r="B14" s="62"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
@@ -10717,8 +10827,8 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="4"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -10728,8 +10838,8 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -10739,7 +10849,8 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
-      <c r="B20" s="10"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -10747,14 +10858,31 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A22" s="3"/>
+      <c r="B22" s="10"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="B15:B19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10764,10 +10892,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -10819,22 +10947,22 @@
     </row>
     <row r="3" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B3" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="17" t="s">
         <v>114</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E3" s="56" t="s">
         <v>95</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -10843,16 +10971,16 @@
     </row>
     <row r="4" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
+        <v>135</v>
+      </c>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E4" s="57"/>
       <c r="F4" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>25</v>
@@ -10861,12 +10989,12 @@
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
+        <v>136</v>
+      </c>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E5" s="57"/>
       <c r="F5" s="2" t="s">
@@ -10879,16 +11007,16 @@
     </row>
     <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
+        <v>137</v>
+      </c>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="2" t="s">
         <v>120</v>
       </c>
       <c r="E6" s="57"/>
       <c r="F6" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>25</v>
@@ -10897,16 +11025,16 @@
     </row>
     <row r="7" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
+        <v>138</v>
+      </c>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
       <c r="D7" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E7" s="57"/>
       <c r="F7" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>32</v>
@@ -10915,16 +11043,16 @@
     </row>
     <row r="8" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
+        <v>139</v>
+      </c>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
       <c r="D8" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E8" s="57"/>
       <c r="F8" s="19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>37</v>
@@ -10933,16 +11061,16 @@
     </row>
     <row r="9" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
+        <v>140</v>
+      </c>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
       <c r="D9" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E9" s="57"/>
       <c r="F9" s="19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>25</v>
@@ -10951,30 +11079,30 @@
     </row>
     <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A10" s="35" t="s">
-        <v>213</v>
-      </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
+        <v>212</v>
+      </c>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
       <c r="D10" s="35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E10" s="58"/>
       <c r="F10" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="G10" s="37" t="s">
         <v>211</v>
-      </c>
-      <c r="G10" s="37" t="s">
-        <v>212</v>
       </c>
       <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
+        <v>213</v>
+      </c>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
       <c r="D11" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>108</v>
@@ -10989,213 +11117,249 @@
     </row>
     <row r="12" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
-        <v>215</v>
-      </c>
-      <c r="B12" s="61"/>
-      <c r="C12" s="61"/>
+        <v>214</v>
+      </c>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>121</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G12" s="21" t="s">
         <v>25</v>
       </c>
       <c r="H12" s="26"/>
     </row>
-    <row r="15" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A15" s="2" t="s">
+    <row r="13" spans="1:8" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A13" s="27" t="s">
+        <v>322</v>
+      </c>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="21"/>
+    </row>
+    <row r="16" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B16" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C16" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F16" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G16" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H16" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="114" x14ac:dyDescent="0.15">
-      <c r="A16" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="B16" s="59" t="s">
+    <row r="17" spans="1:8" ht="114" x14ac:dyDescent="0.15">
+      <c r="A17" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="59" t="s">
+      <c r="C17" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="D16" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="E16" s="56" t="s">
+      <c r="D17" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="E17" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="F16" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="14"/>
-    </row>
-    <row r="17" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
-      <c r="A17" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="B17" s="60"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="E17" s="57"/>
       <c r="F17" s="14" t="s">
-        <v>82</v>
+        <v>247</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>25</v>
       </c>
       <c r="H17" s="14"/>
     </row>
-    <row r="18" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A18" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
+        <v>144</v>
+      </c>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
       <c r="D18" s="14" t="s">
-        <v>58</v>
+        <v>270</v>
       </c>
       <c r="E18" s="57"/>
       <c r="F18" s="14" t="s">
-        <v>249</v>
+        <v>82</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>25</v>
       </c>
       <c r="H18" s="14"/>
     </row>
-    <row r="19" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A19" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
+        <v>145</v>
+      </c>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
       <c r="D19" s="14" t="s">
-        <v>272</v>
+        <v>58</v>
       </c>
       <c r="E19" s="57"/>
       <c r="F19" s="14" t="s">
-        <v>81</v>
+        <v>248</v>
       </c>
       <c r="G19" s="14" t="s">
         <v>25</v>
       </c>
       <c r="H19" s="14"/>
     </row>
-    <row r="20" spans="1:8" ht="114" x14ac:dyDescent="0.15">
-      <c r="A20" s="11" t="s">
+    <row r="20" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+      <c r="A20" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="E20" s="57"/>
+      <c r="F20" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21" spans="1:8" ht="114" x14ac:dyDescent="0.15">
+      <c r="A21" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="E21" s="57"/>
+      <c r="F21" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="16"/>
+    </row>
+    <row r="22" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+      <c r="A22" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="E22" s="58"/>
+      <c r="F22" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="G22" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="H22" s="37"/>
+    </row>
+    <row r="23" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A23" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="E20" s="57"/>
-      <c r="F20" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="G20" s="15" t="s">
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="H23" s="21"/>
+    </row>
+    <row r="24" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
+      <c r="A24" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="G24" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H20" s="16"/>
-    </row>
-    <row r="21" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
-      <c r="A21" s="35" t="s">
-        <v>218</v>
-      </c>
-      <c r="B21" s="60"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="35" t="s">
-        <v>216</v>
-      </c>
-      <c r="E21" s="58"/>
-      <c r="F21" s="36" t="s">
-        <v>220</v>
-      </c>
-      <c r="G21" s="37" t="s">
-        <v>212</v>
-      </c>
-      <c r="H21" s="37"/>
-    </row>
-    <row r="22" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A22" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="B22" s="60"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="G22" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="H22" s="21"/>
-    </row>
-    <row r="23" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
-      <c r="A23" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="B23" s="61"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="G23" s="21" t="s">
+      <c r="H24" s="21"/>
+    </row>
+    <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A25" s="27" t="s">
+        <v>323</v>
+      </c>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="G25" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="21"/>
+      <c r="H25" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E10"/>
-    <mergeCell ref="B3:B12"/>
-    <mergeCell ref="C3:C12"/>
-    <mergeCell ref="B16:B23"/>
-    <mergeCell ref="C16:C23"/>
-    <mergeCell ref="E16:E21"/>
+    <mergeCell ref="E17:E22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11205,7 +11369,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -11261,22 +11425,22 @@
     </row>
     <row r="3" spans="1:8" s="23" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="B3" s="65" t="s">
-        <v>188</v>
-      </c>
-      <c r="C3" s="65" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="69" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="69" t="s">
         <v>115</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="E3" s="68" t="s">
+        <v>272</v>
+      </c>
+      <c r="E3" s="65" t="s">
         <v>122</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>35</v>
@@ -11285,14 +11449,14 @@
     </row>
     <row r="4" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
+        <v>195</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="E4" s="69"/>
+        <v>273</v>
+      </c>
+      <c r="E4" s="66"/>
       <c r="F4" s="6" t="s">
         <v>84</v>
       </c>
@@ -11303,16 +11467,16 @@
     </row>
     <row r="5" spans="1:8" s="23" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
+        <v>196</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
       <c r="D5" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="69"/>
+      <c r="E5" s="66"/>
       <c r="F5" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>34</v>
@@ -11321,14 +11485,14 @@
     </row>
     <row r="6" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
+        <v>197</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="E6" s="69"/>
+        <v>274</v>
+      </c>
+      <c r="E6" s="66"/>
       <c r="F6" s="6" t="s">
         <v>84</v>
       </c>
@@ -11339,16 +11503,16 @@
     </row>
     <row r="7" spans="1:8" s="23" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="29" t="s">
-        <v>199</v>
-      </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
+        <v>198</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="29" t="s">
-        <v>192</v>
-      </c>
-      <c r="E7" s="69"/>
+        <v>191</v>
+      </c>
+      <c r="E7" s="66"/>
       <c r="F7" s="29" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G7" s="30" t="s">
         <v>61</v>
@@ -11357,30 +11521,30 @@
     </row>
     <row r="8" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A8" s="38" t="s">
-        <v>223</v>
-      </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
+        <v>222</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="35" t="s">
-        <v>226</v>
-      </c>
-      <c r="E8" s="70"/>
+        <v>225</v>
+      </c>
+      <c r="E8" s="67"/>
       <c r="F8" s="36" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H8" s="40"/>
     </row>
     <row r="9" spans="1:8" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A9" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
+        <v>199</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
       <c r="D9" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>110</v>
@@ -11395,179 +11559,181 @@
     </row>
     <row r="10" spans="1:8" s="33" customFormat="1" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A10" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
+        <v>221</v>
+      </c>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" spans="1:8" s="33" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="9"/>
-      <c r="H11" s="34"/>
+    <row r="11" spans="1:8" s="33" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A11" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="21"/>
     </row>
     <row r="12" spans="1:8" s="33" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="9"/>
+      <c r="H12" s="34"/>
+    </row>
+    <row r="13" spans="1:8" s="33" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B13" s="59" t="s">
-        <v>189</v>
-      </c>
-      <c r="C13" s="65" t="s">
-        <v>115</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E13" s="56" t="s">
-        <v>109</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B14" s="60"/>
-      <c r="C14" s="66"/>
+        <v>200</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="C14" s="69" t="s">
+        <v>115</v>
+      </c>
       <c r="D14" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="E14" s="57"/>
+        <v>189</v>
+      </c>
+      <c r="E14" s="56" t="s">
+        <v>109</v>
+      </c>
       <c r="F14" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="57" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B15" s="60"/>
-      <c r="C15" s="66"/>
+        <v>201</v>
+      </c>
+      <c r="B15" s="43"/>
+      <c r="C15" s="7"/>
       <c r="D15" s="2" t="s">
-        <v>276</v>
+        <v>190</v>
       </c>
       <c r="E15" s="57"/>
       <c r="F15" s="2" t="s">
-        <v>86</v>
+        <v>254</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B16" s="60"/>
-      <c r="C16" s="66"/>
+        <v>202</v>
+      </c>
+      <c r="B16" s="43"/>
+      <c r="C16" s="7"/>
       <c r="D16" s="2" t="s">
-        <v>60</v>
+        <v>275</v>
       </c>
       <c r="E16" s="57"/>
       <c r="F16" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="G16" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
-      <c r="A17" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="B17" s="60"/>
-      <c r="C17" s="66"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
+      <c r="A17" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B17" s="43"/>
+      <c r="C17" s="7"/>
       <c r="D17" s="2" t="s">
-        <v>277</v>
+        <v>60</v>
       </c>
       <c r="E17" s="57"/>
       <c r="F17" s="2" t="s">
-        <v>85</v>
+        <v>255</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
-      <c r="A18" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="B18" s="60"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="11" t="s">
-        <v>194</v>
+    <row r="18" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+      <c r="A18" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B18" s="43"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="2" t="s">
+        <v>276</v>
       </c>
       <c r="E18" s="57"/>
-      <c r="F18" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="H18" s="16"/>
+      <c r="F18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="B19" s="60"/>
-      <c r="C19" s="66"/>
+        <v>205</v>
+      </c>
+      <c r="B19" s="43"/>
+      <c r="C19" s="7"/>
       <c r="D19" s="11" t="s">
         <v>193</v>
       </c>
@@ -11576,76 +11742,110 @@
         <v>76</v>
       </c>
       <c r="G19" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="16"/>
+    </row>
+    <row r="20" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
+      <c r="A20" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="B20" s="43"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="E20" s="57"/>
+      <c r="F20" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H19" s="16"/>
-    </row>
-    <row r="20" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
-      <c r="A20" s="35" t="s">
-        <v>225</v>
-      </c>
-      <c r="B20" s="60"/>
-      <c r="C20" s="66"/>
-      <c r="D20" s="35" t="s">
-        <v>227</v>
-      </c>
-      <c r="E20" s="58"/>
-      <c r="F20" s="36" t="s">
+      <c r="H20" s="16"/>
+    </row>
+    <row r="21" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
+      <c r="A21" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="G20" s="41" t="s">
-        <v>212</v>
-      </c>
-      <c r="H20" s="42"/>
-    </row>
-    <row r="21" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A21" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="B21" s="60"/>
-      <c r="C21" s="66"/>
-      <c r="D21" s="20" t="s">
+      <c r="B21" s="43"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="E21" s="58"/>
+      <c r="F21" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="G21" s="41" t="s">
+        <v>211</v>
+      </c>
+      <c r="H21" s="42"/>
+    </row>
+    <row r="22" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A22" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B22" s="43"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="H22" s="21"/>
+    </row>
+    <row r="23" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
+      <c r="A23" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B23" s="44"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="E21" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="G21" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="H21" s="21"/>
-    </row>
-    <row r="22" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
-      <c r="A22" s="20" t="s">
-        <v>221</v>
-      </c>
-      <c r="B22" s="61"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="E22" s="20" t="s">
+      <c r="E23" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="F22" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="G22" s="21" t="s">
+      <c r="G23" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H22" s="21"/>
+      <c r="H23" s="21"/>
+    </row>
+    <row r="24" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A24" s="27" t="s">
+        <v>325</v>
+      </c>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="G24" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B13:B22"/>
-    <mergeCell ref="C13:C22"/>
-    <mergeCell ref="E13:E20"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="E14:E21"/>
     <mergeCell ref="E3:E8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -11656,7 +11856,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -11714,17 +11914,17 @@
       <c r="A3" s="22">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="17" t="s">
         <v>116</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>100</v>
@@ -11738,10 +11938,10 @@
       <c r="A4" s="22">
         <v>5.2</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E4" s="57"/>
       <c r="F4" s="2" t="s">
@@ -11756,10 +11956,10 @@
       <c r="A5" s="22">
         <v>5.3</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E5" s="57"/>
       <c r="F5" s="2" t="s">
@@ -11774,14 +11974,14 @@
       <c r="A6" s="22">
         <v>5.4</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E6" s="58"/>
       <c r="F6" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>31</v>
@@ -11792,19 +11992,19 @@
       <c r="A7" s="22">
         <v>5.5</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
       <c r="D7" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E7" s="52" t="s">
         <v>300</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="F7" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>302</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>303</v>
       </c>
       <c r="H7" s="13"/>
     </row>
@@ -11812,10 +12012,10 @@
       <c r="A8" s="27">
         <v>5.6</v>
       </c>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>104</v>
@@ -11828,18 +12028,36 @@
       </c>
       <c r="H8" s="21"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B9" s="8"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="8"/>
+    <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.15">
+      <c r="A9" s="27">
+        <v>5.7</v>
+      </c>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="21"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B10" s="8"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E6"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="C3:C8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11849,7 +12067,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -11902,7 +12120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="228" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="213.75" x14ac:dyDescent="0.15">
       <c r="A3" s="22">
         <v>6.1</v>
       </c>
@@ -11913,13 +12131,13 @@
         <v>117</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -11937,21 +12155,21 @@
       </c>
       <c r="E4" s="57"/>
       <c r="F4" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>31</v>
       </c>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A5" s="22">
         <v>6.3</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="D5" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E5" s="58"/>
       <c r="F5" s="2" t="s">
@@ -11969,16 +12187,16 @@
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="D6" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H6" s="6"/>
     </row>
@@ -11989,13 +12207,13 @@
       <c r="B7" s="43"/>
       <c r="C7" s="43"/>
       <c r="D7" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E7" s="54" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -12007,7 +12225,7 @@
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
       <c r="D8" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>104</v>
@@ -12020,8 +12238,28 @@
       </c>
       <c r="H8" s="21"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B11" s="8"/>
+    <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.15">
+      <c r="A9" s="27">
+        <v>6.7</v>
+      </c>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="21"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B12" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -12036,10 +12274,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A8" sqref="A8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -12092,12 +12330,12 @@
     </row>
     <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B3" s="59" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="17" t="s">
         <v>118</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -12107,7 +12345,7 @@
         <v>97</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>29</v>
@@ -12116,12 +12354,12 @@
     </row>
     <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
+        <v>154</v>
+      </c>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E4" s="57"/>
       <c r="F4" s="2" t="s">
@@ -12134,12 +12372,12 @@
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
+        <v>155</v>
+      </c>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E5" s="57"/>
       <c r="F5" s="2" t="s">
@@ -12152,10 +12390,10 @@
     </row>
     <row r="6" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
+        <v>156</v>
+      </c>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="6" t="s">
         <v>66</v>
       </c>
@@ -12170,12 +12408,12 @@
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
+        <v>157</v>
+      </c>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>108</v>
@@ -12188,68 +12426,70 @@
       </c>
       <c r="H7" s="21"/>
     </row>
-    <row r="9" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
+    <row r="8" spans="1:8" ht="57" x14ac:dyDescent="0.15">
+      <c r="A8" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="21"/>
+    </row>
+    <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="114" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B10" s="59" t="s">
+    <row r="11" spans="1:8" ht="114" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="59" t="s">
+      <c r="C11" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E11" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E11" s="57"/>
       <c r="F11" s="2" t="s">
-        <v>153</v>
+        <v>257</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>25</v>
@@ -12258,69 +12498,103 @@
     </row>
     <row r="12" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
+        <v>159</v>
+      </c>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
       <c r="D12" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E12" s="57"/>
       <c r="F12" s="2" t="s">
-        <v>67</v>
+        <v>152</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E13" s="57"/>
+      <c r="F13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
+      <c r="A14" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="58"/>
+      <c r="F14" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A15" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="58"/>
-      <c r="F13" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="6" t="s">
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="H15" s="21"/>
+    </row>
+    <row r="16" spans="1:8" ht="57" x14ac:dyDescent="0.15">
+      <c r="A16" s="27" t="s">
+        <v>326</v>
+      </c>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="G16" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A14" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="H14" s="21"/>
+      <c r="H16" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C3:C7"/>
     <mergeCell ref="E3:E6"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="E11:E14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12330,7 +12604,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -12387,34 +12661,34 @@
       <c r="A3" s="22">
         <v>8.1</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="17" t="s">
         <v>119</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A4" s="22">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
@@ -12431,10 +12705,10 @@
       <c r="A5" s="22">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E5" s="58"/>
       <c r="F5" s="2" t="s">
@@ -12449,19 +12723,19 @@
       <c r="A6" s="22">
         <v>8.4</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E6" s="56" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -12469,17 +12743,17 @@
       <c r="A7" s="22">
         <v>8.5</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
       <c r="D7" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E7" s="57"/>
       <c r="F7" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>311</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>312</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -12487,17 +12761,17 @@
       <c r="A8" s="22">
         <v>8.6</v>
       </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
       <c r="D8" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E8" s="58"/>
       <c r="F8" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -12505,10 +12779,10 @@
       <c r="A9" s="27">
         <v>8.6999999999999993</v>
       </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>108</v>
@@ -12521,16 +12795,34 @@
       </c>
       <c r="H9" s="21"/>
     </row>
-    <row r="11" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A11" s="9"/>
-      <c r="B11" s="8"/>
+    <row r="10" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A10" s="27">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="21"/>
+    </row>
+    <row r="12" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A12" s="9"/>
+      <c r="B12" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E5"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="C3:C9"/>
     <mergeCell ref="E6:E8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Update the test case file for FileOperation as rename function updated
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="334">
   <si>
     <t>删除文件夹</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3882,10 +3882,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>7.1.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>7.2.1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3899,10 +3895,6 @@
   </si>
   <si>
     <t>7.2.4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7.2.5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -9068,6 +9060,116 @@
   </si>
   <si>
     <t>7.1.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.1.7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.1.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件夹名字
+2.输入替换的空文件夹名</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.2.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示新命名文件夹不能为空（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cannot rename with empty path. Please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件夹不应被重命名成功</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件夹名字
+2.输入替换的空文件名</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.2.7</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -9301,7 +9403,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -9467,6 +9569,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -9478,15 +9589,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -9506,14 +9608,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9822,7 +9927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -9839,14 +9944,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
+      <c r="A1" s="58"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -9887,11 +9992,11 @@
       <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="59" t="s">
         <v>103</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>26</v>
@@ -9907,7 +10012,7 @@
       <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="57"/>
+      <c r="E4" s="60"/>
       <c r="F4" s="2" t="s">
         <v>101</v>
       </c>
@@ -9923,9 +10028,9 @@
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="D5" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="E5" s="57"/>
+        <v>257</v>
+      </c>
+      <c r="E5" s="60"/>
       <c r="F5" s="2" t="s">
         <v>80</v>
       </c>
@@ -9943,7 +10048,7 @@
       <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="58"/>
+      <c r="E6" s="61"/>
       <c r="F6" s="2" t="s">
         <v>79</v>
       </c>
@@ -9959,13 +10064,13 @@
       <c r="B7" s="43"/>
       <c r="C7" s="43"/>
       <c r="D7" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>298</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="E7" s="52" t="s">
-        <v>300</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>301</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="18"/>
@@ -9997,13 +10102,13 @@
       <c r="B9" s="44"/>
       <c r="C9" s="44"/>
       <c r="D9" s="20" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>25</v>
@@ -10085,23 +10190,23 @@
       <c r="A3" s="46">
         <v>10.1</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="71" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="71" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="71" t="s">
         <v>165</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="E3" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D3" s="68" t="s">
-        <v>167</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -10109,14 +10214,14 @@
       <c r="A4" s="46">
         <v>10.199999999999999</v>
       </c>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
       <c r="E4" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>151</v>
@@ -10127,14 +10232,14 @@
       <c r="A5" s="46">
         <v>10.3</v>
       </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
       <c r="E5" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>151</v>
@@ -10145,14 +10250,14 @@
       <c r="A6" s="46">
         <v>10.4</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
       <c r="E6" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>151</v>
@@ -10163,14 +10268,14 @@
       <c r="A7" s="46">
         <v>10.5</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
       <c r="E7" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>151</v>
@@ -10181,14 +10286,14 @@
       <c r="A8" s="46">
         <v>10.6</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
       <c r="E8" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>151</v>
@@ -10199,14 +10304,14 @@
       <c r="A9" s="46">
         <v>10.7</v>
       </c>
-      <c r="B9" s="68"/>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
       <c r="E9" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>151</v>
@@ -10217,14 +10322,14 @@
       <c r="A10" s="46">
         <v>10.8</v>
       </c>
-      <c r="B10" s="68"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
       <c r="E10" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>151</v>
@@ -10235,30 +10340,30 @@
       <c r="A11" s="46">
         <v>10.9</v>
       </c>
-      <c r="B11" s="68"/>
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
       <c r="E11" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A12" s="53" t="s">
-        <v>294</v>
-      </c>
-      <c r="B12" s="68"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
+        <v>292</v>
+      </c>
+      <c r="B12" s="71"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
       <c r="E12" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>25</v>
@@ -10269,14 +10374,14 @@
       <c r="A13" s="48">
         <v>10.11</v>
       </c>
-      <c r="B13" s="68"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
       <c r="E13" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>151</v>
@@ -10287,14 +10392,14 @@
       <c r="A14" s="46">
         <v>10.119999999999999</v>
       </c>
-      <c r="B14" s="68"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
       <c r="E14" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>151</v>
@@ -10374,20 +10479,20 @@
       <c r="A3" s="22">
         <v>11.1</v>
       </c>
-      <c r="B3" s="59" t="s">
-        <v>281</v>
-      </c>
-      <c r="C3" s="59" t="s">
-        <v>282</v>
+      <c r="B3" s="68" t="s">
+        <v>279</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>280</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="E3" s="56" t="s">
+        <v>284</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>288</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>290</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>292</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -10398,14 +10503,14 @@
       <c r="A4" s="49">
         <v>11.2</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
       <c r="D4" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E4" s="61"/>
+      <c r="F4" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="2" t="s">
-        <v>289</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>25</v>
@@ -10416,16 +10521,16 @@
       <c r="A5" s="49">
         <v>11.3</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="E5" s="56" t="s">
+        <v>282</v>
+      </c>
+      <c r="E5" s="59" t="s">
+        <v>289</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>291</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>293</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>25</v>
@@ -10436,14 +10541,14 @@
       <c r="A6" s="50">
         <v>11.4</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="E6" s="58"/>
+        <v>283</v>
+      </c>
+      <c r="E6" s="61"/>
       <c r="F6" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>25</v>
@@ -10454,8 +10559,8 @@
       <c r="A7" s="51">
         <v>11.5</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
       <c r="D7" s="20" t="s">
         <v>149</v>
       </c>
@@ -10506,14 +10611,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
+      <c r="A1" s="58"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10558,7 +10663,7 @@
         <v>73</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>30</v>
@@ -10572,13 +10677,13 @@
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
       <c r="D4" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>25</v>
@@ -10592,7 +10697,7 @@
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="D5" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>73</v>
@@ -10615,7 +10720,7 @@
         <v>149</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>105</v>
@@ -10627,18 +10732,18 @@
     </row>
     <row r="7" spans="1:9" ht="57" x14ac:dyDescent="0.15">
       <c r="A7" s="27" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B7" s="44"/>
       <c r="C7" s="44"/>
       <c r="D7" s="20" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>25</v>
@@ -10700,7 +10805,7 @@
         <v>107</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>25</v>
@@ -10721,7 +10826,7 @@
         <v>94</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>72</v>
@@ -10738,7 +10843,7 @@
       <c r="B12" s="43"/>
       <c r="C12" s="43"/>
       <c r="D12" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>93</v>
@@ -10774,18 +10879,18 @@
     </row>
     <row r="14" spans="1:9" s="23" customFormat="1" ht="57" x14ac:dyDescent="0.15">
       <c r="A14" s="27" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B14" s="44"/>
       <c r="C14" s="44"/>
       <c r="D14" s="20" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G14" s="21" t="s">
         <v>25</v>
@@ -10956,13 +11061,13 @@
         <v>114</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="E3" s="56" t="s">
+        <v>264</v>
+      </c>
+      <c r="E3" s="59" t="s">
         <v>95</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -10976,11 +11081,11 @@
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
       <c r="D4" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="E4" s="57"/>
+        <v>265</v>
+      </c>
+      <c r="E4" s="60"/>
       <c r="F4" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>25</v>
@@ -10994,9 +11099,9 @@
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="D5" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="E5" s="57"/>
+        <v>266</v>
+      </c>
+      <c r="E5" s="60"/>
       <c r="F5" s="2" t="s">
         <v>83</v>
       </c>
@@ -11014,9 +11119,9 @@
       <c r="D6" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E6" s="57"/>
+      <c r="E6" s="60"/>
       <c r="F6" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>25</v>
@@ -11030,11 +11135,11 @@
       <c r="B7" s="43"/>
       <c r="C7" s="43"/>
       <c r="D7" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="E7" s="57"/>
+        <v>267</v>
+      </c>
+      <c r="E7" s="60"/>
       <c r="F7" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>32</v>
@@ -11050,9 +11155,9 @@
       <c r="D8" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E8" s="57"/>
+      <c r="E8" s="60"/>
       <c r="F8" s="19" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>37</v>
@@ -11066,11 +11171,11 @@
       <c r="B9" s="43"/>
       <c r="C9" s="43"/>
       <c r="D9" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="E9" s="57"/>
+        <v>206</v>
+      </c>
+      <c r="E9" s="60"/>
       <c r="F9" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>25</v>
@@ -11079,25 +11184,25 @@
     </row>
     <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A10" s="35" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B10" s="43"/>
       <c r="C10" s="43"/>
       <c r="D10" s="35" t="s">
-        <v>216</v>
-      </c>
-      <c r="E10" s="58"/>
+        <v>214</v>
+      </c>
+      <c r="E10" s="61"/>
       <c r="F10" s="36" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B11" s="43"/>
       <c r="C11" s="43"/>
@@ -11117,7 +11222,7 @@
     </row>
     <row r="12" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
@@ -11137,18 +11242,18 @@
     </row>
     <row r="13" spans="1:8" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A13" s="27" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
       <c r="D13" s="20" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G13" s="21" t="s">
         <v>25</v>
@@ -11194,11 +11299,11 @@
       <c r="D17" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="E17" s="56" t="s">
+      <c r="E17" s="59" t="s">
         <v>96</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>25</v>
@@ -11212,9 +11317,9 @@
       <c r="B18" s="43"/>
       <c r="C18" s="43"/>
       <c r="D18" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="E18" s="57"/>
+        <v>268</v>
+      </c>
+      <c r="E18" s="60"/>
       <c r="F18" s="14" t="s">
         <v>82</v>
       </c>
@@ -11232,9 +11337,9 @@
       <c r="D19" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="57"/>
+      <c r="E19" s="60"/>
       <c r="F19" s="14" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G19" s="14" t="s">
         <v>25</v>
@@ -11248,9 +11353,9 @@
       <c r="B20" s="43"/>
       <c r="C20" s="43"/>
       <c r="D20" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="E20" s="57"/>
+        <v>269</v>
+      </c>
+      <c r="E20" s="60"/>
       <c r="F20" s="14" t="s">
         <v>81</v>
       </c>
@@ -11268,9 +11373,9 @@
       <c r="D21" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="E21" s="57"/>
+      <c r="E21" s="60"/>
       <c r="F21" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G21" s="15" t="s">
         <v>25</v>
@@ -11279,19 +11384,19 @@
     </row>
     <row r="22" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A22" s="35" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B22" s="43"/>
       <c r="C22" s="43"/>
       <c r="D22" s="35" t="s">
-        <v>215</v>
-      </c>
-      <c r="E22" s="58"/>
+        <v>213</v>
+      </c>
+      <c r="E22" s="61"/>
       <c r="F22" s="36" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H22" s="37"/>
     </row>
@@ -11317,7 +11422,7 @@
     </row>
     <row r="24" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A24" s="20" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B24" s="44"/>
       <c r="C24" s="44"/>
@@ -11337,18 +11442,18 @@
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A25" s="27" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
       <c r="D25" s="20" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G25" s="21" t="s">
         <v>25</v>
@@ -11425,22 +11530,22 @@
     </row>
     <row r="3" spans="1:8" s="23" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="B3" s="69" t="s">
-        <v>187</v>
-      </c>
-      <c r="C3" s="69" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="56" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" s="56" t="s">
         <v>115</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E3" s="65" t="s">
         <v>122</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>35</v>
@@ -11449,12 +11554,12 @@
     </row>
     <row r="4" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E4" s="66"/>
       <c r="F4" s="6" t="s">
@@ -11467,7 +11572,7 @@
     </row>
     <row r="5" spans="1:8" s="23" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -11476,7 +11581,7 @@
       </c>
       <c r="E5" s="66"/>
       <c r="F5" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>34</v>
@@ -11485,12 +11590,12 @@
     </row>
     <row r="6" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E6" s="66"/>
       <c r="F6" s="6" t="s">
@@ -11503,16 +11608,16 @@
     </row>
     <row r="7" spans="1:8" s="23" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="29" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="29" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E7" s="66"/>
       <c r="F7" s="29" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G7" s="30" t="s">
         <v>61</v>
@@ -11521,25 +11626,25 @@
     </row>
     <row r="8" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A8" s="38" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="35" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E8" s="67"/>
       <c r="F8" s="36" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H8" s="40"/>
     </row>
     <row r="9" spans="1:8" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A9" s="20" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -11559,10 +11664,10 @@
     </row>
     <row r="10" spans="1:8" s="33" customFormat="1" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A10" s="20" t="s">
-        <v>221</v>
-      </c>
-      <c r="B10" s="70"/>
-      <c r="C10" s="70"/>
+        <v>219</v>
+      </c>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
       <c r="D10" s="20" t="s">
         <v>150</v>
       </c>
@@ -11579,18 +11684,18 @@
     </row>
     <row r="11" spans="1:8" s="33" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="27" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B11" s="44"/>
       <c r="C11" s="44"/>
       <c r="D11" s="20" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G11" s="21" t="s">
         <v>25</v>
@@ -11634,22 +11739,22 @@
     </row>
     <row r="14" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="C14" s="69" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14" s="56" t="s">
         <v>115</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E14" s="56" t="s">
+        <v>187</v>
+      </c>
+      <c r="E14" s="59" t="s">
         <v>109</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>25</v>
@@ -11658,16 +11763,16 @@
     </row>
     <row r="15" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B15" s="43"/>
       <c r="C15" s="7"/>
       <c r="D15" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E15" s="57"/>
+        <v>188</v>
+      </c>
+      <c r="E15" s="60"/>
       <c r="F15" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>25</v>
@@ -11676,14 +11781,14 @@
     </row>
     <row r="16" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B16" s="43"/>
       <c r="C16" s="7"/>
       <c r="D16" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="E16" s="57"/>
+        <v>273</v>
+      </c>
+      <c r="E16" s="60"/>
       <c r="F16" s="2" t="s">
         <v>86</v>
       </c>
@@ -11694,16 +11799,16 @@
     </row>
     <row r="17" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B17" s="43"/>
       <c r="C17" s="7"/>
       <c r="D17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="57"/>
+      <c r="E17" s="60"/>
       <c r="F17" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>25</v>
@@ -11712,14 +11817,14 @@
     </row>
     <row r="18" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B18" s="43"/>
       <c r="C18" s="7"/>
       <c r="D18" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="E18" s="57"/>
+        <v>274</v>
+      </c>
+      <c r="E18" s="60"/>
       <c r="F18" s="2" t="s">
         <v>85</v>
       </c>
@@ -11730,14 +11835,14 @@
     </row>
     <row r="19" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B19" s="43"/>
       <c r="C19" s="7"/>
       <c r="D19" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="E19" s="57"/>
+        <v>191</v>
+      </c>
+      <c r="E19" s="60"/>
       <c r="F19" s="11" t="s">
         <v>76</v>
       </c>
@@ -11748,14 +11853,14 @@
     </row>
     <row r="20" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A20" s="11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B20" s="43"/>
       <c r="C20" s="7"/>
       <c r="D20" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="E20" s="57"/>
+        <v>190</v>
+      </c>
+      <c r="E20" s="60"/>
       <c r="F20" s="11" t="s">
         <v>76</v>
       </c>
@@ -11766,25 +11871,25 @@
     </row>
     <row r="21" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A21" s="35" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B21" s="43"/>
       <c r="C21" s="7"/>
       <c r="D21" s="35" t="s">
-        <v>226</v>
-      </c>
-      <c r="E21" s="58"/>
+        <v>224</v>
+      </c>
+      <c r="E21" s="61"/>
       <c r="F21" s="36" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G21" s="41" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H21" s="42"/>
     </row>
     <row r="22" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B22" s="43"/>
       <c r="C22" s="7"/>
@@ -11804,10 +11909,10 @@
     </row>
     <row r="23" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A23" s="20" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B23" s="44"/>
-      <c r="C23" s="70"/>
+      <c r="C23" s="57"/>
       <c r="D23" s="20" t="s">
         <v>150</v>
       </c>
@@ -11824,18 +11929,18 @@
     </row>
     <row r="24" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A24" s="27" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B24" s="44"/>
       <c r="C24" s="44"/>
       <c r="D24" s="20" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G24" s="21" t="s">
         <v>25</v>
@@ -11923,8 +12028,8 @@
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="56" t="s">
-        <v>234</v>
+      <c r="E3" s="59" t="s">
+        <v>232</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>100</v>
@@ -11941,9 +12046,9 @@
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
       <c r="D4" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="E4" s="57"/>
+        <v>258</v>
+      </c>
+      <c r="E4" s="60"/>
       <c r="F4" s="2" t="s">
         <v>99</v>
       </c>
@@ -11959,9 +12064,9 @@
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="D5" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="E5" s="57"/>
+        <v>275</v>
+      </c>
+      <c r="E5" s="60"/>
       <c r="F5" s="2" t="s">
         <v>87</v>
       </c>
@@ -11977,11 +12082,11 @@
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="D6" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E6" s="61"/>
+      <c r="F6" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="E6" s="58"/>
-      <c r="F6" s="2" t="s">
-        <v>235</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>31</v>
@@ -11995,16 +12100,16 @@
       <c r="B7" s="43"/>
       <c r="C7" s="43"/>
       <c r="D7" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>298</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="G7" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>302</v>
       </c>
       <c r="H7" s="13"/>
     </row>
@@ -12035,13 +12140,13 @@
       <c r="B9" s="44"/>
       <c r="C9" s="44"/>
       <c r="D9" s="20" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>25</v>
@@ -12131,13 +12236,13 @@
         <v>117</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>281</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="E3" s="56" t="s">
-        <v>283</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -12153,9 +12258,9 @@
       <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="57"/>
+      <c r="E4" s="60"/>
       <c r="F4" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>31</v>
@@ -12169,9 +12274,9 @@
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="D5" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="E5" s="58"/>
+        <v>259</v>
+      </c>
+      <c r="E5" s="61"/>
       <c r="F5" s="2" t="s">
         <v>88</v>
       </c>
@@ -12187,13 +12292,13 @@
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="D6" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>311</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>229</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>313</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>231</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>151</v>
@@ -12207,13 +12312,13 @@
       <c r="B7" s="43"/>
       <c r="C7" s="43"/>
       <c r="D7" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E7" s="54" t="s">
         <v>312</v>
       </c>
-      <c r="E7" s="54" t="s">
-        <v>314</v>
-      </c>
       <c r="F7" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -12245,13 +12350,13 @@
       <c r="B9" s="44"/>
       <c r="C9" s="44"/>
       <c r="D9" s="20" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>25</v>
@@ -12274,10 +12379,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -12341,11 +12446,11 @@
       <c r="D3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="59" t="s">
         <v>97</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>29</v>
@@ -12359,9 +12464,9 @@
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
       <c r="D4" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="E4" s="57"/>
+        <v>260</v>
+      </c>
+      <c r="E4" s="60"/>
       <c r="F4" s="2" t="s">
         <v>62</v>
       </c>
@@ -12377,9 +12482,9 @@
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="D5" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="E5" s="57"/>
+        <v>259</v>
+      </c>
+      <c r="E5" s="60"/>
       <c r="F5" s="2" t="s">
         <v>89</v>
       </c>
@@ -12397,7 +12502,7 @@
       <c r="D6" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="58"/>
+      <c r="E6" s="61"/>
       <c r="F6" s="6" t="s">
         <v>63</v>
       </c>
@@ -12406,108 +12511,108 @@
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A7" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="21"/>
-    </row>
-    <row r="8" spans="1:8" ht="57" x14ac:dyDescent="0.15">
-      <c r="A8" s="27" t="s">
+    <row r="7" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
+      <c r="A7" s="6" t="s">
         <v>327</v>
+      </c>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E7" s="55"/>
+      <c r="F7" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A8" s="20" t="s">
+        <v>325</v>
       </c>
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
       <c r="D8" s="20" t="s">
-        <v>315</v>
+        <v>149</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>319</v>
+        <v>108</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>320</v>
+        <v>105</v>
       </c>
       <c r="G8" s="21" t="s">
         <v>25</v>
       </c>
       <c r="H8" s="21"/>
     </row>
-    <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
+    <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.15">
+      <c r="A9" s="27" t="s">
+        <v>326</v>
+      </c>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="21"/>
+    </row>
+    <row r="11" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="114" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B11" s="17" t="s">
+    <row r="12" spans="1:8" ht="114" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C12" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="56" t="s">
+      <c r="E12" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="E12" s="57"/>
       <c r="F12" s="2" t="s">
-        <v>152</v>
+        <v>255</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>25</v>
@@ -12516,85 +12621,121 @@
     </row>
     <row r="13" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B13" s="43"/>
       <c r="C13" s="43"/>
       <c r="D13" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E13" s="57"/>
+        <v>261</v>
+      </c>
+      <c r="E13" s="60"/>
       <c r="F13" s="2" t="s">
-        <v>67</v>
+        <v>152</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
-      <c r="A14" s="6" t="s">
-        <v>161</v>
+    <row r="14" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+      <c r="A14" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="B14" s="43"/>
       <c r="C14" s="43"/>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="E14" s="60"/>
+      <c r="F14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
+      <c r="A15" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="58"/>
-      <c r="F14" s="6" t="s">
+      <c r="E15" s="61"/>
+      <c r="F15" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A15" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="20" t="s">
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
+      <c r="A16" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E16" s="55"/>
+      <c r="F16" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A17" s="20" t="s">
+        <v>324</v>
+      </c>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E17" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F17" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G17" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="H15" s="21"/>
-    </row>
-    <row r="16" spans="1:8" ht="57" x14ac:dyDescent="0.15">
-      <c r="A16" s="27" t="s">
-        <v>326</v>
-      </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="20" t="s">
-        <v>315</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>319</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>320</v>
-      </c>
-      <c r="G16" s="21" t="s">
+      <c r="H17" s="21"/>
+    </row>
+    <row r="18" spans="1:8" ht="57" x14ac:dyDescent="0.15">
+      <c r="A18" s="27" t="s">
+        <v>333</v>
+      </c>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="G18" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="21"/>
+      <c r="H18" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E6"/>
-    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="E12:E15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12668,19 +12809,19 @@
         <v>119</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E3" s="56" t="s">
-        <v>306</v>
+        <v>161</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>304</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
@@ -12692,7 +12833,7 @@
       <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="57"/>
+      <c r="E4" s="60"/>
       <c r="F4" s="2" t="s">
         <v>52</v>
       </c>
@@ -12708,9 +12849,9 @@
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="D5" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="E5" s="58"/>
+        <v>263</v>
+      </c>
+      <c r="E5" s="61"/>
       <c r="F5" s="2" t="s">
         <v>90</v>
       </c>
@@ -12726,16 +12867,16 @@
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="D6" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="E6" s="56" t="s">
+        <v>302</v>
+      </c>
+      <c r="E6" s="59" t="s">
+        <v>305</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>311</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -12746,14 +12887,14 @@
       <c r="B7" s="43"/>
       <c r="C7" s="43"/>
       <c r="D7" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E7" s="57"/>
+        <v>303</v>
+      </c>
+      <c r="E7" s="60"/>
       <c r="F7" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -12764,14 +12905,14 @@
       <c r="B8" s="43"/>
       <c r="C8" s="43"/>
       <c r="D8" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="E8" s="58"/>
+        <v>301</v>
+      </c>
+      <c r="E8" s="61"/>
       <c r="F8" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -12802,13 +12943,13 @@
       <c r="B10" s="44"/>
       <c r="C10" s="44"/>
       <c r="D10" s="20" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>25</v>
@@ -12891,10 +13032,10 @@
       <c r="A3" s="22">
         <v>9.1</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="68" t="s">
         <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -12903,7 +13044,7 @@
       <c r="E3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -12915,15 +13056,15 @@
       <c r="A4" s="22">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
       <c r="D4" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="60"/>
+      <c r="F4" s="69"/>
       <c r="G4" s="2" t="s">
         <v>47</v>
       </c>
@@ -12933,15 +13074,15 @@
       <c r="A5" s="22">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="60"/>
+      <c r="F5" s="69"/>
       <c r="G5" s="2" t="s">
         <v>47</v>
       </c>
@@ -12951,15 +13092,15 @@
       <c r="A6" s="22">
         <v>9.4</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="60"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="5" t="s">
         <v>47</v>
       </c>
@@ -12969,15 +13110,15 @@
       <c r="A7" s="22">
         <v>9.5</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
       <c r="D7" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="61"/>
+      <c r="F7" s="70"/>
       <c r="G7" s="5" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Update the test case file of FileOperation as updated before
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="350">
   <si>
     <t>删除文件夹</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -9043,15 +9043,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3.2.9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>4.1.9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.2.11</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -9170,6 +9162,272 @@
   </si>
   <si>
     <t>7.2.7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.1.12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示输入需要被目标文件夹路径时，输入存在路径不带'\'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件夹的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入空字符串</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在提示信息"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"出现时，输入存在路径不带'\'</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示输入需要被复制文件夹路径时，输入存在路径不带'\'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.2.9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.2.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件夹的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入空字符串</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在提示信息"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"出现时，输入存在路径不带'\'</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示输入需要被复制文件路径时，输入存在路径不带'\'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示输入需要被目标文件路径时，输入存在路径不带'\'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.2.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.2.12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.1.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示输入需要被移动文件夹或者文件路径时，输入存在路径不带'\'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示输入需要被目标文件夹路径移动时，输入存在路径不带'\'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示输入需要被目标文件路径移动时，输入存在路径不带'\'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示输入需要被移动文件夹或者文件路径时，输入存在路径不带'\'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -9403,7 +9661,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -9533,12 +9791,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -9572,12 +9824,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -9589,6 +9835,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -9608,13 +9863,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -9944,14 +10199,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="58"/>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
+      <c r="A1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -9983,16 +10238,16 @@
       <c r="A3" s="22">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="58" t="s">
         <v>111</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="55" t="s">
         <v>103</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -10007,12 +10262,12 @@
       <c r="A4" s="22">
         <v>1.2</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="60"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="2" t="s">
         <v>101</v>
       </c>
@@ -10025,12 +10280,12 @@
       <c r="A5" s="22">
         <v>1.3</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="E5" s="60"/>
+      <c r="E5" s="56"/>
       <c r="F5" s="2" t="s">
         <v>80</v>
       </c>
@@ -10043,12 +10298,12 @@
       <c r="A6" s="22">
         <v>1.4</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="61"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="2" t="s">
         <v>79</v>
       </c>
@@ -10061,12 +10316,12 @@
       <c r="A7" s="22">
         <v>1.5</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="E7" s="50" t="s">
         <v>298</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -10079,8 +10334,8 @@
       <c r="A8" s="27">
         <v>1.6</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
       <c r="D8" s="20" t="s">
         <v>149</v>
       </c>
@@ -10099,8 +10354,8 @@
       <c r="A9" s="27">
         <v>1.7</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
       <c r="D9" s="20" t="s">
         <v>313</v>
       </c>
@@ -10120,9 +10375,11 @@
       <c r="B10" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E6"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="C3:C9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10140,7 +10397,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.875" style="47" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.875" style="45" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.875" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="28.375" customWidth="1"/>
@@ -10151,17 +10408,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="64"/>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -10187,16 +10444,16 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A3" s="46">
+      <c r="A3" s="44">
         <v>10.1</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="70" t="s">
         <v>163</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="70" t="s">
         <v>164</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="D3" s="70" t="s">
         <v>165</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -10211,12 +10468,12 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A4" s="46">
+      <c r="A4" s="44">
         <v>10.199999999999999</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
       <c r="E4" s="2" t="s">
         <v>167</v>
       </c>
@@ -10229,12 +10486,12 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A5" s="46">
+      <c r="A5" s="44">
         <v>10.3</v>
       </c>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
       <c r="E5" s="2" t="s">
         <v>168</v>
       </c>
@@ -10247,12 +10504,12 @@
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A6" s="46">
+      <c r="A6" s="44">
         <v>10.4</v>
       </c>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
       <c r="E6" s="2" t="s">
         <v>169</v>
       </c>
@@ -10265,12 +10522,12 @@
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A7" s="46">
+      <c r="A7" s="44">
         <v>10.5</v>
       </c>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
       <c r="E7" s="2" t="s">
         <v>170</v>
       </c>
@@ -10283,12 +10540,12 @@
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A8" s="46">
+      <c r="A8" s="44">
         <v>10.6</v>
       </c>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
       <c r="E8" s="2" t="s">
         <v>171</v>
       </c>
@@ -10301,12 +10558,12 @@
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A9" s="46">
+      <c r="A9" s="44">
         <v>10.7</v>
       </c>
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
       <c r="E9" s="2" t="s">
         <v>172</v>
       </c>
@@ -10319,12 +10576,12 @@
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A10" s="46">
+      <c r="A10" s="44">
         <v>10.8</v>
       </c>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
       <c r="E10" s="2" t="s">
         <v>173</v>
       </c>
@@ -10337,12 +10594,12 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A11" s="46">
+      <c r="A11" s="44">
         <v>10.9</v>
       </c>
-      <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
       <c r="E11" s="2" t="s">
         <v>295</v>
       </c>
@@ -10353,12 +10610,12 @@
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="51" t="s">
         <v>292</v>
       </c>
-      <c r="B12" s="71"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
       <c r="E12" s="2" t="s">
         <v>293</v>
       </c>
@@ -10371,12 +10628,12 @@
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A13" s="48">
+      <c r="A13" s="46">
         <v>10.11</v>
       </c>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
       <c r="E13" s="2" t="s">
         <v>294</v>
       </c>
@@ -10389,12 +10646,12 @@
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A14" s="46">
+      <c r="A14" s="44">
         <v>10.119999999999999</v>
       </c>
-      <c r="B14" s="71"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
       <c r="E14" s="2" t="s">
         <v>174</v>
       </c>
@@ -10421,9 +10678,9 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -10440,14 +10697,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="64"/>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10479,16 +10736,16 @@
       <c r="A3" s="22">
         <v>11.1</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="70" t="s">
         <v>279</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="70" t="s">
         <v>280</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="55" t="s">
         <v>288</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -10500,15 +10757,15 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="57" x14ac:dyDescent="0.15">
-      <c r="A4" s="49">
+      <c r="A4" s="47">
         <v>11.2</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="E4" s="61"/>
+      <c r="E4" s="57"/>
       <c r="F4" s="2" t="s">
         <v>287</v>
       </c>
@@ -10518,15 +10775,15 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.15">
-      <c r="A5" s="49">
+      <c r="A5" s="47">
         <v>11.3</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
       <c r="D5" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="55" t="s">
         <v>289</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -10538,15 +10795,15 @@
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="57" x14ac:dyDescent="0.15">
-      <c r="A6" s="50">
+      <c r="A6" s="48">
         <v>11.4</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="E6" s="61"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="2" t="s">
         <v>286</v>
       </c>
@@ -10556,7 +10813,7 @@
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A7" s="51">
+      <c r="A7" s="49">
         <v>11.5</v>
       </c>
       <c r="B7" s="70"/>
@@ -10575,13 +10832,33 @@
       </c>
       <c r="H7" s="21"/>
     </row>
+    <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A8" s="49">
+        <v>11.6</v>
+      </c>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>314</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="21"/>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C3:C7"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="E3:E4"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="C3:C8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10611,14 +10888,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="58"/>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
+      <c r="A1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10650,10 +10927,10 @@
       <c r="A3" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="58" t="s">
         <v>112</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -10674,8 +10951,8 @@
       <c r="A4" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
         <v>276</v>
       </c>
@@ -10694,8 +10971,8 @@
       <c r="A5" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
         <v>277</v>
       </c>
@@ -10714,8 +10991,8 @@
       <c r="A6" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="20" t="s">
         <v>149</v>
       </c>
@@ -10734,8 +11011,8 @@
       <c r="A7" s="27" t="s">
         <v>315</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="20" t="s">
         <v>313</v>
       </c>
@@ -10792,10 +11069,10 @@
       <c r="A10" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="58" t="s">
         <v>112</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -10817,8 +11094,8 @@
       <c r="A11" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
@@ -10840,8 +11117,8 @@
       <c r="A12" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
       <c r="D12" s="2" t="s">
         <v>278</v>
       </c>
@@ -10861,8 +11138,8 @@
       <c r="A13" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
       <c r="D13" s="20" t="s">
         <v>149</v>
       </c>
@@ -10881,8 +11158,8 @@
       <c r="A14" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
       <c r="D14" s="20" t="s">
         <v>313</v>
       </c>
@@ -10899,7 +11176,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
-      <c r="B15" s="62"/>
+      <c r="B15" s="61"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -10910,7 +11187,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
-      <c r="B16" s="62"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -10921,7 +11198,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
-      <c r="B17" s="62"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -10932,7 +11209,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
-      <c r="B18" s="62"/>
+      <c r="B18" s="61"/>
       <c r="C18" s="4"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -10943,7 +11220,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
-      <c r="B19" s="62"/>
+      <c r="B19" s="61"/>
       <c r="C19" s="4"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -10985,9 +11262,13 @@
       <c r="I22" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B15:B19"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="C10:C14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10997,10 +11278,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:H13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -11015,14 +11296,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A1" s="63"/>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="A1" s="62"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11054,16 +11335,16 @@
       <c r="A3" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="58" t="s">
         <v>114</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="55" t="s">
         <v>95</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -11078,12 +11359,12 @@
       <c r="A4" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="E4" s="60"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="2" t="s">
         <v>241</v>
       </c>
@@ -11096,12 +11377,12 @@
       <c r="A5" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="E5" s="60"/>
+      <c r="E5" s="56"/>
       <c r="F5" s="2" t="s">
         <v>83</v>
       </c>
@@ -11114,12 +11395,12 @@
       <c r="A6" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E6" s="60"/>
+      <c r="E6" s="56"/>
       <c r="F6" s="2" t="s">
         <v>242</v>
       </c>
@@ -11132,12 +11413,12 @@
       <c r="A7" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="E7" s="60"/>
+      <c r="E7" s="56"/>
       <c r="F7" s="2" t="s">
         <v>207</v>
       </c>
@@ -11150,12 +11431,12 @@
       <c r="A8" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
       <c r="D8" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E8" s="60"/>
+      <c r="E8" s="56"/>
       <c r="F8" s="19" t="s">
         <v>243</v>
       </c>
@@ -11168,12 +11449,12 @@
       <c r="A9" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
       <c r="D9" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="E9" s="60"/>
+      <c r="E9" s="56"/>
       <c r="F9" s="19" t="s">
         <v>244</v>
       </c>
@@ -11186,12 +11467,12 @@
       <c r="A10" s="35" t="s">
         <v>210</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
       <c r="D10" s="35" t="s">
         <v>214</v>
       </c>
-      <c r="E10" s="61"/>
+      <c r="E10" s="57"/>
       <c r="F10" s="36" t="s">
         <v>208</v>
       </c>
@@ -11204,8 +11485,8 @@
       <c r="A11" s="20" t="s">
         <v>211</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
       <c r="D11" s="20" t="s">
         <v>149</v>
       </c>
@@ -11224,13 +11505,13 @@
       <c r="A12" s="20" t="s">
         <v>212</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
       <c r="D12" s="20" t="s">
         <v>150</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>121</v>
+        <v>334</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>124</v>
@@ -11244,10 +11525,10 @@
       <c r="A13" s="27" t="s">
         <v>320</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
       <c r="D13" s="20" t="s">
-        <v>313</v>
+        <v>341</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>317</v>
@@ -11259,6 +11540,26 @@
         <v>25</v>
       </c>
       <c r="H13" s="21"/>
+    </row>
+    <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A14" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="21"/>
     </row>
     <row r="16" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
@@ -11290,16 +11591,16 @@
       <c r="A17" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="58" t="s">
         <v>113</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="E17" s="59" t="s">
+      <c r="E17" s="55" t="s">
         <v>96</v>
       </c>
       <c r="F17" s="14" t="s">
@@ -11314,12 +11615,12 @@
       <c r="A18" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
       <c r="D18" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="E18" s="60"/>
+      <c r="E18" s="56"/>
       <c r="F18" s="14" t="s">
         <v>82</v>
       </c>
@@ -11332,12 +11633,12 @@
       <c r="A19" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
       <c r="D19" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="60"/>
+      <c r="E19" s="56"/>
       <c r="F19" s="14" t="s">
         <v>246</v>
       </c>
@@ -11350,12 +11651,12 @@
       <c r="A20" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
       <c r="D20" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="E20" s="60"/>
+      <c r="E20" s="56"/>
       <c r="F20" s="14" t="s">
         <v>81</v>
       </c>
@@ -11368,12 +11669,12 @@
       <c r="A21" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
       <c r="D21" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="E21" s="60"/>
+      <c r="E21" s="56"/>
       <c r="F21" s="11" t="s">
         <v>247</v>
       </c>
@@ -11386,12 +11687,12 @@
       <c r="A22" s="35" t="s">
         <v>215</v>
       </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
       <c r="D22" s="35" t="s">
         <v>213</v>
       </c>
-      <c r="E22" s="61"/>
+      <c r="E22" s="57"/>
       <c r="F22" s="36" t="s">
         <v>217</v>
       </c>
@@ -11404,8 +11705,8 @@
       <c r="A23" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
       <c r="D23" s="20" t="s">
         <v>102</v>
       </c>
@@ -11424,13 +11725,13 @@
       <c r="A24" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
       <c r="D24" s="20" t="s">
         <v>150</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>121</v>
+        <v>339</v>
       </c>
       <c r="F24" s="20" t="s">
         <v>124</v>
@@ -11442,15 +11743,15 @@
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A25" s="27" t="s">
-        <v>321</v>
-      </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
+        <v>337</v>
+      </c>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
       <c r="D25" s="20" t="s">
-        <v>313</v>
+        <v>336</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>317</v>
+        <v>340</v>
       </c>
       <c r="F25" s="20" t="s">
         <v>318</v>
@@ -11460,11 +11761,35 @@
       </c>
       <c r="H25" s="21"/>
     </row>
+    <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A26" s="27" t="s">
+        <v>338</v>
+      </c>
+      <c r="B26" s="60"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" s="21"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E10"/>
     <mergeCell ref="E17:E22"/>
+    <mergeCell ref="B3:B14"/>
+    <mergeCell ref="C3:C14"/>
+    <mergeCell ref="B17:B26"/>
+    <mergeCell ref="C17:C26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11474,7 +11799,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -11493,14 +11818,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="64"/>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11532,16 +11857,16 @@
       <c r="A3" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="67" t="s">
         <v>185</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="67" t="s">
         <v>115</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="64" t="s">
         <v>122</v>
       </c>
       <c r="F3" s="6" t="s">
@@ -11556,12 +11881,12 @@
       <c r="A4" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="E4" s="66"/>
+      <c r="E4" s="65"/>
       <c r="F4" s="6" t="s">
         <v>84</v>
       </c>
@@ -11574,12 +11899,12 @@
       <c r="A5" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
       <c r="D5" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="66"/>
+      <c r="E5" s="65"/>
       <c r="F5" s="6" t="s">
         <v>249</v>
       </c>
@@ -11592,12 +11917,12 @@
       <c r="A6" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
       <c r="D6" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="E6" s="66"/>
+      <c r="E6" s="65"/>
       <c r="F6" s="6" t="s">
         <v>84</v>
       </c>
@@ -11610,12 +11935,12 @@
       <c r="A7" s="29" t="s">
         <v>196</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
       <c r="D7" s="29" t="s">
         <v>189</v>
       </c>
-      <c r="E7" s="66"/>
+      <c r="E7" s="65"/>
       <c r="F7" s="29" t="s">
         <v>250</v>
       </c>
@@ -11628,12 +11953,12 @@
       <c r="A8" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
       <c r="D8" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="E8" s="67"/>
+      <c r="E8" s="66"/>
       <c r="F8" s="36" t="s">
         <v>225</v>
       </c>
@@ -11646,8 +11971,8 @@
       <c r="A9" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="68"/>
       <c r="D9" s="20" t="s">
         <v>149</v>
       </c>
@@ -11666,8 +11991,8 @@
       <c r="A10" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
       <c r="D10" s="20" t="s">
         <v>150</v>
       </c>
@@ -11684,12 +12009,12 @@
     </row>
     <row r="11" spans="1:8" s="33" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="27" t="s">
-        <v>322</v>
-      </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
+        <v>321</v>
+      </c>
+      <c r="B11" s="68"/>
+      <c r="C11" s="68"/>
       <c r="D11" s="20" t="s">
-        <v>313</v>
+        <v>346</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>317</v>
@@ -11702,256 +12027,300 @@
       </c>
       <c r="H11" s="21"/>
     </row>
-    <row r="12" spans="1:8" s="33" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="9"/>
-      <c r="H12" s="34"/>
+    <row r="12" spans="1:8" s="33" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A12" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="21"/>
     </row>
     <row r="13" spans="1:8" s="33" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="9"/>
+      <c r="H13" s="34"/>
+    </row>
+    <row r="14" spans="1:8" s="33" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="C14" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E14" s="59" t="s">
-        <v>109</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="7"/>
+        <v>198</v>
+      </c>
+      <c r="B15" s="58" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" s="67" t="s">
+        <v>115</v>
+      </c>
       <c r="D15" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E15" s="60"/>
+        <v>187</v>
+      </c>
+      <c r="E15" s="55" t="s">
+        <v>109</v>
+      </c>
       <c r="F15" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="57" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="7"/>
+        <v>199</v>
+      </c>
+      <c r="B16" s="59"/>
+      <c r="C16" s="68"/>
       <c r="D16" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E16" s="60"/>
+        <v>188</v>
+      </c>
+      <c r="E16" s="56"/>
       <c r="F16" s="2" t="s">
-        <v>86</v>
+        <v>252</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B17" s="59"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E17" s="56"/>
+      <c r="F17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
+      <c r="A18" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B17" s="43"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="2" t="s">
+      <c r="B18" s="59"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="60"/>
-      <c r="F17" s="2" t="s">
+      <c r="E18" s="56"/>
+      <c r="F18" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
-      <c r="A18" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E18" s="60"/>
-      <c r="F18" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
-      <c r="A19" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="E19" s="60"/>
-      <c r="F19" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="H19" s="16"/>
+    <row r="19" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+      <c r="A19" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B19" s="59"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="E19" s="56"/>
+      <c r="F19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A20" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="7"/>
+        <v>203</v>
+      </c>
+      <c r="B20" s="59"/>
+      <c r="C20" s="68"/>
       <c r="D20" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="E20" s="60"/>
+        <v>191</v>
+      </c>
+      <c r="E20" s="56"/>
       <c r="F20" s="11" t="s">
         <v>76</v>
       </c>
       <c r="G20" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H20" s="16"/>
+    </row>
+    <row r="21" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
+      <c r="A21" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B21" s="59"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="E21" s="56"/>
+      <c r="F21" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H20" s="16"/>
-    </row>
-    <row r="21" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
-      <c r="A21" s="35" t="s">
+      <c r="H21" s="16"/>
+    </row>
+    <row r="22" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
+      <c r="A22" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="35" t="s">
+      <c r="B22" s="59"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="E21" s="61"/>
-      <c r="F21" s="36" t="s">
+      <c r="E22" s="57"/>
+      <c r="F22" s="36" t="s">
         <v>221</v>
       </c>
-      <c r="G21" s="41" t="s">
+      <c r="G22" s="41" t="s">
         <v>209</v>
       </c>
-      <c r="H21" s="42"/>
-    </row>
-    <row r="22" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A22" s="20" t="s">
+      <c r="H22" s="42"/>
+    </row>
+    <row r="23" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A23" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="20" t="s">
+      <c r="B23" s="59"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E23" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F23" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="G22" s="21" t="s">
+      <c r="G23" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="H22" s="21"/>
-    </row>
-    <row r="23" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
-      <c r="A23" s="20" t="s">
+      <c r="H23" s="21"/>
+    </row>
+    <row r="24" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
+      <c r="A24" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="20" t="s">
+      <c r="B24" s="59"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E24" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F24" s="20" t="s">
         <v>124</v>
-      </c>
-      <c r="G23" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="H23" s="21"/>
-    </row>
-    <row r="24" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A24" s="27" t="s">
-        <v>323</v>
-      </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="20" t="s">
-        <v>313</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>317</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>318</v>
       </c>
       <c r="G24" s="21" t="s">
         <v>25</v>
       </c>
       <c r="H24" s="21"/>
     </row>
+    <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A25" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="B25" s="59"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="21"/>
+    </row>
+    <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A26" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B26" s="60"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" s="21"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="E14:E21"/>
+    <mergeCell ref="E15:E22"/>
     <mergeCell ref="E3:E8"/>
+    <mergeCell ref="B3:B12"/>
+    <mergeCell ref="C3:C12"/>
+    <mergeCell ref="B15:B26"/>
+    <mergeCell ref="C15:C26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11980,14 +12349,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="64"/>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -12019,16 +12388,16 @@
       <c r="A3" s="22">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="58" t="s">
         <v>116</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="55" t="s">
         <v>232</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -12043,12 +12412,12 @@
       <c r="A4" s="22">
         <v>5.2</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="E4" s="60"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="2" t="s">
         <v>99</v>
       </c>
@@ -12061,12 +12430,12 @@
       <c r="A5" s="22">
         <v>5.3</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="E5" s="60"/>
+      <c r="E5" s="56"/>
       <c r="F5" s="2" t="s">
         <v>87</v>
       </c>
@@ -12079,12 +12448,12 @@
       <c r="A6" s="22">
         <v>5.4</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="E6" s="61"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="2" t="s">
         <v>233</v>
       </c>
@@ -12097,12 +12466,12 @@
       <c r="A7" s="22">
         <v>5.5</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="E7" s="50" t="s">
         <v>298</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -12117,8 +12486,8 @@
       <c r="A8" s="27">
         <v>5.6</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
       <c r="D8" s="20" t="s">
         <v>149</v>
       </c>
@@ -12137,8 +12506,8 @@
       <c r="A9" s="27">
         <v>5.7</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
       <c r="D9" s="20" t="s">
         <v>313</v>
       </c>
@@ -12160,9 +12529,11 @@
       <c r="A14" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E6"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="C3:C9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12190,14 +12561,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="64"/>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -12229,16 +12600,16 @@
       <c r="A3" s="22">
         <v>6.1</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="58" t="s">
         <v>117</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="55" t="s">
         <v>281</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -12253,12 +12624,12 @@
       <c r="A4" s="22">
         <v>6.2</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="60"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="2" t="s">
         <v>230</v>
       </c>
@@ -12271,12 +12642,12 @@
       <c r="A5" s="22">
         <v>6.3</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="E5" s="61"/>
+      <c r="E5" s="57"/>
       <c r="F5" s="2" t="s">
         <v>88</v>
       </c>
@@ -12289,8 +12660,8 @@
       <c r="A6" s="24">
         <v>6.4</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="6" t="s">
         <v>227</v>
       </c>
@@ -12309,12 +12680,12 @@
       <c r="A7" s="24">
         <v>6.5</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="E7" s="54" t="s">
+      <c r="E7" s="52" t="s">
         <v>312</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -12327,8 +12698,8 @@
       <c r="A8" s="27">
         <v>6.6</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
       <c r="D8" s="20" t="s">
         <v>149</v>
       </c>
@@ -12347,8 +12718,8 @@
       <c r="A9" s="27">
         <v>6.7</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
       <c r="D9" s="20" t="s">
         <v>313</v>
       </c>
@@ -12367,9 +12738,11 @@
       <c r="B12" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E5"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="C3:C9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12381,7 +12754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -12398,14 +12771,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="64"/>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -12437,16 +12810,16 @@
       <c r="A3" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="58" t="s">
         <v>118</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="55" t="s">
         <v>97</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -12461,12 +12834,12 @@
       <c r="A4" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E4" s="60"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="2" t="s">
         <v>62</v>
       </c>
@@ -12479,12 +12852,12 @@
       <c r="A5" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="E5" s="60"/>
+      <c r="E5" s="56"/>
       <c r="F5" s="2" t="s">
         <v>89</v>
       </c>
@@ -12497,12 +12870,12 @@
       <c r="A6" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="61"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="6" t="s">
         <v>63</v>
       </c>
@@ -12513,28 +12886,28 @@
     </row>
     <row r="7" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
+        <v>325</v>
+      </c>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E7" s="53"/>
+      <c r="F7" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="E7" s="55"/>
-      <c r="F7" s="6" t="s">
-        <v>330</v>
-      </c>
       <c r="G7" s="6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A8" s="20" t="s">
-        <v>325</v>
-      </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
+        <v>323</v>
+      </c>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
       <c r="D8" s="20" t="s">
         <v>149</v>
       </c>
@@ -12551,10 +12924,10 @@
     </row>
     <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A9" s="27" t="s">
-        <v>326</v>
-      </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
+        <v>324</v>
+      </c>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
       <c r="D9" s="20" t="s">
         <v>313</v>
       </c>
@@ -12599,16 +12972,16 @@
       <c r="A12" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="58" t="s">
         <v>75</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="59" t="s">
+      <c r="E12" s="55" t="s">
         <v>98</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -12623,12 +12996,12 @@
       <c r="A13" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
       <c r="D13" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="E13" s="60"/>
+      <c r="E13" s="56"/>
       <c r="F13" s="2" t="s">
         <v>152</v>
       </c>
@@ -12641,12 +13014,12 @@
       <c r="A14" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
       <c r="D14" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="E14" s="60"/>
+      <c r="E14" s="56"/>
       <c r="F14" s="2" t="s">
         <v>67</v>
       </c>
@@ -12659,12 +13032,12 @@
       <c r="A15" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
       <c r="D15" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="61"/>
+      <c r="E15" s="57"/>
       <c r="F15" s="6" t="s">
         <v>70</v>
       </c>
@@ -12675,28 +13048,28 @@
     </row>
     <row r="16" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="B16" s="59"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E16" s="53"/>
+      <c r="F16" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>329</v>
-      </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="E16" s="55"/>
-      <c r="F16" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>331</v>
       </c>
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A17" s="20" t="s">
-        <v>324</v>
-      </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
+        <v>322</v>
+      </c>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
       <c r="D17" s="20" t="s">
         <v>149</v>
       </c>
@@ -12713,10 +13086,10 @@
     </row>
     <row r="18" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A18" s="27" t="s">
-        <v>333</v>
-      </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
+        <v>331</v>
+      </c>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
       <c r="D18" s="20" t="s">
         <v>313</v>
       </c>
@@ -12732,10 +13105,14 @@
       <c r="H18" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E6"/>
     <mergeCell ref="E12:E15"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="C3:C9"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="C12:C18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12763,14 +13140,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="64"/>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -12802,16 +13179,16 @@
       <c r="A3" s="22">
         <v>8.1</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="58" t="s">
         <v>119</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="55" t="s">
         <v>304</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -12828,12 +13205,12 @@
       <c r="A4" s="22">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="60"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="2" t="s">
         <v>52</v>
       </c>
@@ -12846,12 +13223,12 @@
       <c r="A5" s="22">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="E5" s="61"/>
+      <c r="E5" s="57"/>
       <c r="F5" s="2" t="s">
         <v>90</v>
       </c>
@@ -12864,12 +13241,12 @@
       <c r="A6" s="22">
         <v>8.4</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="55" t="s">
         <v>305</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -12884,12 +13261,12 @@
       <c r="A7" s="22">
         <v>8.5</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="E7" s="60"/>
+      <c r="E7" s="56"/>
       <c r="F7" s="2" t="s">
         <v>308</v>
       </c>
@@ -12902,12 +13279,12 @@
       <c r="A8" s="22">
         <v>8.6</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
       <c r="D8" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="E8" s="61"/>
+      <c r="E8" s="57"/>
       <c r="F8" s="2" t="s">
         <v>306</v>
       </c>
@@ -12920,8 +13297,8 @@
       <c r="A9" s="27">
         <v>8.6999999999999993</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
       <c r="D9" s="20" t="s">
         <v>149</v>
       </c>
@@ -12940,8 +13317,8 @@
       <c r="A10" s="27">
         <v>8.8000000000000007</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
       <c r="D10" s="20" t="s">
         <v>313</v>
       </c>
@@ -12961,10 +13338,12 @@
       <c r="B12" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="E6:E8"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="C3:C10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12993,14 +13372,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="64"/>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -13032,10 +13411,10 @@
       <c r="A3" s="22">
         <v>9.1</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="58" t="s">
         <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -13044,7 +13423,7 @@
       <c r="E3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="68" t="s">
+      <c r="F3" s="58" t="s">
         <v>45</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -13056,15 +13435,15 @@
       <c r="A4" s="22">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="69"/>
+      <c r="F4" s="59"/>
       <c r="G4" s="2" t="s">
         <v>47</v>
       </c>
@@ -13074,15 +13453,15 @@
       <c r="A5" s="22">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="69"/>
+      <c r="F5" s="59"/>
       <c r="G5" s="2" t="s">
         <v>47</v>
       </c>
@@ -13092,15 +13471,15 @@
       <c r="A6" s="22">
         <v>9.4</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="69"/>
+      <c r="F6" s="59"/>
       <c r="G6" s="5" t="s">
         <v>47</v>
       </c>
@@ -13110,15 +13489,15 @@
       <c r="A7" s="22">
         <v>9.5</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="70"/>
+      <c r="F7" s="60"/>
       <c r="G7" s="5" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Update the test file of FileOperation as #31 has been fixed
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="374">
   <si>
     <t>删除文件夹</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4606,60 +4606,6 @@
       </rPr>
       <t>）
 2.文件不应该被移动到指定路径</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径
-2.输入文件夹下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件名或扩展名</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -10315,6 +10261,174 @@
         <scheme val="minor"/>
       </rPr>
       <t>Do not input the empty content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2.输入文件夹下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件名或扩展名</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2.在需要找的文件夹或文件输入框内输入空字符串</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:D:\Test
+2.在"P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lease input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" 输入空字符串
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示不能输入空的搜索内容的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Do not input the empty folder or file name, please input again!</t>
     </r>
     <r>
       <rPr>
@@ -10575,7 +10689,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -10759,6 +10873,15 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -10810,20 +10933,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -11150,14 +11267,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="61"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11189,20 +11306,20 @@
       <c r="A3" s="21">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="68" t="s">
         <v>100</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E3" s="65" t="s">
+        <v>329</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="E3" s="62" t="s">
-        <v>330</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>333</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>22</v>
@@ -11213,14 +11330,14 @@
       <c r="A4" s="21">
         <v>1.2</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
       <c r="D4" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E4" s="66"/>
+      <c r="F4" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="E4" s="63"/>
-      <c r="F4" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>23</v>
@@ -11231,14 +11348,14 @@
       <c r="A5" s="21">
         <v>1.3</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="E5" s="66"/>
+      <c r="F5" s="2" t="s">
         <v>336</v>
-      </c>
-      <c r="E5" s="63"/>
-      <c r="F5" s="2" t="s">
-        <v>337</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>24</v>
@@ -11249,14 +11366,14 @@
       <c r="A6" s="21">
         <v>1.4</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E6" s="67"/>
+      <c r="F6" s="2" t="s">
         <v>338</v>
-      </c>
-      <c r="E6" s="64"/>
-      <c r="F6" s="2" t="s">
-        <v>339</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>27</v>
@@ -11267,16 +11384,16 @@
       <c r="A7" s="21">
         <v>1.5</v>
       </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E7" s="52" t="s">
         <v>340</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="F7" s="2" t="s">
         <v>341</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>342</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="57"/>
@@ -11285,16 +11402,16 @@
       <c r="A8" s="26">
         <v>1.6</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
       <c r="D8" s="19" t="s">
         <v>138</v>
       </c>
       <c r="E8" s="19" t="s">
+        <v>342</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>343</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>344</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>95</v>
@@ -11305,16 +11422,16 @@
       <c r="A9" s="26">
         <v>1.7</v>
       </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
       <c r="D9" s="19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E9" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>345</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>346</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -11325,16 +11442,16 @@
       <c r="A10" s="55">
         <v>1.8</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="66"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
       <c r="D10" s="54" t="s">
+        <v>346</v>
+      </c>
+      <c r="E10" s="54" t="s">
         <v>347</v>
       </c>
-      <c r="E10" s="54" t="s">
+      <c r="F10" s="54" t="s">
         <v>348</v>
-      </c>
-      <c r="F10" s="54" t="s">
-        <v>349</v>
       </c>
       <c r="G10" s="59"/>
       <c r="H10" s="59"/>
@@ -11343,16 +11460,16 @@
       <c r="A11" s="60">
         <v>1.9</v>
       </c>
-      <c r="B11" s="67"/>
-      <c r="C11" s="67"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="54" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E11" s="54" t="s">
+        <v>349</v>
+      </c>
+      <c r="F11" s="54" t="s">
         <v>350</v>
-      </c>
-      <c r="F11" s="54" t="s">
-        <v>351</v>
       </c>
       <c r="G11" s="59"/>
       <c r="H11" s="59"/>
@@ -11391,14 +11508,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="71"/>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
+      <c r="A1" s="74"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="42" t="s">
@@ -11430,13 +11547,13 @@
       <c r="A3" s="43">
         <v>10.1</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="82" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="82" t="s">
         <v>153</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="82" t="s">
         <v>154</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -11454,9 +11571,9 @@
       <c r="A4" s="43">
         <v>10.199999999999999</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
       <c r="E4" s="2" t="s">
         <v>156</v>
       </c>
@@ -11472,9 +11589,9 @@
       <c r="A5" s="43">
         <v>10.3</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
       <c r="E5" s="2" t="s">
         <v>157</v>
       </c>
@@ -11490,9 +11607,9 @@
       <c r="A6" s="43">
         <v>10.4</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
       <c r="E6" s="2" t="s">
         <v>158</v>
       </c>
@@ -11508,9 +11625,9 @@
       <c r="A7" s="43">
         <v>10.5</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
       <c r="E7" s="2" t="s">
         <v>159</v>
       </c>
@@ -11526,9 +11643,9 @@
       <c r="A8" s="43">
         <v>10.6</v>
       </c>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
       <c r="E8" s="2" t="s">
         <v>160</v>
       </c>
@@ -11544,9 +11661,9 @@
       <c r="A9" s="43">
         <v>10.7</v>
       </c>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
       <c r="E9" s="2" t="s">
         <v>161</v>
       </c>
@@ -11562,9 +11679,9 @@
       <c r="A10" s="43">
         <v>10.8</v>
       </c>
-      <c r="B10" s="78"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
       <c r="E10" s="2" t="s">
         <v>162</v>
       </c>
@@ -11580,30 +11697,30 @@
       <c r="A11" s="43">
         <v>10.9</v>
       </c>
-      <c r="B11" s="78"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="78"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
       <c r="E11" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>278</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A12" s="49" t="s">
+        <v>273</v>
+      </c>
+      <c r="B12" s="82"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="B12" s="78"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="2" t="s">
-        <v>275</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>21</v>
@@ -11614,11 +11731,11 @@
       <c r="A13" s="45">
         <v>10.11</v>
       </c>
-      <c r="B13" s="78"/>
-      <c r="C13" s="78"/>
-      <c r="D13" s="78"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
       <c r="E13" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>164</v>
@@ -11632,9 +11749,9 @@
       <c r="A14" s="43">
         <v>10.119999999999999</v>
       </c>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
+      <c r="B14" s="82"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="82"/>
       <c r="E14" s="2" t="s">
         <v>163</v>
       </c>
@@ -11680,14 +11797,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="71"/>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
+      <c r="A1" s="74"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11719,20 +11836,20 @@
       <c r="A3" s="21">
         <v>11.1</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="82" t="s">
+        <v>260</v>
+      </c>
+      <c r="C3" s="82" t="s">
         <v>261</v>
       </c>
-      <c r="C3" s="78" t="s">
-        <v>262</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="E3" s="62" t="s">
-        <v>270</v>
+        <v>265</v>
+      </c>
+      <c r="E3" s="65" t="s">
+        <v>269</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>21</v>
@@ -11743,14 +11860,14 @@
       <c r="A4" s="46">
         <v>11.2</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
       <c r="D4" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="E4" s="64"/>
+        <v>266</v>
+      </c>
+      <c r="E4" s="67"/>
       <c r="F4" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>21</v>
@@ -11761,16 +11878,16 @@
       <c r="A5" s="46">
         <v>11.3</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="82"/>
       <c r="D5" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E5" s="62" t="s">
-        <v>271</v>
+        <v>263</v>
+      </c>
+      <c r="E5" s="65" t="s">
+        <v>270</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>21</v>
@@ -11781,14 +11898,14 @@
       <c r="A6" s="47">
         <v>11.4</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
       <c r="D6" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="E6" s="64"/>
+        <v>264</v>
+      </c>
+      <c r="E6" s="67"/>
       <c r="F6" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>21</v>
@@ -11799,8 +11916,8 @@
       <c r="A7" s="48">
         <v>11.5</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
       <c r="D7" s="19" t="s">
         <v>138</v>
       </c>
@@ -11819,16 +11936,16 @@
       <c r="A8" s="48">
         <v>11.6</v>
       </c>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
       <c r="D8" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="E8" s="19" t="s">
         <v>293</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>294</v>
-      </c>
       <c r="F8" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>21</v>
@@ -11871,14 +11988,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="68"/>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
+      <c r="A1" s="71"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11910,10 +12027,10 @@
       <c r="A3" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="68" t="s">
         <v>101</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -11923,7 +12040,7 @@
         <v>69</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>26</v>
@@ -11934,16 +12051,16 @@
       <c r="A4" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
       <c r="D4" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>21</v>
@@ -11954,10 +12071,10 @@
       <c r="A5" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>69</v>
@@ -11974,13 +12091,13 @@
       <c r="A6" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="19" t="s">
         <v>138</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>94</v>
@@ -11992,18 +12109,18 @@
     </row>
     <row r="7" spans="1:9" ht="57" x14ac:dyDescent="0.15">
       <c r="A7" s="26" t="s">
-        <v>295</v>
-      </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
+        <v>294</v>
+      </c>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
       <c r="D7" s="19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E7" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>297</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>298</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>21</v>
@@ -12052,10 +12169,10 @@
       <c r="A10" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="68" t="s">
         <v>101</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -12065,7 +12182,7 @@
         <v>96</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>21</v>
@@ -12077,8 +12194,8 @@
       <c r="A11" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="66"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
@@ -12086,7 +12203,7 @@
         <v>87</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>68</v>
@@ -12100,10 +12217,10 @@
       <c r="A12" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B12" s="66"/>
-      <c r="C12" s="66"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
       <c r="D12" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>86</v>
@@ -12121,8 +12238,8 @@
       <c r="A13" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
       <c r="D13" s="19" t="s">
         <v>138</v>
       </c>
@@ -12139,18 +12256,18 @@
     </row>
     <row r="14" spans="1:9" s="22" customFormat="1" ht="57" x14ac:dyDescent="0.15">
       <c r="A14" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="B14" s="67"/>
-      <c r="C14" s="67"/>
+        <v>298</v>
+      </c>
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
       <c r="D14" s="19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E14" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>297</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>298</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>21</v>
@@ -12159,7 +12276,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
-      <c r="B15" s="69"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -12170,7 +12287,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
-      <c r="B16" s="69"/>
+      <c r="B16" s="72"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -12181,7 +12298,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
-      <c r="B17" s="69"/>
+      <c r="B17" s="72"/>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -12192,7 +12309,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
-      <c r="B18" s="69"/>
+      <c r="B18" s="72"/>
       <c r="C18" s="4"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -12203,7 +12320,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
-      <c r="B19" s="69"/>
+      <c r="B19" s="72"/>
       <c r="C19" s="4"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -12279,14 +12396,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A1" s="70"/>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
+      <c r="A1" s="73"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -12318,20 +12435,20 @@
       <c r="A3" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="68" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="68" t="s">
         <v>103</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E3" s="62" t="s">
+        <v>246</v>
+      </c>
+      <c r="E3" s="65" t="s">
         <v>88</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>21</v>
@@ -12342,14 +12459,14 @@
       <c r="A4" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
       <c r="D4" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E4" s="63"/>
+        <v>247</v>
+      </c>
+      <c r="E4" s="66"/>
       <c r="F4" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>21</v>
@@ -12360,12 +12477,12 @@
       <c r="A5" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="E5" s="63"/>
+        <v>248</v>
+      </c>
+      <c r="E5" s="66"/>
       <c r="F5" s="2" t="s">
         <v>77</v>
       </c>
@@ -12378,14 +12495,14 @@
       <c r="A6" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E6" s="63"/>
+      <c r="E6" s="66"/>
       <c r="F6" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>21</v>
@@ -12396,12 +12513,12 @@
       <c r="A7" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="E7" s="63"/>
+        <v>249</v>
+      </c>
+      <c r="E7" s="66"/>
       <c r="F7" s="2" t="s">
         <v>196</v>
       </c>
@@ -12414,14 +12531,14 @@
       <c r="A8" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
       <c r="D8" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="E8" s="63"/>
+      <c r="E8" s="66"/>
       <c r="F8" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>33</v>
@@ -12432,14 +12549,14 @@
       <c r="A9" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
       <c r="D9" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="E9" s="63"/>
+      <c r="E9" s="66"/>
       <c r="F9" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>21</v>
@@ -12450,12 +12567,12 @@
       <c r="A10" s="34" t="s">
         <v>199</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="66"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
       <c r="D10" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="E10" s="64"/>
+      <c r="E10" s="67"/>
       <c r="F10" s="35" t="s">
         <v>197</v>
       </c>
@@ -12468,8 +12585,8 @@
       <c r="A11" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="66"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="19" t="s">
         <v>138</v>
       </c>
@@ -12488,13 +12605,13 @@
       <c r="A12" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="B12" s="66"/>
-      <c r="C12" s="66"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
       <c r="D12" s="19" t="s">
         <v>139</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F12" s="19" t="s">
         <v>113</v>
@@ -12506,18 +12623,18 @@
     </row>
     <row r="13" spans="1:8" s="22" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A13" s="26" t="s">
-        <v>300</v>
-      </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
+        <v>299</v>
+      </c>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
       <c r="D13" s="19" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E13" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="F13" s="19" t="s">
         <v>297</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>298</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>21</v>
@@ -12526,18 +12643,18 @@
     </row>
     <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A14" s="26" t="s">
-        <v>312</v>
-      </c>
-      <c r="B14" s="67"/>
-      <c r="C14" s="67"/>
+        <v>311</v>
+      </c>
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
       <c r="D14" s="19" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>21</v>
@@ -12574,20 +12691,20 @@
       <c r="A17" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="B17" s="65" t="s">
+      <c r="B17" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="65" t="s">
+      <c r="C17" s="68" t="s">
         <v>102</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="E17" s="62" t="s">
+      <c r="E17" s="65" t="s">
         <v>89</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>21</v>
@@ -12598,12 +12715,12 @@
       <c r="A18" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B18" s="66"/>
-      <c r="C18" s="66"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="69"/>
       <c r="D18" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="E18" s="63"/>
+        <v>250</v>
+      </c>
+      <c r="E18" s="66"/>
       <c r="F18" s="14" t="s">
         <v>76</v>
       </c>
@@ -12616,14 +12733,14 @@
       <c r="A19" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="B19" s="66"/>
-      <c r="C19" s="66"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="69"/>
       <c r="D19" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="63"/>
+      <c r="E19" s="66"/>
       <c r="F19" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G19" s="14" t="s">
         <v>21</v>
@@ -12634,12 +12751,12 @@
       <c r="A20" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="B20" s="66"/>
-      <c r="C20" s="66"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="69"/>
       <c r="D20" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="E20" s="63"/>
+        <v>251</v>
+      </c>
+      <c r="E20" s="66"/>
       <c r="F20" s="14" t="s">
         <v>75</v>
       </c>
@@ -12652,14 +12769,14 @@
       <c r="A21" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B21" s="66"/>
-      <c r="C21" s="66"/>
+      <c r="B21" s="69"/>
+      <c r="C21" s="69"/>
       <c r="D21" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="E21" s="63"/>
+      <c r="E21" s="66"/>
       <c r="F21" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G21" s="15" t="s">
         <v>21</v>
@@ -12670,12 +12787,12 @@
       <c r="A22" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="B22" s="66"/>
-      <c r="C22" s="66"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="69"/>
       <c r="D22" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="E22" s="64"/>
+      <c r="E22" s="67"/>
       <c r="F22" s="35" t="s">
         <v>206</v>
       </c>
@@ -12688,8 +12805,8 @@
       <c r="A23" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B23" s="66"/>
-      <c r="C23" s="66"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="69"/>
       <c r="D23" s="19" t="s">
         <v>92</v>
       </c>
@@ -12708,13 +12825,13 @@
       <c r="A24" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="B24" s="66"/>
-      <c r="C24" s="66"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
       <c r="D24" s="19" t="s">
         <v>139</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F24" s="19" t="s">
         <v>113</v>
@@ -12726,18 +12843,18 @@
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
-        <v>317</v>
-      </c>
-      <c r="B25" s="66"/>
-      <c r="C25" s="66"/>
+        <v>316</v>
+      </c>
+      <c r="B25" s="69"/>
+      <c r="C25" s="69"/>
       <c r="D25" s="19" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>21</v>
@@ -12746,18 +12863,18 @@
     </row>
     <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
-        <v>318</v>
-      </c>
-      <c r="B26" s="67"/>
-      <c r="C26" s="67"/>
+        <v>317</v>
+      </c>
+      <c r="B26" s="70"/>
+      <c r="C26" s="70"/>
       <c r="D26" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>21</v>
@@ -12801,14 +12918,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="71"/>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
+      <c r="A1" s="74"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -12840,20 +12957,20 @@
       <c r="A3" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="78" t="s">
         <v>174</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="78" t="s">
         <v>104</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="E3" s="72" t="s">
+        <v>252</v>
+      </c>
+      <c r="E3" s="75" t="s">
         <v>111</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>31</v>
@@ -12864,12 +12981,12 @@
       <c r="A4" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
       <c r="D4" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="E4" s="73"/>
+        <v>253</v>
+      </c>
+      <c r="E4" s="76"/>
       <c r="F4" s="6" t="s">
         <v>78</v>
       </c>
@@ -12882,14 +12999,14 @@
       <c r="A5" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
       <c r="D5" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="73"/>
+      <c r="E5" s="76"/>
       <c r="F5" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>30</v>
@@ -12900,12 +13017,12 @@
       <c r="A6" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="B6" s="76"/>
-      <c r="C6" s="76"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="79"/>
       <c r="D6" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="E6" s="73"/>
+        <v>254</v>
+      </c>
+      <c r="E6" s="76"/>
       <c r="F6" s="6" t="s">
         <v>78</v>
       </c>
@@ -12918,14 +13035,14 @@
       <c r="A7" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="B7" s="76"/>
-      <c r="C7" s="76"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="79"/>
       <c r="D7" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="E7" s="73"/>
+      <c r="E7" s="76"/>
       <c r="F7" s="28" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G7" s="29" t="s">
         <v>57</v>
@@ -12936,12 +13053,12 @@
       <c r="A8" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="79"/>
       <c r="D8" s="34" t="s">
         <v>212</v>
       </c>
-      <c r="E8" s="74"/>
+      <c r="E8" s="77"/>
       <c r="F8" s="35" t="s">
         <v>214</v>
       </c>
@@ -12954,8 +13071,8 @@
       <c r="A9" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
       <c r="D9" s="19" t="s">
         <v>138</v>
       </c>
@@ -12974,8 +13091,8 @@
       <c r="A10" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="B10" s="76"/>
-      <c r="C10" s="76"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
       <c r="D10" s="19" t="s">
         <v>139</v>
       </c>
@@ -12992,18 +13109,18 @@
     </row>
     <row r="11" spans="1:8" s="32" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="26" t="s">
-        <v>301</v>
-      </c>
-      <c r="B11" s="76"/>
-      <c r="C11" s="76"/>
+        <v>300</v>
+      </c>
+      <c r="B11" s="79"/>
+      <c r="C11" s="79"/>
       <c r="D11" s="19" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E11" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="F11" s="19" t="s">
         <v>297</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>298</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>21</v>
@@ -13012,18 +13129,18 @@
     </row>
     <row r="12" spans="1:8" s="32" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="26" t="s">
-        <v>325</v>
-      </c>
-      <c r="B12" s="77"/>
-      <c r="C12" s="77"/>
+        <v>324</v>
+      </c>
+      <c r="B12" s="80"/>
+      <c r="C12" s="80"/>
       <c r="D12" s="19" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>21</v>
@@ -13069,20 +13186,20 @@
       <c r="A15" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B15" s="65" t="s">
+      <c r="B15" s="68" t="s">
         <v>175</v>
       </c>
-      <c r="C15" s="75" t="s">
+      <c r="C15" s="78" t="s">
         <v>104</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E15" s="62" t="s">
+      <c r="E15" s="65" t="s">
         <v>98</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>21</v>
@@ -13093,14 +13210,14 @@
       <c r="A16" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B16" s="66"/>
-      <c r="C16" s="76"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="79"/>
       <c r="D16" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E16" s="63"/>
+      <c r="E16" s="66"/>
       <c r="F16" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>21</v>
@@ -13111,12 +13228,12 @@
       <c r="A17" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B17" s="66"/>
-      <c r="C17" s="76"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="79"/>
       <c r="D17" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="E17" s="63"/>
+        <v>255</v>
+      </c>
+      <c r="E17" s="66"/>
       <c r="F17" s="2" t="s">
         <v>80</v>
       </c>
@@ -13129,14 +13246,14 @@
       <c r="A18" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B18" s="66"/>
-      <c r="C18" s="76"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="79"/>
       <c r="D18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="63"/>
+      <c r="E18" s="66"/>
       <c r="F18" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>21</v>
@@ -13147,12 +13264,12 @@
       <c r="A19" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="B19" s="66"/>
-      <c r="C19" s="76"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="79"/>
       <c r="D19" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="E19" s="63"/>
+        <v>256</v>
+      </c>
+      <c r="E19" s="66"/>
       <c r="F19" s="2" t="s">
         <v>79</v>
       </c>
@@ -13165,12 +13282,12 @@
       <c r="A20" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="B20" s="66"/>
-      <c r="C20" s="76"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="79"/>
       <c r="D20" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="E20" s="63"/>
+      <c r="E20" s="66"/>
       <c r="F20" s="11" t="s">
         <v>72</v>
       </c>
@@ -13183,12 +13300,12 @@
       <c r="A21" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="B21" s="66"/>
-      <c r="C21" s="76"/>
+      <c r="B21" s="69"/>
+      <c r="C21" s="79"/>
       <c r="D21" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="E21" s="63"/>
+      <c r="E21" s="66"/>
       <c r="F21" s="11" t="s">
         <v>72</v>
       </c>
@@ -13201,12 +13318,12 @@
       <c r="A22" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="B22" s="66"/>
-      <c r="C22" s="76"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="79"/>
       <c r="D22" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="E22" s="64"/>
+      <c r="E22" s="67"/>
       <c r="F22" s="35" t="s">
         <v>210</v>
       </c>
@@ -13219,8 +13336,8 @@
       <c r="A23" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="B23" s="66"/>
-      <c r="C23" s="76"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="79"/>
       <c r="D23" s="19" t="s">
         <v>138</v>
       </c>
@@ -13239,8 +13356,8 @@
       <c r="A24" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="B24" s="66"/>
-      <c r="C24" s="76"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="79"/>
       <c r="D24" s="19" t="s">
         <v>139</v>
       </c>
@@ -13257,18 +13374,18 @@
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
-        <v>323</v>
-      </c>
-      <c r="B25" s="66"/>
-      <c r="C25" s="76"/>
+        <v>322</v>
+      </c>
+      <c r="B25" s="69"/>
+      <c r="C25" s="79"/>
       <c r="D25" s="19" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E25" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="F25" s="19" t="s">
         <v>297</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>298</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>21</v>
@@ -13277,18 +13394,18 @@
     </row>
     <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
-        <v>324</v>
-      </c>
-      <c r="B26" s="67"/>
-      <c r="C26" s="77"/>
+        <v>323</v>
+      </c>
+      <c r="B26" s="70"/>
+      <c r="C26" s="80"/>
       <c r="D26" s="19" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>21</v>
@@ -13315,32 +13432,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.875" style="80" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" style="80" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.375" style="80" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.875" style="80" customWidth="1"/>
-    <col min="5" max="5" width="34.25" style="80" customWidth="1"/>
-    <col min="6" max="6" width="34" style="80" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="80" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.875" style="80" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="80"/>
+    <col min="1" max="1" width="13.875" style="61" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" style="61" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.875" style="61" customWidth="1"/>
+    <col min="5" max="5" width="34.25" style="61" customWidth="1"/>
+    <col min="6" max="6" width="34" style="61" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="61" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.875" style="61" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="61"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="79"/>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
+      <c r="A1" s="81"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
@@ -13372,56 +13489,56 @@
       <c r="A3" s="21">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="68" t="s">
         <v>105</v>
       </c>
       <c r="D3" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="E3" s="65" t="s">
         <v>354</v>
       </c>
-      <c r="E3" s="62" t="s">
+      <c r="F3" s="14" t="s">
         <v>355</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>356</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="81"/>
+      <c r="H3" s="62"/>
     </row>
     <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A4" s="21">
         <v>5.2</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
       <c r="D4" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="E4" s="66"/>
+      <c r="F4" s="14" t="s">
         <v>357</v>
-      </c>
-      <c r="E4" s="63"/>
-      <c r="F4" s="14" t="s">
-        <v>358</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="81"/>
+      <c r="H4" s="62"/>
     </row>
     <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A5" s="21">
         <v>5.3</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="E5" s="66"/>
+      <c r="F5" s="14" t="s">
         <v>359</v>
-      </c>
-      <c r="E5" s="63"/>
-      <c r="F5" s="14" t="s">
-        <v>360</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>22</v>
@@ -13432,54 +13549,54 @@
       <c r="A6" s="21">
         <v>5.4</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="E6" s="67"/>
+      <c r="F6" s="14" t="s">
         <v>361</v>
-      </c>
-      <c r="E6" s="64"/>
-      <c r="F6" s="14" t="s">
-        <v>362</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="81"/>
+      <c r="H6" s="62"/>
     </row>
     <row r="7" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A7" s="21">
         <v>5.5</v>
       </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="E7" s="53" t="s">
         <v>363</v>
       </c>
-      <c r="E7" s="53" t="s">
+      <c r="F7" s="14" t="s">
         <v>364</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>365</v>
-      </c>
       <c r="G7" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="H7" s="81"/>
+        <v>279</v>
+      </c>
+      <c r="H7" s="62"/>
     </row>
     <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A8" s="26">
         <v>5.6</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
       <c r="D8" s="19" t="s">
         <v>138</v>
       </c>
       <c r="E8" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>366</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>367</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>95</v>
@@ -13490,16 +13607,16 @@
       <c r="A9" s="26">
         <v>5.7</v>
       </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
       <c r="D9" s="19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -13510,16 +13627,16 @@
       <c r="A10" s="60">
         <v>5.8</v>
       </c>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="54" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E10" s="54" t="s">
+        <v>368</v>
+      </c>
+      <c r="F10" s="54" t="s">
         <v>369</v>
-      </c>
-      <c r="F10" s="54" t="s">
-        <v>370</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -13527,7 +13644,7 @@
       <c r="H10" s="59"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="82"/>
+      <c r="A14" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -13546,7 +13663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -13562,14 +13679,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="71"/>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
+      <c r="A1" s="74"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -13601,20 +13718,20 @@
       <c r="A3" s="21">
         <v>6.1</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="82" t="s">
         <v>106</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="E3" s="62" t="s">
-        <v>263</v>
+        <v>370</v>
+      </c>
+      <c r="E3" s="65" t="s">
+        <v>262</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>21</v>
@@ -13625,14 +13742,14 @@
       <c r="A4" s="21">
         <v>6.2</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="63"/>
+      <c r="E4" s="66"/>
       <c r="F4" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>27</v>
@@ -13643,12 +13760,12 @@
       <c r="A5" s="21">
         <v>6.3</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="82"/>
       <c r="D5" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="E5" s="64"/>
+        <v>241</v>
+      </c>
+      <c r="E5" s="67"/>
       <c r="F5" s="2" t="s">
         <v>81</v>
       </c>
@@ -13661,16 +13778,16 @@
       <c r="A6" s="23">
         <v>6.4</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
       <c r="D6" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>140</v>
@@ -13681,16 +13798,16 @@
       <c r="A7" s="23">
         <v>6.5</v>
       </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
       <c r="D7" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -13699,8 +13816,8 @@
       <c r="A8" s="26">
         <v>6.6</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
       <c r="D8" s="19" t="s">
         <v>138</v>
       </c>
@@ -13719,21 +13836,41 @@
       <c r="A9" s="26">
         <v>6.7</v>
       </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="67"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="82"/>
       <c r="D9" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>293</v>
       </c>
-      <c r="E9" s="19" t="s">
-        <v>294</v>
-      </c>
       <c r="F9" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="20"/>
+    </row>
+    <row r="10" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
+      <c r="A10" s="83">
+        <v>6.8</v>
+      </c>
+      <c r="B10" s="82"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="54" t="s">
+        <v>371</v>
+      </c>
+      <c r="E10" s="54" t="s">
+        <v>372</v>
+      </c>
+      <c r="F10" s="54" t="s">
+        <v>373</v>
+      </c>
+      <c r="G10" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="59"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B12" s="8"/>
@@ -13742,8 +13879,8 @@
   <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E5"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="C3:C9"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="C3:C10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13772,14 +13909,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="71"/>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
+      <c r="A1" s="74"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -13811,20 +13948,20 @@
       <c r="A3" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="68" t="s">
         <v>107</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="62" t="s">
+      <c r="E3" s="65" t="s">
         <v>90</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -13835,12 +13972,12 @@
       <c r="A4" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
       <c r="D4" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="E4" s="63"/>
+        <v>242</v>
+      </c>
+      <c r="E4" s="66"/>
       <c r="F4" s="2" t="s">
         <v>58</v>
       </c>
@@ -13853,12 +13990,12 @@
       <c r="A5" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="E5" s="63"/>
+        <v>241</v>
+      </c>
+      <c r="E5" s="66"/>
       <c r="F5" s="2" t="s">
         <v>82</v>
       </c>
@@ -13871,12 +14008,12 @@
       <c r="A6" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="64"/>
+      <c r="E6" s="67"/>
       <c r="F6" s="6" t="s">
         <v>59</v>
       </c>
@@ -13887,28 +14024,28 @@
     </row>
     <row r="7" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="2" t="s">
-        <v>306</v>
       </c>
       <c r="E7" s="51"/>
       <c r="F7" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>308</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>309</v>
       </c>
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A8" s="19" t="s">
-        <v>303</v>
-      </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
+        <v>302</v>
+      </c>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
       <c r="D8" s="19" t="s">
         <v>138</v>
       </c>
@@ -13925,18 +14062,18 @@
     </row>
     <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A9" s="26" t="s">
-        <v>304</v>
-      </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="67"/>
+        <v>303</v>
+      </c>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E9" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>297</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>298</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -13973,20 +14110,20 @@
       <c r="A12" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C12" s="68" t="s">
         <v>71</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="62" t="s">
+      <c r="E12" s="65" t="s">
         <v>91</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>21</v>
@@ -13997,12 +14134,12 @@
       <c r="A13" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
       <c r="D13" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="E13" s="63"/>
+        <v>243</v>
+      </c>
+      <c r="E13" s="66"/>
       <c r="F13" s="2" t="s">
         <v>141</v>
       </c>
@@ -14015,12 +14152,12 @@
       <c r="A14" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
       <c r="D14" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="E14" s="63"/>
+        <v>244</v>
+      </c>
+      <c r="E14" s="66"/>
       <c r="F14" s="2" t="s">
         <v>63</v>
       </c>
@@ -14033,12 +14170,12 @@
       <c r="A15" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="B15" s="66"/>
-      <c r="C15" s="66"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
       <c r="D15" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="64"/>
+      <c r="E15" s="67"/>
       <c r="F15" s="6" t="s">
         <v>66</v>
       </c>
@@ -14049,28 +14186,28 @@
     </row>
     <row r="16" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="B16" s="66"/>
-      <c r="C16" s="66"/>
+        <v>306</v>
+      </c>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
       <c r="D16" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E16" s="51"/>
       <c r="F16" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>308</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>309</v>
       </c>
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A17" s="19" t="s">
-        <v>302</v>
-      </c>
-      <c r="B17" s="66"/>
-      <c r="C17" s="66"/>
+        <v>301</v>
+      </c>
+      <c r="B17" s="69"/>
+      <c r="C17" s="69"/>
       <c r="D17" s="19" t="s">
         <v>138</v>
       </c>
@@ -14087,18 +14224,18 @@
     </row>
     <row r="18" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A18" s="26" t="s">
-        <v>311</v>
-      </c>
-      <c r="B18" s="67"/>
-      <c r="C18" s="67"/>
+        <v>310</v>
+      </c>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
       <c r="D18" s="19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E18" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="F18" s="19" t="s">
         <v>297</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>298</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>21</v>
@@ -14141,14 +14278,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="71"/>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
+      <c r="A1" s="74"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -14180,20 +14317,20 @@
       <c r="A3" s="21">
         <v>8.1</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="68" t="s">
         <v>108</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E3" s="62" t="s">
-        <v>284</v>
+      <c r="E3" s="65" t="s">
+        <v>283</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>21</v>
@@ -14206,12 +14343,12 @@
       <c r="A4" s="21">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="63"/>
+      <c r="E4" s="66"/>
       <c r="F4" s="2" t="s">
         <v>48</v>
       </c>
@@ -14224,12 +14361,12 @@
       <c r="A5" s="21">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E5" s="64"/>
+        <v>245</v>
+      </c>
+      <c r="E5" s="67"/>
       <c r="F5" s="2" t="s">
         <v>83</v>
       </c>
@@ -14242,19 +14379,19 @@
       <c r="A6" s="21">
         <v>8.4</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="E6" s="62" t="s">
-        <v>285</v>
+        <v>281</v>
+      </c>
+      <c r="E6" s="65" t="s">
+        <v>284</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -14262,17 +14399,17 @@
       <c r="A7" s="21">
         <v>8.5</v>
       </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="E7" s="63"/>
+        <v>282</v>
+      </c>
+      <c r="E7" s="66"/>
       <c r="F7" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>288</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>289</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -14280,17 +14417,17 @@
       <c r="A8" s="21">
         <v>8.6</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
       <c r="D8" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="E8" s="64"/>
+        <v>280</v>
+      </c>
+      <c r="E8" s="67"/>
       <c r="F8" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -14298,8 +14435,8 @@
       <c r="A9" s="26">
         <v>8.6999999999999993</v>
       </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
       <c r="D9" s="19" t="s">
         <v>138</v>
       </c>
@@ -14318,16 +14455,16 @@
       <c r="A10" s="26">
         <v>8.8000000000000007</v>
       </c>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E10" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="F10" s="19" t="s">
         <v>297</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>298</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>21</v>
@@ -14373,14 +14510,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="71"/>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
+      <c r="A1" s="74"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -14412,10 +14549,10 @@
       <c r="A3" s="21">
         <v>9.1</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="68" t="s">
         <v>36</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -14424,7 +14561,7 @@
       <c r="E3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="68" t="s">
         <v>41</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -14436,15 +14573,15 @@
       <c r="A4" s="21">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="66"/>
+      <c r="F4" s="69"/>
       <c r="G4" s="2" t="s">
         <v>43</v>
       </c>
@@ -14454,15 +14591,15 @@
       <c r="A5" s="21">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="66"/>
+      <c r="F5" s="69"/>
       <c r="G5" s="2" t="s">
         <v>43</v>
       </c>
@@ -14472,15 +14609,15 @@
       <c r="A6" s="21">
         <v>9.4</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="66"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="5" t="s">
         <v>43</v>
       </c>
@@ -14490,15 +14627,15 @@
       <c r="A7" s="21">
         <v>9.5</v>
       </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
       <c r="D7" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="67"/>
+      <c r="F7" s="70"/>
       <c r="G7" s="5" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Update the test file of FileOperation as #32 has been fixed
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="390">
   <si>
     <t>删除文件夹</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -7367,141 +7367,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What word do you want find?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alonso</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What word do you want replace?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Button</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the file or folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>D:\Test\Alonso.txt</t>
     </r>
     <r>
@@ -10440,6 +10305,751 @@
         <scheme val="minor"/>
       </rPr>
       <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the file or folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want find?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alonso</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want replace?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Button</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:D:\Test
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want find?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">",输入空字符
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示需要被替换字符不能为空的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Do not input the empty find content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:D:\Test
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want find?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如Alonso
+3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want replace?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">",输入新的想要被替换的文件夹名为空字符
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示需要新替换字符名称不能为空的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Do not input the empty replace content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2. 根据</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件中的某一字段，输入想要被替换的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>为空字符</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2. 根据</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件中的某一字段，输入想要被替换的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>已有字段</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3. 输入想要被替换的新名称为空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.1.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.2.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件夹名字
+2.输入替换的文件夹名字为</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如D:\TesT39
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what word you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字为空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The format of " D:Test Folder " is incorrect! Should with '\'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示替换内容不能为空的信息
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Do not input empty replace name. Please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件名字
+2.输入替换的文件名字为</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件名字，如D:\TesT39\ALO.bmp
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what word you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件名字为空字符</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -10689,7 +11299,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -10882,6 +11492,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -10939,8 +11552,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -11249,8 +11865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -11267,14 +11883,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="64"/>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
+      <c r="A1" s="65"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11306,20 +11922,20 @@
       <c r="A3" s="21">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="69" t="s">
         <v>100</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E3" s="66" t="s">
+        <v>328</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>331</v>
-      </c>
-      <c r="E3" s="65" t="s">
-        <v>329</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>332</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>22</v>
@@ -11330,14 +11946,14 @@
       <c r="A4" s="21">
         <v>1.2</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E4" s="67"/>
+      <c r="F4" s="2" t="s">
         <v>333</v>
-      </c>
-      <c r="E4" s="66"/>
-      <c r="F4" s="2" t="s">
-        <v>334</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>23</v>
@@ -11348,14 +11964,14 @@
       <c r="A5" s="21">
         <v>1.3</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
       <c r="D5" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E5" s="67"/>
+      <c r="F5" s="2" t="s">
         <v>335</v>
-      </c>
-      <c r="E5" s="66"/>
-      <c r="F5" s="2" t="s">
-        <v>336</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>24</v>
@@ -11366,14 +11982,14 @@
       <c r="A6" s="21">
         <v>1.4</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E6" s="68"/>
+      <c r="F6" s="2" t="s">
         <v>337</v>
-      </c>
-      <c r="E6" s="67"/>
-      <c r="F6" s="2" t="s">
-        <v>338</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>27</v>
@@ -11384,16 +12000,16 @@
       <c r="A7" s="21">
         <v>1.5</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
       <c r="D7" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E7" s="52" t="s">
         <v>339</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="F7" s="2" t="s">
         <v>340</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>341</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="57"/>
@@ -11402,16 +12018,16 @@
       <c r="A8" s="26">
         <v>1.6</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
       <c r="D8" s="19" t="s">
         <v>138</v>
       </c>
       <c r="E8" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>342</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>343</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>95</v>
@@ -11422,16 +12038,16 @@
       <c r="A9" s="26">
         <v>1.7</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E9" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>344</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>345</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -11442,16 +12058,16 @@
       <c r="A10" s="55">
         <v>1.8</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="54" t="s">
+        <v>345</v>
+      </c>
+      <c r="E10" s="54" t="s">
         <v>346</v>
       </c>
-      <c r="E10" s="54" t="s">
+      <c r="F10" s="54" t="s">
         <v>347</v>
-      </c>
-      <c r="F10" s="54" t="s">
-        <v>348</v>
       </c>
       <c r="G10" s="59"/>
       <c r="H10" s="59"/>
@@ -11460,16 +12076,16 @@
       <c r="A11" s="60">
         <v>1.9</v>
       </c>
-      <c r="B11" s="70"/>
-      <c r="C11" s="70"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="71"/>
       <c r="D11" s="54" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E11" s="54" t="s">
+        <v>348</v>
+      </c>
+      <c r="F11" s="54" t="s">
         <v>349</v>
-      </c>
-      <c r="F11" s="54" t="s">
-        <v>350</v>
       </c>
       <c r="G11" s="59"/>
       <c r="H11" s="59"/>
@@ -11508,14 +12124,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
+      <c r="A1" s="75"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="42" t="s">
@@ -11547,13 +12163,13 @@
       <c r="A3" s="43">
         <v>10.1</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="83" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="83" t="s">
         <v>153</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="83" t="s">
         <v>154</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -11571,9 +12187,9 @@
       <c r="A4" s="43">
         <v>10.199999999999999</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
       <c r="E4" s="2" t="s">
         <v>156</v>
       </c>
@@ -11589,9 +12205,9 @@
       <c r="A5" s="43">
         <v>10.3</v>
       </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
       <c r="E5" s="2" t="s">
         <v>157</v>
       </c>
@@ -11607,9 +12223,9 @@
       <c r="A6" s="43">
         <v>10.4</v>
       </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
       <c r="E6" s="2" t="s">
         <v>158</v>
       </c>
@@ -11625,9 +12241,9 @@
       <c r="A7" s="43">
         <v>10.5</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
       <c r="E7" s="2" t="s">
         <v>159</v>
       </c>
@@ -11643,9 +12259,9 @@
       <c r="A8" s="43">
         <v>10.6</v>
       </c>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
       <c r="E8" s="2" t="s">
         <v>160</v>
       </c>
@@ -11661,9 +12277,9 @@
       <c r="A9" s="43">
         <v>10.7</v>
       </c>
-      <c r="B9" s="82"/>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="83"/>
       <c r="E9" s="2" t="s">
         <v>161</v>
       </c>
@@ -11679,9 +12295,9 @@
       <c r="A10" s="43">
         <v>10.8</v>
       </c>
-      <c r="B10" s="82"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="83"/>
       <c r="E10" s="2" t="s">
         <v>162</v>
       </c>
@@ -11697,9 +12313,9 @@
       <c r="A11" s="43">
         <v>10.9</v>
       </c>
-      <c r="B11" s="82"/>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="83"/>
       <c r="E11" s="2" t="s">
         <v>276</v>
       </c>
@@ -11713,9 +12329,9 @@
       <c r="A12" s="49" t="s">
         <v>273</v>
       </c>
-      <c r="B12" s="82"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="82"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
       <c r="E12" s="2" t="s">
         <v>274</v>
       </c>
@@ -11731,9 +12347,9 @@
       <c r="A13" s="45">
         <v>10.11</v>
       </c>
-      <c r="B13" s="82"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="83"/>
       <c r="E13" s="2" t="s">
         <v>275</v>
       </c>
@@ -11749,9 +12365,9 @@
       <c r="A14" s="43">
         <v>10.119999999999999</v>
       </c>
-      <c r="B14" s="82"/>
-      <c r="C14" s="82"/>
-      <c r="D14" s="82"/>
+      <c r="B14" s="83"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="83"/>
       <c r="E14" s="2" t="s">
         <v>163</v>
       </c>
@@ -11797,14 +12413,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
+      <c r="A1" s="75"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11836,16 +12452,16 @@
       <c r="A3" s="21">
         <v>11.1</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="83" t="s">
         <v>260</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="83" t="s">
         <v>261</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="66" t="s">
         <v>269</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -11860,12 +12476,12 @@
       <c r="A4" s="46">
         <v>11.2</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="E4" s="67"/>
+      <c r="E4" s="68"/>
       <c r="F4" s="2" t="s">
         <v>268</v>
       </c>
@@ -11878,12 +12494,12 @@
       <c r="A5" s="46">
         <v>11.3</v>
       </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
       <c r="D5" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="66" t="s">
         <v>270</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -11898,12 +12514,12 @@
       <c r="A6" s="47">
         <v>11.4</v>
       </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
       <c r="D6" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="E6" s="67"/>
+      <c r="E6" s="68"/>
       <c r="F6" s="2" t="s">
         <v>267</v>
       </c>
@@ -11916,8 +12532,8 @@
       <c r="A7" s="48">
         <v>11.5</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
       <c r="D7" s="19" t="s">
         <v>138</v>
       </c>
@@ -11936,16 +12552,16 @@
       <c r="A8" s="48">
         <v>11.6</v>
       </c>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="83"/>
       <c r="D8" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="E8" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>293</v>
-      </c>
       <c r="F8" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>21</v>
@@ -11988,14 +12604,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="71"/>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
+      <c r="A1" s="72"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -12027,10 +12643,10 @@
       <c r="A3" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="69" t="s">
         <v>101</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -12051,8 +12667,8 @@
       <c r="A4" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="2" t="s">
         <v>257</v>
       </c>
@@ -12071,8 +12687,8 @@
       <c r="A5" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
       <c r="D5" s="2" t="s">
         <v>258</v>
       </c>
@@ -12091,13 +12707,13 @@
       <c r="A6" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="19" t="s">
         <v>138</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>94</v>
@@ -12109,18 +12725,18 @@
     </row>
     <row r="7" spans="1:9" ht="57" x14ac:dyDescent="0.15">
       <c r="A7" s="26" t="s">
-        <v>294</v>
-      </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
+        <v>293</v>
+      </c>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
       <c r="D7" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E7" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>296</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>297</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>21</v>
@@ -12169,10 +12785,10 @@
       <c r="A10" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="68" t="s">
+      <c r="C10" s="69" t="s">
         <v>101</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -12194,8 +12810,8 @@
       <c r="A11" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
@@ -12217,8 +12833,8 @@
       <c r="A12" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="2" t="s">
         <v>259</v>
       </c>
@@ -12238,8 +12854,8 @@
       <c r="A13" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
       <c r="D13" s="19" t="s">
         <v>138</v>
       </c>
@@ -12256,18 +12872,18 @@
     </row>
     <row r="14" spans="1:9" s="22" customFormat="1" ht="57" x14ac:dyDescent="0.15">
       <c r="A14" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="70"/>
+        <v>297</v>
+      </c>
+      <c r="B14" s="71"/>
+      <c r="C14" s="71"/>
       <c r="D14" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E14" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>296</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>297</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>21</v>
@@ -12276,7 +12892,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
-      <c r="B15" s="72"/>
+      <c r="B15" s="73"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -12287,7 +12903,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
-      <c r="B16" s="72"/>
+      <c r="B16" s="73"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -12298,7 +12914,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
-      <c r="B17" s="72"/>
+      <c r="B17" s="73"/>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -12309,7 +12925,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
-      <c r="B18" s="72"/>
+      <c r="B18" s="73"/>
       <c r="C18" s="4"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -12320,7 +12936,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
-      <c r="B19" s="72"/>
+      <c r="B19" s="73"/>
       <c r="C19" s="4"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -12396,14 +13012,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A1" s="73"/>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
+      <c r="A1" s="74"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -12435,16 +13051,16 @@
       <c r="A3" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="69" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="69" t="s">
         <v>103</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="66" t="s">
         <v>88</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -12459,12 +13075,12 @@
       <c r="A4" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="66"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="2" t="s">
         <v>225</v>
       </c>
@@ -12477,12 +13093,12 @@
       <c r="A5" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
       <c r="D5" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="E5" s="66"/>
+      <c r="E5" s="67"/>
       <c r="F5" s="2" t="s">
         <v>77</v>
       </c>
@@ -12495,12 +13111,12 @@
       <c r="A6" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E6" s="66"/>
+      <c r="E6" s="67"/>
       <c r="F6" s="2" t="s">
         <v>226</v>
       </c>
@@ -12513,12 +13129,12 @@
       <c r="A7" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
       <c r="D7" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="E7" s="66"/>
+      <c r="E7" s="67"/>
       <c r="F7" s="2" t="s">
         <v>196</v>
       </c>
@@ -12531,12 +13147,12 @@
       <c r="A8" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
       <c r="D8" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="E8" s="66"/>
+      <c r="E8" s="67"/>
       <c r="F8" s="18" t="s">
         <v>227</v>
       </c>
@@ -12549,12 +13165,12 @@
       <c r="A9" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="E9" s="66"/>
+      <c r="E9" s="67"/>
       <c r="F9" s="18" t="s">
         <v>228</v>
       </c>
@@ -12567,12 +13183,12 @@
       <c r="A10" s="34" t="s">
         <v>199</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="E10" s="67"/>
+      <c r="E10" s="68"/>
       <c r="F10" s="35" t="s">
         <v>197</v>
       </c>
@@ -12585,8 +13201,8 @@
       <c r="A11" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="19" t="s">
         <v>138</v>
       </c>
@@ -12605,13 +13221,13 @@
       <c r="A12" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="19" t="s">
         <v>139</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F12" s="19" t="s">
         <v>113</v>
@@ -12623,18 +13239,18 @@
     </row>
     <row r="13" spans="1:8" s="22" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A13" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
+        <v>298</v>
+      </c>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
       <c r="D13" s="19" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E13" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="F13" s="19" t="s">
         <v>296</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>297</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>21</v>
@@ -12643,18 +13259,18 @@
     </row>
     <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A14" s="26" t="s">
-        <v>311</v>
-      </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="70"/>
+        <v>310</v>
+      </c>
+      <c r="B14" s="71"/>
+      <c r="C14" s="71"/>
       <c r="D14" s="19" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>21</v>
@@ -12691,16 +13307,16 @@
       <c r="A17" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="68" t="s">
+      <c r="C17" s="69" t="s">
         <v>102</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="E17" s="65" t="s">
+      <c r="E17" s="66" t="s">
         <v>89</v>
       </c>
       <c r="F17" s="14" t="s">
@@ -12715,12 +13331,12 @@
       <c r="A18" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B18" s="69"/>
-      <c r="C18" s="69"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
       <c r="D18" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="E18" s="66"/>
+      <c r="E18" s="67"/>
       <c r="F18" s="14" t="s">
         <v>76</v>
       </c>
@@ -12733,12 +13349,12 @@
       <c r="A19" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="B19" s="69"/>
-      <c r="C19" s="69"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
       <c r="D19" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="66"/>
+      <c r="E19" s="67"/>
       <c r="F19" s="14" t="s">
         <v>230</v>
       </c>
@@ -12751,12 +13367,12 @@
       <c r="A20" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="B20" s="69"/>
-      <c r="C20" s="69"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
       <c r="D20" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="E20" s="66"/>
+      <c r="E20" s="67"/>
       <c r="F20" s="14" t="s">
         <v>75</v>
       </c>
@@ -12769,12 +13385,12 @@
       <c r="A21" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B21" s="69"/>
-      <c r="C21" s="69"/>
+      <c r="B21" s="70"/>
+      <c r="C21" s="70"/>
       <c r="D21" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="E21" s="66"/>
+      <c r="E21" s="67"/>
       <c r="F21" s="11" t="s">
         <v>231</v>
       </c>
@@ -12787,12 +13403,12 @@
       <c r="A22" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="B22" s="69"/>
-      <c r="C22" s="69"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="70"/>
       <c r="D22" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="E22" s="67"/>
+      <c r="E22" s="68"/>
       <c r="F22" s="35" t="s">
         <v>206</v>
       </c>
@@ -12805,8 +13421,8 @@
       <c r="A23" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B23" s="69"/>
-      <c r="C23" s="69"/>
+      <c r="B23" s="70"/>
+      <c r="C23" s="70"/>
       <c r="D23" s="19" t="s">
         <v>92</v>
       </c>
@@ -12825,13 +13441,13 @@
       <c r="A24" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="B24" s="69"/>
-      <c r="C24" s="69"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="70"/>
       <c r="D24" s="19" t="s">
         <v>139</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F24" s="19" t="s">
         <v>113</v>
@@ -12843,18 +13459,18 @@
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
-        <v>316</v>
-      </c>
-      <c r="B25" s="69"/>
-      <c r="C25" s="69"/>
+        <v>315</v>
+      </c>
+      <c r="B25" s="70"/>
+      <c r="C25" s="70"/>
       <c r="D25" s="19" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>21</v>
@@ -12863,18 +13479,18 @@
     </row>
     <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
-        <v>317</v>
-      </c>
-      <c r="B26" s="70"/>
-      <c r="C26" s="70"/>
+        <v>316</v>
+      </c>
+      <c r="B26" s="71"/>
+      <c r="C26" s="71"/>
       <c r="D26" s="19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>21</v>
@@ -12918,14 +13534,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
+      <c r="A1" s="75"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -12957,16 +13573,16 @@
       <c r="A3" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="79" t="s">
         <v>174</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="79" t="s">
         <v>104</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="76" t="s">
         <v>111</v>
       </c>
       <c r="F3" s="6" t="s">
@@ -12981,12 +13597,12 @@
       <c r="A4" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
       <c r="D4" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="E4" s="76"/>
+      <c r="E4" s="77"/>
       <c r="F4" s="6" t="s">
         <v>78</v>
       </c>
@@ -12999,12 +13615,12 @@
       <c r="A5" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
       <c r="D5" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="76"/>
+      <c r="E5" s="77"/>
       <c r="F5" s="6" t="s">
         <v>233</v>
       </c>
@@ -13017,12 +13633,12 @@
       <c r="A6" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
       <c r="D6" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="E6" s="76"/>
+      <c r="E6" s="77"/>
       <c r="F6" s="6" t="s">
         <v>78</v>
       </c>
@@ -13035,12 +13651,12 @@
       <c r="A7" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
       <c r="D7" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="E7" s="76"/>
+      <c r="E7" s="77"/>
       <c r="F7" s="28" t="s">
         <v>234</v>
       </c>
@@ -13053,12 +13669,12 @@
       <c r="A8" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
       <c r="D8" s="34" t="s">
         <v>212</v>
       </c>
-      <c r="E8" s="77"/>
+      <c r="E8" s="78"/>
       <c r="F8" s="35" t="s">
         <v>214</v>
       </c>
@@ -13071,8 +13687,8 @@
       <c r="A9" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="19" t="s">
         <v>138</v>
       </c>
@@ -13091,8 +13707,8 @@
       <c r="A10" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="19" t="s">
         <v>139</v>
       </c>
@@ -13109,18 +13725,18 @@
     </row>
     <row r="11" spans="1:8" s="32" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="26" t="s">
-        <v>300</v>
-      </c>
-      <c r="B11" s="79"/>
-      <c r="C11" s="79"/>
+        <v>299</v>
+      </c>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E11" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="F11" s="19" t="s">
         <v>296</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>297</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>21</v>
@@ -13129,18 +13745,18 @@
     </row>
     <row r="12" spans="1:8" s="32" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="26" t="s">
-        <v>324</v>
-      </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
+        <v>323</v>
+      </c>
+      <c r="B12" s="81"/>
+      <c r="C12" s="81"/>
       <c r="D12" s="19" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>21</v>
@@ -13186,16 +13802,16 @@
       <c r="A15" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="69" t="s">
         <v>175</v>
       </c>
-      <c r="C15" s="78" t="s">
+      <c r="C15" s="79" t="s">
         <v>104</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E15" s="65" t="s">
+      <c r="E15" s="66" t="s">
         <v>98</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -13210,12 +13826,12 @@
       <c r="A16" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="79"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="80"/>
       <c r="D16" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E16" s="66"/>
+      <c r="E16" s="67"/>
       <c r="F16" s="2" t="s">
         <v>236</v>
       </c>
@@ -13228,12 +13844,12 @@
       <c r="A17" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="79"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="80"/>
       <c r="D17" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E17" s="66"/>
+      <c r="E17" s="67"/>
       <c r="F17" s="2" t="s">
         <v>80</v>
       </c>
@@ -13246,12 +13862,12 @@
       <c r="A18" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B18" s="69"/>
-      <c r="C18" s="79"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="80"/>
       <c r="D18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="66"/>
+      <c r="E18" s="67"/>
       <c r="F18" s="2" t="s">
         <v>237</v>
       </c>
@@ -13264,12 +13880,12 @@
       <c r="A19" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="B19" s="69"/>
-      <c r="C19" s="79"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="80"/>
       <c r="D19" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="E19" s="66"/>
+      <c r="E19" s="67"/>
       <c r="F19" s="2" t="s">
         <v>79</v>
       </c>
@@ -13282,12 +13898,12 @@
       <c r="A20" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="B20" s="69"/>
-      <c r="C20" s="79"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="80"/>
       <c r="D20" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="E20" s="66"/>
+      <c r="E20" s="67"/>
       <c r="F20" s="11" t="s">
         <v>72</v>
       </c>
@@ -13300,12 +13916,12 @@
       <c r="A21" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="B21" s="69"/>
-      <c r="C21" s="79"/>
+      <c r="B21" s="70"/>
+      <c r="C21" s="80"/>
       <c r="D21" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="E21" s="66"/>
+      <c r="E21" s="67"/>
       <c r="F21" s="11" t="s">
         <v>72</v>
       </c>
@@ -13318,12 +13934,12 @@
       <c r="A22" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="B22" s="69"/>
-      <c r="C22" s="79"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="80"/>
       <c r="D22" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="E22" s="67"/>
+      <c r="E22" s="68"/>
       <c r="F22" s="35" t="s">
         <v>210</v>
       </c>
@@ -13336,8 +13952,8 @@
       <c r="A23" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="B23" s="69"/>
-      <c r="C23" s="79"/>
+      <c r="B23" s="70"/>
+      <c r="C23" s="80"/>
       <c r="D23" s="19" t="s">
         <v>138</v>
       </c>
@@ -13356,8 +13972,8 @@
       <c r="A24" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="B24" s="69"/>
-      <c r="C24" s="79"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="80"/>
       <c r="D24" s="19" t="s">
         <v>139</v>
       </c>
@@ -13374,18 +13990,18 @@
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
-        <v>322</v>
-      </c>
-      <c r="B25" s="69"/>
-      <c r="C25" s="79"/>
+        <v>321</v>
+      </c>
+      <c r="B25" s="70"/>
+      <c r="C25" s="80"/>
       <c r="D25" s="19" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E25" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="F25" s="19" t="s">
         <v>296</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>297</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>21</v>
@@ -13394,18 +14010,18 @@
     </row>
     <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
-        <v>323</v>
-      </c>
-      <c r="B26" s="70"/>
-      <c r="C26" s="80"/>
+        <v>322</v>
+      </c>
+      <c r="B26" s="71"/>
+      <c r="C26" s="81"/>
       <c r="D26" s="19" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>21</v>
@@ -13432,8 +14048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:H10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -13450,14 +14066,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="81"/>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
+      <c r="A1" s="82"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
@@ -13489,20 +14105,20 @@
       <c r="A3" s="21">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="69" t="s">
         <v>105</v>
       </c>
       <c r="D3" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="E3" s="66" t="s">
         <v>353</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="F3" s="14" t="s">
         <v>354</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>355</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>34</v>
@@ -13513,14 +14129,14 @@
       <c r="A4" s="21">
         <v>5.2</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="E4" s="67"/>
+      <c r="F4" s="14" t="s">
         <v>356</v>
-      </c>
-      <c r="E4" s="66"/>
-      <c r="F4" s="14" t="s">
-        <v>357</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>27</v>
@@ -13531,14 +14147,14 @@
       <c r="A5" s="21">
         <v>5.3</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
       <c r="D5" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="E5" s="67"/>
+      <c r="F5" s="14" t="s">
         <v>358</v>
-      </c>
-      <c r="E5" s="66"/>
-      <c r="F5" s="14" t="s">
-        <v>359</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>22</v>
@@ -13549,14 +14165,14 @@
       <c r="A6" s="21">
         <v>5.4</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="E6" s="68"/>
+      <c r="F6" s="14" t="s">
         <v>360</v>
-      </c>
-      <c r="E6" s="67"/>
-      <c r="F6" s="14" t="s">
-        <v>361</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>27</v>
@@ -13567,16 +14183,16 @@
       <c r="A7" s="21">
         <v>5.5</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
       <c r="D7" s="14" t="s">
+        <v>361</v>
+      </c>
+      <c r="E7" s="53" t="s">
         <v>362</v>
       </c>
-      <c r="E7" s="53" t="s">
+      <c r="F7" s="14" t="s">
         <v>363</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>364</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>279</v>
@@ -13587,16 +14203,16 @@
       <c r="A8" s="26">
         <v>5.6</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
       <c r="D8" s="19" t="s">
         <v>138</v>
       </c>
       <c r="E8" s="19" t="s">
+        <v>364</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>365</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>366</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>95</v>
@@ -13607,16 +14223,16 @@
       <c r="A9" s="26">
         <v>5.7</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -13627,16 +14243,16 @@
       <c r="A10" s="60">
         <v>5.8</v>
       </c>
-      <c r="B10" s="70"/>
-      <c r="C10" s="70"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
       <c r="D10" s="54" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E10" s="54" t="s">
+        <v>367</v>
+      </c>
+      <c r="F10" s="54" t="s">
         <v>368</v>
-      </c>
-      <c r="F10" s="54" t="s">
-        <v>369</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -13663,7 +14279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -13679,14 +14295,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
+      <c r="A1" s="75"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -13718,16 +14334,16 @@
       <c r="A3" s="21">
         <v>6.1</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="83" t="s">
         <v>106</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="E3" s="65" t="s">
+        <v>369</v>
+      </c>
+      <c r="E3" s="66" t="s">
         <v>262</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -13742,12 +14358,12 @@
       <c r="A4" s="21">
         <v>6.2</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="66"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="2" t="s">
         <v>218</v>
       </c>
@@ -13760,12 +14376,12 @@
       <c r="A5" s="21">
         <v>6.3</v>
       </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
       <c r="D5" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="E5" s="67"/>
+      <c r="E5" s="68"/>
       <c r="F5" s="2" t="s">
         <v>81</v>
       </c>
@@ -13778,13 +14394,13 @@
       <c r="A6" s="23">
         <v>6.4</v>
       </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
       <c r="D6" s="6" t="s">
         <v>215</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>217</v>
@@ -13798,13 +14414,13 @@
       <c r="A7" s="23">
         <v>6.5</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
       <c r="D7" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>278</v>
@@ -13816,8 +14432,8 @@
       <c r="A8" s="26">
         <v>6.6</v>
       </c>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="83"/>
       <c r="D8" s="19" t="s">
         <v>138</v>
       </c>
@@ -13836,16 +14452,16 @@
       <c r="A9" s="26">
         <v>6.7</v>
       </c>
-      <c r="B9" s="82"/>
-      <c r="C9" s="82"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="83"/>
       <c r="D9" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="E9" s="19" t="s">
-        <v>293</v>
-      </c>
       <c r="F9" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -13853,19 +14469,19 @@
       <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
-      <c r="A10" s="83">
+      <c r="A10" s="64">
         <v>6.8</v>
       </c>
-      <c r="B10" s="82"/>
-      <c r="C10" s="82"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="83"/>
       <c r="D10" s="54" t="s">
+        <v>370</v>
+      </c>
+      <c r="E10" s="54" t="s">
         <v>371</v>
       </c>
-      <c r="E10" s="54" t="s">
+      <c r="F10" s="54" t="s">
         <v>372</v>
-      </c>
-      <c r="F10" s="54" t="s">
-        <v>373</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -13890,7 +14506,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -13909,14 +14525,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
+      <c r="A1" s="75"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -13948,16 +14564,16 @@
       <c r="A3" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="69" t="s">
         <v>107</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="66" t="s">
         <v>90</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -13972,12 +14588,12 @@
       <c r="A4" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="E4" s="66"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="2" t="s">
         <v>58</v>
       </c>
@@ -13990,12 +14606,12 @@
       <c r="A5" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
       <c r="D5" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="E5" s="66"/>
+      <c r="E5" s="67"/>
       <c r="F5" s="2" t="s">
         <v>82</v>
       </c>
@@ -14008,12 +14624,12 @@
       <c r="A6" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="67"/>
+      <c r="E6" s="68"/>
       <c r="F6" s="6" t="s">
         <v>59</v>
       </c>
@@ -14024,28 +14640,28 @@
     </row>
     <row r="7" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="2" t="s">
-        <v>305</v>
       </c>
       <c r="E7" s="51"/>
       <c r="F7" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>307</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>308</v>
       </c>
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A8" s="19" t="s">
-        <v>302</v>
-      </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
+        <v>301</v>
+      </c>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
       <c r="D8" s="19" t="s">
         <v>138</v>
       </c>
@@ -14062,86 +14678,88 @@
     </row>
     <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A9" s="26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B9" s="70"/>
       <c r="C9" s="70"/>
       <c r="D9" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>297</v>
+        <v>385</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="20"/>
     </row>
-    <row r="11" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
+    <row r="10" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
+      <c r="A10" s="55" t="s">
+        <v>381</v>
+      </c>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="54" t="s">
+        <v>383</v>
+      </c>
+      <c r="E10" s="54" t="s">
+        <v>384</v>
+      </c>
+      <c r="F10" s="54" t="s">
+        <v>386</v>
+      </c>
+      <c r="G10" s="59" t="s">
+        <v>387</v>
+      </c>
+      <c r="H10" s="59"/>
+    </row>
+    <row r="12" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="114" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:8" ht="114" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B12" s="68" t="s">
+      <c r="B13" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="68" t="s">
+      <c r="C13" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="65" t="s">
+      <c r="E13" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
-      <c r="A13" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="E13" s="66"/>
-      <c r="F13" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>21</v>
@@ -14150,107 +14768,145 @@
     </row>
     <row r="14" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B14" s="69"/>
-      <c r="C14" s="69"/>
+        <v>147</v>
+      </c>
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
       <c r="D14" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="E14" s="66"/>
+        <v>243</v>
+      </c>
+      <c r="E14" s="67"/>
       <c r="F14" s="2" t="s">
-        <v>63</v>
+        <v>141</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+      <c r="A15" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E15" s="67"/>
+      <c r="F15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
+      <c r="A16" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="6" t="s">
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="67"/>
-      <c r="F15" s="6" t="s">
+      <c r="E16" s="68"/>
+      <c r="F16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
-      <c r="A16" s="6" t="s">
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
+      <c r="A17" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E17" s="51"/>
+      <c r="F17" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E16" s="51"/>
-      <c r="F16" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A17" s="19" t="s">
-        <v>301</v>
-      </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="H17" s="20"/>
-    </row>
-    <row r="18" spans="1:8" ht="57" x14ac:dyDescent="0.15">
-      <c r="A18" s="26" t="s">
-        <v>310</v>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A18" s="19" t="s">
+        <v>300</v>
       </c>
       <c r="B18" s="70"/>
       <c r="C18" s="70"/>
       <c r="D18" s="19" t="s">
-        <v>292</v>
+        <v>138</v>
       </c>
       <c r="E18" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H18" s="20"/>
+    </row>
+    <row r="19" spans="1:8" ht="57" x14ac:dyDescent="0.15">
+      <c r="A19" s="26" t="s">
+        <v>309</v>
+      </c>
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="F19" s="19" t="s">
         <v>296</v>
       </c>
-      <c r="F18" s="19" t="s">
-        <v>297</v>
-      </c>
-      <c r="G18" s="20" t="s">
+      <c r="G19" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="20"/>
+      <c r="H19" s="20"/>
+    </row>
+    <row r="20" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
+      <c r="A20" s="55" t="s">
+        <v>382</v>
+      </c>
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="54" t="s">
+        <v>388</v>
+      </c>
+      <c r="E20" s="54" t="s">
+        <v>389</v>
+      </c>
+      <c r="F20" s="54" t="s">
+        <v>386</v>
+      </c>
+      <c r="G20" s="59" t="s">
+        <v>387</v>
+      </c>
+      <c r="H20" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E6"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="C3:C9"/>
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="C12:C18"/>
+    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="B13:B20"/>
+    <mergeCell ref="C13:C20"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="C3:C10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14278,14 +14934,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
+      <c r="A1" s="75"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -14317,17 +14973,17 @@
       <c r="A3" s="21">
         <v>8.1</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="69" t="s">
         <v>108</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E3" s="65" t="s">
-        <v>283</v>
+      <c r="E3" s="66" t="s">
+        <v>373</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>240</v>
@@ -14343,12 +14999,12 @@
       <c r="A4" s="21">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="66"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="2" t="s">
         <v>48</v>
       </c>
@@ -14361,12 +15017,12 @@
       <c r="A5" s="21">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
       <c r="D5" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="E5" s="67"/>
+      <c r="E5" s="68"/>
       <c r="F5" s="2" t="s">
         <v>83</v>
       </c>
@@ -14379,19 +15035,19 @@
       <c r="A6" s="21">
         <v>8.4</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="E6" s="65" t="s">
-        <v>284</v>
+      <c r="E6" s="66" t="s">
+        <v>283</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -14399,17 +15055,17 @@
       <c r="A7" s="21">
         <v>8.5</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
       <c r="D7" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="E7" s="66"/>
+      <c r="E7" s="67"/>
       <c r="F7" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>288</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -14417,17 +15073,17 @@
       <c r="A8" s="21">
         <v>8.6</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
       <c r="D8" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="E8" s="67"/>
+      <c r="E8" s="68"/>
       <c r="F8" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -14435,8 +15091,8 @@
       <c r="A9" s="26">
         <v>8.6999999999999993</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="19" t="s">
         <v>138</v>
       </c>
@@ -14458,30 +15114,66 @@
       <c r="B10" s="70"/>
       <c r="C10" s="70"/>
       <c r="D10" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E10" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="F10" s="19" t="s">
         <v>296</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>297</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>21</v>
       </c>
       <c r="H10" s="20"/>
     </row>
-    <row r="12" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A12" s="9"/>
-      <c r="B12" s="8"/>
+    <row r="11" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+      <c r="A11" s="84">
+        <v>8.9</v>
+      </c>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="54" t="s">
+        <v>379</v>
+      </c>
+      <c r="E11" s="55" t="s">
+        <v>374</v>
+      </c>
+      <c r="F11" s="55" t="s">
+        <v>375</v>
+      </c>
+      <c r="G11" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="60"/>
+    </row>
+    <row r="12" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
+      <c r="A12" s="85" t="s">
+        <v>378</v>
+      </c>
+      <c r="B12" s="71"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="54" t="s">
+        <v>380</v>
+      </c>
+      <c r="E12" s="55" t="s">
+        <v>376</v>
+      </c>
+      <c r="F12" s="55" t="s">
+        <v>377</v>
+      </c>
+      <c r="G12" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="E6:E8"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="B3:B12"/>
+    <mergeCell ref="C3:C12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14510,14 +15202,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
+      <c r="A1" s="75"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -14549,10 +15241,10 @@
       <c r="A3" s="21">
         <v>9.1</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="69" t="s">
         <v>36</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -14561,7 +15253,7 @@
       <c r="E3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="68" t="s">
+      <c r="F3" s="69" t="s">
         <v>41</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -14573,15 +15265,15 @@
       <c r="A4" s="21">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="69"/>
+      <c r="F4" s="70"/>
       <c r="G4" s="2" t="s">
         <v>43</v>
       </c>
@@ -14591,15 +15283,15 @@
       <c r="A5" s="21">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
       <c r="D5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="69"/>
+      <c r="F5" s="70"/>
       <c r="G5" s="2" t="s">
         <v>43</v>
       </c>
@@ -14609,15 +15301,15 @@
       <c r="A6" s="21">
         <v>9.4</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="69"/>
+      <c r="F6" s="70"/>
       <c r="G6" s="5" t="s">
         <v>43</v>
       </c>
@@ -14627,15 +15319,15 @@
       <c r="A7" s="21">
         <v>9.5</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
       <c r="D7" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="70"/>
+      <c r="F7" s="71"/>
       <c r="G7" s="5" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Update the test case file after updated hint message on replace content on txt files
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -9166,36 +9166,6 @@
   </si>
   <si>
     <r>
-      <t>提示请不要输入空查找内容的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Do not input the empty original name,please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1.在"</t>
     </r>
     <r>
@@ -9268,36 +9238,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>",输入想要替换成的新内容，输入空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示请不要输入空的替换内容信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Do not input the empty replace name,please input again</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>!）</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -11050,6 +10990,66 @@
         <scheme val="minor"/>
       </rPr>
       <t>",输入新的想要被替换的文件名字为空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示请不要输入空的替换内容信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty replace content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示请不要输入空查找内容的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty search content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -11495,6 +11495,12 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -11551,12 +11557,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -11883,14 +11883,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="65"/>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
+      <c r="A1" s="67"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11922,16 +11922,16 @@
       <c r="A3" s="21">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="71" t="s">
         <v>100</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="E3" s="66" t="s">
+      <c r="E3" s="68" t="s">
         <v>328</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -11946,12 +11946,12 @@
       <c r="A4" s="21">
         <v>1.2</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
       <c r="D4" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="E4" s="67"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="2" t="s">
         <v>333</v>
       </c>
@@ -11964,12 +11964,12 @@
       <c r="A5" s="21">
         <v>1.3</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
       <c r="D5" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="E5" s="67"/>
+      <c r="E5" s="69"/>
       <c r="F5" s="2" t="s">
         <v>335</v>
       </c>
@@ -11982,12 +11982,12 @@
       <c r="A6" s="21">
         <v>1.4</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
       <c r="D6" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="E6" s="68"/>
+      <c r="E6" s="70"/>
       <c r="F6" s="2" t="s">
         <v>337</v>
       </c>
@@ -12000,8 +12000,8 @@
       <c r="A7" s="21">
         <v>1.5</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
       <c r="D7" s="2" t="s">
         <v>338</v>
       </c>
@@ -12018,8 +12018,8 @@
       <c r="A8" s="26">
         <v>1.6</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
       <c r="D8" s="19" t="s">
         <v>138</v>
       </c>
@@ -12038,8 +12038,8 @@
       <c r="A9" s="26">
         <v>1.7</v>
       </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="70"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="72"/>
       <c r="D9" s="19" t="s">
         <v>291</v>
       </c>
@@ -12058,8 +12058,8 @@
       <c r="A10" s="55">
         <v>1.8</v>
       </c>
-      <c r="B10" s="70"/>
-      <c r="C10" s="70"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="72"/>
       <c r="D10" s="54" t="s">
         <v>345</v>
       </c>
@@ -12067,7 +12067,7 @@
         <v>346</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>347</v>
+        <v>389</v>
       </c>
       <c r="G10" s="59"/>
       <c r="H10" s="59"/>
@@ -12076,16 +12076,16 @@
       <c r="A11" s="60">
         <v>1.9</v>
       </c>
-      <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
       <c r="D11" s="54" t="s">
         <v>329</v>
       </c>
       <c r="E11" s="54" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F11" s="54" t="s">
-        <v>349</v>
+        <v>388</v>
       </c>
       <c r="G11" s="59"/>
       <c r="H11" s="59"/>
@@ -12124,14 +12124,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="75"/>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
+      <c r="A1" s="77"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="42" t="s">
@@ -12163,13 +12163,13 @@
       <c r="A3" s="43">
         <v>10.1</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="85" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="85" t="s">
         <v>153</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="85" t="s">
         <v>154</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -12187,9 +12187,9 @@
       <c r="A4" s="43">
         <v>10.199999999999999</v>
       </c>
-      <c r="B4" s="83"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
       <c r="E4" s="2" t="s">
         <v>156</v>
       </c>
@@ -12205,9 +12205,9 @@
       <c r="A5" s="43">
         <v>10.3</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
       <c r="E5" s="2" t="s">
         <v>157</v>
       </c>
@@ -12223,9 +12223,9 @@
       <c r="A6" s="43">
         <v>10.4</v>
       </c>
-      <c r="B6" s="83"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
       <c r="E6" s="2" t="s">
         <v>158</v>
       </c>
@@ -12241,9 +12241,9 @@
       <c r="A7" s="43">
         <v>10.5</v>
       </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
       <c r="E7" s="2" t="s">
         <v>159</v>
       </c>
@@ -12259,9 +12259,9 @@
       <c r="A8" s="43">
         <v>10.6</v>
       </c>
-      <c r="B8" s="83"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="85"/>
       <c r="E8" s="2" t="s">
         <v>160</v>
       </c>
@@ -12277,9 +12277,9 @@
       <c r="A9" s="43">
         <v>10.7</v>
       </c>
-      <c r="B9" s="83"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="83"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="85"/>
       <c r="E9" s="2" t="s">
         <v>161</v>
       </c>
@@ -12295,9 +12295,9 @@
       <c r="A10" s="43">
         <v>10.8</v>
       </c>
-      <c r="B10" s="83"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="83"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
       <c r="E10" s="2" t="s">
         <v>162</v>
       </c>
@@ -12313,9 +12313,9 @@
       <c r="A11" s="43">
         <v>10.9</v>
       </c>
-      <c r="B11" s="83"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="83"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="85"/>
+      <c r="D11" s="85"/>
       <c r="E11" s="2" t="s">
         <v>276</v>
       </c>
@@ -12329,9 +12329,9 @@
       <c r="A12" s="49" t="s">
         <v>273</v>
       </c>
-      <c r="B12" s="83"/>
-      <c r="C12" s="83"/>
-      <c r="D12" s="83"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="85"/>
       <c r="E12" s="2" t="s">
         <v>274</v>
       </c>
@@ -12347,9 +12347,9 @@
       <c r="A13" s="45">
         <v>10.11</v>
       </c>
-      <c r="B13" s="83"/>
-      <c r="C13" s="83"/>
-      <c r="D13" s="83"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
       <c r="E13" s="2" t="s">
         <v>275</v>
       </c>
@@ -12365,9 +12365,9 @@
       <c r="A14" s="43">
         <v>10.119999999999999</v>
       </c>
-      <c r="B14" s="83"/>
-      <c r="C14" s="83"/>
-      <c r="D14" s="83"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
       <c r="E14" s="2" t="s">
         <v>163</v>
       </c>
@@ -12413,14 +12413,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="75"/>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
+      <c r="A1" s="77"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -12452,16 +12452,16 @@
       <c r="A3" s="21">
         <v>11.1</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="85" t="s">
         <v>260</v>
       </c>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="85" t="s">
         <v>261</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="E3" s="66" t="s">
+      <c r="E3" s="68" t="s">
         <v>269</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -12476,12 +12476,12 @@
       <c r="A4" s="46">
         <v>11.2</v>
       </c>
-      <c r="B4" s="83"/>
-      <c r="C4" s="83"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
       <c r="D4" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="E4" s="68"/>
+      <c r="E4" s="70"/>
       <c r="F4" s="2" t="s">
         <v>268</v>
       </c>
@@ -12494,12 +12494,12 @@
       <c r="A5" s="46">
         <v>11.3</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
       <c r="D5" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="E5" s="66" t="s">
+      <c r="E5" s="68" t="s">
         <v>270</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -12514,12 +12514,12 @@
       <c r="A6" s="47">
         <v>11.4</v>
       </c>
-      <c r="B6" s="83"/>
-      <c r="C6" s="83"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="E6" s="68"/>
+      <c r="E6" s="70"/>
       <c r="F6" s="2" t="s">
         <v>267</v>
       </c>
@@ -12532,8 +12532,8 @@
       <c r="A7" s="48">
         <v>11.5</v>
       </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="83"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
       <c r="D7" s="19" t="s">
         <v>138</v>
       </c>
@@ -12552,8 +12552,8 @@
       <c r="A8" s="48">
         <v>11.6</v>
       </c>
-      <c r="B8" s="83"/>
-      <c r="C8" s="83"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
       <c r="D8" s="19" t="s">
         <v>291</v>
       </c>
@@ -12604,14 +12604,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="72"/>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
+      <c r="A1" s="74"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -12643,10 +12643,10 @@
       <c r="A3" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="71" t="s">
         <v>101</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -12667,8 +12667,8 @@
       <c r="A4" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
       <c r="D4" s="2" t="s">
         <v>257</v>
       </c>
@@ -12687,8 +12687,8 @@
       <c r="A5" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
       <c r="D5" s="2" t="s">
         <v>258</v>
       </c>
@@ -12707,8 +12707,8 @@
       <c r="A6" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
       <c r="D6" s="19" t="s">
         <v>138</v>
       </c>
@@ -12727,8 +12727,8 @@
       <c r="A7" s="26" t="s">
         <v>293</v>
       </c>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
       <c r="D7" s="19" t="s">
         <v>291</v>
       </c>
@@ -12785,10 +12785,10 @@
       <c r="A10" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="69" t="s">
+      <c r="C10" s="71" t="s">
         <v>101</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -12810,8 +12810,8 @@
       <c r="A11" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="70"/>
-      <c r="C11" s="70"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="72"/>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
@@ -12833,8 +12833,8 @@
       <c r="A12" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B12" s="70"/>
-      <c r="C12" s="70"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="72"/>
       <c r="D12" s="2" t="s">
         <v>259</v>
       </c>
@@ -12854,8 +12854,8 @@
       <c r="A13" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="B13" s="70"/>
-      <c r="C13" s="70"/>
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
       <c r="D13" s="19" t="s">
         <v>138</v>
       </c>
@@ -12874,8 +12874,8 @@
       <c r="A14" s="26" t="s">
         <v>297</v>
       </c>
-      <c r="B14" s="71"/>
-      <c r="C14" s="71"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
       <c r="D14" s="19" t="s">
         <v>291</v>
       </c>
@@ -12892,7 +12892,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
-      <c r="B15" s="73"/>
+      <c r="B15" s="75"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -12903,7 +12903,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
-      <c r="B16" s="73"/>
+      <c r="B16" s="75"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -12914,7 +12914,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
-      <c r="B17" s="73"/>
+      <c r="B17" s="75"/>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -12925,7 +12925,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
-      <c r="B18" s="73"/>
+      <c r="B18" s="75"/>
       <c r="C18" s="4"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -12936,7 +12936,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
-      <c r="B19" s="73"/>
+      <c r="B19" s="75"/>
       <c r="C19" s="4"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -13012,14 +13012,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
+      <c r="A1" s="76"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -13051,16 +13051,16 @@
       <c r="A3" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="71" t="s">
         <v>103</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="E3" s="66" t="s">
+      <c r="E3" s="68" t="s">
         <v>88</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -13075,12 +13075,12 @@
       <c r="A4" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
       <c r="D4" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="67"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="2" t="s">
         <v>225</v>
       </c>
@@ -13093,12 +13093,12 @@
       <c r="A5" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
       <c r="D5" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="E5" s="67"/>
+      <c r="E5" s="69"/>
       <c r="F5" s="2" t="s">
         <v>77</v>
       </c>
@@ -13111,12 +13111,12 @@
       <c r="A6" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
       <c r="D6" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E6" s="67"/>
+      <c r="E6" s="69"/>
       <c r="F6" s="2" t="s">
         <v>226</v>
       </c>
@@ -13129,12 +13129,12 @@
       <c r="A7" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
       <c r="D7" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="E7" s="67"/>
+      <c r="E7" s="69"/>
       <c r="F7" s="2" t="s">
         <v>196</v>
       </c>
@@ -13147,12 +13147,12 @@
       <c r="A8" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
       <c r="D8" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="E8" s="67"/>
+      <c r="E8" s="69"/>
       <c r="F8" s="18" t="s">
         <v>227</v>
       </c>
@@ -13165,12 +13165,12 @@
       <c r="A9" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="70"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="72"/>
       <c r="D9" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="E9" s="67"/>
+      <c r="E9" s="69"/>
       <c r="F9" s="18" t="s">
         <v>228</v>
       </c>
@@ -13183,12 +13183,12 @@
       <c r="A10" s="34" t="s">
         <v>199</v>
       </c>
-      <c r="B10" s="70"/>
-      <c r="C10" s="70"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="72"/>
       <c r="D10" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="E10" s="68"/>
+      <c r="E10" s="70"/>
       <c r="F10" s="35" t="s">
         <v>197</v>
       </c>
@@ -13201,8 +13201,8 @@
       <c r="A11" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="B11" s="70"/>
-      <c r="C11" s="70"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="72"/>
       <c r="D11" s="19" t="s">
         <v>138</v>
       </c>
@@ -13221,8 +13221,8 @@
       <c r="A12" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="B12" s="70"/>
-      <c r="C12" s="70"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="72"/>
       <c r="D12" s="19" t="s">
         <v>139</v>
       </c>
@@ -13241,8 +13241,8 @@
       <c r="A13" s="26" t="s">
         <v>298</v>
       </c>
-      <c r="B13" s="70"/>
-      <c r="C13" s="70"/>
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
       <c r="D13" s="19" t="s">
         <v>319</v>
       </c>
@@ -13261,8 +13261,8 @@
       <c r="A14" s="26" t="s">
         <v>310</v>
       </c>
-      <c r="B14" s="71"/>
-      <c r="C14" s="71"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
       <c r="D14" s="19" t="s">
         <v>320</v>
       </c>
@@ -13307,16 +13307,16 @@
       <c r="A17" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="B17" s="69" t="s">
+      <c r="B17" s="71" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="69" t="s">
+      <c r="C17" s="71" t="s">
         <v>102</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="E17" s="66" t="s">
+      <c r="E17" s="68" t="s">
         <v>89</v>
       </c>
       <c r="F17" s="14" t="s">
@@ -13331,12 +13331,12 @@
       <c r="A18" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B18" s="70"/>
-      <c r="C18" s="70"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="72"/>
       <c r="D18" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="E18" s="67"/>
+      <c r="E18" s="69"/>
       <c r="F18" s="14" t="s">
         <v>76</v>
       </c>
@@ -13349,12 +13349,12 @@
       <c r="A19" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="B19" s="70"/>
-      <c r="C19" s="70"/>
+      <c r="B19" s="72"/>
+      <c r="C19" s="72"/>
       <c r="D19" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="67"/>
+      <c r="E19" s="69"/>
       <c r="F19" s="14" t="s">
         <v>230</v>
       </c>
@@ -13367,12 +13367,12 @@
       <c r="A20" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
+      <c r="B20" s="72"/>
+      <c r="C20" s="72"/>
       <c r="D20" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="E20" s="67"/>
+      <c r="E20" s="69"/>
       <c r="F20" s="14" t="s">
         <v>75</v>
       </c>
@@ -13385,12 +13385,12 @@
       <c r="A21" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B21" s="70"/>
-      <c r="C21" s="70"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="72"/>
       <c r="D21" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="E21" s="67"/>
+      <c r="E21" s="69"/>
       <c r="F21" s="11" t="s">
         <v>231</v>
       </c>
@@ -13403,12 +13403,12 @@
       <c r="A22" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="B22" s="70"/>
-      <c r="C22" s="70"/>
+      <c r="B22" s="72"/>
+      <c r="C22" s="72"/>
       <c r="D22" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="E22" s="68"/>
+      <c r="E22" s="70"/>
       <c r="F22" s="35" t="s">
         <v>206</v>
       </c>
@@ -13421,8 +13421,8 @@
       <c r="A23" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B23" s="70"/>
-      <c r="C23" s="70"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="72"/>
       <c r="D23" s="19" t="s">
         <v>92</v>
       </c>
@@ -13441,8 +13441,8 @@
       <c r="A24" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="B24" s="70"/>
-      <c r="C24" s="70"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
       <c r="D24" s="19" t="s">
         <v>139</v>
       </c>
@@ -13461,8 +13461,8 @@
       <c r="A25" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="B25" s="70"/>
-      <c r="C25" s="70"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="72"/>
       <c r="D25" s="19" t="s">
         <v>314</v>
       </c>
@@ -13481,8 +13481,8 @@
       <c r="A26" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="B26" s="71"/>
-      <c r="C26" s="71"/>
+      <c r="B26" s="73"/>
+      <c r="C26" s="73"/>
       <c r="D26" s="19" t="s">
         <v>311</v>
       </c>
@@ -13534,14 +13534,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="75"/>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
+      <c r="A1" s="77"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -13573,16 +13573,16 @@
       <c r="A3" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="81" t="s">
         <v>174</v>
       </c>
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="81" t="s">
         <v>104</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="E3" s="76" t="s">
+      <c r="E3" s="78" t="s">
         <v>111</v>
       </c>
       <c r="F3" s="6" t="s">
@@ -13597,12 +13597,12 @@
       <c r="A4" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
       <c r="D4" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="E4" s="77"/>
+      <c r="E4" s="79"/>
       <c r="F4" s="6" t="s">
         <v>78</v>
       </c>
@@ -13615,12 +13615,12 @@
       <c r="A5" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="82"/>
       <c r="D5" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="77"/>
+      <c r="E5" s="79"/>
       <c r="F5" s="6" t="s">
         <v>233</v>
       </c>
@@ -13633,12 +13633,12 @@
       <c r="A6" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="B6" s="80"/>
-      <c r="C6" s="80"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
       <c r="D6" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="E6" s="77"/>
+      <c r="E6" s="79"/>
       <c r="F6" s="6" t="s">
         <v>78</v>
       </c>
@@ -13651,12 +13651,12 @@
       <c r="A7" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
       <c r="D7" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="E7" s="77"/>
+      <c r="E7" s="79"/>
       <c r="F7" s="28" t="s">
         <v>234</v>
       </c>
@@ -13669,12 +13669,12 @@
       <c r="A8" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="B8" s="80"/>
-      <c r="C8" s="80"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
       <c r="D8" s="34" t="s">
         <v>212</v>
       </c>
-      <c r="E8" s="78"/>
+      <c r="E8" s="80"/>
       <c r="F8" s="35" t="s">
         <v>214</v>
       </c>
@@ -13687,8 +13687,8 @@
       <c r="A9" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="B9" s="80"/>
-      <c r="C9" s="80"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="82"/>
       <c r="D9" s="19" t="s">
         <v>138</v>
       </c>
@@ -13707,8 +13707,8 @@
       <c r="A10" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="B10" s="80"/>
-      <c r="C10" s="80"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="82"/>
       <c r="D10" s="19" t="s">
         <v>139</v>
       </c>
@@ -13727,8 +13727,8 @@
       <c r="A11" s="26" t="s">
         <v>299</v>
       </c>
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="82"/>
       <c r="D11" s="19" t="s">
         <v>324</v>
       </c>
@@ -13747,8 +13747,8 @@
       <c r="A12" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="B12" s="81"/>
-      <c r="C12" s="81"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="83"/>
       <c r="D12" s="19" t="s">
         <v>325</v>
       </c>
@@ -13802,16 +13802,16 @@
       <c r="A15" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B15" s="69" t="s">
+      <c r="B15" s="71" t="s">
         <v>175</v>
       </c>
-      <c r="C15" s="79" t="s">
+      <c r="C15" s="81" t="s">
         <v>104</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E15" s="66" t="s">
+      <c r="E15" s="68" t="s">
         <v>98</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -13826,12 +13826,12 @@
       <c r="A16" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B16" s="70"/>
-      <c r="C16" s="80"/>
+      <c r="B16" s="72"/>
+      <c r="C16" s="82"/>
       <c r="D16" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E16" s="67"/>
+      <c r="E16" s="69"/>
       <c r="F16" s="2" t="s">
         <v>236</v>
       </c>
@@ -13844,12 +13844,12 @@
       <c r="A17" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B17" s="70"/>
-      <c r="C17" s="80"/>
+      <c r="B17" s="72"/>
+      <c r="C17" s="82"/>
       <c r="D17" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E17" s="67"/>
+      <c r="E17" s="69"/>
       <c r="F17" s="2" t="s">
         <v>80</v>
       </c>
@@ -13862,12 +13862,12 @@
       <c r="A18" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B18" s="70"/>
-      <c r="C18" s="80"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="82"/>
       <c r="D18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="67"/>
+      <c r="E18" s="69"/>
       <c r="F18" s="2" t="s">
         <v>237</v>
       </c>
@@ -13880,12 +13880,12 @@
       <c r="A19" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="B19" s="70"/>
-      <c r="C19" s="80"/>
+      <c r="B19" s="72"/>
+      <c r="C19" s="82"/>
       <c r="D19" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="E19" s="67"/>
+      <c r="E19" s="69"/>
       <c r="F19" s="2" t="s">
         <v>79</v>
       </c>
@@ -13898,12 +13898,12 @@
       <c r="A20" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="B20" s="70"/>
-      <c r="C20" s="80"/>
+      <c r="B20" s="72"/>
+      <c r="C20" s="82"/>
       <c r="D20" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="E20" s="67"/>
+      <c r="E20" s="69"/>
       <c r="F20" s="11" t="s">
         <v>72</v>
       </c>
@@ -13916,12 +13916,12 @@
       <c r="A21" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="B21" s="70"/>
-      <c r="C21" s="80"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="82"/>
       <c r="D21" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="E21" s="67"/>
+      <c r="E21" s="69"/>
       <c r="F21" s="11" t="s">
         <v>72</v>
       </c>
@@ -13934,12 +13934,12 @@
       <c r="A22" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="B22" s="70"/>
-      <c r="C22" s="80"/>
+      <c r="B22" s="72"/>
+      <c r="C22" s="82"/>
       <c r="D22" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="E22" s="68"/>
+      <c r="E22" s="70"/>
       <c r="F22" s="35" t="s">
         <v>210</v>
       </c>
@@ -13952,8 +13952,8 @@
       <c r="A23" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="B23" s="70"/>
-      <c r="C23" s="80"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="82"/>
       <c r="D23" s="19" t="s">
         <v>138</v>
       </c>
@@ -13972,8 +13972,8 @@
       <c r="A24" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="B24" s="70"/>
-      <c r="C24" s="80"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="82"/>
       <c r="D24" s="19" t="s">
         <v>139</v>
       </c>
@@ -13992,8 +13992,8 @@
       <c r="A25" s="26" t="s">
         <v>321</v>
       </c>
-      <c r="B25" s="70"/>
-      <c r="C25" s="80"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="82"/>
       <c r="D25" s="19" t="s">
         <v>327</v>
       </c>
@@ -14012,8 +14012,8 @@
       <c r="A26" s="26" t="s">
         <v>322</v>
       </c>
-      <c r="B26" s="71"/>
-      <c r="C26" s="81"/>
+      <c r="B26" s="73"/>
+      <c r="C26" s="83"/>
       <c r="D26" s="19" t="s">
         <v>326</v>
       </c>
@@ -14066,14 +14066,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="82"/>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
+      <c r="A1" s="84"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
@@ -14105,20 +14105,20 @@
       <c r="A3" s="21">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="71" t="s">
         <v>105</v>
       </c>
       <c r="D3" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="E3" s="68" t="s">
+        <v>351</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>352</v>
-      </c>
-      <c r="E3" s="66" t="s">
-        <v>353</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>354</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>34</v>
@@ -14129,14 +14129,14 @@
       <c r="A4" s="21">
         <v>5.2</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
       <c r="D4" s="14" t="s">
-        <v>355</v>
-      </c>
-      <c r="E4" s="67"/>
+        <v>353</v>
+      </c>
+      <c r="E4" s="69"/>
       <c r="F4" s="14" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>27</v>
@@ -14147,14 +14147,14 @@
       <c r="A5" s="21">
         <v>5.3</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
       <c r="D5" s="14" t="s">
-        <v>357</v>
-      </c>
-      <c r="E5" s="67"/>
+        <v>355</v>
+      </c>
+      <c r="E5" s="69"/>
       <c r="F5" s="14" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>22</v>
@@ -14165,14 +14165,14 @@
       <c r="A6" s="21">
         <v>5.4</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
       <c r="D6" s="14" t="s">
-        <v>359</v>
-      </c>
-      <c r="E6" s="68"/>
+        <v>357</v>
+      </c>
+      <c r="E6" s="70"/>
       <c r="F6" s="14" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>27</v>
@@ -14183,16 +14183,16 @@
       <c r="A7" s="21">
         <v>5.5</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
       <c r="D7" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>360</v>
+      </c>
+      <c r="F7" s="14" t="s">
         <v>361</v>
-      </c>
-      <c r="E7" s="53" t="s">
-        <v>362</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>363</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>279</v>
@@ -14203,16 +14203,16 @@
       <c r="A8" s="26">
         <v>5.6</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
       <c r="D8" s="19" t="s">
         <v>138</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>95</v>
@@ -14223,16 +14223,16 @@
       <c r="A9" s="26">
         <v>5.7</v>
       </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="70"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="72"/>
       <c r="D9" s="19" t="s">
         <v>291</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -14243,16 +14243,16 @@
       <c r="A10" s="60">
         <v>5.8</v>
       </c>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
       <c r="D10" s="54" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -14295,14 +14295,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="75"/>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
+      <c r="A1" s="77"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -14334,16 +14334,16 @@
       <c r="A3" s="21">
         <v>6.1</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="85" t="s">
         <v>106</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="E3" s="66" t="s">
+        <v>367</v>
+      </c>
+      <c r="E3" s="68" t="s">
         <v>262</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -14358,12 +14358,12 @@
       <c r="A4" s="21">
         <v>6.2</v>
       </c>
-      <c r="B4" s="83"/>
-      <c r="C4" s="83"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="67"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="2" t="s">
         <v>218</v>
       </c>
@@ -14376,12 +14376,12 @@
       <c r="A5" s="21">
         <v>6.3</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
       <c r="D5" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="E5" s="68"/>
+      <c r="E5" s="70"/>
       <c r="F5" s="2" t="s">
         <v>81</v>
       </c>
@@ -14394,8 +14394,8 @@
       <c r="A6" s="23">
         <v>6.4</v>
       </c>
-      <c r="B6" s="83"/>
-      <c r="C6" s="83"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="6" t="s">
         <v>215</v>
       </c>
@@ -14414,8 +14414,8 @@
       <c r="A7" s="23">
         <v>6.5</v>
       </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="83"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
       <c r="D7" s="2" t="s">
         <v>288</v>
       </c>
@@ -14432,8 +14432,8 @@
       <c r="A8" s="26">
         <v>6.6</v>
       </c>
-      <c r="B8" s="83"/>
-      <c r="C8" s="83"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
       <c r="D8" s="19" t="s">
         <v>138</v>
       </c>
@@ -14452,8 +14452,8 @@
       <c r="A9" s="26">
         <v>6.7</v>
       </c>
-      <c r="B9" s="83"/>
-      <c r="C9" s="83"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
       <c r="D9" s="19" t="s">
         <v>291</v>
       </c>
@@ -14472,16 +14472,16 @@
       <c r="A10" s="64">
         <v>6.8</v>
       </c>
-      <c r="B10" s="83"/>
-      <c r="C10" s="83"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="54" t="s">
+        <v>368</v>
+      </c>
+      <c r="E10" s="54" t="s">
+        <v>369</v>
+      </c>
+      <c r="F10" s="54" t="s">
         <v>370</v>
-      </c>
-      <c r="E10" s="54" t="s">
-        <v>371</v>
-      </c>
-      <c r="F10" s="54" t="s">
-        <v>372</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -14525,14 +14525,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="75"/>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
+      <c r="A1" s="77"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -14564,16 +14564,16 @@
       <c r="A3" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="71" t="s">
         <v>107</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="66" t="s">
+      <c r="E3" s="68" t="s">
         <v>90</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -14588,12 +14588,12 @@
       <c r="A4" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
       <c r="D4" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="E4" s="67"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="2" t="s">
         <v>58</v>
       </c>
@@ -14606,12 +14606,12 @@
       <c r="A5" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
       <c r="D5" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="E5" s="67"/>
+      <c r="E5" s="69"/>
       <c r="F5" s="2" t="s">
         <v>82</v>
       </c>
@@ -14624,12 +14624,12 @@
       <c r="A6" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
       <c r="D6" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="68"/>
+      <c r="E6" s="70"/>
       <c r="F6" s="6" t="s">
         <v>59</v>
       </c>
@@ -14642,8 +14642,8 @@
       <c r="A7" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
       <c r="D7" s="2" t="s">
         <v>304</v>
       </c>
@@ -14660,8 +14660,8 @@
       <c r="A8" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
       <c r="D8" s="19" t="s">
         <v>138</v>
       </c>
@@ -14680,8 +14680,8 @@
       <c r="A9" s="26" t="s">
         <v>302</v>
       </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="70"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="72"/>
       <c r="D9" s="19" t="s">
         <v>291</v>
       </c>
@@ -14689,7 +14689,7 @@
         <v>295</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -14698,21 +14698,21 @@
     </row>
     <row r="10" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A10" s="55" t="s">
+        <v>379</v>
+      </c>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="54" t="s">
         <v>381</v>
       </c>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="54" t="s">
-        <v>383</v>
-      </c>
       <c r="E10" s="54" t="s">
+        <v>382</v>
+      </c>
+      <c r="F10" s="54" t="s">
         <v>384</v>
       </c>
-      <c r="F10" s="54" t="s">
-        <v>386</v>
-      </c>
       <c r="G10" s="59" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H10" s="59"/>
     </row>
@@ -14746,16 +14746,16 @@
       <c r="A13" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="69" t="s">
+      <c r="B13" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="71" t="s">
         <v>71</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="66" t="s">
+      <c r="E13" s="68" t="s">
         <v>91</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -14770,12 +14770,12 @@
       <c r="A14" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="70"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
       <c r="D14" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="E14" s="67"/>
+      <c r="E14" s="69"/>
       <c r="F14" s="2" t="s">
         <v>141</v>
       </c>
@@ -14788,12 +14788,12 @@
       <c r="A15" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
+      <c r="B15" s="72"/>
+      <c r="C15" s="72"/>
       <c r="D15" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="E15" s="67"/>
+      <c r="E15" s="69"/>
       <c r="F15" s="2" t="s">
         <v>63</v>
       </c>
@@ -14806,12 +14806,12 @@
       <c r="A16" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="B16" s="70"/>
-      <c r="C16" s="70"/>
+      <c r="B16" s="72"/>
+      <c r="C16" s="72"/>
       <c r="D16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="68"/>
+      <c r="E16" s="70"/>
       <c r="F16" s="6" t="s">
         <v>66</v>
       </c>
@@ -14824,8 +14824,8 @@
       <c r="A17" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="B17" s="70"/>
-      <c r="C17" s="70"/>
+      <c r="B17" s="72"/>
+      <c r="C17" s="72"/>
       <c r="D17" s="2" t="s">
         <v>308</v>
       </c>
@@ -14842,8 +14842,8 @@
       <c r="A18" s="19" t="s">
         <v>300</v>
       </c>
-      <c r="B18" s="70"/>
-      <c r="C18" s="70"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="72"/>
       <c r="D18" s="19" t="s">
         <v>138</v>
       </c>
@@ -14862,8 +14862,8 @@
       <c r="A19" s="26" t="s">
         <v>309</v>
       </c>
-      <c r="B19" s="70"/>
-      <c r="C19" s="70"/>
+      <c r="B19" s="72"/>
+      <c r="C19" s="72"/>
       <c r="D19" s="19" t="s">
         <v>291</v>
       </c>
@@ -14880,21 +14880,21 @@
     </row>
     <row r="20" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A20" s="55" t="s">
-        <v>382</v>
-      </c>
-      <c r="B20" s="71"/>
-      <c r="C20" s="71"/>
+        <v>380</v>
+      </c>
+      <c r="B20" s="73"/>
+      <c r="C20" s="73"/>
       <c r="D20" s="54" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E20" s="54" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F20" s="54" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G20" s="59" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H20" s="59"/>
     </row>
@@ -14934,14 +14934,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="75"/>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
+      <c r="A1" s="77"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -14973,17 +14973,17 @@
       <c r="A3" s="21">
         <v>8.1</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="71" t="s">
         <v>108</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E3" s="66" t="s">
-        <v>373</v>
+      <c r="E3" s="68" t="s">
+        <v>371</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>240</v>
@@ -14999,12 +14999,12 @@
       <c r="A4" s="21">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="67"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="2" t="s">
         <v>48</v>
       </c>
@@ -15017,12 +15017,12 @@
       <c r="A5" s="21">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
       <c r="D5" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="E5" s="68"/>
+      <c r="E5" s="70"/>
       <c r="F5" s="2" t="s">
         <v>83</v>
       </c>
@@ -15035,12 +15035,12 @@
       <c r="A6" s="21">
         <v>8.4</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
       <c r="D6" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="E6" s="66" t="s">
+      <c r="E6" s="68" t="s">
         <v>283</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -15055,12 +15055,12 @@
       <c r="A7" s="21">
         <v>8.5</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
       <c r="D7" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="E7" s="67"/>
+      <c r="E7" s="69"/>
       <c r="F7" s="2" t="s">
         <v>286</v>
       </c>
@@ -15073,12 +15073,12 @@
       <c r="A8" s="21">
         <v>8.6</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
       <c r="D8" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="E8" s="68"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="2" t="s">
         <v>284</v>
       </c>
@@ -15091,8 +15091,8 @@
       <c r="A9" s="26">
         <v>8.6999999999999993</v>
       </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="70"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="72"/>
       <c r="D9" s="19" t="s">
         <v>138</v>
       </c>
@@ -15111,8 +15111,8 @@
       <c r="A10" s="26">
         <v>8.8000000000000007</v>
       </c>
-      <c r="B10" s="70"/>
-      <c r="C10" s="70"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="72"/>
       <c r="D10" s="19" t="s">
         <v>291</v>
       </c>
@@ -15128,19 +15128,19 @@
       <c r="H10" s="20"/>
     </row>
     <row r="11" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
-      <c r="A11" s="84">
+      <c r="A11" s="65">
         <v>8.9</v>
       </c>
-      <c r="B11" s="70"/>
-      <c r="C11" s="70"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="72"/>
       <c r="D11" s="54" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F11" s="55" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="G11" s="60" t="s">
         <v>21</v>
@@ -15148,19 +15148,19 @@
       <c r="H11" s="60"/>
     </row>
     <row r="12" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
-      <c r="A12" s="85" t="s">
+      <c r="A12" s="66" t="s">
+        <v>376</v>
+      </c>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="54" t="s">
         <v>378</v>
       </c>
-      <c r="B12" s="71"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="54" t="s">
-        <v>380</v>
-      </c>
       <c r="E12" s="55" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F12" s="55" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G12" s="60" t="s">
         <v>21</v>
@@ -15202,14 +15202,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="75"/>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
+      <c r="A1" s="77"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -15241,10 +15241,10 @@
       <c r="A3" s="21">
         <v>9.1</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="71" t="s">
         <v>36</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -15253,7 +15253,7 @@
       <c r="E3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="69" t="s">
+      <c r="F3" s="71" t="s">
         <v>41</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -15265,15 +15265,15 @@
       <c r="A4" s="21">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="70"/>
+      <c r="F4" s="72"/>
       <c r="G4" s="2" t="s">
         <v>43</v>
       </c>
@@ -15283,15 +15283,15 @@
       <c r="A5" s="21">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
       <c r="D5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="70"/>
+      <c r="F5" s="72"/>
       <c r="G5" s="2" t="s">
         <v>43</v>
       </c>
@@ -15301,15 +15301,15 @@
       <c r="A6" s="21">
         <v>9.4</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
       <c r="D6" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="70"/>
+      <c r="F6" s="72"/>
       <c r="G6" s="5" t="s">
         <v>43</v>
       </c>
@@ -15319,15 +15319,15 @@
       <c r="A7" s="21">
         <v>9.5</v>
       </c>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
       <c r="D7" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="71"/>
+      <c r="F7" s="73"/>
       <c r="G7" s="5" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Update the test case file after updated hint message on find contents on txt files
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -10052,6 +10052,144 @@
   </si>
   <si>
     <r>
+      <t>1.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2.输入文件夹下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件名或扩展名</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2.在需要找的文件夹或文件输入框内输入空字符串</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:D:\Test
+2.在"P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lease input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" 输入空字符串
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t>提示不能输入空的搜索内容的信息 
 （</t>
     </r>
@@ -10065,174 +10203,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Do not input the empty content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径
-2.输入文件夹下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件名或扩展名</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径
-2.在需要找的文件夹或文件输入框内输入空字符串</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:D:\Test
-2.在"P</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>lease input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" 输入空字符串
-</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示不能输入空的搜索内容的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Do not input the empty folder or file name, please input again!</t>
     </r>
     <r>
@@ -11026,6 +10996,36 @@
   <si>
     <r>
       <t>提示请不要输入空查找内容的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty search content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示不能输入空的搜索内容的信息 
 （</t>
     </r>
     <r>
@@ -11865,8 +11865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -12067,7 +12067,7 @@
         <v>346</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G10" s="59"/>
       <c r="H10" s="59"/>
@@ -12085,7 +12085,7 @@
         <v>347</v>
       </c>
       <c r="F11" s="54" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G11" s="59"/>
       <c r="H11" s="59"/>
@@ -14048,7 +14048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -14252,7 +14252,7 @@
         <v>365</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>366</v>
+        <v>389</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -14341,7 +14341,7 @@
         <v>106</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E3" s="68" t="s">
         <v>262</v>
@@ -14475,13 +14475,13 @@
       <c r="B10" s="85"/>
       <c r="C10" s="85"/>
       <c r="D10" s="54" t="s">
+        <v>367</v>
+      </c>
+      <c r="E10" s="54" t="s">
         <v>368</v>
       </c>
-      <c r="E10" s="54" t="s">
+      <c r="F10" s="54" t="s">
         <v>369</v>
-      </c>
-      <c r="F10" s="54" t="s">
-        <v>370</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -14689,7 +14689,7 @@
         <v>295</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -14698,21 +14698,21 @@
     </row>
     <row r="10" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A10" s="55" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B10" s="73"/>
       <c r="C10" s="73"/>
       <c r="D10" s="54" t="s">
+        <v>380</v>
+      </c>
+      <c r="E10" s="54" t="s">
         <v>381</v>
       </c>
-      <c r="E10" s="54" t="s">
-        <v>382</v>
-      </c>
       <c r="F10" s="54" t="s">
+        <v>383</v>
+      </c>
+      <c r="G10" s="59" t="s">
         <v>384</v>
-      </c>
-      <c r="G10" s="59" t="s">
-        <v>385</v>
       </c>
       <c r="H10" s="59"/>
     </row>
@@ -14880,21 +14880,21 @@
     </row>
     <row r="20" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A20" s="55" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B20" s="73"/>
       <c r="C20" s="73"/>
       <c r="D20" s="54" t="s">
+        <v>385</v>
+      </c>
+      <c r="E20" s="54" t="s">
         <v>386</v>
       </c>
-      <c r="E20" s="54" t="s">
-        <v>387</v>
-      </c>
       <c r="F20" s="54" t="s">
+        <v>383</v>
+      </c>
+      <c r="G20" s="59" t="s">
         <v>384</v>
-      </c>
-      <c r="G20" s="59" t="s">
-        <v>385</v>
       </c>
       <c r="H20" s="59"/>
     </row>
@@ -14983,7 +14983,7 @@
         <v>150</v>
       </c>
       <c r="E3" s="68" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>240</v>
@@ -15134,13 +15134,13 @@
       <c r="B11" s="72"/>
       <c r="C11" s="72"/>
       <c r="D11" s="54" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E11" s="55" t="s">
+        <v>371</v>
+      </c>
+      <c r="F11" s="55" t="s">
         <v>372</v>
-      </c>
-      <c r="F11" s="55" t="s">
-        <v>373</v>
       </c>
       <c r="G11" s="60" t="s">
         <v>21</v>
@@ -15149,18 +15149,18 @@
     </row>
     <row r="12" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A12" s="66" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B12" s="73"/>
       <c r="C12" s="73"/>
       <c r="D12" s="54" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E12" s="55" t="s">
+        <v>373</v>
+      </c>
+      <c r="F12" s="55" t="s">
         <v>374</v>
-      </c>
-      <c r="F12" s="55" t="s">
-        <v>375</v>
       </c>
       <c r="G12" s="60" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Update the test case file after updated hint message on find files or folder on folder
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -10190,6 +10190,811 @@
   </si>
   <si>
     <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the file or folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want find?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alonso</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want replace?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Button</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:D:\Test
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want find?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">",输入空字符
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示需要被替换字符不能为空的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Do not input the empty find content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:D:\Test
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want find?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如Alonso
+3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want replace?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">",输入新的想要被替换的文件夹名为空字符
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示需要新替换字符名称不能为空的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Do not input the empty replace content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2. 根据</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件中的某一字段，输入想要被替换的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>为空字符</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2. 根据</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件中的某一字段，输入想要被替换的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>已有字段</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3. 输入想要被替换的新名称为空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.1.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.2.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件夹名字
+2.输入替换的文件夹名字为</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如D:\TesT39
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what word you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字为空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The format of " D:Test Folder " is incorrect! Should with '\'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示替换内容不能为空的信息
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Do not input empty replace name. Please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件名字
+2.输入替换的文件名字为</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件名字，如D:\TesT39\ALO.bmp
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what word you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件名字为空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示请不要输入空的替换内容信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty replace content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示请不要输入空查找内容的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty search content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t>提示不能输入空的搜索内容的信息 
 （</t>
     </r>
@@ -10203,811 +11008,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Do not input the empty folder or file name, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the file or folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What word do you want find?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alonso</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What word do you want replace?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Button</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:D:\Test
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What word do you want find?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">",输入空字符
-</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示需要被替换字符不能为空的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Do not input the empty find content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:D:\Test
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What word do you want find?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如Alonso
-3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What word do you want replace?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">",输入新的想要被替换的文件夹名为空字符
-</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示需要新替换字符名称不能为空的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Do not input the empty replace content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8.10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径
-2. 根据</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件中的某一字段，输入想要被替换的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>为空字符</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径
-2. 根据</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件中的某一字段，输入想要被替换的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>已有字段</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3. 输入想要被替换的新名称为空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7.1.8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7.2.8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件夹名字
-2.输入替换的文件夹名字为</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如D:\TesT39
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what word you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字为空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The format of " D:Test Folder " is incorrect! Should with '\'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示替换内容不能为空的信息
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Do not input empty replace name. Please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pass</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件名字
-2.输入替换的文件名字为</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件名字，如D:\TesT39\ALO.bmp
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what word you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件名字为空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示请不要输入空的替换内容信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Illegal -- cannot input empty replace content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示请不要输入空查找内容的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Illegal -- cannot input empty search content, please input again!</t>
     </r>
     <r>
@@ -11038,7 +11038,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Illegal -- cannot input empty search content, please input again!</t>
+      <t>Illegal -- cannot input empty file or folder name, please input again!</t>
     </r>
     <r>
       <rPr>
@@ -12067,7 +12067,7 @@
         <v>346</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G10" s="59"/>
       <c r="H10" s="59"/>
@@ -12085,7 +12085,7 @@
         <v>347</v>
       </c>
       <c r="F11" s="54" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G11" s="59"/>
       <c r="H11" s="59"/>
@@ -14048,7 +14048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -14252,7 +14252,7 @@
         <v>365</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -14279,7 +14279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -14481,7 +14481,7 @@
         <v>368</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>369</v>
+        <v>389</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -14689,7 +14689,7 @@
         <v>295</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -14698,21 +14698,21 @@
     </row>
     <row r="10" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A10" s="55" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B10" s="73"/>
       <c r="C10" s="73"/>
       <c r="D10" s="54" t="s">
+        <v>379</v>
+      </c>
+      <c r="E10" s="54" t="s">
         <v>380</v>
       </c>
-      <c r="E10" s="54" t="s">
-        <v>381</v>
-      </c>
       <c r="F10" s="54" t="s">
+        <v>382</v>
+      </c>
+      <c r="G10" s="59" t="s">
         <v>383</v>
-      </c>
-      <c r="G10" s="59" t="s">
-        <v>384</v>
       </c>
       <c r="H10" s="59"/>
     </row>
@@ -14880,21 +14880,21 @@
     </row>
     <row r="20" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A20" s="55" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B20" s="73"/>
       <c r="C20" s="73"/>
       <c r="D20" s="54" t="s">
+        <v>384</v>
+      </c>
+      <c r="E20" s="54" t="s">
         <v>385</v>
       </c>
-      <c r="E20" s="54" t="s">
-        <v>386</v>
-      </c>
       <c r="F20" s="54" t="s">
+        <v>382</v>
+      </c>
+      <c r="G20" s="59" t="s">
         <v>383</v>
-      </c>
-      <c r="G20" s="59" t="s">
-        <v>384</v>
       </c>
       <c r="H20" s="59"/>
     </row>
@@ -14983,7 +14983,7 @@
         <v>150</v>
       </c>
       <c r="E3" s="68" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>240</v>
@@ -15134,13 +15134,13 @@
       <c r="B11" s="72"/>
       <c r="C11" s="72"/>
       <c r="D11" s="54" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E11" s="55" t="s">
+        <v>370</v>
+      </c>
+      <c r="F11" s="55" t="s">
         <v>371</v>
-      </c>
-      <c r="F11" s="55" t="s">
-        <v>372</v>
       </c>
       <c r="G11" s="60" t="s">
         <v>21</v>
@@ -15149,18 +15149,18 @@
     </row>
     <row r="12" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A12" s="66" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B12" s="73"/>
       <c r="C12" s="73"/>
       <c r="D12" s="54" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E12" s="55" t="s">
+        <v>372</v>
+      </c>
+      <c r="F12" s="55" t="s">
         <v>373</v>
-      </c>
-      <c r="F12" s="55" t="s">
-        <v>374</v>
       </c>
       <c r="G12" s="60" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Update the test case file after updated hint message on rename file or folder
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -2592,10 +2592,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>7. Rename file or folder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>8. Rename file with specificname</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -10805,6 +10801,225 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件名字
+2.输入替换的文件名字为</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件名字，如D:\TesT39\ALO.bmp
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what word you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件名字为空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示请不要输入空的替换内容信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty replace content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示请不要输入空查找内容的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty search content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示不能输入空的搜索内容的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty search content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示不能输入空的搜索内容的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty file or folder name, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t>提示替换内容不能为空的信息
 （</t>
@@ -10819,7 +11034,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Do not input empty replace name. Please input again!</t>
+      <t>Illegal -- cannot input empty replace content, please input again!</t>
     </r>
     <r>
       <rPr>
@@ -10835,222 +11050,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Pass</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件名字
-2.输入替换的文件名字为</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件名字，如D:\TesT39\ALO.bmp
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what word you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件名字为空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示请不要输入空的替换内容信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Illegal -- cannot input empty replace content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示请不要输入空查找内容的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Illegal -- cannot input empty search content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示不能输入空的搜索内容的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Illegal -- cannot input empty search content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示不能输入空的搜索内容的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Illegal -- cannot input empty file or folder name, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
+    <t>7. Rename file or folder</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -11929,13 +11929,13 @@
         <v>100</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E3" s="68" t="s">
+        <v>327</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>330</v>
-      </c>
-      <c r="E3" s="68" t="s">
-        <v>328</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>331</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>22</v>
@@ -11949,11 +11949,11 @@
       <c r="B4" s="72"/>
       <c r="C4" s="72"/>
       <c r="D4" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E4" s="69"/>
       <c r="F4" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>23</v>
@@ -11967,11 +11967,11 @@
       <c r="B5" s="72"/>
       <c r="C5" s="72"/>
       <c r="D5" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E5" s="69"/>
       <c r="F5" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>24</v>
@@ -11985,11 +11985,11 @@
       <c r="B6" s="72"/>
       <c r="C6" s="72"/>
       <c r="D6" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E6" s="70"/>
       <c r="F6" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>27</v>
@@ -12003,13 +12003,13 @@
       <c r="B7" s="72"/>
       <c r="C7" s="72"/>
       <c r="D7" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E7" s="52" t="s">
         <v>338</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="F7" s="2" t="s">
         <v>339</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>340</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="57"/>
@@ -12021,13 +12021,13 @@
       <c r="B8" s="72"/>
       <c r="C8" s="72"/>
       <c r="D8" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E8" s="19" t="s">
+        <v>340</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>341</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>342</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>95</v>
@@ -12041,13 +12041,13 @@
       <c r="B9" s="72"/>
       <c r="C9" s="72"/>
       <c r="D9" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E9" s="19" t="s">
+        <v>342</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>343</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>344</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -12061,13 +12061,13 @@
       <c r="B10" s="72"/>
       <c r="C10" s="72"/>
       <c r="D10" s="54" t="s">
+        <v>344</v>
+      </c>
+      <c r="E10" s="54" t="s">
         <v>345</v>
       </c>
-      <c r="E10" s="54" t="s">
-        <v>346</v>
-      </c>
       <c r="F10" s="54" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G10" s="59"/>
       <c r="H10" s="59"/>
@@ -12079,13 +12079,13 @@
       <c r="B11" s="73"/>
       <c r="C11" s="73"/>
       <c r="D11" s="54" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E11" s="54" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F11" s="54" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G11" s="59"/>
       <c r="H11" s="59"/>
@@ -12164,22 +12164,22 @@
         <v>10.1</v>
       </c>
       <c r="B3" s="85" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="85" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="85" t="s">
+      <c r="D3" s="85" t="s">
         <v>153</v>
       </c>
-      <c r="D3" s="85" t="s">
+      <c r="E3" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="F3" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -12191,13 +12191,13 @@
       <c r="C4" s="85"/>
       <c r="D4" s="85"/>
       <c r="E4" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -12209,13 +12209,13 @@
       <c r="C5" s="85"/>
       <c r="D5" s="85"/>
       <c r="E5" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -12227,13 +12227,13 @@
       <c r="C6" s="85"/>
       <c r="D6" s="85"/>
       <c r="E6" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H6" s="5"/>
     </row>
@@ -12245,13 +12245,13 @@
       <c r="C7" s="85"/>
       <c r="D7" s="85"/>
       <c r="E7" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H7" s="5"/>
     </row>
@@ -12263,13 +12263,13 @@
       <c r="C8" s="85"/>
       <c r="D8" s="85"/>
       <c r="E8" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H8" s="5"/>
     </row>
@@ -12281,13 +12281,13 @@
       <c r="C9" s="85"/>
       <c r="D9" s="85"/>
       <c r="E9" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H9" s="5"/>
     </row>
@@ -12299,13 +12299,13 @@
       <c r="C10" s="85"/>
       <c r="D10" s="85"/>
       <c r="E10" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H10" s="5"/>
     </row>
@@ -12317,26 +12317,26 @@
       <c r="C11" s="85"/>
       <c r="D11" s="85"/>
       <c r="E11" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>277</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A12" s="49" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B12" s="85"/>
       <c r="C12" s="85"/>
       <c r="D12" s="85"/>
       <c r="E12" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>21</v>
@@ -12351,13 +12351,13 @@
       <c r="C13" s="85"/>
       <c r="D13" s="85"/>
       <c r="E13" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H13" s="5"/>
     </row>
@@ -12369,13 +12369,13 @@
       <c r="C14" s="85"/>
       <c r="D14" s="85"/>
       <c r="E14" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="G14" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H14" s="5"/>
     </row>
@@ -12453,19 +12453,19 @@
         <v>11.1</v>
       </c>
       <c r="B3" s="85" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" s="85" t="s">
         <v>260</v>
       </c>
-      <c r="C3" s="85" t="s">
-        <v>261</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E3" s="68" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>21</v>
@@ -12479,11 +12479,11 @@
       <c r="B4" s="85"/>
       <c r="C4" s="85"/>
       <c r="D4" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E4" s="70"/>
       <c r="F4" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>21</v>
@@ -12497,13 +12497,13 @@
       <c r="B5" s="85"/>
       <c r="C5" s="85"/>
       <c r="D5" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E5" s="68" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>21</v>
@@ -12517,11 +12517,11 @@
       <c r="B6" s="85"/>
       <c r="C6" s="85"/>
       <c r="D6" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E6" s="70"/>
       <c r="F6" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>21</v>
@@ -12535,7 +12535,7 @@
       <c r="B7" s="85"/>
       <c r="C7" s="85"/>
       <c r="D7" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>93</v>
@@ -12555,13 +12555,13 @@
       <c r="B8" s="85"/>
       <c r="C8" s="85"/>
       <c r="D8" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="E8" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>292</v>
-      </c>
       <c r="F8" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>21</v>
@@ -12641,7 +12641,7 @@
     </row>
     <row r="3" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" s="71" t="s">
         <v>0</v>
@@ -12656,7 +12656,7 @@
         <v>69</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>26</v>
@@ -12665,18 +12665,18 @@
     </row>
     <row r="4" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4" s="72"/>
       <c r="C4" s="72"/>
       <c r="D4" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>21</v>
@@ -12685,12 +12685,12 @@
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" s="72"/>
       <c r="C5" s="72"/>
       <c r="D5" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>69</v>
@@ -12705,15 +12705,15 @@
     </row>
     <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A6" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" s="72"/>
       <c r="C6" s="72"/>
       <c r="D6" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>94</v>
@@ -12725,18 +12725,18 @@
     </row>
     <row r="7" spans="1:9" ht="57" x14ac:dyDescent="0.15">
       <c r="A7" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B7" s="73"/>
       <c r="C7" s="73"/>
       <c r="D7" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E7" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>295</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>296</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>21</v>
@@ -12783,7 +12783,7 @@
     </row>
     <row r="10" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B10" s="71" t="s">
         <v>4</v>
@@ -12798,7 +12798,7 @@
         <v>96</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>21</v>
@@ -12808,7 +12808,7 @@
     </row>
     <row r="11" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B11" s="72"/>
       <c r="C11" s="72"/>
@@ -12819,7 +12819,7 @@
         <v>87</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>68</v>
@@ -12831,12 +12831,12 @@
     </row>
     <row r="12" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B12" s="72"/>
       <c r="C12" s="72"/>
       <c r="D12" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>86</v>
@@ -12852,12 +12852,12 @@
     </row>
     <row r="13" spans="1:9" s="22" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A13" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B13" s="72"/>
       <c r="C13" s="72"/>
       <c r="D13" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>97</v>
@@ -12872,18 +12872,18 @@
     </row>
     <row r="14" spans="1:9" s="22" customFormat="1" ht="57" x14ac:dyDescent="0.15">
       <c r="A14" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B14" s="73"/>
       <c r="C14" s="73"/>
       <c r="D14" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E14" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>295</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>296</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>21</v>
@@ -13049,7 +13049,7 @@
     </row>
     <row r="3" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="71" t="s">
         <v>84</v>
@@ -13058,13 +13058,13 @@
         <v>103</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E3" s="68" t="s">
         <v>88</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>21</v>
@@ -13073,16 +13073,16 @@
     </row>
     <row r="4" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B4" s="72"/>
       <c r="C4" s="72"/>
       <c r="D4" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E4" s="69"/>
       <c r="F4" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>21</v>
@@ -13091,12 +13091,12 @@
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="72"/>
       <c r="C5" s="72"/>
       <c r="D5" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E5" s="69"/>
       <c r="F5" s="2" t="s">
@@ -13109,16 +13109,16 @@
     </row>
     <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B6" s="72"/>
       <c r="C6" s="72"/>
       <c r="D6" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E6" s="69"/>
       <c r="F6" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>21</v>
@@ -13127,16 +13127,16 @@
     </row>
     <row r="7" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B7" s="72"/>
       <c r="C7" s="72"/>
       <c r="D7" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E7" s="69"/>
       <c r="F7" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>28</v>
@@ -13145,16 +13145,16 @@
     </row>
     <row r="8" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B8" s="72"/>
       <c r="C8" s="72"/>
       <c r="D8" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E8" s="69"/>
       <c r="F8" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>33</v>
@@ -13163,16 +13163,16 @@
     </row>
     <row r="9" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B9" s="72"/>
       <c r="C9" s="72"/>
       <c r="D9" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E9" s="69"/>
       <c r="F9" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>21</v>
@@ -13181,30 +13181,30 @@
     </row>
     <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A10" s="34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B10" s="72"/>
       <c r="C10" s="72"/>
       <c r="D10" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E10" s="70"/>
       <c r="F10" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="G10" s="36" t="s">
         <v>197</v>
-      </c>
-      <c r="G10" s="36" t="s">
-        <v>198</v>
       </c>
       <c r="H10" s="36"/>
     </row>
     <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B11" s="72"/>
       <c r="C11" s="72"/>
       <c r="D11" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>97</v>
@@ -13219,18 +13219,18 @@
     </row>
     <row r="12" spans="1:8" s="22" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A12" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B12" s="72"/>
       <c r="C12" s="72"/>
       <c r="D12" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>21</v>
@@ -13239,18 +13239,18 @@
     </row>
     <row r="13" spans="1:8" s="22" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A13" s="26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B13" s="72"/>
       <c r="C13" s="72"/>
       <c r="D13" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E13" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="F13" s="19" t="s">
         <v>295</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>296</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>21</v>
@@ -13259,18 +13259,18 @@
     </row>
     <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A14" s="26" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B14" s="73"/>
       <c r="C14" s="73"/>
       <c r="D14" s="19" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>21</v>
@@ -13305,7 +13305,7 @@
     </row>
     <row r="17" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A17" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B17" s="71" t="s">
         <v>85</v>
@@ -13314,13 +13314,13 @@
         <v>102</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E17" s="68" t="s">
         <v>89</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>21</v>
@@ -13329,12 +13329,12 @@
     </row>
     <row r="18" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A18" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B18" s="72"/>
       <c r="C18" s="72"/>
       <c r="D18" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E18" s="69"/>
       <c r="F18" s="14" t="s">
@@ -13347,7 +13347,7 @@
     </row>
     <row r="19" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A19" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B19" s="72"/>
       <c r="C19" s="72"/>
@@ -13356,7 +13356,7 @@
       </c>
       <c r="E19" s="69"/>
       <c r="F19" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G19" s="14" t="s">
         <v>21</v>
@@ -13365,12 +13365,12 @@
     </row>
     <row r="20" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A20" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B20" s="72"/>
       <c r="C20" s="72"/>
       <c r="D20" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E20" s="69"/>
       <c r="F20" s="14" t="s">
@@ -13383,16 +13383,16 @@
     </row>
     <row r="21" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A21" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B21" s="72"/>
       <c r="C21" s="72"/>
       <c r="D21" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E21" s="69"/>
       <c r="F21" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G21" s="15" t="s">
         <v>21</v>
@@ -13401,25 +13401,25 @@
     </row>
     <row r="22" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A22" s="34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B22" s="72"/>
       <c r="C22" s="72"/>
       <c r="D22" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E22" s="70"/>
       <c r="F22" s="35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G22" s="36" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H22" s="36"/>
     </row>
     <row r="23" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A23" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B23" s="72"/>
       <c r="C23" s="72"/>
@@ -13439,18 +13439,18 @@
     </row>
     <row r="24" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A24" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B24" s="72"/>
       <c r="C24" s="72"/>
       <c r="D24" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>21</v>
@@ -13459,18 +13459,18 @@
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B25" s="72"/>
       <c r="C25" s="72"/>
       <c r="D25" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>21</v>
@@ -13479,18 +13479,18 @@
     </row>
     <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B26" s="73"/>
       <c r="C26" s="73"/>
       <c r="D26" s="19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>21</v>
@@ -13571,22 +13571,22 @@
     </row>
     <row r="3" spans="1:8" s="22" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B3" s="81" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C3" s="81" t="s">
         <v>104</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E3" s="78" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>31</v>
@@ -13595,12 +13595,12 @@
     </row>
     <row r="4" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B4" s="82"/>
       <c r="C4" s="82"/>
       <c r="D4" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E4" s="79"/>
       <c r="F4" s="6" t="s">
@@ -13613,7 +13613,7 @@
     </row>
     <row r="5" spans="1:8" s="22" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B5" s="82"/>
       <c r="C5" s="82"/>
@@ -13622,7 +13622,7 @@
       </c>
       <c r="E5" s="79"/>
       <c r="F5" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>30</v>
@@ -13631,12 +13631,12 @@
     </row>
     <row r="6" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B6" s="82"/>
       <c r="C6" s="82"/>
       <c r="D6" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E6" s="79"/>
       <c r="F6" s="6" t="s">
@@ -13649,16 +13649,16 @@
     </row>
     <row r="7" spans="1:8" s="22" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B7" s="82"/>
       <c r="C7" s="82"/>
       <c r="D7" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E7" s="79"/>
       <c r="F7" s="28" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G7" s="29" t="s">
         <v>57</v>
@@ -13667,30 +13667,30 @@
     </row>
     <row r="8" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A8" s="37" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B8" s="82"/>
       <c r="C8" s="82"/>
       <c r="D8" s="34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E8" s="80"/>
       <c r="F8" s="35" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G8" s="38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H8" s="39"/>
     </row>
     <row r="9" spans="1:8" s="22" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A9" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B9" s="82"/>
       <c r="C9" s="82"/>
       <c r="D9" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>99</v>
@@ -13705,18 +13705,18 @@
     </row>
     <row r="10" spans="1:8" s="32" customFormat="1" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A10" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B10" s="82"/>
       <c r="C10" s="82"/>
       <c r="D10" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>21</v>
@@ -13725,18 +13725,18 @@
     </row>
     <row r="11" spans="1:8" s="32" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="26" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B11" s="82"/>
       <c r="C11" s="82"/>
       <c r="D11" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E11" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="F11" s="19" t="s">
         <v>295</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>296</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>21</v>
@@ -13745,18 +13745,18 @@
     </row>
     <row r="12" spans="1:8" s="32" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="26" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B12" s="83"/>
       <c r="C12" s="83"/>
       <c r="D12" s="19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>21</v>
@@ -13800,22 +13800,22 @@
     </row>
     <row r="15" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B15" s="71" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C15" s="81" t="s">
         <v>104</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E15" s="68" t="s">
         <v>98</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>21</v>
@@ -13824,16 +13824,16 @@
     </row>
     <row r="16" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B16" s="72"/>
       <c r="C16" s="82"/>
       <c r="D16" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E16" s="69"/>
       <c r="F16" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>21</v>
@@ -13842,12 +13842,12 @@
     </row>
     <row r="17" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B17" s="72"/>
       <c r="C17" s="82"/>
       <c r="D17" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E17" s="69"/>
       <c r="F17" s="2" t="s">
@@ -13860,7 +13860,7 @@
     </row>
     <row r="18" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B18" s="72"/>
       <c r="C18" s="82"/>
@@ -13869,7 +13869,7 @@
       </c>
       <c r="E18" s="69"/>
       <c r="F18" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>21</v>
@@ -13878,12 +13878,12 @@
     </row>
     <row r="19" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B19" s="72"/>
       <c r="C19" s="82"/>
       <c r="D19" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E19" s="69"/>
       <c r="F19" s="2" t="s">
@@ -13896,12 +13896,12 @@
     </row>
     <row r="20" spans="1:8" s="22" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A20" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B20" s="72"/>
       <c r="C20" s="82"/>
       <c r="D20" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E20" s="69"/>
       <c r="F20" s="11" t="s">
@@ -13914,12 +13914,12 @@
     </row>
     <row r="21" spans="1:8" s="22" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A21" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B21" s="72"/>
       <c r="C21" s="82"/>
       <c r="D21" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E21" s="69"/>
       <c r="F21" s="11" t="s">
@@ -13932,30 +13932,30 @@
     </row>
     <row r="22" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A22" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B22" s="72"/>
       <c r="C22" s="82"/>
       <c r="D22" s="34" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E22" s="70"/>
       <c r="F22" s="35" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G22" s="40" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H22" s="41"/>
     </row>
     <row r="23" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A23" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B23" s="72"/>
       <c r="C23" s="82"/>
       <c r="D23" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>99</v>
@@ -13970,18 +13970,18 @@
     </row>
     <row r="24" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A24" s="19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B24" s="72"/>
       <c r="C24" s="82"/>
       <c r="D24" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E24" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="F24" s="19" t="s">
         <v>112</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>113</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>21</v>
@@ -13990,18 +13990,18 @@
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B25" s="72"/>
       <c r="C25" s="82"/>
       <c r="D25" s="19" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E25" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="F25" s="19" t="s">
         <v>295</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>296</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>21</v>
@@ -14010,18 +14010,18 @@
     </row>
     <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B26" s="73"/>
       <c r="C26" s="83"/>
       <c r="D26" s="19" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>21</v>
@@ -14112,13 +14112,13 @@
         <v>105</v>
       </c>
       <c r="D3" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="E3" s="68" t="s">
         <v>350</v>
       </c>
-      <c r="E3" s="68" t="s">
+      <c r="F3" s="14" t="s">
         <v>351</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>352</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>34</v>
@@ -14132,11 +14132,11 @@
       <c r="B4" s="72"/>
       <c r="C4" s="72"/>
       <c r="D4" s="14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E4" s="69"/>
       <c r="F4" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>27</v>
@@ -14150,11 +14150,11 @@
       <c r="B5" s="72"/>
       <c r="C5" s="72"/>
       <c r="D5" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E5" s="69"/>
       <c r="F5" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>22</v>
@@ -14168,11 +14168,11 @@
       <c r="B6" s="72"/>
       <c r="C6" s="72"/>
       <c r="D6" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E6" s="70"/>
       <c r="F6" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>27</v>
@@ -14186,16 +14186,16 @@
       <c r="B7" s="72"/>
       <c r="C7" s="72"/>
       <c r="D7" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="E7" s="53" t="s">
         <v>359</v>
       </c>
-      <c r="E7" s="53" t="s">
+      <c r="F7" s="14" t="s">
         <v>360</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>361</v>
-      </c>
       <c r="G7" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H7" s="62"/>
     </row>
@@ -14206,13 +14206,13 @@
       <c r="B8" s="72"/>
       <c r="C8" s="72"/>
       <c r="D8" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E8" s="19" t="s">
+        <v>361</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>362</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>363</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>95</v>
@@ -14226,13 +14226,13 @@
       <c r="B9" s="72"/>
       <c r="C9" s="72"/>
       <c r="D9" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -14246,13 +14246,13 @@
       <c r="B10" s="73"/>
       <c r="C10" s="73"/>
       <c r="D10" s="54" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -14279,7 +14279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -14341,13 +14341,13 @@
         <v>106</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E3" s="68" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>21</v>
@@ -14365,7 +14365,7 @@
       </c>
       <c r="E4" s="69"/>
       <c r="F4" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>27</v>
@@ -14379,7 +14379,7 @@
       <c r="B5" s="85"/>
       <c r="C5" s="85"/>
       <c r="D5" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E5" s="70"/>
       <c r="F5" s="2" t="s">
@@ -14397,16 +14397,16 @@
       <c r="B6" s="85"/>
       <c r="C6" s="85"/>
       <c r="D6" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H6" s="6"/>
     </row>
@@ -14417,13 +14417,13 @@
       <c r="B7" s="85"/>
       <c r="C7" s="85"/>
       <c r="D7" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -14435,7 +14435,7 @@
       <c r="B8" s="85"/>
       <c r="C8" s="85"/>
       <c r="D8" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>93</v>
@@ -14455,13 +14455,13 @@
       <c r="B9" s="85"/>
       <c r="C9" s="85"/>
       <c r="D9" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="E9" s="19" t="s">
-        <v>292</v>
-      </c>
       <c r="F9" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -14475,13 +14475,13 @@
       <c r="B10" s="85"/>
       <c r="C10" s="85"/>
       <c r="D10" s="54" t="s">
+        <v>366</v>
+      </c>
+      <c r="E10" s="54" t="s">
         <v>367</v>
       </c>
-      <c r="E10" s="54" t="s">
-        <v>368</v>
-      </c>
       <c r="F10" s="54" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -14508,7 +14508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -14562,13 +14562,13 @@
     </row>
     <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B3" s="71" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="71" t="s">
-        <v>107</v>
+        <v>389</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>61</v>
@@ -14577,7 +14577,7 @@
         <v>90</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -14586,12 +14586,12 @@
     </row>
     <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4" s="72"/>
       <c r="C4" s="72"/>
       <c r="D4" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E4" s="69"/>
       <c r="F4" s="2" t="s">
@@ -14604,12 +14604,12 @@
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B5" s="72"/>
       <c r="C5" s="72"/>
       <c r="D5" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E5" s="69"/>
       <c r="F5" s="2" t="s">
@@ -14622,7 +14622,7 @@
     </row>
     <row r="6" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B6" s="72"/>
       <c r="C6" s="72"/>
@@ -14640,30 +14640,30 @@
     </row>
     <row r="7" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B7" s="72"/>
       <c r="C7" s="72"/>
       <c r="D7" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E7" s="51"/>
       <c r="F7" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>306</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>307</v>
       </c>
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A8" s="19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B8" s="72"/>
       <c r="C8" s="72"/>
       <c r="D8" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>97</v>
@@ -14678,18 +14678,18 @@
     </row>
     <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A9" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B9" s="72"/>
       <c r="C9" s="72"/>
       <c r="D9" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -14698,21 +14698,21 @@
     </row>
     <row r="10" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A10" s="55" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B10" s="73"/>
       <c r="C10" s="73"/>
       <c r="D10" s="54" t="s">
+        <v>378</v>
+      </c>
+      <c r="E10" s="54" t="s">
         <v>379</v>
       </c>
-      <c r="E10" s="54" t="s">
-        <v>380</v>
-      </c>
       <c r="F10" s="54" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="G10" s="59" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H10" s="59"/>
     </row>
@@ -14744,7 +14744,7 @@
     </row>
     <row r="13" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B13" s="71" t="s">
         <v>16</v>
@@ -14759,7 +14759,7 @@
         <v>91</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>21</v>
@@ -14768,16 +14768,16 @@
     </row>
     <row r="14" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B14" s="72"/>
       <c r="C14" s="72"/>
       <c r="D14" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E14" s="69"/>
       <c r="F14" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>21</v>
@@ -14786,12 +14786,12 @@
     </row>
     <row r="15" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B15" s="72"/>
       <c r="C15" s="72"/>
       <c r="D15" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E15" s="69"/>
       <c r="F15" s="2" t="s">
@@ -14804,7 +14804,7 @@
     </row>
     <row r="16" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B16" s="72"/>
       <c r="C16" s="72"/>
@@ -14822,30 +14822,30 @@
     </row>
     <row r="17" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B17" s="72"/>
       <c r="C17" s="72"/>
       <c r="D17" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E17" s="51"/>
       <c r="F17" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>306</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>307</v>
       </c>
       <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A18" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B18" s="72"/>
       <c r="C18" s="72"/>
       <c r="D18" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>97</v>
@@ -14860,18 +14860,18 @@
     </row>
     <row r="19" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A19" s="26" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B19" s="72"/>
       <c r="C19" s="72"/>
       <c r="D19" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E19" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="F19" s="19" t="s">
         <v>295</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>296</v>
       </c>
       <c r="G19" s="20" t="s">
         <v>21</v>
@@ -14880,21 +14880,21 @@
     </row>
     <row r="20" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A20" s="55" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B20" s="73"/>
       <c r="C20" s="73"/>
       <c r="D20" s="54" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E20" s="54" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F20" s="54" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="G20" s="59" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H20" s="59"/>
     </row>
@@ -14977,22 +14977,22 @@
         <v>17</v>
       </c>
       <c r="C3" s="71" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E3" s="68" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
@@ -15020,7 +15020,7 @@
       <c r="B5" s="72"/>
       <c r="C5" s="72"/>
       <c r="D5" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E5" s="70"/>
       <c r="F5" s="2" t="s">
@@ -15038,16 +15038,16 @@
       <c r="B6" s="72"/>
       <c r="C6" s="72"/>
       <c r="D6" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E6" s="68" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -15058,14 +15058,14 @@
       <c r="B7" s="72"/>
       <c r="C7" s="72"/>
       <c r="D7" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E7" s="69"/>
       <c r="F7" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>286</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>287</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -15076,14 +15076,14 @@
       <c r="B8" s="72"/>
       <c r="C8" s="72"/>
       <c r="D8" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E8" s="70"/>
       <c r="F8" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -15094,7 +15094,7 @@
       <c r="B9" s="72"/>
       <c r="C9" s="72"/>
       <c r="D9" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>97</v>
@@ -15114,13 +15114,13 @@
       <c r="B10" s="72"/>
       <c r="C10" s="72"/>
       <c r="D10" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E10" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="F10" s="19" t="s">
         <v>295</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>296</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>21</v>
@@ -15134,13 +15134,13 @@
       <c r="B11" s="72"/>
       <c r="C11" s="72"/>
       <c r="D11" s="54" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E11" s="55" t="s">
+        <v>369</v>
+      </c>
+      <c r="F11" s="55" t="s">
         <v>370</v>
-      </c>
-      <c r="F11" s="55" t="s">
-        <v>371</v>
       </c>
       <c r="G11" s="60" t="s">
         <v>21</v>
@@ -15149,18 +15149,18 @@
     </row>
     <row r="12" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A12" s="66" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B12" s="73"/>
       <c r="C12" s="73"/>
       <c r="D12" s="54" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E12" s="55" t="s">
+        <v>371</v>
+      </c>
+      <c r="F12" s="55" t="s">
         <v>372</v>
-      </c>
-      <c r="F12" s="55" t="s">
-        <v>373</v>
       </c>
       <c r="G12" s="60" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Update the test case file after updated hint message on rename file with specificname
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -10375,6 +10375,626 @@
   </si>
   <si>
     <r>
+      <t>1.在</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:D:\Test
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want find?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如Alonso
+3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want replace?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">",输入新的想要被替换的文件夹名为空字符
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2. 根据</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件中的某一字段，输入想要被替换的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>为空字符</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2. 根据</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件中的某一字段，输入想要被替换的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>已有字段</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3. 输入想要被替换的新名称为空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.1.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.2.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件夹名字
+2.输入替换的文件夹名字为</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如D:\TesT39
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what word you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字为空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The format of " D:Test Folder " is incorrect! Should with '\'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件名字
+2.输入替换的文件名字为</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件名字，如D:\TesT39\ALO.bmp
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what word you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件名字为空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示请不要输入空的替换内容信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty replace content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示请不要输入空查找内容的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty search content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示不能输入空的搜索内容的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty search content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示不能输入空的搜索内容的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty file or folder name, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示替换内容不能为空的信息
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty replace content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. Rename file or folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t>提示需要被替换字符不能为空的信息 
 （</t>
     </r>
@@ -10388,7 +11008,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Do not input the empty find content, please input again!</t>
+      <t>Illegal -- cannot input empty search content, please input again!</t>
     </r>
     <r>
       <rPr>
@@ -10400,84 +11020,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:D:\Test
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What word do you want find?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如Alonso
-3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What word do you want replace?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">",输入新的想要被替换的文件夹名为空字符
-</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -10496,7 +11038,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Do not input the empty replace content, please input again!</t>
+      <t>Illegal -- cannot input empty replace content, please input again!</t>
     </r>
     <r>
       <rPr>
@@ -10509,548 +11051,6 @@
       </rPr>
       <t>）</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8.10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径
-2. 根据</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件中的某一字段，输入想要被替换的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>为空字符</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径
-2. 根据</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件中的某一字段，输入想要被替换的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>已有字段</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3. 输入想要被替换的新名称为空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7.1.8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7.2.8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件夹名字
-2.输入替换的文件夹名字为</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如D:\TesT39
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what word you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字为空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The format of " D:Test Folder " is incorrect! Should with '\'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pass</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件名字
-2.输入替换的文件名字为</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件名字，如D:\TesT39\ALO.bmp
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what word you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件名字为空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示请不要输入空的替换内容信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Illegal -- cannot input empty replace content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示请不要输入空查找内容的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Illegal -- cannot input empty search content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示不能输入空的搜索内容的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Illegal -- cannot input empty search content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示不能输入空的搜索内容的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Illegal -- cannot input empty file or folder name, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示替换内容不能为空的信息
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Illegal -- cannot input empty replace content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7. Rename file or folder</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -12067,7 +12067,7 @@
         <v>345</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G10" s="59"/>
       <c r="H10" s="59"/>
@@ -12085,7 +12085,7 @@
         <v>346</v>
       </c>
       <c r="F11" s="54" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G11" s="59"/>
       <c r="H11" s="59"/>
@@ -14252,7 +14252,7 @@
         <v>364</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -14481,7 +14481,7 @@
         <v>367</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -14508,7 +14508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -14568,7 +14568,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="71" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>61</v>
@@ -14689,7 +14689,7 @@
         <v>294</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -14698,21 +14698,21 @@
     </row>
     <row r="10" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A10" s="55" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B10" s="73"/>
       <c r="C10" s="73"/>
       <c r="D10" s="54" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E10" s="54" t="s">
+        <v>377</v>
+      </c>
+      <c r="F10" s="54" t="s">
+        <v>386</v>
+      </c>
+      <c r="G10" s="59" t="s">
         <v>379</v>
-      </c>
-      <c r="F10" s="54" t="s">
-        <v>388</v>
-      </c>
-      <c r="G10" s="59" t="s">
-        <v>381</v>
       </c>
       <c r="H10" s="59"/>
     </row>
@@ -14880,21 +14880,21 @@
     </row>
     <row r="20" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A20" s="55" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B20" s="73"/>
       <c r="C20" s="73"/>
       <c r="D20" s="54" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E20" s="54" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F20" s="54" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="G20" s="59" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H20" s="59"/>
     </row>
@@ -14918,7 +14918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -15134,13 +15134,13 @@
       <c r="B11" s="72"/>
       <c r="C11" s="72"/>
       <c r="D11" s="54" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E11" s="55" t="s">
         <v>369</v>
       </c>
       <c r="F11" s="55" t="s">
-        <v>370</v>
+        <v>388</v>
       </c>
       <c r="G11" s="60" t="s">
         <v>21</v>
@@ -15149,18 +15149,18 @@
     </row>
     <row r="12" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A12" s="66" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B12" s="73"/>
       <c r="C12" s="73"/>
       <c r="D12" s="54" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E12" s="55" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F12" s="55" t="s">
-        <v>372</v>
+        <v>389</v>
       </c>
       <c r="G12" s="60" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Update the test case file after updated hint message for most functions
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -7328,19 +7328,144 @@
   </si>
   <si>
     <r>
+      <t>1. 显示指定的文件夹路径不存在 （</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso1.jpg is NOT exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2. 重命名失败</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 显示成功的将相同字段的文件被替换为指定的新名称
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\alonso.txt has been replaced as D:\Test\Button.txt successfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+2.可以在本地计算机中查到新名称文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 显示查找的文件不包含指定字段 （</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Didn't found file named with alonso on file D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2. 重命名失败</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">文件路径
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t>1.在"</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the file or folder path:</t>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
     </r>
     <r>
       <rPr>
@@ -7363,7 +7488,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>D:\Test\Alonso.txt</t>
+      <t>D:\Test9</t>
     </r>
     <r>
       <rPr>
@@ -7381,101 +7506,282 @@
       <rPr>
         <b/>
         <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What file or folder you want to find on this folder?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入文件夹名，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>McLaren</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
         <color theme="4"/>
         <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>What word do you want find?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alonso</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What word do you want replace?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Button</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 显示指定的文件夹路径不存在 （</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso1.jpg is NOT exist!</t>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test9\123.txt</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示输入需要被复制文件夹或者文件路径时，输入存在路径不带'\'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在提示信息"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"出现时，输入存在路径不带'\'</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.1.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在提示信息"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"出现时，输入一串空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在提示信息"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"出现时，输入存在路径不带'\'</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The format of " D:Test Folder " is incorrect! Should with '\'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.2.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.1.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.1.9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.2.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.1.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.1.7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.1.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件夹名字
+2.输入替换的空文件夹名</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.2.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示新命名文件夹不能为空（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cannot rename with empty path. Please input again!</t>
     </r>
     <r>
       <rPr>
@@ -7487,68 +7793,7 @@
         <scheme val="minor"/>
       </rPr>
       <t>）
-2. 重命名失败</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 显示成功的将相同字段的文件被替换为指定的新名称
-(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\alonso.txt has been replaced as D:\Test\Button.txt successfully!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)
-2.可以在本地计算机中查到新名称文件</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 显示查找的文件不包含指定字段 （</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Didn't found file named with alonso on file D:\Test\Alonso.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2. 重命名失败</t>
+2.文件夹不应被重命名成功</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7558,7 +7803,7 @@
   </si>
   <si>
     <r>
-      <t>1.输入</t>
+      <t>1.输入该路径下</t>
     </r>
     <r>
       <rPr>
@@ -7581,9 +7826,21 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">文件路径
-</t>
-    </r>
+      <t>原来的文件夹名字
+2.输入替换的空文件名</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.2.7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.1.12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示输入需要被目标文件夹路径时，输入存在路径不带'\'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -7594,36 +7851,36 @@
       <rPr>
         <b/>
         <sz val="12"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test9</t>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件夹的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
     </r>
     <r>
       <rPr>
@@ -7641,82 +7898,25 @@
       <rPr>
         <b/>
         <sz val="12"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What file or folder you want to find on this folder?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入文件夹名，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>McLaren</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test9\123.txt</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>提示输入需要被复制文件夹或者文件路径时，输入存在路径不带'\'</t>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入空字符串</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -7733,7 +7933,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please input the folder path:</t>
+      <t>Please input target folder path:</t>
     </r>
     <r>
       <rPr>
@@ -7749,233 +7949,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2.1.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>在提示信息"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"出现时，输入一串空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>在提示信息"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"出现时，输入存在路径不带'\'</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The format of " D:Test Folder " is incorrect! Should with '\'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.2.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.1.11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.1.9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7.2.6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7.1.6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7.1.7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7.1.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件夹名字
-2.输入替换的空文件夹名</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7.2.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示新命名文件夹不能为空（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cannot rename with empty path. Please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件夹不应被重命名成功</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pass</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件夹名字
-2.输入替换的空文件名</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7.2.7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.1.12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>提示输入需要被目标文件夹路径时，输入存在路径不带'\'</t>
+    <t>提示输入需要被复制文件夹路径时，输入存在路径不带'\'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.2.9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.2.10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -8068,7 +8050,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please input target folder path:</t>
+      <t>Please input the folder or file path:</t>
     </r>
     <r>
       <rPr>
@@ -8084,123 +8066,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>提示输入需要被复制文件夹路径时，输入存在路径不带'\'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.2.9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.2.10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入被复制文件夹的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input target folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入空字符串</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>在提示信息"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"出现时，输入存在路径不带'\'</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>提示输入需要被复制文件路径时，输入存在路径不带'\'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -8234,141 +8099,6 @@
   </si>
   <si>
     <t>提示输入需要被移动文件夹或者文件路径时，输入存在路径不带'\'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what word you want to find:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入txt文件内存在的内容，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Alonso
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what word you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入想要替换成的新内容，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alo</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -9109,136 +8839,6 @@
   </si>
   <si>
     <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:" 输入路径，如:D:\Test
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what word you want to find</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:",输入空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:" 输入路径，如:D:\Test
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what word you want to find:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入txt文件内存在的内容，如Alonso
-3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what word you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入想要替换成的新内容，输入空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1.输入</t>
     </r>
     <r>
@@ -10185,6 +9785,212 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>8.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2. 根据</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件中的某一字段，输入想要被替换的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>为空字符</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2. 根据</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件中的某一字段，输入想要被替换的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>已有字段</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3. 输入想要被替换的新名称为空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.1.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.2.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件夹名字
+2.输入替换的文件夹名字为</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t>1.在"</t>
     </r>
@@ -10192,13 +9998,409 @@
       <rPr>
         <b/>
         <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如D:\TesT39
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what word you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字为空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The format of " D:Test Folder " is incorrect! Should with '\'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件名字
+2.输入替换的文件名字为</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件名字，如D:\TesT39\ALO.bmp
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what word you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件名字为空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示请不要输入空的替换内容信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty replace content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示请不要输入空查找内容的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty search content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示不能输入空的搜索内容的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty search content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示不能输入空的搜索内容的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty file or folder name, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示替换内容不能为空的信息
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty replace content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. Rename file or folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示需要被替换字符不能为空的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty search content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示需要新替换字符名称不能为空的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illegal -- cannot input empty replace content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
         <color theme="4"/>
         <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please input the file or folder path:</t>
+      <t>Please input the folder path:</t>
     </r>
     <r>
       <rPr>
@@ -10245,7 +10447,272 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>What word do you want find?</t>
+      <t>Please input what content you want to find:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入txt文件内存在的内容，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Alonso
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what content you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入想要替换成的新内容，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alo</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:" 输入路径，如:D:\Test
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what content you want to find</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:",输入空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:" 输入路径，如:D:\Test
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what content you want to find:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入txt文件内存在的内容，如Alonso
+3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what content you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入想要替换成的新内容，输入空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the file or folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What content do you want find?</t>
     </r>
     <r>
       <rPr>
@@ -10292,7 +10759,142 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>What word do you want replace?</t>
+      <t>What content do you want replace?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Button</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the file or folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What content do you want find?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alonso</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What content do you want replace?</t>
     </r>
     <r>
       <rPr>
@@ -10357,7 +10959,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>What word do you want find?</t>
+      <t>What content do you want find?</t>
     </r>
     <r>
       <rPr>
@@ -10411,7 +11013,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>What word do you want find?</t>
+      <t>What content do you want find?</t>
     </r>
     <r>
       <rPr>
@@ -10435,7 +11037,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>What word do you want replace?</t>
+      <t>What content do you want replace?</t>
     </r>
     <r>
       <rPr>
@@ -10448,608 +11050,6 @@
       </rPr>
       <t xml:space="preserve">",输入新的想要被替换的文件夹名为空字符
 </t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8.10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径
-2. 根据</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件中的某一字段，输入想要被替换的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>为空字符</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径
-2. 根据</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件中的某一字段，输入想要被替换的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>已有字段</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3. 输入想要被替换的新名称为空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7.1.8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7.2.8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件夹名字
-2.输入替换的文件夹名字为</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如D:\TesT39
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what word you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字为空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The format of " D:Test Folder " is incorrect! Should with '\'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pass</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件名字
-2.输入替换的文件名字为</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件名字，如D:\TesT39\ALO.bmp
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what word you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件名字为空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示请不要输入空的替换内容信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Illegal -- cannot input empty replace content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示请不要输入空查找内容的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Illegal -- cannot input empty search content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示不能输入空的搜索内容的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Illegal -- cannot input empty search content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示不能输入空的搜索内容的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Illegal -- cannot input empty file or folder name, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示替换内容不能为空的信息
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Illegal -- cannot input empty replace content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7. Rename file or folder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示需要被替换字符不能为空的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Illegal -- cannot input empty search content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示需要新替换字符名称不能为空的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Illegal -- cannot input empty replace content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -11865,8 +11865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -11929,13 +11929,13 @@
         <v>100</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E3" s="68" t="s">
-        <v>327</v>
+        <v>383</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>22</v>
@@ -11949,11 +11949,11 @@
       <c r="B4" s="72"/>
       <c r="C4" s="72"/>
       <c r="D4" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E4" s="69"/>
       <c r="F4" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>23</v>
@@ -11967,11 +11967,11 @@
       <c r="B5" s="72"/>
       <c r="C5" s="72"/>
       <c r="D5" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E5" s="69"/>
       <c r="F5" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>24</v>
@@ -11985,11 +11985,11 @@
       <c r="B6" s="72"/>
       <c r="C6" s="72"/>
       <c r="D6" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E6" s="70"/>
       <c r="F6" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>27</v>
@@ -12003,13 +12003,13 @@
       <c r="B7" s="72"/>
       <c r="C7" s="72"/>
       <c r="D7" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>336</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>337</v>
-      </c>
-      <c r="E7" s="52" t="s">
-        <v>338</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>339</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="57"/>
@@ -12024,10 +12024,10 @@
         <v>137</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>95</v>
@@ -12041,13 +12041,13 @@
       <c r="B9" s="72"/>
       <c r="C9" s="72"/>
       <c r="D9" s="19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -12061,13 +12061,13 @@
       <c r="B10" s="72"/>
       <c r="C10" s="72"/>
       <c r="D10" s="54" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>345</v>
+        <v>384</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="G10" s="59"/>
       <c r="H10" s="59"/>
@@ -12079,13 +12079,13 @@
       <c r="B11" s="73"/>
       <c r="C11" s="73"/>
       <c r="D11" s="54" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E11" s="54" t="s">
-        <v>346</v>
+        <v>385</v>
       </c>
       <c r="F11" s="54" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="G11" s="59"/>
       <c r="H11" s="59"/>
@@ -12555,13 +12555,13 @@
       <c r="B8" s="85"/>
       <c r="C8" s="85"/>
       <c r="D8" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="E8" s="19" t="s">
         <v>290</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>291</v>
-      </c>
       <c r="F8" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>21</v>
@@ -12713,7 +12713,7 @@
         <v>137</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>94</v>
@@ -12725,18 +12725,18 @@
     </row>
     <row r="7" spans="1:9" ht="57" x14ac:dyDescent="0.15">
       <c r="A7" s="26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B7" s="73"/>
       <c r="C7" s="73"/>
       <c r="D7" s="19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E7" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>294</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>295</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>21</v>
@@ -12872,18 +12872,18 @@
     </row>
     <row r="14" spans="1:9" s="22" customFormat="1" ht="57" x14ac:dyDescent="0.15">
       <c r="A14" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B14" s="73"/>
       <c r="C14" s="73"/>
       <c r="D14" s="19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E14" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>294</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>295</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>21</v>
@@ -13227,7 +13227,7 @@
         <v>138</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F12" s="19" t="s">
         <v>112</v>
@@ -13239,18 +13239,18 @@
     </row>
     <row r="13" spans="1:8" s="22" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A13" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B13" s="72"/>
       <c r="C13" s="72"/>
       <c r="D13" s="19" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E13" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="F13" s="19" t="s">
         <v>294</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>295</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>21</v>
@@ -13259,18 +13259,18 @@
     </row>
     <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A14" s="26" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B14" s="73"/>
       <c r="C14" s="73"/>
       <c r="D14" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>21</v>
@@ -13447,7 +13447,7 @@
         <v>138</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F24" s="19" t="s">
         <v>112</v>
@@ -13459,18 +13459,18 @@
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B25" s="72"/>
       <c r="C25" s="72"/>
       <c r="D25" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>21</v>
@@ -13479,18 +13479,18 @@
     </row>
     <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B26" s="73"/>
       <c r="C26" s="73"/>
       <c r="D26" s="19" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>21</v>
@@ -13725,18 +13725,18 @@
     </row>
     <row r="11" spans="1:8" s="32" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B11" s="82"/>
       <c r="C11" s="82"/>
       <c r="D11" s="19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E11" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="F11" s="19" t="s">
         <v>294</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>295</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>21</v>
@@ -13745,18 +13745,18 @@
     </row>
     <row r="12" spans="1:8" s="32" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B12" s="83"/>
       <c r="C12" s="83"/>
       <c r="D12" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>21</v>
@@ -13990,18 +13990,18 @@
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B25" s="72"/>
       <c r="C25" s="82"/>
       <c r="D25" s="19" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E25" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="F25" s="19" t="s">
         <v>294</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>295</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>21</v>
@@ -14010,18 +14010,18 @@
     </row>
     <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B26" s="73"/>
       <c r="C26" s="83"/>
       <c r="D26" s="19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>21</v>
@@ -14112,13 +14112,13 @@
         <v>105</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E3" s="68" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>34</v>
@@ -14132,11 +14132,11 @@
       <c r="B4" s="72"/>
       <c r="C4" s="72"/>
       <c r="D4" s="14" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E4" s="69"/>
       <c r="F4" s="14" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>27</v>
@@ -14150,11 +14150,11 @@
       <c r="B5" s="72"/>
       <c r="C5" s="72"/>
       <c r="D5" s="14" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E5" s="69"/>
       <c r="F5" s="14" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>22</v>
@@ -14168,11 +14168,11 @@
       <c r="B6" s="72"/>
       <c r="C6" s="72"/>
       <c r="D6" s="14" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E6" s="70"/>
       <c r="F6" s="14" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>27</v>
@@ -14186,13 +14186,13 @@
       <c r="B7" s="72"/>
       <c r="C7" s="72"/>
       <c r="D7" s="14" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E7" s="53" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>278</v>
@@ -14209,10 +14209,10 @@
         <v>137</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>95</v>
@@ -14226,13 +14226,13 @@
       <c r="B9" s="72"/>
       <c r="C9" s="72"/>
       <c r="D9" s="19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -14246,13 +14246,13 @@
       <c r="B10" s="73"/>
       <c r="C10" s="73"/>
       <c r="D10" s="54" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -14341,7 +14341,7 @@
         <v>106</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E3" s="68" t="s">
         <v>261</v>
@@ -14400,7 +14400,7 @@
         <v>214</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>216</v>
@@ -14417,10 +14417,10 @@
       <c r="B7" s="85"/>
       <c r="C7" s="85"/>
       <c r="D7" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>277</v>
@@ -14455,13 +14455,13 @@
       <c r="B9" s="85"/>
       <c r="C9" s="85"/>
       <c r="D9" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>290</v>
       </c>
-      <c r="E9" s="19" t="s">
-        <v>291</v>
-      </c>
       <c r="F9" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -14475,13 +14475,13 @@
       <c r="B10" s="85"/>
       <c r="C10" s="85"/>
       <c r="D10" s="54" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -14568,7 +14568,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="71" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>61</v>
@@ -14640,25 +14640,25 @@
     </row>
     <row r="7" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B7" s="72"/>
       <c r="C7" s="72"/>
       <c r="D7" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E7" s="51"/>
       <c r="F7" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>305</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>306</v>
       </c>
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A8" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B8" s="72"/>
       <c r="C8" s="72"/>
@@ -14678,18 +14678,18 @@
     </row>
     <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A9" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B9" s="72"/>
       <c r="C9" s="72"/>
       <c r="D9" s="19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -14698,21 +14698,21 @@
     </row>
     <row r="10" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A10" s="55" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="B10" s="73"/>
       <c r="C10" s="73"/>
       <c r="D10" s="54" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="G10" s="59" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="H10" s="59"/>
     </row>
@@ -14822,25 +14822,25 @@
     </row>
     <row r="17" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B17" s="72"/>
       <c r="C17" s="72"/>
       <c r="D17" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E17" s="51"/>
       <c r="F17" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>305</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>306</v>
       </c>
       <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A18" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B18" s="72"/>
       <c r="C18" s="72"/>
@@ -14860,18 +14860,18 @@
     </row>
     <row r="19" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A19" s="26" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B19" s="72"/>
       <c r="C19" s="72"/>
       <c r="D19" s="19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E19" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="F19" s="19" t="s">
         <v>294</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>295</v>
       </c>
       <c r="G19" s="20" t="s">
         <v>21</v>
@@ -14880,21 +14880,21 @@
     </row>
     <row r="20" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A20" s="55" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="B20" s="73"/>
       <c r="C20" s="73"/>
       <c r="D20" s="54" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="E20" s="54" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="F20" s="54" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="G20" s="59" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="H20" s="59"/>
     </row>
@@ -14918,7 +14918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -14983,7 +14983,7 @@
         <v>149</v>
       </c>
       <c r="E3" s="68" t="s">
-        <v>368</v>
+        <v>386</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>239</v>
@@ -15041,13 +15041,13 @@
         <v>280</v>
       </c>
       <c r="E6" s="68" t="s">
-        <v>282</v>
+        <v>387</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -15062,10 +15062,10 @@
       </c>
       <c r="E7" s="69"/>
       <c r="F7" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>286</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -15080,10 +15080,10 @@
       </c>
       <c r="E8" s="70"/>
       <c r="F8" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -15114,13 +15114,13 @@
       <c r="B10" s="72"/>
       <c r="C10" s="72"/>
       <c r="D10" s="19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E10" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="F10" s="19" t="s">
         <v>294</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>295</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>21</v>
@@ -15134,13 +15134,13 @@
       <c r="B11" s="72"/>
       <c r="C11" s="72"/>
       <c r="D11" s="54" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>369</v>
+        <v>388</v>
       </c>
       <c r="F11" s="55" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="G11" s="60" t="s">
         <v>21</v>
@@ -15149,18 +15149,18 @@
     </row>
     <row r="12" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A12" s="66" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="B12" s="73"/>
       <c r="C12" s="73"/>
       <c r="D12" s="54" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="E12" s="55" t="s">
-        <v>370</v>
+        <v>389</v>
       </c>
       <c r="F12" s="55" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="G12" s="60" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Update the test case file after updated hint message on empty string again
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -7840,10 +7840,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>提示输入需要被目标文件夹路径时，输入存在路径不带'\'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>1.在"</t>
     </r>
@@ -8067,10 +8063,6 @@
   </si>
   <si>
     <t>提示输入需要被复制文件路径时，输入存在路径不带'\'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>提示输入需要被目标文件路径时，输入存在路径不带'\'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -10173,6 +10165,707 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>7. Rename file or folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what content you want to find:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入txt文件内存在的内容，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Alonso
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what content you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入想要替换成的新内容，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alo</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:" 输入路径，如:D:\Test
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what content you want to find</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:",输入空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:" 输入路径，如:D:\Test
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what content you want to find:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入txt文件内存在的内容，如Alonso
+3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what content you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入想要替换成的新内容，输入空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the file or folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What content do you want find?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alonso</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What content do you want replace?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Button</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the file or folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What content do you want find?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alonso</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What content do you want replace?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Button</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:D:\Test
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What content do you want find?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">",输入空字符
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:D:\Test
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What content do you want find?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如Alonso
+3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What content do you want replace?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">",输入新的想要被替换的文件夹名为空字符
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示请不要输入空查找内容的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cannot input empty search content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t>提示请不要输入空的替换内容信息 
 （</t>
@@ -10187,37 +10880,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Illegal -- cannot input empty replace content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示请不要输入空查找内容的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Illegal -- cannot input empty search content, please input again!</t>
+      <t>Cannot input empty replace content, please input again!</t>
     </r>
     <r>
       <rPr>
@@ -10247,7 +10910,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Illegal -- cannot input empty search content, please input again!</t>
+      <t>Cannot input empty search content, please input again!</t>
     </r>
     <r>
       <rPr>
@@ -10277,7 +10940,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Illegal -- cannot input empty file or folder name, please input again!</t>
+      <t>Cannot input empty file or folder name, please input again!</t>
     </r>
     <r>
       <rPr>
@@ -10307,7 +10970,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Illegal -- cannot input empty replace content, please input again!</t>
+      <t>Cannot input empty replace content, please input again!</t>
     </r>
     <r>
       <rPr>
@@ -10320,10 +10983,6 @@
       </rPr>
       <t>）</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7. Rename file or folder</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -10341,7 +11000,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Illegal -- cannot input empty search content, please input again!</t>
+      <t>Cannot input empty search content, please input again!</t>
     </r>
     <r>
       <rPr>
@@ -10371,7 +11030,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Illegal -- cannot input empty replace content, please input again!</t>
+      <t>Cannot input empty replace content, please input again!</t>
     </r>
     <r>
       <rPr>
@@ -10387,670 +11046,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what content you want to find:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入txt文件内存在的内容，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Alonso
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what content you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入想要替换成的新内容，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alo</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:" 输入路径，如:D:\Test
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what content you want to find</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:",输入空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:" 输入路径，如:D:\Test
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what content you want to find:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入txt文件内存在的内容，如Alonso
-3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what content you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入想要替换成的新内容，输入空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the file or folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What content do you want find?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alonso</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What content do you want replace?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Button</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the file or folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What content do you want find?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alonso</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What content do you want replace?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Button</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:D:\Test
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What content do you want find?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">",输入空字符
-</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:D:\Test
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What content do you want find?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如Alonso
-3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What content do you want replace?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">",输入新的想要被替换的文件夹名为空字符
-</t>
-    </r>
+    <t>提示输入需要被目标文件夹路径时，输入存在路径不带'\'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示输入需要被目标文件路径时，输入存在路径不带'\'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -11929,13 +11929,13 @@
         <v>100</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E3" s="68" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>22</v>
@@ -11949,11 +11949,11 @@
       <c r="B4" s="72"/>
       <c r="C4" s="72"/>
       <c r="D4" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E4" s="69"/>
       <c r="F4" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>23</v>
@@ -11967,11 +11967,11 @@
       <c r="B5" s="72"/>
       <c r="C5" s="72"/>
       <c r="D5" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E5" s="69"/>
       <c r="F5" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>24</v>
@@ -11985,11 +11985,11 @@
       <c r="B6" s="72"/>
       <c r="C6" s="72"/>
       <c r="D6" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E6" s="70"/>
       <c r="F6" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>27</v>
@@ -12003,13 +12003,13 @@
       <c r="B7" s="72"/>
       <c r="C7" s="72"/>
       <c r="D7" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>334</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>335</v>
-      </c>
-      <c r="E7" s="52" t="s">
-        <v>336</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>337</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="57"/>
@@ -12024,10 +12024,10 @@
         <v>137</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>95</v>
@@ -12044,10 +12044,10 @@
         <v>289</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -12061,13 +12061,13 @@
       <c r="B10" s="72"/>
       <c r="C10" s="72"/>
       <c r="D10" s="54" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="G10" s="59"/>
       <c r="H10" s="59"/>
@@ -12079,13 +12079,13 @@
       <c r="B11" s="73"/>
       <c r="C11" s="73"/>
       <c r="D11" s="54" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E11" s="54" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="F11" s="54" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="G11" s="59"/>
       <c r="H11" s="59"/>
@@ -13227,7 +13227,7 @@
         <v>138</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F12" s="19" t="s">
         <v>112</v>
@@ -13244,7 +13244,7 @@
       <c r="B13" s="72"/>
       <c r="C13" s="72"/>
       <c r="D13" s="19" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>293</v>
@@ -13264,10 +13264,10 @@
       <c r="B14" s="73"/>
       <c r="C14" s="73"/>
       <c r="D14" s="19" t="s">
-        <v>318</v>
+        <v>388</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>294</v>
@@ -13447,7 +13447,7 @@
         <v>138</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F24" s="19" t="s">
         <v>112</v>
@@ -13459,15 +13459,15 @@
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B25" s="72"/>
       <c r="C25" s="72"/>
       <c r="D25" s="19" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F25" s="19" t="s">
         <v>294</v>
@@ -13479,15 +13479,15 @@
     </row>
     <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B26" s="73"/>
       <c r="C26" s="73"/>
       <c r="D26" s="19" t="s">
-        <v>309</v>
+        <v>389</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F26" s="19" t="s">
         <v>294</v>
@@ -13730,7 +13730,7 @@
       <c r="B11" s="82"/>
       <c r="C11" s="82"/>
       <c r="D11" s="19" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>293</v>
@@ -13745,15 +13745,15 @@
     </row>
     <row r="12" spans="1:8" s="32" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="26" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B12" s="83"/>
       <c r="C12" s="83"/>
       <c r="D12" s="19" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F12" s="19" t="s">
         <v>294</v>
@@ -13990,12 +13990,12 @@
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B25" s="72"/>
       <c r="C25" s="82"/>
       <c r="D25" s="19" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>293</v>
@@ -14010,15 +14010,15 @@
     </row>
     <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B26" s="73"/>
       <c r="C26" s="83"/>
       <c r="D26" s="19" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F26" s="19" t="s">
         <v>294</v>
@@ -14112,13 +14112,13 @@
         <v>105</v>
       </c>
       <c r="D3" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="E3" s="68" t="s">
+        <v>344</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>345</v>
-      </c>
-      <c r="E3" s="68" t="s">
-        <v>346</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>347</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>34</v>
@@ -14132,11 +14132,11 @@
       <c r="B4" s="72"/>
       <c r="C4" s="72"/>
       <c r="D4" s="14" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E4" s="69"/>
       <c r="F4" s="14" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>27</v>
@@ -14150,11 +14150,11 @@
       <c r="B5" s="72"/>
       <c r="C5" s="72"/>
       <c r="D5" s="14" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E5" s="69"/>
       <c r="F5" s="14" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>22</v>
@@ -14168,11 +14168,11 @@
       <c r="B6" s="72"/>
       <c r="C6" s="72"/>
       <c r="D6" s="14" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E6" s="70"/>
       <c r="F6" s="14" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>27</v>
@@ -14186,13 +14186,13 @@
       <c r="B7" s="72"/>
       <c r="C7" s="72"/>
       <c r="D7" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>353</v>
+      </c>
+      <c r="F7" s="14" t="s">
         <v>354</v>
-      </c>
-      <c r="E7" s="53" t="s">
-        <v>355</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>356</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>278</v>
@@ -14209,10 +14209,10 @@
         <v>137</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>95</v>
@@ -14229,10 +14229,10 @@
         <v>289</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -14246,13 +14246,13 @@
       <c r="B10" s="73"/>
       <c r="C10" s="73"/>
       <c r="D10" s="54" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -14341,7 +14341,7 @@
         <v>106</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E3" s="68" t="s">
         <v>261</v>
@@ -14475,13 +14475,13 @@
       <c r="B10" s="85"/>
       <c r="C10" s="85"/>
       <c r="D10" s="54" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -14508,7 +14508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -14568,7 +14568,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="71" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>61</v>
@@ -14689,7 +14689,7 @@
         <v>293</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -14698,21 +14698,21 @@
     </row>
     <row r="10" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A10" s="55" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B10" s="73"/>
       <c r="C10" s="73"/>
       <c r="D10" s="54" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E10" s="54" t="s">
+        <v>368</v>
+      </c>
+      <c r="F10" s="54" t="s">
+        <v>385</v>
+      </c>
+      <c r="G10" s="59" t="s">
         <v>370</v>
-      </c>
-      <c r="F10" s="54" t="s">
-        <v>379</v>
-      </c>
-      <c r="G10" s="59" t="s">
-        <v>372</v>
       </c>
       <c r="H10" s="59"/>
     </row>
@@ -14880,21 +14880,21 @@
     </row>
     <row r="20" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A20" s="55" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B20" s="73"/>
       <c r="C20" s="73"/>
       <c r="D20" s="54" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E20" s="54" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F20" s="54" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="G20" s="59" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="H20" s="59"/>
     </row>
@@ -14983,7 +14983,7 @@
         <v>149</v>
       </c>
       <c r="E3" s="68" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>239</v>
@@ -15041,7 +15041,7 @@
         <v>280</v>
       </c>
       <c r="E6" s="68" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>283</v>
@@ -15134,13 +15134,13 @@
       <c r="B11" s="72"/>
       <c r="C11" s="72"/>
       <c r="D11" s="54" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="F11" s="55" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
       <c r="G11" s="60" t="s">
         <v>21</v>
@@ -15149,18 +15149,18 @@
     </row>
     <row r="12" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A12" s="66" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B12" s="73"/>
       <c r="C12" s="73"/>
       <c r="D12" s="54" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E12" s="55" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="F12" s="55" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="G12" s="60" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Update the test case file of FileOperation after fixed #33
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="398">
   <si>
     <t>删除文件夹</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1952,94 +1952,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>D:\Test1</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入被复制文件夹的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input target folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入需要复制到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\Program Files</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -5702,93 +5614,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>需要被复制的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>非空文件夹</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的路径和</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>目标路径
-2.输入被复制文件夹路径和目标文件夹路径</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>需要被复制</t>
     </r>
     <r>
@@ -11046,11 +10871,507 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>3.1.13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.2.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被复制的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>非空文件夹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>目标路径
+2.输入被复制文件夹路径和目标文件夹路径</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示输入需要被目标文件路径时，输入存在路径不带'\'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>提示输入需要被目标文件夹路径时，输入存在路径不带'\'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>提示输入需要被目标文件路径时，输入存在路径不带'\'</t>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被复制的文件夹路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的本地磁盘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的文件夹路径
+2.输入被复制文件夹路径和目标文件夹路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件夹的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Program Files</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件夹的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I:\Program Files</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示目标本地磁盘不存在，无法复制的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I: is not exists on this PC, cannot copy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I:\Program Files</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被复制的文件路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的本地磁盘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的文件夹路径
+2.输入被复制文件路径和目标文件夹路径</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -11189,7 +11510,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -11217,6 +11538,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11299,7 +11626,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -11500,6 +11827,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -11865,7 +12201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -11883,14 +12219,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="67"/>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
+      <c r="A1" s="70"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11922,20 +12258,20 @@
       <c r="A3" s="21">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="71" t="s">
-        <v>100</v>
+      <c r="C3" s="74" t="s">
+        <v>99</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="E3" s="68" t="s">
-        <v>374</v>
+        <v>323</v>
+      </c>
+      <c r="E3" s="71" t="s">
+        <v>372</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>22</v>
@@ -11946,14 +12282,14 @@
       <c r="A4" s="21">
         <v>1.2</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="E4" s="69"/>
+        <v>325</v>
+      </c>
+      <c r="E4" s="72"/>
       <c r="F4" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>23</v>
@@ -11964,14 +12300,14 @@
       <c r="A5" s="21">
         <v>1.3</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
       <c r="D5" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="E5" s="69"/>
+        <v>327</v>
+      </c>
+      <c r="E5" s="72"/>
       <c r="F5" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>24</v>
@@ -11982,14 +12318,14 @@
       <c r="A6" s="21">
         <v>1.4</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
       <c r="D6" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="E6" s="70"/>
+        <v>329</v>
+      </c>
+      <c r="E6" s="73"/>
       <c r="F6" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>27</v>
@@ -12000,16 +12336,16 @@
       <c r="A7" s="21">
         <v>1.5</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
       <c r="D7" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>332</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>333</v>
-      </c>
-      <c r="E7" s="52" t="s">
-        <v>334</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="57"/>
@@ -12018,19 +12354,19 @@
       <c r="A8" s="26">
         <v>1.6</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
       <c r="D8" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H8" s="20"/>
     </row>
@@ -12038,16 +12374,16 @@
       <c r="A9" s="26">
         <v>1.7</v>
       </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="75"/>
       <c r="D9" s="19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -12058,16 +12394,16 @@
       <c r="A10" s="55">
         <v>1.8</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
       <c r="D10" s="54" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G10" s="59"/>
       <c r="H10" s="59"/>
@@ -12076,16 +12412,16 @@
       <c r="A11" s="60">
         <v>1.9</v>
       </c>
-      <c r="B11" s="73"/>
-      <c r="C11" s="73"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
       <c r="D11" s="54" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E11" s="54" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F11" s="54" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G11" s="59"/>
       <c r="H11" s="59"/>
@@ -12124,14 +12460,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="77"/>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
+      <c r="A1" s="80"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="42" t="s">
@@ -12163,23 +12499,23 @@
       <c r="A3" s="43">
         <v>10.1</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="88" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="88" t="s">
         <v>151</v>
       </c>
-      <c r="C3" s="85" t="s">
+      <c r="D3" s="88" t="s">
         <v>152</v>
       </c>
-      <c r="D3" s="85" t="s">
+      <c r="E3" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="F3" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>165</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -12187,17 +12523,17 @@
       <c r="A4" s="43">
         <v>10.199999999999999</v>
       </c>
-      <c r="B4" s="85"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
+      <c r="B4" s="88"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
       <c r="E4" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -12205,17 +12541,17 @@
       <c r="A5" s="43">
         <v>10.3</v>
       </c>
-      <c r="B5" s="85"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
       <c r="E5" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -12223,17 +12559,17 @@
       <c r="A6" s="43">
         <v>10.4</v>
       </c>
-      <c r="B6" s="85"/>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85"/>
+      <c r="B6" s="88"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
       <c r="E6" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H6" s="5"/>
     </row>
@@ -12241,17 +12577,17 @@
       <c r="A7" s="43">
         <v>10.5</v>
       </c>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
       <c r="E7" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H7" s="5"/>
     </row>
@@ -12259,17 +12595,17 @@
       <c r="A8" s="43">
         <v>10.6</v>
       </c>
-      <c r="B8" s="85"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
       <c r="E8" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H8" s="5"/>
     </row>
@@ -12277,17 +12613,17 @@
       <c r="A9" s="43">
         <v>10.7</v>
       </c>
-      <c r="B9" s="85"/>
-      <c r="C9" s="85"/>
-      <c r="D9" s="85"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
       <c r="E9" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H9" s="5"/>
     </row>
@@ -12295,17 +12631,17 @@
       <c r="A10" s="43">
         <v>10.8</v>
       </c>
-      <c r="B10" s="85"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="85"/>
+      <c r="B10" s="88"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
       <c r="E10" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H10" s="5"/>
     </row>
@@ -12313,30 +12649,30 @@
       <c r="A11" s="43">
         <v>10.9</v>
       </c>
-      <c r="B11" s="85"/>
-      <c r="C11" s="85"/>
-      <c r="D11" s="85"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
       <c r="E11" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A12" s="49" t="s">
-        <v>272</v>
-      </c>
-      <c r="B12" s="85"/>
-      <c r="C12" s="85"/>
-      <c r="D12" s="85"/>
+        <v>270</v>
+      </c>
+      <c r="B12" s="88"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
       <c r="E12" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>21</v>
@@ -12347,17 +12683,17 @@
       <c r="A13" s="45">
         <v>10.11</v>
       </c>
-      <c r="B13" s="85"/>
-      <c r="C13" s="85"/>
-      <c r="D13" s="85"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="88"/>
+      <c r="D13" s="88"/>
       <c r="E13" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H13" s="5"/>
     </row>
@@ -12365,17 +12701,17 @@
       <c r="A14" s="43">
         <v>10.119999999999999</v>
       </c>
-      <c r="B14" s="85"/>
-      <c r="C14" s="85"/>
-      <c r="D14" s="85"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
       <c r="E14" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="G14" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H14" s="5"/>
     </row>
@@ -12413,14 +12749,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="77"/>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
+      <c r="A1" s="80"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -12452,20 +12788,20 @@
       <c r="A3" s="21">
         <v>11.1</v>
       </c>
-      <c r="B3" s="85" t="s">
-        <v>259</v>
-      </c>
-      <c r="C3" s="85" t="s">
-        <v>260</v>
+      <c r="B3" s="88" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" s="88" t="s">
+        <v>258</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E3" s="68" t="s">
+        <v>262</v>
+      </c>
+      <c r="E3" s="71" t="s">
+        <v>266</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>21</v>
@@ -12476,14 +12812,14 @@
       <c r="A4" s="46">
         <v>11.2</v>
       </c>
-      <c r="B4" s="85"/>
-      <c r="C4" s="85"/>
+      <c r="B4" s="88"/>
+      <c r="C4" s="88"/>
       <c r="D4" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E4" s="73"/>
+      <c r="F4" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="E4" s="70"/>
-      <c r="F4" s="2" t="s">
-        <v>267</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>21</v>
@@ -12494,16 +12830,16 @@
       <c r="A5" s="46">
         <v>11.3</v>
       </c>
-      <c r="B5" s="85"/>
-      <c r="C5" s="85"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
       <c r="D5" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="E5" s="68" t="s">
+        <v>260</v>
+      </c>
+      <c r="E5" s="71" t="s">
+        <v>267</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>271</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>21</v>
@@ -12514,14 +12850,14 @@
       <c r="A6" s="47">
         <v>11.4</v>
       </c>
-      <c r="B6" s="85"/>
-      <c r="C6" s="85"/>
+      <c r="B6" s="88"/>
+      <c r="C6" s="88"/>
       <c r="D6" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="E6" s="70"/>
+        <v>261</v>
+      </c>
+      <c r="E6" s="73"/>
       <c r="F6" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>21</v>
@@ -12532,16 +12868,16 @@
       <c r="A7" s="48">
         <v>11.5</v>
       </c>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="88"/>
       <c r="D7" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E7" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>93</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>94</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>21</v>
@@ -12552,16 +12888,16 @@
       <c r="A8" s="48">
         <v>11.6</v>
       </c>
-      <c r="B8" s="85"/>
-      <c r="C8" s="85"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="88"/>
       <c r="D8" s="19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>21</v>
@@ -12604,14 +12940,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
+      <c r="A1" s="77"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -12641,13 +12977,13 @@
     </row>
     <row r="3" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="71" t="s">
-        <v>101</v>
+      <c r="C3" s="74" t="s">
+        <v>100</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -12656,7 +12992,7 @@
         <v>69</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>26</v>
@@ -12665,18 +13001,18 @@
     </row>
     <row r="4" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
+        <v>113</v>
+      </c>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>21</v>
@@ -12685,12 +13021,12 @@
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
+        <v>114</v>
+      </c>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
       <c r="D5" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>69</v>
@@ -12705,18 +13041,18 @@
     </row>
     <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A6" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
+        <v>119</v>
+      </c>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
       <c r="D6" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G6" s="20" t="s">
         <v>21</v>
@@ -12725,18 +13061,18 @@
     </row>
     <row r="7" spans="1:9" ht="57" x14ac:dyDescent="0.15">
       <c r="A7" s="26" t="s">
+        <v>289</v>
+      </c>
+      <c r="B7" s="76"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="E7" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="19" t="s">
-        <v>289</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>293</v>
-      </c>
       <c r="F7" s="19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>21</v>
@@ -12783,22 +13119,22 @@
     </row>
     <row r="10" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" s="71" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="71" t="s">
-        <v>101</v>
+      <c r="C10" s="74" t="s">
+        <v>100</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>21</v>
@@ -12808,10 +13144,10 @@
     </row>
     <row r="11" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B11" s="72"/>
-      <c r="C11" s="72"/>
+        <v>116</v>
+      </c>
+      <c r="B11" s="75"/>
+      <c r="C11" s="75"/>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
@@ -12819,7 +13155,7 @@
         <v>87</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>68</v>
@@ -12831,12 +13167,12 @@
     </row>
     <row r="12" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="72"/>
-      <c r="C12" s="72"/>
+        <v>117</v>
+      </c>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>86</v>
@@ -12852,38 +13188,38 @@
     </row>
     <row r="13" spans="1:9" s="22" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A13" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
+        <v>118</v>
+      </c>
+      <c r="B13" s="75"/>
+      <c r="C13" s="75"/>
       <c r="D13" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F13" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="20" t="s">
         <v>94</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>95</v>
       </c>
       <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:9" s="22" customFormat="1" ht="57" x14ac:dyDescent="0.15">
       <c r="A14" s="26" t="s">
-        <v>295</v>
-      </c>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
+        <v>293</v>
+      </c>
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
       <c r="D14" s="19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>21</v>
@@ -12892,7 +13228,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
-      <c r="B15" s="75"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -12903,7 +13239,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
-      <c r="B16" s="75"/>
+      <c r="B16" s="78"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -12914,7 +13250,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
-      <c r="B17" s="75"/>
+      <c r="B17" s="78"/>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -12925,7 +13261,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
-      <c r="B18" s="75"/>
+      <c r="B18" s="78"/>
       <c r="C18" s="4"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -12936,7 +13272,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
-      <c r="B19" s="75"/>
+      <c r="B19" s="78"/>
       <c r="C19" s="4"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -12994,9 +13330,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -13012,14 +13348,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A1" s="76"/>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
+      <c r="A1" s="79"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -13049,22 +13385,22 @@
     </row>
     <row r="3" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B3" s="71" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="71" t="s">
-        <v>103</v>
+      <c r="C3" s="74" t="s">
+        <v>102</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="E3" s="68" t="s">
-        <v>88</v>
+        <v>389</v>
+      </c>
+      <c r="E3" s="71" t="s">
+        <v>393</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>21</v>
@@ -13073,16 +13409,16 @@
     </row>
     <row r="4" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
+        <v>122</v>
+      </c>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E4" s="69"/>
+        <v>244</v>
+      </c>
+      <c r="E4" s="72"/>
       <c r="F4" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>21</v>
@@ -13091,14 +13427,14 @@
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
+        <v>123</v>
+      </c>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
       <c r="D5" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E5" s="69"/>
+        <v>245</v>
+      </c>
+      <c r="E5" s="72"/>
       <c r="F5" s="2" t="s">
         <v>77</v>
       </c>
@@ -13109,16 +13445,16 @@
     </row>
     <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
+        <v>124</v>
+      </c>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
       <c r="D6" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E6" s="69"/>
+        <v>107</v>
+      </c>
+      <c r="E6" s="72"/>
       <c r="F6" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>21</v>
@@ -13127,16 +13463,16 @@
     </row>
     <row r="7" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
+        <v>125</v>
+      </c>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
       <c r="D7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E7" s="69"/>
+        <v>246</v>
+      </c>
+      <c r="E7" s="72"/>
       <c r="F7" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>28</v>
@@ -13145,16 +13481,16 @@
     </row>
     <row r="8" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
+        <v>126</v>
+      </c>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
       <c r="D8" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="E8" s="69"/>
+        <v>120</v>
+      </c>
+      <c r="E8" s="72"/>
       <c r="F8" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>33</v>
@@ -13163,16 +13499,16 @@
     </row>
     <row r="9" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
+        <v>127</v>
+      </c>
+      <c r="B9" s="75"/>
+      <c r="C9" s="75"/>
       <c r="D9" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="E9" s="69"/>
+        <v>193</v>
+      </c>
+      <c r="E9" s="72"/>
       <c r="F9" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>21</v>
@@ -13181,36 +13517,36 @@
     </row>
     <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A10" s="34" t="s">
-        <v>198</v>
-      </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
+        <v>197</v>
+      </c>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
       <c r="D10" s="34" t="s">
-        <v>202</v>
-      </c>
-      <c r="E10" s="70"/>
+        <v>201</v>
+      </c>
+      <c r="E10" s="73"/>
       <c r="F10" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="G10" s="36" t="s">
         <v>196</v>
-      </c>
-      <c r="G10" s="36" t="s">
-        <v>197</v>
       </c>
       <c r="H10" s="36"/>
     </row>
     <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="B11" s="72"/>
-      <c r="C11" s="72"/>
+        <v>198</v>
+      </c>
+      <c r="B11" s="75"/>
+      <c r="C11" s="75"/>
       <c r="D11" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>21</v>
@@ -13219,18 +13555,18 @@
     </row>
     <row r="12" spans="1:8" s="22" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A12" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="B12" s="72"/>
-      <c r="C12" s="72"/>
+        <v>199</v>
+      </c>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>21</v>
@@ -13239,18 +13575,18 @@
     </row>
     <row r="13" spans="1:8" s="22" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A13" s="26" t="s">
-        <v>296</v>
-      </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
+        <v>294</v>
+      </c>
+      <c r="B13" s="75"/>
+      <c r="C13" s="75"/>
       <c r="D13" s="19" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>21</v>
@@ -13259,218 +13595,218 @@
     </row>
     <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A14" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="B14" s="75"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="E14" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="19" t="s">
-        <v>388</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>310</v>
-      </c>
       <c r="F14" s="19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>21</v>
       </c>
       <c r="H14" s="20"/>
     </row>
-    <row r="16" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A16" s="2" t="s">
+    <row r="15" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+      <c r="A15" s="67" t="s">
+        <v>386</v>
+      </c>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="68" t="s">
+        <v>392</v>
+      </c>
+      <c r="E15" s="68" t="s">
+        <v>394</v>
+      </c>
+      <c r="F15" s="68" t="s">
+        <v>395</v>
+      </c>
+      <c r="G15" s="69" t="s">
+        <v>387</v>
+      </c>
+      <c r="H15" s="69"/>
+    </row>
+    <row r="17" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B17" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C17" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F17" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G17" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H17" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="114" x14ac:dyDescent="0.15">
-      <c r="A17" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="B17" s="71" t="s">
+    <row r="18" spans="1:8" ht="114" x14ac:dyDescent="0.15">
+      <c r="A18" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="71" t="s">
-        <v>102</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="E17" s="68" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="14"/>
-    </row>
-    <row r="18" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
-      <c r="A18" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="B18" s="72"/>
-      <c r="C18" s="72"/>
+      <c r="C18" s="74" t="s">
+        <v>101</v>
+      </c>
       <c r="D18" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="E18" s="69"/>
+        <v>128</v>
+      </c>
+      <c r="E18" s="71" t="s">
+        <v>88</v>
+      </c>
       <c r="F18" s="14" t="s">
-        <v>76</v>
+        <v>227</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>21</v>
       </c>
       <c r="H18" s="14"/>
     </row>
-    <row r="19" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A19" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="B19" s="72"/>
-      <c r="C19" s="72"/>
+        <v>131</v>
+      </c>
+      <c r="B19" s="75"/>
+      <c r="C19" s="75"/>
       <c r="D19" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="69"/>
+        <v>247</v>
+      </c>
+      <c r="E19" s="72"/>
       <c r="F19" s="14" t="s">
-        <v>229</v>
+        <v>76</v>
       </c>
       <c r="G19" s="14" t="s">
         <v>21</v>
       </c>
       <c r="H19" s="14"/>
     </row>
-    <row r="20" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A20" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="B20" s="72"/>
-      <c r="C20" s="72"/>
+        <v>132</v>
+      </c>
+      <c r="B20" s="75"/>
+      <c r="C20" s="75"/>
       <c r="D20" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="E20" s="69"/>
+        <v>54</v>
+      </c>
+      <c r="E20" s="72"/>
       <c r="F20" s="14" t="s">
-        <v>75</v>
+        <v>228</v>
       </c>
       <c r="G20" s="14" t="s">
         <v>21</v>
       </c>
       <c r="H20" s="14"/>
     </row>
-    <row r="21" spans="1:8" ht="114" x14ac:dyDescent="0.15">
-      <c r="A21" s="11" t="s">
+    <row r="21" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+      <c r="A21" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="75"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="E21" s="72"/>
+      <c r="F21" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="14"/>
+    </row>
+    <row r="22" spans="1:8" ht="114" x14ac:dyDescent="0.15">
+      <c r="A22" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" s="75"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E22" s="72"/>
+      <c r="F22" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="16"/>
+    </row>
+    <row r="23" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+      <c r="A23" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="E23" s="73"/>
+      <c r="F23" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="G23" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H23" s="36"/>
+    </row>
+    <row r="24" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A24" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="B21" s="72"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="E21" s="69"/>
-      <c r="F21" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="G21" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" s="16"/>
-    </row>
-    <row r="22" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
-      <c r="A22" s="34" t="s">
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24" s="20"/>
+    </row>
+    <row r="25" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
+      <c r="A25" s="19" t="s">
         <v>203</v>
       </c>
-      <c r="B22" s="72"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="34" t="s">
-        <v>201</v>
-      </c>
-      <c r="E22" s="70"/>
-      <c r="F22" s="35" t="s">
-        <v>205</v>
-      </c>
-      <c r="G22" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="H22" s="36"/>
-    </row>
-    <row r="23" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A23" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="B23" s="72"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="H23" s="20"/>
-    </row>
-    <row r="24" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
-      <c r="A24" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="B24" s="72"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>314</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H24" s="20"/>
-    </row>
-    <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A25" s="26" t="s">
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="E25" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="19" t="s">
-        <v>316</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>315</v>
-      </c>
       <c r="F25" s="19" t="s">
-        <v>294</v>
+        <v>111</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>21</v>
@@ -13479,33 +13815,73 @@
     </row>
     <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
+        <v>310</v>
+      </c>
+      <c r="B26" s="75"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="E26" s="19" t="s">
         <v>313</v>
       </c>
-      <c r="B26" s="73"/>
-      <c r="C26" s="73"/>
-      <c r="D26" s="19" t="s">
-        <v>389</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>310</v>
-      </c>
       <c r="F26" s="19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="H26" s="20"/>
+    </row>
+    <row r="27" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A27" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="B27" s="75"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="19" t="s">
+        <v>390</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="20"/>
+    </row>
+    <row r="28" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+      <c r="A28" s="67" t="s">
+        <v>388</v>
+      </c>
+      <c r="B28" s="76"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="68" t="s">
+        <v>397</v>
+      </c>
+      <c r="E28" s="68" t="s">
+        <v>396</v>
+      </c>
+      <c r="F28" s="68" t="s">
+        <v>395</v>
+      </c>
+      <c r="G28" s="69" t="s">
+        <v>387</v>
+      </c>
+      <c r="H28" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E10"/>
-    <mergeCell ref="E17:E22"/>
-    <mergeCell ref="B3:B14"/>
-    <mergeCell ref="C3:C14"/>
-    <mergeCell ref="B17:B26"/>
-    <mergeCell ref="C17:C26"/>
+    <mergeCell ref="E18:E23"/>
+    <mergeCell ref="B3:B15"/>
+    <mergeCell ref="C3:C15"/>
+    <mergeCell ref="B18:B28"/>
+    <mergeCell ref="C18:C28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13534,14 +13910,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="77"/>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
+      <c r="A1" s="80"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -13571,22 +13947,22 @@
     </row>
     <row r="3" spans="1:8" s="22" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="B3" s="81" t="s">
-        <v>173</v>
-      </c>
-      <c r="C3" s="81" t="s">
-        <v>104</v>
+        <v>179</v>
+      </c>
+      <c r="B3" s="84" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="84" t="s">
+        <v>103</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="E3" s="78" t="s">
-        <v>110</v>
+        <v>249</v>
+      </c>
+      <c r="E3" s="81" t="s">
+        <v>109</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>31</v>
@@ -13595,14 +13971,14 @@
     </row>
     <row r="4" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
+        <v>180</v>
+      </c>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
       <c r="D4" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="E4" s="79"/>
+        <v>250</v>
+      </c>
+      <c r="E4" s="82"/>
       <c r="F4" s="6" t="s">
         <v>78</v>
       </c>
@@ -13613,16 +13989,16 @@
     </row>
     <row r="5" spans="1:8" s="22" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
+        <v>181</v>
+      </c>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
       <c r="D5" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="79"/>
+      <c r="E5" s="82"/>
       <c r="F5" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>30</v>
@@ -13631,14 +14007,14 @@
     </row>
     <row r="6" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
+        <v>182</v>
+      </c>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="E6" s="79"/>
+        <v>251</v>
+      </c>
+      <c r="E6" s="82"/>
       <c r="F6" s="6" t="s">
         <v>78</v>
       </c>
@@ -13649,16 +14025,16 @@
     </row>
     <row r="7" spans="1:8" s="22" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
+        <v>183</v>
+      </c>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
       <c r="D7" s="28" t="s">
-        <v>177</v>
-      </c>
-      <c r="E7" s="79"/>
+        <v>176</v>
+      </c>
+      <c r="E7" s="82"/>
       <c r="F7" s="28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G7" s="29" t="s">
         <v>57</v>
@@ -13667,36 +14043,36 @@
     </row>
     <row r="8" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A8" s="37" t="s">
-        <v>208</v>
-      </c>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
+        <v>207</v>
+      </c>
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
       <c r="D8" s="34" t="s">
-        <v>211</v>
-      </c>
-      <c r="E8" s="80"/>
+        <v>210</v>
+      </c>
+      <c r="E8" s="83"/>
       <c r="F8" s="35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G8" s="38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H8" s="39"/>
     </row>
     <row r="9" spans="1:8" s="22" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A9" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="B9" s="82"/>
-      <c r="C9" s="82"/>
+        <v>184</v>
+      </c>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
       <c r="D9" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -13705,18 +14081,18 @@
     </row>
     <row r="10" spans="1:8" s="32" customFormat="1" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A10" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="B10" s="82"/>
-      <c r="C10" s="82"/>
+        <v>206</v>
+      </c>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>21</v>
@@ -13725,18 +14101,18 @@
     </row>
     <row r="11" spans="1:8" s="32" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="26" t="s">
-        <v>297</v>
-      </c>
-      <c r="B11" s="82"/>
-      <c r="C11" s="82"/>
+        <v>295</v>
+      </c>
+      <c r="B11" s="85"/>
+      <c r="C11" s="85"/>
       <c r="D11" s="19" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>21</v>
@@ -13745,18 +14121,18 @@
     </row>
     <row r="12" spans="1:8" s="32" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="B12" s="86"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="19" t="s">
         <v>319</v>
       </c>
-      <c r="B12" s="83"/>
-      <c r="C12" s="83"/>
-      <c r="D12" s="19" t="s">
-        <v>321</v>
-      </c>
       <c r="E12" s="19" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>21</v>
@@ -13800,22 +14176,22 @@
     </row>
     <row r="15" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B15" s="71" t="s">
+        <v>185</v>
+      </c>
+      <c r="B15" s="74" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="84" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C15" s="81" t="s">
-        <v>104</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E15" s="68" t="s">
-        <v>98</v>
+      <c r="E15" s="71" t="s">
+        <v>97</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>21</v>
@@ -13824,16 +14200,16 @@
     </row>
     <row r="16" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B16" s="72"/>
-      <c r="C16" s="82"/>
+        <v>186</v>
+      </c>
+      <c r="B16" s="75"/>
+      <c r="C16" s="85"/>
       <c r="D16" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E16" s="69"/>
+        <v>175</v>
+      </c>
+      <c r="E16" s="72"/>
       <c r="F16" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>21</v>
@@ -13842,14 +14218,14 @@
     </row>
     <row r="17" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B17" s="72"/>
-      <c r="C17" s="82"/>
+        <v>187</v>
+      </c>
+      <c r="B17" s="75"/>
+      <c r="C17" s="85"/>
       <c r="D17" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="E17" s="69"/>
+        <v>252</v>
+      </c>
+      <c r="E17" s="72"/>
       <c r="F17" s="2" t="s">
         <v>80</v>
       </c>
@@ -13860,16 +14236,16 @@
     </row>
     <row r="18" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B18" s="72"/>
-      <c r="C18" s="82"/>
+        <v>188</v>
+      </c>
+      <c r="B18" s="75"/>
+      <c r="C18" s="85"/>
       <c r="D18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="69"/>
+      <c r="E18" s="72"/>
       <c r="F18" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>21</v>
@@ -13878,14 +14254,14 @@
     </row>
     <row r="19" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="B19" s="72"/>
-      <c r="C19" s="82"/>
+        <v>189</v>
+      </c>
+      <c r="B19" s="75"/>
+      <c r="C19" s="85"/>
       <c r="D19" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="E19" s="69"/>
+        <v>253</v>
+      </c>
+      <c r="E19" s="72"/>
       <c r="F19" s="2" t="s">
         <v>79</v>
       </c>
@@ -13896,14 +14272,14 @@
     </row>
     <row r="20" spans="1:8" s="22" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A20" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="B20" s="72"/>
-      <c r="C20" s="82"/>
+        <v>190</v>
+      </c>
+      <c r="B20" s="75"/>
+      <c r="C20" s="85"/>
       <c r="D20" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="E20" s="69"/>
+        <v>178</v>
+      </c>
+      <c r="E20" s="72"/>
       <c r="F20" s="11" t="s">
         <v>72</v>
       </c>
@@ -13914,14 +14290,14 @@
     </row>
     <row r="21" spans="1:8" s="22" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A21" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="B21" s="72"/>
-      <c r="C21" s="82"/>
+        <v>191</v>
+      </c>
+      <c r="B21" s="75"/>
+      <c r="C21" s="85"/>
       <c r="D21" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="E21" s="69"/>
+        <v>177</v>
+      </c>
+      <c r="E21" s="72"/>
       <c r="F21" s="11" t="s">
         <v>72</v>
       </c>
@@ -13932,56 +14308,56 @@
     </row>
     <row r="22" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A22" s="34" t="s">
-        <v>210</v>
-      </c>
-      <c r="B22" s="72"/>
-      <c r="C22" s="82"/>
+        <v>209</v>
+      </c>
+      <c r="B22" s="75"/>
+      <c r="C22" s="85"/>
       <c r="D22" s="34" t="s">
-        <v>212</v>
-      </c>
-      <c r="E22" s="70"/>
+        <v>211</v>
+      </c>
+      <c r="E22" s="73"/>
       <c r="F22" s="35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G22" s="40" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H22" s="41"/>
     </row>
     <row r="23" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A23" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="B23" s="72"/>
-      <c r="C23" s="82"/>
+        <v>192</v>
+      </c>
+      <c r="B23" s="75"/>
+      <c r="C23" s="85"/>
       <c r="D23" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F23" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G23" s="20" t="s">
         <v>94</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>95</v>
       </c>
       <c r="H23" s="20"/>
     </row>
     <row r="24" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A24" s="19" t="s">
-        <v>206</v>
-      </c>
-      <c r="B24" s="72"/>
-      <c r="C24" s="82"/>
+        <v>205</v>
+      </c>
+      <c r="B24" s="75"/>
+      <c r="C24" s="85"/>
       <c r="D24" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E24" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F24" s="19" t="s">
         <v>111</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>112</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>21</v>
@@ -13990,18 +14366,18 @@
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
-        <v>317</v>
-      </c>
-      <c r="B25" s="72"/>
-      <c r="C25" s="82"/>
+        <v>315</v>
+      </c>
+      <c r="B25" s="75"/>
+      <c r="C25" s="85"/>
       <c r="D25" s="19" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>21</v>
@@ -14010,18 +14386,18 @@
     </row>
     <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
-        <v>318</v>
-      </c>
-      <c r="B26" s="73"/>
-      <c r="C26" s="83"/>
+        <v>316</v>
+      </c>
+      <c r="B26" s="76"/>
+      <c r="C26" s="86"/>
       <c r="D26" s="19" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>21</v>
@@ -14066,14 +14442,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="84"/>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
+      <c r="A1" s="87"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
@@ -14105,20 +14481,20 @@
       <c r="A3" s="21">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="71" t="s">
-        <v>105</v>
+      <c r="C3" s="74" t="s">
+        <v>104</v>
       </c>
       <c r="D3" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="E3" s="71" t="s">
+        <v>342</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>343</v>
-      </c>
-      <c r="E3" s="68" t="s">
-        <v>344</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>345</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>34</v>
@@ -14129,14 +14505,14 @@
       <c r="A4" s="21">
         <v>5.2</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="E4" s="69"/>
+        <v>344</v>
+      </c>
+      <c r="E4" s="72"/>
       <c r="F4" s="14" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>27</v>
@@ -14147,14 +14523,14 @@
       <c r="A5" s="21">
         <v>5.3</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
       <c r="D5" s="14" t="s">
-        <v>348</v>
-      </c>
-      <c r="E5" s="69"/>
+        <v>346</v>
+      </c>
+      <c r="E5" s="72"/>
       <c r="F5" s="14" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>22</v>
@@ -14165,14 +14541,14 @@
       <c r="A6" s="21">
         <v>5.4</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
       <c r="D6" s="14" t="s">
-        <v>350</v>
-      </c>
-      <c r="E6" s="70"/>
+        <v>348</v>
+      </c>
+      <c r="E6" s="73"/>
       <c r="F6" s="14" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>27</v>
@@ -14183,19 +14559,19 @@
       <c r="A7" s="21">
         <v>5.5</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
       <c r="D7" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>351</v>
+      </c>
+      <c r="F7" s="14" t="s">
         <v>352</v>
       </c>
-      <c r="E7" s="53" t="s">
-        <v>353</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>354</v>
-      </c>
       <c r="G7" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H7" s="62"/>
     </row>
@@ -14203,19 +14579,19 @@
       <c r="A8" s="26">
         <v>5.6</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
       <c r="D8" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H8" s="20"/>
     </row>
@@ -14223,16 +14599,16 @@
       <c r="A9" s="26">
         <v>5.7</v>
       </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="75"/>
       <c r="D9" s="19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -14243,16 +14619,16 @@
       <c r="A10" s="60">
         <v>5.8</v>
       </c>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
       <c r="D10" s="54" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -14295,14 +14671,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="77"/>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
+      <c r="A1" s="80"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -14334,20 +14710,20 @@
       <c r="A3" s="21">
         <v>6.1</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="85" t="s">
-        <v>106</v>
+      <c r="C3" s="88" t="s">
+        <v>105</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="E3" s="68" t="s">
-        <v>261</v>
+        <v>357</v>
+      </c>
+      <c r="E3" s="71" t="s">
+        <v>259</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>21</v>
@@ -14358,14 +14734,14 @@
       <c r="A4" s="21">
         <v>6.2</v>
       </c>
-      <c r="B4" s="85"/>
-      <c r="C4" s="85"/>
+      <c r="B4" s="88"/>
+      <c r="C4" s="88"/>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="69"/>
+      <c r="E4" s="72"/>
       <c r="F4" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>27</v>
@@ -14376,12 +14752,12 @@
       <c r="A5" s="21">
         <v>6.3</v>
       </c>
-      <c r="B5" s="85"/>
-      <c r="C5" s="85"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
       <c r="D5" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E5" s="70"/>
+        <v>239</v>
+      </c>
+      <c r="E5" s="73"/>
       <c r="F5" s="2" t="s">
         <v>81</v>
       </c>
@@ -14394,19 +14770,19 @@
       <c r="A6" s="23">
         <v>6.4</v>
       </c>
-      <c r="B6" s="85"/>
-      <c r="C6" s="85"/>
+      <c r="B6" s="88"/>
+      <c r="C6" s="88"/>
       <c r="D6" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H6" s="6"/>
     </row>
@@ -14414,16 +14790,16 @@
       <c r="A7" s="23">
         <v>6.5</v>
       </c>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="88"/>
       <c r="D7" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E7" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="E7" s="50" t="s">
-        <v>288</v>
-      </c>
       <c r="F7" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -14432,19 +14808,19 @@
       <c r="A8" s="26">
         <v>6.6</v>
       </c>
-      <c r="B8" s="85"/>
-      <c r="C8" s="85"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="88"/>
       <c r="D8" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E8" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="G8" s="20" t="s">
         <v>94</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>95</v>
       </c>
       <c r="H8" s="20"/>
     </row>
@@ -14452,16 +14828,16 @@
       <c r="A9" s="26">
         <v>6.7</v>
       </c>
-      <c r="B9" s="85"/>
-      <c r="C9" s="85"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
       <c r="D9" s="19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -14472,16 +14848,16 @@
       <c r="A10" s="64">
         <v>6.8</v>
       </c>
-      <c r="B10" s="85"/>
-      <c r="C10" s="85"/>
+      <c r="B10" s="88"/>
+      <c r="C10" s="88"/>
       <c r="D10" s="54" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -14525,14 +14901,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="77"/>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
+      <c r="A1" s="80"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -14562,22 +14938,22 @@
     </row>
     <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B3" s="71" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="71" t="s">
-        <v>373</v>
+      <c r="C3" s="74" t="s">
+        <v>371</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="68" t="s">
-        <v>90</v>
+      <c r="E3" s="71" t="s">
+        <v>89</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -14586,14 +14962,14 @@
     </row>
     <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
+        <v>141</v>
+      </c>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="E4" s="69"/>
+        <v>240</v>
+      </c>
+      <c r="E4" s="72"/>
       <c r="F4" s="2" t="s">
         <v>58</v>
       </c>
@@ -14604,14 +14980,14 @@
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
+        <v>142</v>
+      </c>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
       <c r="D5" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E5" s="69"/>
+        <v>239</v>
+      </c>
+      <c r="E5" s="72"/>
       <c r="F5" s="2" t="s">
         <v>82</v>
       </c>
@@ -14622,14 +14998,14 @@
     </row>
     <row r="6" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
+        <v>143</v>
+      </c>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
       <c r="D6" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="70"/>
+      <c r="E6" s="73"/>
       <c r="F6" s="6" t="s">
         <v>59</v>
       </c>
@@ -14640,36 +15016,36 @@
     </row>
     <row r="7" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
+        <v>299</v>
+      </c>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
       <c r="D7" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E7" s="51"/>
       <c r="F7" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A8" s="19" t="s">
-        <v>299</v>
-      </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
+        <v>297</v>
+      </c>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
       <c r="D8" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>21</v>
@@ -14678,18 +15054,18 @@
     </row>
     <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A9" s="26" t="s">
-        <v>300</v>
-      </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
+        <v>298</v>
+      </c>
+      <c r="B9" s="75"/>
+      <c r="C9" s="75"/>
       <c r="D9" s="19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -14698,21 +15074,21 @@
     </row>
     <row r="10" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A10" s="55" t="s">
+        <v>363</v>
+      </c>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="54" t="s">
         <v>365</v>
       </c>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="54" t="s">
-        <v>367</v>
-      </c>
       <c r="E10" s="54" t="s">
+        <v>366</v>
+      </c>
+      <c r="F10" s="54" t="s">
+        <v>383</v>
+      </c>
+      <c r="G10" s="59" t="s">
         <v>368</v>
-      </c>
-      <c r="F10" s="54" t="s">
-        <v>385</v>
-      </c>
-      <c r="G10" s="59" t="s">
-        <v>370</v>
       </c>
       <c r="H10" s="59"/>
     </row>
@@ -14744,22 +15120,22 @@
     </row>
     <row r="13" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B13" s="71" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="71" t="s">
+      <c r="C13" s="74" t="s">
         <v>71</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="68" t="s">
-        <v>91</v>
+      <c r="E13" s="71" t="s">
+        <v>90</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>21</v>
@@ -14768,16 +15144,16 @@
     </row>
     <row r="14" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
+        <v>145</v>
+      </c>
+      <c r="B14" s="75"/>
+      <c r="C14" s="75"/>
       <c r="D14" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="E14" s="69"/>
+        <v>241</v>
+      </c>
+      <c r="E14" s="72"/>
       <c r="F14" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>21</v>
@@ -14786,14 +15162,14 @@
     </row>
     <row r="15" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B15" s="72"/>
-      <c r="C15" s="72"/>
+        <v>146</v>
+      </c>
+      <c r="B15" s="75"/>
+      <c r="C15" s="75"/>
       <c r="D15" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="E15" s="69"/>
+        <v>242</v>
+      </c>
+      <c r="E15" s="72"/>
       <c r="F15" s="2" t="s">
         <v>63</v>
       </c>
@@ -14804,14 +15180,14 @@
     </row>
     <row r="16" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="B16" s="72"/>
-      <c r="C16" s="72"/>
+        <v>147</v>
+      </c>
+      <c r="B16" s="75"/>
+      <c r="C16" s="75"/>
       <c r="D16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="70"/>
+      <c r="E16" s="73"/>
       <c r="F16" s="6" t="s">
         <v>66</v>
       </c>
@@ -14822,56 +15198,56 @@
     </row>
     <row r="17" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="B17" s="72"/>
-      <c r="C17" s="72"/>
+        <v>301</v>
+      </c>
+      <c r="B17" s="75"/>
+      <c r="C17" s="75"/>
       <c r="D17" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E17" s="51"/>
       <c r="F17" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A18" s="19" t="s">
-        <v>298</v>
-      </c>
-      <c r="B18" s="72"/>
-      <c r="C18" s="72"/>
+        <v>296</v>
+      </c>
+      <c r="B18" s="75"/>
+      <c r="C18" s="75"/>
       <c r="D18" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F18" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" s="20" t="s">
         <v>94</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>95</v>
       </c>
       <c r="H18" s="20"/>
     </row>
     <row r="19" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A19" s="26" t="s">
-        <v>307</v>
-      </c>
-      <c r="B19" s="72"/>
-      <c r="C19" s="72"/>
+        <v>305</v>
+      </c>
+      <c r="B19" s="75"/>
+      <c r="C19" s="75"/>
       <c r="D19" s="19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G19" s="20" t="s">
         <v>21</v>
@@ -14880,21 +15256,21 @@
     </row>
     <row r="20" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A20" s="55" t="s">
-        <v>366</v>
-      </c>
-      <c r="B20" s="73"/>
-      <c r="C20" s="73"/>
+        <v>364</v>
+      </c>
+      <c r="B20" s="76"/>
+      <c r="C20" s="76"/>
       <c r="D20" s="54" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E20" s="54" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F20" s="54" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G20" s="59" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="H20" s="59"/>
     </row>
@@ -14934,14 +15310,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="77"/>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
+      <c r="A1" s="80"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -14973,38 +15349,38 @@
       <c r="A3" s="21">
         <v>8.1</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="71" t="s">
-        <v>107</v>
+      <c r="C3" s="74" t="s">
+        <v>106</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E3" s="68" t="s">
-        <v>377</v>
+        <v>148</v>
+      </c>
+      <c r="E3" s="71" t="s">
+        <v>375</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A4" s="21">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="69"/>
+      <c r="E4" s="72"/>
       <c r="F4" s="2" t="s">
         <v>48</v>
       </c>
@@ -15017,12 +15393,12 @@
       <c r="A5" s="21">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
       <c r="D5" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="E5" s="70"/>
+        <v>243</v>
+      </c>
+      <c r="E5" s="73"/>
       <c r="F5" s="2" t="s">
         <v>83</v>
       </c>
@@ -15035,19 +15411,19 @@
       <c r="A6" s="21">
         <v>8.4</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
       <c r="D6" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="E6" s="68" t="s">
-        <v>378</v>
+        <v>278</v>
+      </c>
+      <c r="E6" s="71" t="s">
+        <v>376</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>285</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -15055,17 +15431,17 @@
       <c r="A7" s="21">
         <v>8.5</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
       <c r="D7" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="E7" s="69"/>
+        <v>279</v>
+      </c>
+      <c r="E7" s="72"/>
       <c r="F7" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -15073,17 +15449,17 @@
       <c r="A8" s="21">
         <v>8.6</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
       <c r="D8" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E8" s="70"/>
+        <v>277</v>
+      </c>
+      <c r="E8" s="73"/>
       <c r="F8" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -15091,19 +15467,19 @@
       <c r="A9" s="26">
         <v>8.6999999999999993</v>
       </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="75"/>
       <c r="D9" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F9" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="20" t="s">
         <v>94</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>95</v>
       </c>
       <c r="H9" s="20"/>
     </row>
@@ -15111,16 +15487,16 @@
       <c r="A10" s="26">
         <v>8.8000000000000007</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
       <c r="D10" s="19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>21</v>
@@ -15131,16 +15507,16 @@
       <c r="A11" s="65">
         <v>8.9</v>
       </c>
-      <c r="B11" s="72"/>
-      <c r="C11" s="72"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="75"/>
       <c r="D11" s="54" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F11" s="55" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G11" s="60" t="s">
         <v>21</v>
@@ -15149,18 +15525,18 @@
     </row>
     <row r="12" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A12" s="66" t="s">
+        <v>360</v>
+      </c>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="54" t="s">
         <v>362</v>
       </c>
-      <c r="B12" s="73"/>
-      <c r="C12" s="73"/>
-      <c r="D12" s="54" t="s">
-        <v>364</v>
-      </c>
       <c r="E12" s="55" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F12" s="55" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G12" s="60" t="s">
         <v>21</v>
@@ -15202,14 +15578,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="77"/>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
+      <c r="A1" s="80"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -15241,10 +15617,10 @@
       <c r="A3" s="21">
         <v>9.1</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="74" t="s">
         <v>36</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -15253,7 +15629,7 @@
       <c r="E3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="71" t="s">
+      <c r="F3" s="74" t="s">
         <v>41</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -15265,15 +15641,15 @@
       <c r="A4" s="21">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="72"/>
+      <c r="F4" s="75"/>
       <c r="G4" s="2" t="s">
         <v>43</v>
       </c>
@@ -15283,15 +15659,15 @@
       <c r="A5" s="21">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
       <c r="D5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="72"/>
+      <c r="F5" s="75"/>
       <c r="G5" s="2" t="s">
         <v>43</v>
       </c>
@@ -15301,15 +15677,15 @@
       <c r="A6" s="21">
         <v>9.4</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
       <c r="D6" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="72"/>
+      <c r="F6" s="75"/>
       <c r="G6" s="5" t="s">
         <v>43</v>
       </c>
@@ -15319,15 +15695,15 @@
       <c r="A7" s="21">
         <v>9.5</v>
       </c>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="76"/>
       <c r="D7" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="73"/>
+      <c r="F7" s="76"/>
       <c r="G7" s="5" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Update the test case file of FileOperation after fixed #34
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="404">
   <si>
     <t>删除文件夹</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -7911,10 +7911,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>提示输入需要被目标文件路径移动时，输入存在路径不带'\'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>提示输入需要被移动文件夹或者文件路径时，输入存在路径不带'\'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -11372,6 +11368,298 @@
       <t>的文件夹路径
 2.输入被复制文件路径和目标文件夹路径</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.2.13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.1.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被移动的文件路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的本地磁盘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的文件夹路径
+2.输入被移动文件路径和目标文件夹路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被移动文件的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要移动到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I:\Program Files</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被移动文件夹的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要移动到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I:\Program Files</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被移动的文件夹路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的本地磁盘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的文件夹路径
+2.输入被移动文件夹路径和目标文件夹路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示输入需要被目标文件夹路径移动时，输入存在路径不带'\'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -11382,7 +11670,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -11509,6 +11797,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -11626,7 +11922,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -11893,6 +12189,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -12265,13 +12567,13 @@
         <v>99</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E3" s="71" t="s">
+        <v>371</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>323</v>
-      </c>
-      <c r="E3" s="71" t="s">
-        <v>372</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>324</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>22</v>
@@ -12285,11 +12587,11 @@
       <c r="B4" s="75"/>
       <c r="C4" s="75"/>
       <c r="D4" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E4" s="72"/>
       <c r="F4" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>23</v>
@@ -12303,11 +12605,11 @@
       <c r="B5" s="75"/>
       <c r="C5" s="75"/>
       <c r="D5" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E5" s="72"/>
       <c r="F5" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>24</v>
@@ -12321,11 +12623,11 @@
       <c r="B6" s="75"/>
       <c r="C6" s="75"/>
       <c r="D6" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E6" s="73"/>
       <c r="F6" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>27</v>
@@ -12339,13 +12641,13 @@
       <c r="B7" s="75"/>
       <c r="C7" s="75"/>
       <c r="D7" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E7" s="52" t="s">
         <v>331</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="F7" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>333</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="57"/>
@@ -12360,10 +12662,10 @@
         <v>136</v>
       </c>
       <c r="E8" s="19" t="s">
+        <v>333</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>334</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>335</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>94</v>
@@ -12380,10 +12682,10 @@
         <v>287</v>
       </c>
       <c r="E9" s="19" t="s">
+        <v>335</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>336</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>337</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -12397,13 +12699,13 @@
       <c r="B10" s="75"/>
       <c r="C10" s="75"/>
       <c r="D10" s="54" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G10" s="59"/>
       <c r="H10" s="59"/>
@@ -12415,13 +12717,13 @@
       <c r="B11" s="76"/>
       <c r="C11" s="76"/>
       <c r="D11" s="54" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E11" s="54" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F11" s="54" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G11" s="59"/>
       <c r="H11" s="59"/>
@@ -13332,8 +13634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView topLeftCell="E25" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -13394,10 +13696,10 @@
         <v>102</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E3" s="71" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>222</v>
@@ -13600,7 +13902,7 @@
       <c r="B14" s="75"/>
       <c r="C14" s="75"/>
       <c r="D14" s="19" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E14" s="19" t="s">
         <v>308</v>
@@ -13615,21 +13917,21 @@
     </row>
     <row r="15" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A15" s="67" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B15" s="76"/>
       <c r="C15" s="76"/>
       <c r="D15" s="68" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E15" s="68" t="s">
+        <v>393</v>
+      </c>
+      <c r="F15" s="68" t="s">
         <v>394</v>
       </c>
-      <c r="F15" s="68" t="s">
-        <v>395</v>
-      </c>
       <c r="G15" s="69" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H15" s="69"/>
     </row>
@@ -13840,7 +14142,7 @@
       <c r="B27" s="75"/>
       <c r="C27" s="75"/>
       <c r="D27" s="19" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E27" s="19" t="s">
         <v>308</v>
@@ -13855,21 +14157,21 @@
     </row>
     <row r="28" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A28" s="67" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B28" s="76"/>
       <c r="C28" s="76"/>
       <c r="D28" s="68" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E28" s="68" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F28" s="68" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G28" s="69" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H28" s="69"/>
     </row>
@@ -13891,9 +14193,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -14123,8 +14425,8 @@
       <c r="A12" s="26" t="s">
         <v>317</v>
       </c>
-      <c r="B12" s="86"/>
-      <c r="C12" s="86"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="85"/>
       <c r="D12" s="19" t="s">
         <v>319</v>
       </c>
@@ -14139,245 +14441,245 @@
       </c>
       <c r="H12" s="20"/>
     </row>
-    <row r="13" spans="1:8" s="32" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="9"/>
-      <c r="H13" s="33"/>
+    <row r="13" spans="1:8" s="32" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
+      <c r="A13" s="89" t="s">
+        <v>398</v>
+      </c>
+      <c r="B13" s="86"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="68" t="s">
+        <v>399</v>
+      </c>
+      <c r="E13" s="68" t="s">
+        <v>400</v>
+      </c>
+      <c r="F13" s="68" t="s">
+        <v>394</v>
+      </c>
+      <c r="G13" s="69" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="90"/>
     </row>
     <row r="14" spans="1:8" s="32" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="9"/>
+      <c r="H14" s="33"/>
+    </row>
+    <row r="15" spans="1:8" s="32" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B15" s="74" t="s">
-        <v>173</v>
-      </c>
-      <c r="C15" s="84" t="s">
-        <v>103</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E15" s="71" t="s">
-        <v>97</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B16" s="75"/>
-      <c r="C16" s="85"/>
+        <v>185</v>
+      </c>
+      <c r="B16" s="74" t="s">
+        <v>173</v>
+      </c>
+      <c r="C16" s="84" t="s">
+        <v>103</v>
+      </c>
       <c r="D16" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E16" s="72"/>
+        <v>174</v>
+      </c>
+      <c r="E16" s="71" t="s">
+        <v>97</v>
+      </c>
       <c r="F16" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="57" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B17" s="75"/>
       <c r="C17" s="85"/>
       <c r="D17" s="2" t="s">
-        <v>252</v>
+        <v>175</v>
       </c>
       <c r="E17" s="72"/>
       <c r="F17" s="2" t="s">
-        <v>80</v>
+        <v>234</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B18" s="75"/>
       <c r="C18" s="85"/>
       <c r="D18" s="2" t="s">
-        <v>56</v>
+        <v>252</v>
       </c>
       <c r="E18" s="72"/>
       <c r="F18" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="G18" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
-      <c r="A19" s="6" t="s">
-        <v>189</v>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
+      <c r="A19" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="B19" s="75"/>
       <c r="C19" s="85"/>
       <c r="D19" s="2" t="s">
-        <v>253</v>
+        <v>56</v>
       </c>
       <c r="E19" s="72"/>
       <c r="F19" s="2" t="s">
-        <v>79</v>
+        <v>235</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>21</v>
       </c>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" s="22" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
-      <c r="A20" s="11" t="s">
-        <v>190</v>
+    <row r="20" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+      <c r="A20" s="6" t="s">
+        <v>189</v>
       </c>
       <c r="B20" s="75"/>
       <c r="C20" s="85"/>
-      <c r="D20" s="11" t="s">
-        <v>178</v>
+      <c r="D20" s="2" t="s">
+        <v>253</v>
       </c>
       <c r="E20" s="72"/>
-      <c r="F20" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="H20" s="16"/>
+      <c r="F20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" s="22" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A21" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B21" s="75"/>
       <c r="C21" s="85"/>
       <c r="D21" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E21" s="72"/>
       <c r="F21" s="11" t="s">
         <v>72</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="H21" s="16"/>
     </row>
-    <row r="22" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
-      <c r="A22" s="34" t="s">
-        <v>209</v>
+    <row r="22" spans="1:8" s="22" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
+      <c r="A22" s="11" t="s">
+        <v>191</v>
       </c>
       <c r="B22" s="75"/>
       <c r="C22" s="85"/>
-      <c r="D22" s="34" t="s">
-        <v>211</v>
-      </c>
-      <c r="E22" s="73"/>
-      <c r="F22" s="35" t="s">
-        <v>208</v>
-      </c>
-      <c r="G22" s="40" t="s">
-        <v>196</v>
-      </c>
-      <c r="H22" s="41"/>
-    </row>
-    <row r="23" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A23" s="19" t="s">
-        <v>192</v>
+      <c r="D22" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="E22" s="72"/>
+      <c r="F22" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="16"/>
+    </row>
+    <row r="23" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
+      <c r="A23" s="34" t="s">
+        <v>209</v>
       </c>
       <c r="B23" s="75"/>
       <c r="C23" s="85"/>
-      <c r="D23" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="H23" s="20"/>
-    </row>
-    <row r="24" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
+      <c r="D23" s="34" t="s">
+        <v>211</v>
+      </c>
+      <c r="E23" s="73"/>
+      <c r="F23" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="G23" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="H23" s="41"/>
+    </row>
+    <row r="24" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A24" s="19" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="B24" s="75"/>
       <c r="C24" s="85"/>
       <c r="D24" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="H24" s="20"/>
     </row>
-    <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A25" s="26" t="s">
-        <v>315</v>
+    <row r="25" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
+      <c r="A25" s="19" t="s">
+        <v>205</v>
       </c>
       <c r="B25" s="75"/>
       <c r="C25" s="85"/>
       <c r="D25" s="19" t="s">
-        <v>321</v>
+        <v>137</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>291</v>
+        <v>110</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>292</v>
+        <v>111</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>21</v>
@@ -14386,15 +14688,15 @@
     </row>
     <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
-        <v>316</v>
-      </c>
-      <c r="B26" s="76"/>
-      <c r="C26" s="86"/>
+        <v>315</v>
+      </c>
+      <c r="B26" s="75"/>
+      <c r="C26" s="85"/>
       <c r="D26" s="19" t="s">
         <v>320</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="F26" s="19" t="s">
         <v>292</v>
@@ -14403,16 +14705,56 @@
         <v>21</v>
       </c>
       <c r="H26" s="20"/>
+    </row>
+    <row r="27" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A27" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="B27" s="75"/>
+      <c r="C27" s="85"/>
+      <c r="D27" s="19" t="s">
+        <v>403</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="20"/>
+    </row>
+    <row r="28" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+      <c r="A28" s="67" t="s">
+        <v>397</v>
+      </c>
+      <c r="B28" s="76"/>
+      <c r="C28" s="86"/>
+      <c r="D28" s="68" t="s">
+        <v>402</v>
+      </c>
+      <c r="E28" s="68" t="s">
+        <v>401</v>
+      </c>
+      <c r="F28" s="68" t="s">
+        <v>394</v>
+      </c>
+      <c r="G28" s="69" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="E15:E22"/>
+    <mergeCell ref="E16:E23"/>
     <mergeCell ref="E3:E8"/>
-    <mergeCell ref="B3:B12"/>
-    <mergeCell ref="C3:C12"/>
-    <mergeCell ref="B15:B26"/>
-    <mergeCell ref="C15:C26"/>
+    <mergeCell ref="B3:B13"/>
+    <mergeCell ref="C3:C13"/>
+    <mergeCell ref="B16:B28"/>
+    <mergeCell ref="C16:C28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14488,13 +14830,13 @@
         <v>104</v>
       </c>
       <c r="D3" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="E3" s="71" t="s">
         <v>341</v>
       </c>
-      <c r="E3" s="71" t="s">
+      <c r="F3" s="14" t="s">
         <v>342</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>343</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>34</v>
@@ -14508,11 +14850,11 @@
       <c r="B4" s="75"/>
       <c r="C4" s="75"/>
       <c r="D4" s="14" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E4" s="72"/>
       <c r="F4" s="14" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>27</v>
@@ -14526,11 +14868,11 @@
       <c r="B5" s="75"/>
       <c r="C5" s="75"/>
       <c r="D5" s="14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E5" s="72"/>
       <c r="F5" s="14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>22</v>
@@ -14544,11 +14886,11 @@
       <c r="B6" s="75"/>
       <c r="C6" s="75"/>
       <c r="D6" s="14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E6" s="73"/>
       <c r="F6" s="14" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>27</v>
@@ -14562,13 +14904,13 @@
       <c r="B7" s="75"/>
       <c r="C7" s="75"/>
       <c r="D7" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="E7" s="53" t="s">
         <v>350</v>
       </c>
-      <c r="E7" s="53" t="s">
+      <c r="F7" s="14" t="s">
         <v>351</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>352</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>276</v>
@@ -14585,10 +14927,10 @@
         <v>136</v>
       </c>
       <c r="E8" s="19" t="s">
+        <v>352</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>353</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>354</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>94</v>
@@ -14605,10 +14947,10 @@
         <v>287</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -14622,13 +14964,13 @@
       <c r="B10" s="76"/>
       <c r="C10" s="76"/>
       <c r="D10" s="54" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -14717,7 +15059,7 @@
         <v>105</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E3" s="71" t="s">
         <v>259</v>
@@ -14851,13 +15193,13 @@
       <c r="B10" s="88"/>
       <c r="C10" s="88"/>
       <c r="D10" s="54" t="s">
+        <v>357</v>
+      </c>
+      <c r="E10" s="54" t="s">
         <v>358</v>
       </c>
-      <c r="E10" s="54" t="s">
-        <v>359</v>
-      </c>
       <c r="F10" s="54" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -14944,7 +15286,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="74" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>61</v>
@@ -15065,7 +15407,7 @@
         <v>291</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>21</v>
@@ -15074,21 +15416,21 @@
     </row>
     <row r="10" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A10" s="55" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B10" s="76"/>
       <c r="C10" s="76"/>
       <c r="D10" s="54" t="s">
+        <v>364</v>
+      </c>
+      <c r="E10" s="54" t="s">
         <v>365</v>
       </c>
-      <c r="E10" s="54" t="s">
-        <v>366</v>
-      </c>
       <c r="F10" s="54" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G10" s="59" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H10" s="59"/>
     </row>
@@ -15256,21 +15598,21 @@
     </row>
     <row r="20" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A20" s="55" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B20" s="76"/>
       <c r="C20" s="76"/>
       <c r="D20" s="54" t="s">
+        <v>368</v>
+      </c>
+      <c r="E20" s="54" t="s">
         <v>369</v>
       </c>
-      <c r="E20" s="54" t="s">
-        <v>370</v>
-      </c>
       <c r="F20" s="54" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G20" s="59" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H20" s="59"/>
     </row>
@@ -15359,7 +15701,7 @@
         <v>148</v>
       </c>
       <c r="E3" s="71" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>238</v>
@@ -15417,7 +15759,7 @@
         <v>278</v>
       </c>
       <c r="E6" s="71" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>281</v>
@@ -15510,13 +15852,13 @@
       <c r="B11" s="75"/>
       <c r="C11" s="75"/>
       <c r="D11" s="54" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F11" s="55" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G11" s="60" t="s">
         <v>21</v>
@@ -15525,18 +15867,18 @@
     </row>
     <row r="12" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A12" s="66" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B12" s="76"/>
       <c r="C12" s="76"/>
       <c r="D12" s="54" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E12" s="55" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F12" s="55" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G12" s="60" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Update the test cases file of FilOperation as hint message updated on Function 8
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Update codes\20170913\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Update codes\20170914\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="48" windowWidth="5352" windowHeight="7608" tabRatio="945" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="48" windowWidth="5352" windowHeight="7608" tabRatio="945" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -9613,6 +9613,375 @@
   </si>
   <si>
     <r>
+      <t>提示请不要输入空查找内容的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cannot input empty search content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示请不要输入空的替换内容信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cannot input empty replace content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示不能输入空的搜索内容的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cannot input empty search content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示不能输入空的搜索内容的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cannot input empty file or folder name, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示替换内容不能为空的信息
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cannot input empty replace content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示需要被替换字符不能为空的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cannot input empty search content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示需要新替换字符名称不能为空的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cannot input empty replace content, please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.1.13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.2.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被复制的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>非空文件夹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>目标路径
+2.输入被复制文件夹路径和目标文件夹路径</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示输入需要被目标文件路径时，输入存在路径不带'\'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示输入需要被目标文件夹路径时，输入存在路径不带'\'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被复制的文件夹路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的本地磁盘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的文件夹路径
+2.输入被复制文件夹路径和目标文件夹路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t>1.在"</t>
     </r>
     <r>
@@ -9625,18 +9994,18 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please input the file or folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件夹的路径，如:</t>
     </r>
     <r>
       <rPr>
@@ -9672,7 +10041,1292 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>What content do you want find?</t>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Program Files</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件夹的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I:\Program Files</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示目标本地磁盘不存在，无法复制的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I: is not exists on this PC, cannot copy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I:\Program Files</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被复制的文件路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的本地磁盘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的文件夹路径
+2.输入被复制文件路径和目标文件夹路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.2.13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.1.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被移动的文件路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的本地磁盘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的文件夹路径
+2.输入被移动文件路径和目标文件夹路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被移动文件的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要移动到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I:\Program Files</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被移动文件夹的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要移动到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I:\Program Files</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被移动的文件夹路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的本地磁盘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的文件夹路径
+2.输入被移动文件夹路径和目标文件夹路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示输入需要被目标文件夹路径移动时，输入存在路径不带'\'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what to find:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入txt文件内存在的内容，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Alonso
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入想要替换成的新内容，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alo</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:" 输入路径，如:D:\Test
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what to find</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:",输入空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:" 输入路径，如:D:\Test
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what to find:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入txt文件内存在的内容，如Alonso
+3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入想要替换成的新内容，输入空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What want to find on txt file?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入txt文件内存在的内容，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Alonso
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:D:\Test
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What want to find on txt file?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">",输入txt文件内存在的内容为空字符
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What want to find on this folder?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入文件名或扩展名，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.txt，456.txt,20170614</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What want to find on this folder?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入文件夹名，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>McLaren</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:D:\Test
+2.在"P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lease input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" 输入空字符串
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the file or folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What name want to find?</t>
     </r>
     <r>
       <rPr>
@@ -9719,7 +11373,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>What content do you want replace?</t>
+      <t>Please input new name want to replace:</t>
     </r>
     <r>
       <rPr>
@@ -9807,7 +11461,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>What content do you want find?</t>
+      <t>What name want to find?</t>
     </r>
     <r>
       <rPr>
@@ -9854,7 +11508,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>What content do you want replace?</t>
+      <t>Please input new name to replace:</t>
     </r>
     <r>
       <rPr>
@@ -9919,18 +11573,42 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>What content do you want find?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">",输入空字符
+      <t>What name want to find?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如Alonso
+3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input new name to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">",输入新的想要被替换的文件夹名为空字符
 </t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -9973,1696 +11651,18 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>What content do you want find?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如Alonso
-3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What content do you want replace?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">",输入新的想要被替换的文件夹名为空字符
-</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示请不要输入空查找内容的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cannot input empty search content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示请不要输入空的替换内容信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cannot input empty replace content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示不能输入空的搜索内容的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cannot input empty search content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示不能输入空的搜索内容的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cannot input empty file or folder name, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示替换内容不能为空的信息
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cannot input empty replace content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示需要被替换字符不能为空的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cannot input empty search content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示需要新替换字符名称不能为空的信息 
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cannot input empty replace content, please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.1.13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pass</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.2.11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>需要被复制的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>非空文件夹</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的路径和</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>目标路径
-2.输入被复制文件夹路径和目标文件夹路径</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>提示输入需要被目标文件路径时，输入存在路径不带'\'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>提示输入需要被目标文件夹路径时，输入存在路径不带'\'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>需要被复制的文件夹路径和</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>不存在的本地磁盘</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的文件夹路径
-2.输入被复制文件夹路径和目标文件夹路径</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入被复制文件夹的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input target folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入需要复制到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\Program Files</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入被复制文件夹的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input target folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入需要复制到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>I:\Program Files</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>提示目标本地磁盘不存在，无法复制的信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>I: is not exists on this PC, cannot copy</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入被复制文件的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input target folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入需要复制到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>I:\Program Files</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>需要被复制的文件路径和</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>不存在的本地磁盘</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的文件夹路径
-2.输入被复制文件路径和目标文件夹路径</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.2.13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.1.11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>需要被移动的文件路径和</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>不存在的本地磁盘</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的文件夹路径
-2.输入被移动文件路径和目标文件夹路径</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入被移动文件的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input target folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入需要移动到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>I:\Program Files</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入被移动文件夹的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input target folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入需要移动到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>I:\Program Files</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>需要被移动的文件夹路径和</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>不存在的本地磁盘</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的文件夹路径
-2.输入被移动文件夹路径和目标文件夹路径</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>提示输入需要被目标文件夹路径移动时，输入存在路径不带'\'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what to find:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入txt文件内存在的内容，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Alonso
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入想要替换成的新内容，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alo</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:" 输入路径，如:D:\Test
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what to find</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:",输入空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:" 输入路径，如:D:\Test
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what to find:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入txt文件内存在的内容，如Alonso
-3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入想要替换成的新内容，输入空字符</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What want to find on txt file?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入txt文件内存在的内容，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Alonso
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:D:\Test
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What want to find on txt file?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">",输入txt文件内存在的内容为空字符
-</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What want to find on this folder?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入文件名或扩展名，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.txt，456.txt,20170614</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What want to find on this folder?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入文件夹名，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>McLaren</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:D:\Test
-2.在"P</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>lease input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" 输入空字符串
+      <t>Please input new name to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">",输入空字符
 </t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -12575,7 +12575,7 @@
         <v>320</v>
       </c>
       <c r="E3" s="73" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>321</v>
@@ -12707,10 +12707,10 @@
         <v>335</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="G10" s="59"/>
       <c r="H10" s="59"/>
@@ -12725,10 +12725,10 @@
         <v>319</v>
       </c>
       <c r="E11" s="54" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="F11" s="54" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="G11" s="59"/>
       <c r="H11" s="59"/>
@@ -13701,10 +13701,10 @@
         <v>102</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="E3" s="73" t="s">
         <v>380</v>
-      </c>
-      <c r="E3" s="73" t="s">
-        <v>384</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>222</v>
@@ -13907,7 +13907,7 @@
       <c r="B14" s="77"/>
       <c r="C14" s="77"/>
       <c r="D14" s="19" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E14" s="19" t="s">
         <v>306</v>
@@ -13922,21 +13922,21 @@
     </row>
     <row r="15" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A15" s="67" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B15" s="78"/>
       <c r="C15" s="78"/>
       <c r="D15" s="68" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="E15" s="68" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="F15" s="68" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G15" s="69" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="H15" s="69"/>
     </row>
@@ -14147,7 +14147,7 @@
       <c r="B27" s="77"/>
       <c r="C27" s="77"/>
       <c r="D27" s="19" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="E27" s="19" t="s">
         <v>306</v>
@@ -14162,21 +14162,21 @@
     </row>
     <row r="28" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
       <c r="A28" s="67" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B28" s="78"/>
       <c r="C28" s="78"/>
       <c r="D28" s="68" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="E28" s="68" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="F28" s="68" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G28" s="69" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="H28" s="69"/>
     </row>
@@ -14448,18 +14448,18 @@
     </row>
     <row r="13" spans="1:8" s="32" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A13" s="70" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B13" s="88"/>
       <c r="C13" s="88"/>
       <c r="D13" s="68" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="E13" s="68" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="F13" s="68" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G13" s="69" t="s">
         <v>21</v>
@@ -14718,7 +14718,7 @@
       <c r="B27" s="77"/>
       <c r="C27" s="87"/>
       <c r="D27" s="19" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="E27" s="19" t="s">
         <v>306</v>
@@ -14733,18 +14733,18 @@
     </row>
     <row r="28" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A28" s="67" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B28" s="78"/>
       <c r="C28" s="88"/>
       <c r="D28" s="68" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="E28" s="68" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="F28" s="68" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G28" s="69" t="s">
         <v>21</v>
@@ -14838,7 +14838,7 @@
         <v>338</v>
       </c>
       <c r="E3" s="73" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>339</v>
@@ -14972,10 +14972,10 @@
         <v>336</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -15002,7 +15002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -15067,7 +15067,7 @@
         <v>352</v>
       </c>
       <c r="E3" s="73" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>214</v>
@@ -15123,7 +15123,7 @@
         <v>213</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>215</v>
@@ -15201,10 +15201,10 @@
         <v>353</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>21</v>
@@ -15432,7 +15432,7 @@
         <v>360</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>362</v>
@@ -15614,7 +15614,7 @@
         <v>364</v>
       </c>
       <c r="F20" s="54" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="G20" s="59" t="s">
         <v>362</v>
@@ -15641,7 +15641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -15706,7 +15706,7 @@
         <v>148</v>
       </c>
       <c r="E3" s="73" t="s">
-        <v>366</v>
+        <v>400</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>238</v>
@@ -15764,7 +15764,7 @@
         <v>277</v>
       </c>
       <c r="E6" s="73" t="s">
-        <v>367</v>
+        <v>401</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>280</v>
@@ -15860,10 +15860,10 @@
         <v>355</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>368</v>
+        <v>403</v>
       </c>
       <c r="F11" s="55" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="G11" s="60" t="s">
         <v>21</v>
@@ -15880,10 +15880,10 @@
         <v>356</v>
       </c>
       <c r="E12" s="55" t="s">
-        <v>369</v>
+        <v>402</v>
       </c>
       <c r="F12" s="55" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="G12" s="60" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Update test case file for FileOperation as function9 has been renamed
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -15,7 +15,7 @@
     <sheet name="6.在Txt文件内搜索" sheetId="8" r:id="rId6"/>
     <sheet name="7.在文件夹中查找文件" sheetId="9" r:id="rId7"/>
     <sheet name="8.重命名文件夹" sheetId="10" r:id="rId8"/>
-    <sheet name="9.根据文件已有字段被替换为新名称" sheetId="13" r:id="rId9"/>
+    <sheet name="9.批量重命名文件" sheetId="13" r:id="rId9"/>
     <sheet name="10.计算文件或文件夹大小" sheetId="17" r:id="rId10"/>
     <sheet name="11.特殊字符测试" sheetId="15" r:id="rId11"/>
     <sheet name="12.主界面基本功能检测" sheetId="16" r:id="rId12"/>
@@ -222,10 +222,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>根据文件已有字段被替换为新名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>1. 输入</t>
     </r>
@@ -2556,47 +2552,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>Rename file or folder</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>进入"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>根据文件已有字段被替换为新名称</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"模块，并输出</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Rename file with specificname</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -11680,10 +11635,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>9. Rename file with specificname</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>9.10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -12133,6 +12084,55 @@
       <t xml:space="preserve">）
 3.本地计算机上这些文件夹确实被删除
 </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9. Batch Rename file or folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>批量重命名文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>进入"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>批量重命名文件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"模块，并输出</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Batch Rename file or folder</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -13001,7 +13001,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -13010,10 +13010,10 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>6</v>
@@ -13030,22 +13030,22 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" s="77" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E3" s="74" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -13056,14 +13056,14 @@
       <c r="B4" s="78"/>
       <c r="C4" s="78"/>
       <c r="D4" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E4" s="75"/>
       <c r="F4" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -13074,14 +13074,14 @@
       <c r="B5" s="78"/>
       <c r="C5" s="78"/>
       <c r="D5" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -13092,14 +13092,14 @@
       <c r="B6" s="78"/>
       <c r="C6" s="78"/>
       <c r="D6" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E6" s="76"/>
       <c r="F6" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="54"/>
     </row>
@@ -13110,13 +13110,13 @@
       <c r="B7" s="78"/>
       <c r="C7" s="78"/>
       <c r="D7" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E7" s="49" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="54"/>
@@ -13128,16 +13128,16 @@
       <c r="B8" s="78"/>
       <c r="C8" s="78"/>
       <c r="D8" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H8" s="20"/>
     </row>
@@ -13148,16 +13148,16 @@
       <c r="B9" s="78"/>
       <c r="C9" s="78"/>
       <c r="D9" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" s="20"/>
     </row>
@@ -13168,13 +13168,13 @@
       <c r="B10" s="78"/>
       <c r="C10" s="78"/>
       <c r="D10" s="51" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E10" s="51" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F10" s="51" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G10" s="56"/>
       <c r="H10" s="56"/>
@@ -13186,13 +13186,13 @@
       <c r="B11" s="79"/>
       <c r="C11" s="79"/>
       <c r="D11" s="51" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E11" s="51" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F11" s="51" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G11" s="56"/>
       <c r="H11" s="56"/>
@@ -13242,7 +13242,7 @@
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -13251,10 +13251,10 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>6</v>
@@ -13271,22 +13271,22 @@
         <v>10.1</v>
       </c>
       <c r="B3" s="83" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C3" s="83" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E3" s="74" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -13297,14 +13297,14 @@
       <c r="B4" s="83"/>
       <c r="C4" s="83"/>
       <c r="D4" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E4" s="76"/>
       <c r="F4" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -13315,16 +13315,16 @@
       <c r="B5" s="83"/>
       <c r="C5" s="83"/>
       <c r="D5" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -13335,14 +13335,14 @@
       <c r="B6" s="83"/>
       <c r="C6" s="83"/>
       <c r="D6" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E6" s="76"/>
       <c r="F6" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6" s="6"/>
     </row>
@@ -13353,16 +13353,16 @@
       <c r="B7" s="83"/>
       <c r="C7" s="83"/>
       <c r="D7" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E7" s="19" t="s">
+        <v>326</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>328</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>330</v>
-      </c>
       <c r="G7" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="20"/>
     </row>
@@ -13373,16 +13373,16 @@
       <c r="B8" s="83"/>
       <c r="C8" s="83"/>
       <c r="D8" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>327</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>329</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>203</v>
-      </c>
       <c r="G8" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8" s="20"/>
     </row>
@@ -13432,7 +13432,7 @@
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -13441,10 +13441,10 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>6</v>
@@ -13461,22 +13461,22 @@
         <v>11.1</v>
       </c>
       <c r="B3" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="77" t="s">
+      <c r="D3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F3" s="77" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -13487,14 +13487,14 @@
       <c r="B4" s="78"/>
       <c r="C4" s="78"/>
       <c r="D4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F4" s="78"/>
       <c r="G4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -13505,14 +13505,14 @@
       <c r="B5" s="78"/>
       <c r="C5" s="78"/>
       <c r="D5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="78"/>
       <c r="G5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -13523,14 +13523,14 @@
       <c r="B6" s="78"/>
       <c r="C6" s="78"/>
       <c r="D6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F6" s="78"/>
       <c r="G6" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H6" s="5"/>
     </row>
@@ -13541,14 +13541,14 @@
       <c r="B7" s="79"/>
       <c r="C7" s="79"/>
       <c r="D7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" s="79"/>
       <c r="G7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H7" s="5"/>
     </row>
@@ -13597,7 +13597,7 @@
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -13606,10 +13606,10 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>6</v>
@@ -13626,22 +13626,22 @@
         <v>12.1</v>
       </c>
       <c r="B3" s="83" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="83" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="83" t="s">
+      <c r="D3" s="83" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="E3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="F3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -13653,13 +13653,13 @@
       <c r="C4" s="83"/>
       <c r="D4" s="83"/>
       <c r="E4" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -13671,13 +13671,13 @@
       <c r="C5" s="83"/>
       <c r="D5" s="83"/>
       <c r="E5" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -13689,13 +13689,13 @@
       <c r="C6" s="83"/>
       <c r="D6" s="83"/>
       <c r="E6" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -13707,13 +13707,13 @@
       <c r="C7" s="83"/>
       <c r="D7" s="83"/>
       <c r="E7" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H7" s="5"/>
     </row>
@@ -13725,13 +13725,13 @@
       <c r="C8" s="83"/>
       <c r="D8" s="83"/>
       <c r="E8" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H8" s="5"/>
     </row>
@@ -13743,13 +13743,13 @@
       <c r="C9" s="83"/>
       <c r="D9" s="83"/>
       <c r="E9" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H9" s="5"/>
     </row>
@@ -13761,13 +13761,13 @@
       <c r="C10" s="83"/>
       <c r="D10" s="83"/>
       <c r="E10" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H10" s="5"/>
     </row>
@@ -13779,31 +13779,31 @@
       <c r="C11" s="83"/>
       <c r="D11" s="83"/>
       <c r="E11" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>118</v>
+        <v>418</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="46" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B12" s="83"/>
       <c r="C12" s="83"/>
       <c r="D12" s="83"/>
       <c r="E12" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H12" s="5"/>
     </row>
@@ -13815,13 +13815,13 @@
       <c r="C13" s="83"/>
       <c r="D13" s="83"/>
       <c r="E13" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H13" s="5"/>
     </row>
@@ -13833,13 +13833,13 @@
       <c r="C14" s="83"/>
       <c r="D14" s="83"/>
       <c r="E14" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H14" s="5"/>
     </row>
@@ -13851,13 +13851,13 @@
       <c r="C15" s="83"/>
       <c r="D15" s="83"/>
       <c r="E15" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="G15" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H15" s="5"/>
     </row>
@@ -13907,7 +13907,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -13916,10 +13916,10 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>6</v>
@@ -13933,105 +13933,105 @@
     </row>
     <row r="3" spans="1:9" ht="171" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="77" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="77" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="171" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" s="78"/>
       <c r="C4" s="78"/>
       <c r="D4" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="78"/>
       <c r="C5" s="78"/>
       <c r="D5" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A6" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" s="78"/>
       <c r="C6" s="78"/>
       <c r="D6" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E6" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="F6" s="19" t="s">
-        <v>276</v>
-      </c>
       <c r="G6" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6" s="20"/>
     </row>
     <row r="7" spans="1:9" ht="57" x14ac:dyDescent="0.15">
       <c r="A7" s="25" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B7" s="79"/>
       <c r="C7" s="79"/>
       <c r="D7" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="E7" s="19" t="s">
-        <v>275</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>203</v>
-      </c>
       <c r="G7" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="20"/>
     </row>
@@ -14048,7 +14048,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
@@ -14057,10 +14057,10 @@
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>6</v>
@@ -14075,32 +14075,32 @@
     </row>
     <row r="10" spans="1:9" ht="171" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" s="77" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="77" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" ht="171" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" s="78"/>
       <c r="C11" s="78"/>
@@ -14108,75 +14108,75 @@
         <v>9</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H11" s="13"/>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B12" s="78"/>
       <c r="C12" s="78"/>
       <c r="D12" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" s="22" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A13" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B13" s="78"/>
       <c r="C13" s="78"/>
       <c r="D13" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E13" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F13" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="F13" s="19" t="s">
-        <v>281</v>
-      </c>
       <c r="G13" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:9" s="22" customFormat="1" ht="57" x14ac:dyDescent="0.15">
       <c r="A14" s="25" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B14" s="79"/>
       <c r="C14" s="79"/>
       <c r="D14" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="E14" s="19" t="s">
-        <v>280</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>203</v>
-      </c>
       <c r="G14" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H14" s="20"/>
     </row>
@@ -14286,7 +14286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -14315,7 +14315,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -14324,10 +14324,10 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>6</v>
@@ -14344,22 +14344,22 @@
         <v>3.1</v>
       </c>
       <c r="B3" s="83" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C3" s="83" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E3" s="74" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -14374,10 +14374,10 @@
       </c>
       <c r="E4" s="75"/>
       <c r="F4" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4" s="13"/>
     </row>
@@ -14388,14 +14388,14 @@
       <c r="B5" s="83"/>
       <c r="C5" s="83"/>
       <c r="D5" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E5" s="76"/>
       <c r="F5" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -14406,16 +14406,16 @@
       <c r="B6" s="83"/>
       <c r="C6" s="83"/>
       <c r="D6" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E6" s="67" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6" s="6"/>
     </row>
@@ -14426,13 +14426,13 @@
       <c r="B7" s="83"/>
       <c r="C7" s="83"/>
       <c r="D7" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E7" s="67" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -14444,16 +14444,16 @@
       <c r="B8" s="83"/>
       <c r="C8" s="83"/>
       <c r="D8" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8" s="20"/>
     </row>
@@ -14464,16 +14464,16 @@
       <c r="B9" s="83"/>
       <c r="C9" s="83"/>
       <c r="D9" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="E9" s="19" t="s">
-        <v>268</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>203</v>
-      </c>
       <c r="G9" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" s="20"/>
     </row>
@@ -14484,16 +14484,16 @@
       <c r="B10" s="83"/>
       <c r="C10" s="83"/>
       <c r="D10" s="51" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E10" s="51" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F10" s="51" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G10" s="56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" s="56"/>
     </row>
@@ -14584,7 +14584,7 @@
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -14593,10 +14593,10 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>6</v>
@@ -14610,257 +14610,257 @@
     </row>
     <row r="3" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B3" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="77" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E3" s="74" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B4" s="78"/>
       <c r="C4" s="78"/>
       <c r="D4" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E4" s="75"/>
       <c r="F4" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B5" s="78"/>
       <c r="C5" s="78"/>
       <c r="D5" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B6" s="78"/>
       <c r="C6" s="78"/>
       <c r="D6" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E6" s="75"/>
       <c r="F6" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="B7" s="78"/>
       <c r="C7" s="78"/>
       <c r="D7" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E7" s="75"/>
       <c r="F7" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B8" s="78"/>
       <c r="C8" s="78"/>
       <c r="D8" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E8" s="75"/>
       <c r="F8" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B9" s="78"/>
       <c r="C9" s="78"/>
       <c r="D9" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E9" s="75"/>
       <c r="F9" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B10" s="78"/>
       <c r="C10" s="78"/>
       <c r="D10" s="33" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E10" s="76"/>
       <c r="F10" s="34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H10" s="35"/>
     </row>
     <row r="11" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B11" s="78"/>
       <c r="C11" s="78"/>
       <c r="D11" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:8" s="22" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A12" s="19" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B12" s="78"/>
       <c r="C12" s="78"/>
       <c r="D12" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H12" s="24"/>
     </row>
     <row r="13" spans="1:8" s="22" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A13" s="25" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B13" s="78"/>
       <c r="C13" s="78"/>
       <c r="D13" s="19" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A14" s="25" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B14" s="78"/>
       <c r="C14" s="78"/>
       <c r="D14" s="19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H14" s="20"/>
     </row>
     <row r="15" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A15" s="62" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B15" s="79"/>
       <c r="C15" s="79"/>
       <c r="D15" s="63" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E15" s="63" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F15" s="63" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G15" s="64" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H15" s="64"/>
     </row>
     <row r="17" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>3</v>
@@ -14869,10 +14869,10 @@
         <v>10</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F17" s="14" t="s">
         <v>6</v>
@@ -14886,215 +14886,215 @@
     </row>
     <row r="18" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A18" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B18" s="77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" s="77" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E18" s="74" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H18" s="14"/>
     </row>
     <row r="19" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A19" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B19" s="78"/>
       <c r="C19" s="78"/>
       <c r="D19" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E19" s="75"/>
       <c r="F19" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A20" s="14" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B20" s="78"/>
       <c r="C20" s="78"/>
       <c r="D20" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E20" s="75"/>
       <c r="F20" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A21" s="14" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B21" s="78"/>
       <c r="C21" s="78"/>
       <c r="D21" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E21" s="75"/>
       <c r="F21" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A22" s="14" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B22" s="78"/>
       <c r="C22" s="78"/>
       <c r="D22" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E22" s="75"/>
       <c r="F22" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H22" s="16"/>
     </row>
     <row r="23" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A23" s="14" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B23" s="78"/>
       <c r="C23" s="78"/>
       <c r="D23" s="33" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E23" s="76"/>
       <c r="F23" s="34" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G23" s="35" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H23" s="35"/>
     </row>
     <row r="24" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A24" s="14" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B24" s="78"/>
       <c r="C24" s="78"/>
       <c r="D24" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="G24" s="20" t="s">
         <v>81</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>283</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>288</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>82</v>
       </c>
       <c r="H24" s="20"/>
     </row>
     <row r="25" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A25" s="14" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B25" s="78"/>
       <c r="C25" s="78"/>
       <c r="D25" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H25" s="20"/>
     </row>
     <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A26" s="14" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B26" s="78"/>
       <c r="C26" s="78"/>
       <c r="D26" s="19" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H26" s="20"/>
     </row>
     <row r="27" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A27" s="25" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B27" s="78"/>
       <c r="C27" s="78"/>
       <c r="D27" s="19" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H27" s="20"/>
     </row>
     <row r="28" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A28" s="62" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B28" s="79"/>
       <c r="C28" s="79"/>
       <c r="D28" s="63" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E28" s="63" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F28" s="63" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G28" s="64" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H28" s="64"/>
     </row>
@@ -15146,7 +15146,7 @@
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -15155,10 +15155,10 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>6</v>
@@ -15172,215 +15172,215 @@
     </row>
     <row r="3" spans="1:8" s="22" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B3" s="89" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C3" s="89" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E3" s="86" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B4" s="90"/>
       <c r="C4" s="90"/>
       <c r="D4" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E4" s="87"/>
       <c r="F4" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" s="22" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B5" s="90"/>
       <c r="C5" s="90"/>
       <c r="D5" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" s="87"/>
       <c r="F5" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B6" s="90"/>
       <c r="C6" s="90"/>
       <c r="D6" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E6" s="87"/>
       <c r="F6" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:8" s="22" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B7" s="90"/>
       <c r="C7" s="90"/>
       <c r="D7" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E7" s="87"/>
       <c r="F7" s="27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H7" s="29"/>
     </row>
     <row r="8" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B8" s="90"/>
       <c r="C8" s="90"/>
       <c r="D8" s="33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E8" s="88"/>
       <c r="F8" s="34" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G8" s="36" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H8" s="37"/>
     </row>
     <row r="9" spans="1:8" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B9" s="90"/>
       <c r="C9" s="90"/>
       <c r="D9" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" s="31" customFormat="1" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B10" s="90"/>
       <c r="C10" s="90"/>
       <c r="D10" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" s="24"/>
     </row>
     <row r="11" spans="1:8" s="31" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B11" s="90"/>
       <c r="C11" s="90"/>
       <c r="D11" s="19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:8" s="31" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="25" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B12" s="90"/>
       <c r="C12" s="90"/>
       <c r="D12" s="19" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H12" s="20"/>
     </row>
     <row r="13" spans="1:8" s="31" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A13" s="65" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B13" s="91"/>
       <c r="C13" s="91"/>
       <c r="D13" s="63" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E13" s="63" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F13" s="63" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G13" s="64" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H13" s="66"/>
     </row>
@@ -15395,7 +15395,7 @@
     </row>
     <row r="15" spans="1:8" s="31" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>3</v>
@@ -15404,10 +15404,10 @@
         <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>6</v>
@@ -15421,251 +15421,251 @@
     </row>
     <row r="16" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B16" s="77" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C16" s="89" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E16" s="74" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B17" s="78"/>
       <c r="C17" s="90"/>
       <c r="D17" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E17" s="75"/>
       <c r="F17" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B18" s="78"/>
       <c r="C18" s="90"/>
       <c r="D18" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E18" s="75"/>
       <c r="F18" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B19" s="78"/>
       <c r="C19" s="90"/>
       <c r="D19" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E19" s="75"/>
       <c r="F19" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B20" s="78"/>
       <c r="C20" s="90"/>
       <c r="D20" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E20" s="75"/>
       <c r="F20" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" s="22" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B21" s="78"/>
       <c r="C21" s="90"/>
       <c r="D21" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E21" s="75"/>
       <c r="F21" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H21" s="16"/>
     </row>
     <row r="22" spans="1:8" s="22" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B22" s="78"/>
       <c r="C22" s="90"/>
       <c r="D22" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E22" s="75"/>
       <c r="F22" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H22" s="16"/>
     </row>
     <row r="23" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B23" s="78"/>
       <c r="C23" s="90"/>
       <c r="D23" s="33" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E23" s="76"/>
       <c r="F23" s="34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G23" s="38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H23" s="39"/>
     </row>
     <row r="24" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B24" s="78"/>
       <c r="C24" s="90"/>
       <c r="D24" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H24" s="20"/>
     </row>
     <row r="25" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A25" s="19" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B25" s="78"/>
       <c r="C25" s="90"/>
       <c r="D25" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H25" s="20"/>
     </row>
     <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A26" s="25" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B26" s="78"/>
       <c r="C26" s="90"/>
       <c r="D26" s="19" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H26" s="20"/>
     </row>
     <row r="27" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A27" s="25" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B27" s="78"/>
       <c r="C27" s="90"/>
       <c r="D27" s="19" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H27" s="20"/>
     </row>
     <row r="28" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A28" s="62" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B28" s="79"/>
       <c r="C28" s="91"/>
       <c r="D28" s="63" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E28" s="63" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F28" s="63" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G28" s="64" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H28" s="66"/>
     </row>
@@ -15718,7 +15718,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>3</v>
@@ -15727,10 +15727,10 @@
         <v>10</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>46</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>6</v>
@@ -15750,19 +15750,19 @@
         <v>12</v>
       </c>
       <c r="C3" s="77" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E3" s="74" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="59"/>
     </row>
@@ -15773,14 +15773,14 @@
       <c r="B4" s="78"/>
       <c r="C4" s="78"/>
       <c r="D4" s="14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E4" s="75"/>
       <c r="F4" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="59"/>
     </row>
@@ -15791,14 +15791,14 @@
       <c r="B5" s="78"/>
       <c r="C5" s="78"/>
       <c r="D5" s="14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="14" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" s="14"/>
     </row>
@@ -15809,14 +15809,14 @@
       <c r="B6" s="78"/>
       <c r="C6" s="78"/>
       <c r="D6" s="14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E6" s="76"/>
       <c r="F6" s="14" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="59"/>
     </row>
@@ -15827,16 +15827,16 @@
       <c r="B7" s="78"/>
       <c r="C7" s="78"/>
       <c r="D7" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H7" s="59"/>
     </row>
@@ -15847,16 +15847,16 @@
       <c r="B8" s="78"/>
       <c r="C8" s="78"/>
       <c r="D8" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H8" s="20"/>
     </row>
@@ -15867,16 +15867,16 @@
       <c r="B9" s="78"/>
       <c r="C9" s="78"/>
       <c r="D9" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" s="20"/>
     </row>
@@ -15887,16 +15887,16 @@
       <c r="B10" s="79"/>
       <c r="C10" s="79"/>
       <c r="D10" s="51" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E10" s="51" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F10" s="51" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G10" s="56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" s="56"/>
     </row>
@@ -15947,7 +15947,7 @@
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -15956,10 +15956,10 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>6</v>
@@ -15979,19 +15979,19 @@
         <v>13</v>
       </c>
       <c r="C3" s="83" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E3" s="74" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -16006,10 +16006,10 @@
       </c>
       <c r="E4" s="75"/>
       <c r="F4" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="13"/>
     </row>
@@ -16020,14 +16020,14 @@
       <c r="B5" s="83"/>
       <c r="C5" s="83"/>
       <c r="D5" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E5" s="76"/>
       <c r="F5" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -16038,16 +16038,16 @@
       <c r="B6" s="83"/>
       <c r="C6" s="83"/>
       <c r="D6" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>307</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E6" s="26" t="s">
-        <v>309</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>143</v>
-      </c>
       <c r="G6" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H6" s="6"/>
     </row>
@@ -16058,13 +16058,13 @@
       <c r="B7" s="83"/>
       <c r="C7" s="83"/>
       <c r="D7" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -16076,16 +16076,16 @@
       <c r="B8" s="83"/>
       <c r="C8" s="83"/>
       <c r="D8" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H8" s="20"/>
     </row>
@@ -16096,16 +16096,16 @@
       <c r="B9" s="83"/>
       <c r="C9" s="83"/>
       <c r="D9" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="E9" s="19" t="s">
-        <v>311</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>203</v>
-      </c>
       <c r="G9" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" s="20"/>
     </row>
@@ -16116,16 +16116,16 @@
       <c r="B10" s="83"/>
       <c r="C10" s="83"/>
       <c r="D10" s="51" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E10" s="51" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F10" s="51" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G10" s="56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" s="56"/>
     </row>
@@ -16177,7 +16177,7 @@
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -16186,10 +16186,10 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>6</v>
@@ -16203,163 +16203,163 @@
     </row>
     <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B3" s="77" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="77" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="74" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B4" s="78"/>
       <c r="C4" s="78"/>
       <c r="D4" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E4" s="75"/>
       <c r="F4" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B5" s="78"/>
       <c r="C5" s="78"/>
       <c r="D5" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B6" s="78"/>
       <c r="C6" s="78"/>
       <c r="D6" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6" s="76"/>
       <c r="F6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B7" s="78"/>
       <c r="C7" s="78"/>
       <c r="D7" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B8" s="78"/>
       <c r="C8" s="78"/>
       <c r="D8" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B9" s="78"/>
       <c r="C9" s="78"/>
       <c r="D9" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B10" s="79"/>
       <c r="C10" s="79"/>
       <c r="D10" s="51" t="s">
+        <v>242</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>312</v>
+      </c>
+      <c r="F10" s="51" t="s">
+        <v>250</v>
+      </c>
+      <c r="G10" s="56" t="s">
         <v>244</v>
-      </c>
-      <c r="E10" s="51" t="s">
-        <v>314</v>
-      </c>
-      <c r="F10" s="51" t="s">
-        <v>252</v>
-      </c>
-      <c r="G10" s="56" t="s">
-        <v>246</v>
       </c>
       <c r="H10" s="56"/>
     </row>
     <row r="12" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>3</v>
@@ -16371,7 +16371,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>6</v>
@@ -16385,157 +16385,157 @@
     </row>
     <row r="13" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B13" s="77" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="77" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E13" s="74" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B14" s="78"/>
       <c r="C14" s="78"/>
       <c r="D14" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E14" s="75"/>
       <c r="F14" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B15" s="78"/>
       <c r="C15" s="78"/>
       <c r="D15" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E15" s="75"/>
       <c r="F15" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B16" s="78"/>
       <c r="C16" s="78"/>
       <c r="D16" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E16" s="76"/>
       <c r="F16" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B17" s="78"/>
       <c r="C17" s="78"/>
       <c r="D17" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E17" s="48"/>
       <c r="F17" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B18" s="78"/>
       <c r="C18" s="78"/>
       <c r="D18" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H18" s="20"/>
     </row>
     <row r="19" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B19" s="78"/>
       <c r="C19" s="78"/>
       <c r="D19" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="F19" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="E19" s="19" t="s">
-        <v>318</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>203</v>
-      </c>
       <c r="G19" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H19" s="20"/>
     </row>
     <row r="20" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B20" s="79"/>
       <c r="C20" s="79"/>
       <c r="D20" s="51" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E20" s="51" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F20" s="51" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G20" s="56" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H20" s="56"/>
     </row>
@@ -16586,7 +16586,7 @@
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -16595,10 +16595,10 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>6</v>
@@ -16615,25 +16615,25 @@
         <v>9.1</v>
       </c>
       <c r="B3" s="77" t="s">
-        <v>17</v>
+        <v>417</v>
       </c>
       <c r="C3" s="77" t="s">
-        <v>344</v>
+        <v>416</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="74" t="s">
+        <v>318</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="E3" s="74" t="s">
-        <v>320</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
@@ -16643,14 +16643,14 @@
       <c r="B4" s="78"/>
       <c r="C4" s="78"/>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="75"/>
       <c r="F4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="13"/>
     </row>
@@ -16661,14 +16661,14 @@
       <c r="B5" s="78"/>
       <c r="C5" s="78"/>
       <c r="D5" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E5" s="76"/>
       <c r="F5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -16679,16 +16679,16 @@
       <c r="B6" s="78"/>
       <c r="C6" s="78"/>
       <c r="D6" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E6" s="74" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>199</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -16699,14 +16699,14 @@
       <c r="B7" s="78"/>
       <c r="C7" s="78"/>
       <c r="D7" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E7" s="75"/>
       <c r="F7" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -16717,14 +16717,14 @@
       <c r="B8" s="78"/>
       <c r="C8" s="78"/>
       <c r="D8" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E8" s="76"/>
       <c r="F8" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -16735,16 +16735,16 @@
       <c r="B9" s="78"/>
       <c r="C9" s="78"/>
       <c r="D9" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H9" s="20"/>
     </row>
@@ -16755,16 +16755,16 @@
       <c r="B10" s="78"/>
       <c r="C10" s="78"/>
       <c r="D10" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>320</v>
+      </c>
+      <c r="F10" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="E10" s="19" t="s">
-        <v>322</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>203</v>
-      </c>
       <c r="G10" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" s="20"/>
     </row>
@@ -16775,36 +16775,36 @@
       <c r="B11" s="78"/>
       <c r="C11" s="78"/>
       <c r="D11" s="51" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F11" s="52" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G11" s="57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H11" s="57"/>
     </row>
     <row r="12" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A12" s="61" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B12" s="79"/>
       <c r="C12" s="79"/>
       <c r="D12" s="51" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F12" s="52" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G12" s="57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H12" s="57"/>
     </row>

</xml_diff>

<commit_message>
Update the Test cases file for FileOperation as #36 fixed
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="421">
   <si>
     <t>删除文件夹</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -12022,9 +12022,168 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>1.能够出现提示输入的信息
-2.显示指定文件被批量删除的信息（</t>
+    <t>9. Batch Rename file or folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>批量重命名文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>进入"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>批量重命名文件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"模块，并输出</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Batch Rename file or folder</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.提示该文件夹会被删除的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Are you sure to delete D:\Test1\cCc? (Y/N)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.若选择Y删除，则显示该文件夹被删除的消息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1\cCc.txt has been deleted successfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）        
+3.本地计算机上该文件夹确实被删除
+4.若选择N不删除，则需要查看本地计算机该文件夹是否未被删除</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 能够出现提示输入的信息
+2. 提示输入的路径为文件路径，并非文件夹路径 (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\123.txt is a file path , please input a folder path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">)
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 能够出现提示输入的信息
+2. 提示批量会被批量删除的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Are you sure to delete them? (Y/N)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.显示指定文件被批量删除的信息（</t>
     </r>
     <r>
       <rPr>
@@ -12049,7 +12208,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">）
-3.本地计算机上这些文件确实被删除
+4.本地计算机上这些文件确实被删除
 </t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -12057,7 +12216,8 @@
   <si>
     <r>
       <t>1.能够出现提示输入的信息
-2.显示指定文件夹被批量删除的信息（</t>
+2. 提示批量会被批量删除的信息（Are you sure to delete them? (Y/N)
+3.显示指定文件夹被批量删除的信息（</t>
     </r>
     <r>
       <rPr>
@@ -12082,57 +12242,8 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">）
-3.本地计算机上这些文件夹确实被删除
+4.本地计算机上这些文件夹确实被删除
 </t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>9. Batch Rename file or folder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>批量重命名文件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>进入"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>批量重命名文件</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"模块，并输出</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Batch Rename file or folder</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -12972,7 +13083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -13782,7 +13893,7 @@
         <v>336</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>98</v>
@@ -13948,7 +14059,7 @@
         <v>410</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -14286,7 +14397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -14339,7 +14450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="256.5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="299.25" x14ac:dyDescent="0.15">
       <c r="A3" s="21">
         <v>3.1</v>
       </c>
@@ -14356,7 +14467,7 @@
         <v>306</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>20</v>
@@ -14399,7 +14510,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="213.75" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="270.75" x14ac:dyDescent="0.15">
       <c r="A6" s="21">
         <v>3.4</v>
       </c>
@@ -14412,7 +14523,7 @@
         <v>307</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>20</v>
@@ -14432,7 +14543,7 @@
         <v>308</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>189</v>
+        <v>418</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -16615,10 +16726,10 @@
         <v>9.1</v>
       </c>
       <c r="B3" s="77" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C3" s="77" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
Update the test cases of FileOperation as pervious update
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -12158,6 +12158,40 @@
   </si>
   <si>
     <r>
+      <t>1.能够出现提示输入的信息
+2. 提示批量会被批量删除的信息（Are you sure to delete them? (Y/N)
+3.显示指定文件夹被批量删除的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test Folder\Test9\McLaren1 has been deleted successfully!
+D:\Test Folder\Test9\McLaren2 has been deleted successfully!
+D:\Test Folder\Test9\McLaren3 has been deleted successfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">）
+4.本地计算机上这些文件夹确实被删除
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t>1. 能够出现提示输入的信息
 2. 提示批量会被批量删除的信息（</t>
     </r>
@@ -12171,7 +12205,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Are you sure to delete them? (Y/N)</t>
+      <t>Are you sure to batch delete files or folders? (Y/N)</t>
     </r>
     <r>
       <rPr>
@@ -12209,40 +12243,6 @@
       </rPr>
       <t xml:space="preserve">）
 4.本地计算机上这些文件确实被删除
-</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.能够出现提示输入的信息
-2. 提示批量会被批量删除的信息（Are you sure to delete them? (Y/N)
-3.显示指定文件夹被批量删除的信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test Folder\Test9\McLaren1 has been deleted successfully!
-D:\Test Folder\Test9\McLaren2 has been deleted successfully!
-D:\Test Folder\Test9\McLaren3 has been deleted successfully!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">）
-4.本地计算机上这些文件夹确实被删除
 </t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -14450,7 +14450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="299.25" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="313.5" x14ac:dyDescent="0.15">
       <c r="A3" s="21">
         <v>3.1</v>
       </c>
@@ -14467,7 +14467,7 @@
         <v>306</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>20</v>
@@ -14523,7 +14523,7 @@
         <v>307</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Update the test case file of FileOpration after big update
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -5650,67 +5650,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>1. 显示成功的将相同字段的文件被替换为指定的新名称
-(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\alonso.txt has been replaced as D:\Test\Button.txt successfully!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)
-2.可以在本地计算机中查到新名称文件</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 显示查找的文件不包含指定字段 （</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Didn't found file named with alonso on file D:\Test\Alonso.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2. 重命名失败</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Pass</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6388,37 +6327,6 @@
   </si>
   <si>
     <r>
-      <t>1. 能够出现提示输入的信息
-2. 提示输入的路径为文件路径，并非文件夹路径 (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\123.txt is a file path , please input a folder path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">)
-</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>提示信息 
 （</t>
     </r>
@@ -12246,6 +12154,96 @@
 </t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 能够出现提示输入的信息
+2. 提示输入的路径为文件路径，并非文件夹路径 (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\123.txt is a file path , please input a folder path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">)
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 能够出现提示输入的信息
+2. 提示输入的路径为文件路径，并非文件夹路径 (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\123.txt is a file path , please input a folder path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 能够出现提示输入的信息
+2. 提示输入的路径为文件路径，并非文件夹路径 (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\124.txt is a file path , please input a folder path)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
   </si>
 </sst>
 </file>
@@ -13083,7 +13081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -13147,13 +13145,13 @@
         <v>82</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E3" s="74" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>21</v>
@@ -13167,11 +13165,11 @@
       <c r="B4" s="78"/>
       <c r="C4" s="78"/>
       <c r="D4" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E4" s="75"/>
       <c r="F4" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>22</v>
@@ -13185,11 +13183,11 @@
       <c r="B5" s="78"/>
       <c r="C5" s="78"/>
       <c r="D5" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>23</v>
@@ -13203,11 +13201,11 @@
       <c r="B6" s="78"/>
       <c r="C6" s="78"/>
       <c r="D6" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E6" s="76"/>
       <c r="F6" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>26</v>
@@ -13221,13 +13219,13 @@
       <c r="B7" s="78"/>
       <c r="C7" s="78"/>
       <c r="D7" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E7" s="49" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>223</v>
+        <v>189</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="54"/>
@@ -13242,10 +13240,10 @@
         <v>96</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>81</v>
@@ -13259,13 +13257,13 @@
       <c r="B9" s="78"/>
       <c r="C9" s="78"/>
       <c r="D9" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>20</v>
@@ -13279,13 +13277,13 @@
       <c r="B10" s="78"/>
       <c r="C10" s="78"/>
       <c r="D10" s="51" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E10" s="51" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F10" s="51" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G10" s="56"/>
       <c r="H10" s="56"/>
@@ -13297,13 +13295,13 @@
       <c r="B11" s="79"/>
       <c r="C11" s="79"/>
       <c r="D11" s="51" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E11" s="51" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F11" s="51" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G11" s="56"/>
       <c r="H11" s="56"/>
@@ -13385,13 +13383,13 @@
         <v>179</v>
       </c>
       <c r="C3" s="83" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>182</v>
       </c>
       <c r="E3" s="74" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>186</v>
@@ -13429,7 +13427,7 @@
         <v>180</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>187</v>
@@ -13467,10 +13465,10 @@
         <v>96</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>20</v>
@@ -13484,13 +13482,13 @@
       <c r="B8" s="83"/>
       <c r="C8" s="83"/>
       <c r="D8" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>324</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>199</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>327</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>201</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>20</v>
@@ -13782,10 +13780,10 @@
       <c r="C5" s="83"/>
       <c r="D5" s="83"/>
       <c r="E5" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>20</v>
@@ -13800,7 +13798,7 @@
       <c r="C6" s="83"/>
       <c r="D6" s="83"/>
       <c r="E6" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>112</v>
@@ -13818,7 +13816,7 @@
       <c r="C7" s="83"/>
       <c r="D7" s="83"/>
       <c r="E7" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>113</v>
@@ -13836,7 +13834,7 @@
       <c r="C8" s="83"/>
       <c r="D8" s="83"/>
       <c r="E8" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>114</v>
@@ -13854,7 +13852,7 @@
       <c r="C9" s="83"/>
       <c r="D9" s="83"/>
       <c r="E9" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>115</v>
@@ -13872,7 +13870,7 @@
       <c r="C10" s="83"/>
       <c r="D10" s="83"/>
       <c r="E10" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>116</v>
@@ -13890,10 +13888,10 @@
       <c r="C11" s="83"/>
       <c r="D11" s="83"/>
       <c r="E11" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>98</v>
@@ -13902,13 +13900,13 @@
     </row>
     <row r="12" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="46" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B12" s="83"/>
       <c r="C12" s="83"/>
       <c r="D12" s="83"/>
       <c r="E12" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>188</v>
@@ -13926,7 +13924,7 @@
       <c r="C13" s="83"/>
       <c r="D13" s="83"/>
       <c r="E13" s="2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>143</v>
@@ -13944,7 +13942,7 @@
       <c r="C14" s="83"/>
       <c r="D14" s="83"/>
       <c r="E14" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>108</v>
@@ -13990,7 +13988,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -14056,10 +14054,10 @@
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -14076,10 +14074,10 @@
         <v>176</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>20</v>
@@ -14096,7 +14094,7 @@
         <v>177</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>67</v>
@@ -14116,10 +14114,10 @@
         <v>96</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G6" s="20" t="s">
         <v>20</v>
@@ -14128,18 +14126,18 @@
     </row>
     <row r="7" spans="1:9" ht="57" x14ac:dyDescent="0.15">
       <c r="A7" s="25" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B7" s="79"/>
       <c r="C7" s="79"/>
       <c r="D7" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>199</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>273</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>201</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>20</v>
@@ -14198,10 +14196,10 @@
         <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>20</v>
@@ -14219,10 +14217,10 @@
         <v>9</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>22</v>
@@ -14240,7 +14238,7 @@
         <v>178</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>68</v>
@@ -14261,10 +14259,10 @@
         <v>96</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>81</v>
@@ -14273,18 +14271,18 @@
     </row>
     <row r="14" spans="1:9" s="22" customFormat="1" ht="57" x14ac:dyDescent="0.15">
       <c r="A14" s="25" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B14" s="79"/>
       <c r="C14" s="79"/>
       <c r="D14" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>199</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>278</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>201</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>20</v>
@@ -14397,7 +14395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -14455,19 +14453,19 @@
         <v>3.1</v>
       </c>
       <c r="B3" s="83" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C3" s="83" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E3" s="74" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>20</v>
@@ -14520,10 +14518,10 @@
         <v>139</v>
       </c>
       <c r="E6" s="67" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>20</v>
@@ -14537,13 +14535,13 @@
       <c r="B7" s="83"/>
       <c r="C7" s="83"/>
       <c r="D7" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E7" s="67" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -14558,10 +14556,10 @@
         <v>96</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>20</v>
@@ -14575,13 +14573,13 @@
       <c r="B9" s="83"/>
       <c r="C9" s="83"/>
       <c r="D9" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>199</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>201</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>20</v>
@@ -14595,13 +14593,13 @@
       <c r="B10" s="83"/>
       <c r="C10" s="83"/>
       <c r="D10" s="51" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E10" s="51" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F10" s="51" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G10" s="56" t="s">
         <v>20</v>
@@ -14727,13 +14725,13 @@
         <v>78</v>
       </c>
       <c r="C3" s="77" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E3" s="74" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>144</v>
@@ -14763,7 +14761,7 @@
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B5" s="78"/>
       <c r="C5" s="78"/>
@@ -14781,7 +14779,7 @@
     </row>
     <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B6" s="78"/>
       <c r="C6" s="78"/>
@@ -14799,7 +14797,7 @@
     </row>
     <row r="7" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B7" s="78"/>
       <c r="C7" s="78"/>
@@ -14817,7 +14815,7 @@
     </row>
     <row r="8" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B8" s="78"/>
       <c r="C8" s="78"/>
@@ -14835,7 +14833,7 @@
     </row>
     <row r="9" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B9" s="78"/>
       <c r="C9" s="78"/>
@@ -14853,7 +14851,7 @@
     </row>
     <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="B10" s="78"/>
       <c r="C10" s="78"/>
@@ -14871,7 +14869,7 @@
     </row>
     <row r="11" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B11" s="78"/>
       <c r="C11" s="78"/>
@@ -14879,10 +14877,10 @@
         <v>96</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>20</v>
@@ -14891,7 +14889,7 @@
     </row>
     <row r="12" spans="1:8" s="22" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A12" s="19" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B12" s="78"/>
       <c r="C12" s="78"/>
@@ -14899,10 +14897,10 @@
         <v>97</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>20</v>
@@ -14911,18 +14909,18 @@
     </row>
     <row r="13" spans="1:8" s="22" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A13" s="25" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B13" s="78"/>
       <c r="C13" s="78"/>
       <c r="D13" s="19" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>20</v>
@@ -14931,18 +14929,18 @@
     </row>
     <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A14" s="25" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B14" s="78"/>
       <c r="C14" s="78"/>
       <c r="D14" s="19" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>20</v>
@@ -14951,21 +14949,21 @@
     </row>
     <row r="15" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A15" s="62" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B15" s="79"/>
       <c r="C15" s="79"/>
       <c r="D15" s="63" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E15" s="63" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F15" s="63" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G15" s="64" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H15" s="64"/>
     </row>
@@ -15003,13 +15001,13 @@
         <v>79</v>
       </c>
       <c r="C18" s="77" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>94</v>
       </c>
       <c r="E18" s="74" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F18" s="14" t="s">
         <v>149</v>
@@ -15039,7 +15037,7 @@
     </row>
     <row r="20" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A20" s="14" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B20" s="78"/>
       <c r="C20" s="78"/>
@@ -15057,7 +15055,7 @@
     </row>
     <row r="21" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A21" s="14" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B21" s="78"/>
       <c r="C21" s="78"/>
@@ -15075,7 +15073,7 @@
     </row>
     <row r="22" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A22" s="14" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B22" s="78"/>
       <c r="C22" s="78"/>
@@ -15093,7 +15091,7 @@
     </row>
     <row r="23" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A23" s="14" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B23" s="78"/>
       <c r="C23" s="78"/>
@@ -15111,7 +15109,7 @@
     </row>
     <row r="24" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A24" s="14" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B24" s="78"/>
       <c r="C24" s="78"/>
@@ -15119,10 +15117,10 @@
         <v>80</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>81</v>
@@ -15131,7 +15129,7 @@
     </row>
     <row r="25" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A25" s="14" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B25" s="78"/>
       <c r="C25" s="78"/>
@@ -15139,10 +15137,10 @@
         <v>97</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>20</v>
@@ -15151,18 +15149,18 @@
     </row>
     <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A26" s="14" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B26" s="78"/>
       <c r="C26" s="78"/>
       <c r="D26" s="19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>20</v>
@@ -15171,18 +15169,18 @@
     </row>
     <row r="27" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A27" s="25" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B27" s="78"/>
       <c r="C27" s="78"/>
       <c r="D27" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G27" s="20" t="s">
         <v>20</v>
@@ -15191,21 +15189,21 @@
     </row>
     <row r="28" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A28" s="62" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B28" s="79"/>
       <c r="C28" s="79"/>
       <c r="D28" s="63" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E28" s="63" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F28" s="63" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G28" s="64" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H28" s="64"/>
     </row>
@@ -15283,19 +15281,19 @@
     </row>
     <row r="3" spans="1:8" s="22" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B3" s="89" t="s">
         <v>117</v>
       </c>
       <c r="C3" s="89" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>171</v>
       </c>
       <c r="E3" s="86" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>152</v>
@@ -15307,7 +15305,7 @@
     </row>
     <row r="4" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B4" s="90"/>
       <c r="C4" s="90"/>
@@ -15325,7 +15323,7 @@
     </row>
     <row r="5" spans="1:8" s="22" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B5" s="90"/>
       <c r="C5" s="90"/>
@@ -15343,7 +15341,7 @@
     </row>
     <row r="6" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B6" s="90"/>
       <c r="C6" s="90"/>
@@ -15361,7 +15359,7 @@
     </row>
     <row r="7" spans="1:8" s="22" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B7" s="90"/>
       <c r="C7" s="90"/>
@@ -15379,7 +15377,7 @@
     </row>
     <row r="8" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B8" s="90"/>
       <c r="C8" s="90"/>
@@ -15397,7 +15395,7 @@
     </row>
     <row r="9" spans="1:8" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B9" s="90"/>
       <c r="C9" s="90"/>
@@ -15405,10 +15403,10 @@
         <v>96</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>20</v>
@@ -15417,7 +15415,7 @@
     </row>
     <row r="10" spans="1:8" s="31" customFormat="1" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B10" s="90"/>
       <c r="C10" s="90"/>
@@ -15425,10 +15423,10 @@
         <v>97</v>
       </c>
       <c r="E10" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="F10" s="19" t="s">
         <v>291</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>294</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>20</v>
@@ -15437,18 +15435,18 @@
     </row>
     <row r="11" spans="1:8" s="31" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B11" s="90"/>
       <c r="C11" s="90"/>
       <c r="D11" s="19" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>20</v>
@@ -15457,18 +15455,18 @@
     </row>
     <row r="12" spans="1:8" s="31" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="25" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B12" s="90"/>
       <c r="C12" s="90"/>
       <c r="D12" s="19" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>20</v>
@@ -15477,18 +15475,18 @@
     </row>
     <row r="13" spans="1:8" s="31" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A13" s="65" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B13" s="91"/>
       <c r="C13" s="91"/>
       <c r="D13" s="63" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E13" s="63" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F13" s="63" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G13" s="64" t="s">
         <v>20</v>
@@ -15532,19 +15530,19 @@
     </row>
     <row r="16" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B16" s="77" t="s">
         <v>118</v>
       </c>
       <c r="C16" s="89" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>119</v>
       </c>
       <c r="E16" s="74" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>155</v>
@@ -15556,7 +15554,7 @@
     </row>
     <row r="17" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B17" s="78"/>
       <c r="C17" s="90"/>
@@ -15574,7 +15572,7 @@
     </row>
     <row r="18" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B18" s="78"/>
       <c r="C18" s="90"/>
@@ -15592,7 +15590,7 @@
     </row>
     <row r="19" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B19" s="78"/>
       <c r="C19" s="90"/>
@@ -15610,7 +15608,7 @@
     </row>
     <row r="20" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B20" s="78"/>
       <c r="C20" s="90"/>
@@ -15628,7 +15626,7 @@
     </row>
     <row r="21" spans="1:8" s="22" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B21" s="78"/>
       <c r="C21" s="90"/>
@@ -15646,7 +15644,7 @@
     </row>
     <row r="22" spans="1:8" s="22" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B22" s="78"/>
       <c r="C22" s="90"/>
@@ -15664,7 +15662,7 @@
     </row>
     <row r="23" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B23" s="78"/>
       <c r="C23" s="90"/>
@@ -15682,7 +15680,7 @@
     </row>
     <row r="24" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B24" s="78"/>
       <c r="C24" s="90"/>
@@ -15690,10 +15688,10 @@
         <v>96</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>81</v>
@@ -15702,7 +15700,7 @@
     </row>
     <row r="25" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A25" s="19" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B25" s="78"/>
       <c r="C25" s="90"/>
@@ -15710,10 +15708,10 @@
         <v>97</v>
       </c>
       <c r="E25" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="F25" s="19" t="s">
         <v>297</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>300</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>20</v>
@@ -15722,18 +15720,18 @@
     </row>
     <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A26" s="25" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B26" s="78"/>
       <c r="C26" s="90"/>
       <c r="D26" s="19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>20</v>
@@ -15742,18 +15740,18 @@
     </row>
     <row r="27" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A27" s="25" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B27" s="78"/>
       <c r="C27" s="90"/>
       <c r="D27" s="19" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G27" s="20" t="s">
         <v>20</v>
@@ -15762,18 +15760,18 @@
     </row>
     <row r="28" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A28" s="62" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B28" s="79"/>
       <c r="C28" s="91"/>
       <c r="D28" s="63" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E28" s="63" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F28" s="63" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G28" s="64" t="s">
         <v>20</v>
@@ -15861,16 +15859,16 @@
         <v>12</v>
       </c>
       <c r="C3" s="77" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E3" s="74" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>33</v>
@@ -15884,11 +15882,11 @@
       <c r="B4" s="78"/>
       <c r="C4" s="78"/>
       <c r="D4" s="14" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E4" s="75"/>
       <c r="F4" s="14" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>26</v>
@@ -15902,11 +15900,11 @@
       <c r="B5" s="78"/>
       <c r="C5" s="78"/>
       <c r="D5" s="14" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="14" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>21</v>
@@ -15920,11 +15918,11 @@
       <c r="B6" s="78"/>
       <c r="C6" s="78"/>
       <c r="D6" s="14" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E6" s="76"/>
       <c r="F6" s="14" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>26</v>
@@ -15938,13 +15936,13 @@
       <c r="B7" s="78"/>
       <c r="C7" s="78"/>
       <c r="D7" s="14" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>190</v>
@@ -15961,10 +15959,10 @@
         <v>96</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>81</v>
@@ -15978,13 +15976,13 @@
       <c r="B9" s="78"/>
       <c r="C9" s="78"/>
       <c r="D9" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>20</v>
@@ -15998,13 +15996,13 @@
       <c r="B10" s="79"/>
       <c r="C10" s="79"/>
       <c r="D10" s="51" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E10" s="51" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F10" s="51" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="G10" s="56" t="s">
         <v>20</v>
@@ -16032,7 +16030,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="A2:H10"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -16090,13 +16088,13 @@
         <v>13</v>
       </c>
       <c r="C3" s="83" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E3" s="74" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>140</v>
@@ -16152,7 +16150,7 @@
         <v>139</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>141</v>
@@ -16169,13 +16167,13 @@
       <c r="B7" s="83"/>
       <c r="C7" s="83"/>
       <c r="D7" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>189</v>
+        <v>418</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -16190,10 +16188,10 @@
         <v>96</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>81</v>
@@ -16207,13 +16205,13 @@
       <c r="B9" s="83"/>
       <c r="C9" s="83"/>
       <c r="D9" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>199</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>309</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>201</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>20</v>
@@ -16227,13 +16225,13 @@
       <c r="B10" s="83"/>
       <c r="C10" s="83"/>
       <c r="D10" s="51" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E10" s="51" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F10" s="51" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G10" s="56" t="s">
         <v>20</v>
@@ -16314,19 +16312,19 @@
     </row>
     <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B3" s="77" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="77" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>60</v>
       </c>
       <c r="E3" s="74" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>158</v>
@@ -16338,7 +16336,7 @@
     </row>
     <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B4" s="78"/>
       <c r="C4" s="78"/>
@@ -16356,7 +16354,7 @@
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B5" s="78"/>
       <c r="C5" s="78"/>
@@ -16374,7 +16372,7 @@
     </row>
     <row r="6" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B6" s="78"/>
       <c r="C6" s="78"/>
@@ -16392,25 +16390,25 @@
     </row>
     <row r="7" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B7" s="78"/>
       <c r="C7" s="78"/>
       <c r="D7" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B8" s="78"/>
       <c r="C8" s="78"/>
@@ -16418,10 +16416,10 @@
         <v>96</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>20</v>
@@ -16430,18 +16428,18 @@
     </row>
     <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B9" s="78"/>
       <c r="C9" s="78"/>
       <c r="D9" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>20</v>
@@ -16450,21 +16448,21 @@
     </row>
     <row r="10" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B10" s="79"/>
       <c r="C10" s="79"/>
       <c r="D10" s="51" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E10" s="51" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="F10" s="51" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G10" s="56" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H10" s="56"/>
     </row>
@@ -16496,19 +16494,19 @@
     </row>
     <row r="13" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B13" s="77" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="77" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E13" s="74" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>159</v>
@@ -16520,7 +16518,7 @@
     </row>
     <row r="14" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B14" s="78"/>
       <c r="C14" s="78"/>
@@ -16538,7 +16536,7 @@
     </row>
     <row r="15" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B15" s="78"/>
       <c r="C15" s="78"/>
@@ -16556,7 +16554,7 @@
     </row>
     <row r="16" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B16" s="78"/>
       <c r="C16" s="78"/>
@@ -16574,25 +16572,25 @@
     </row>
     <row r="17" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B17" s="78"/>
       <c r="C17" s="78"/>
       <c r="D17" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E17" s="48"/>
       <c r="F17" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B18" s="78"/>
       <c r="C18" s="78"/>
@@ -16600,10 +16598,10 @@
         <v>96</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>81</v>
@@ -16612,18 +16610,18 @@
     </row>
     <row r="19" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B19" s="78"/>
       <c r="C19" s="78"/>
       <c r="D19" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="F19" s="19" t="s">
         <v>199</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>316</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>201</v>
       </c>
       <c r="G19" s="20" t="s">
         <v>20</v>
@@ -16632,21 +16630,21 @@
     </row>
     <row r="20" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B20" s="79"/>
       <c r="C20" s="79"/>
       <c r="D20" s="51" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E20" s="51" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F20" s="51" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G20" s="56" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H20" s="56"/>
     </row>
@@ -16726,16 +16724,16 @@
         <v>9.1</v>
       </c>
       <c r="B3" s="77" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C3" s="77" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>100</v>
       </c>
       <c r="E3" s="74" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>160</v>
@@ -16793,13 +16791,13 @@
         <v>192</v>
       </c>
       <c r="E6" s="74" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>197</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -16814,10 +16812,10 @@
       </c>
       <c r="E7" s="75"/>
       <c r="F7" s="2" t="s">
-        <v>196</v>
+        <v>420</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -16835,7 +16833,7 @@
         <v>194</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -16849,10 +16847,10 @@
         <v>96</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>81</v>
@@ -16866,13 +16864,13 @@
       <c r="B10" s="78"/>
       <c r="C10" s="78"/>
       <c r="D10" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="F10" s="19" t="s">
         <v>199</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>320</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>201</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>20</v>
@@ -16886,13 +16884,13 @@
       <c r="B11" s="78"/>
       <c r="C11" s="78"/>
       <c r="D11" s="51" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F11" s="52" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G11" s="57" t="s">
         <v>20</v>
@@ -16901,18 +16899,18 @@
     </row>
     <row r="12" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A12" s="61" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B12" s="79"/>
       <c r="C12" s="79"/>
       <c r="D12" s="51" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="F12" s="52" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G12" s="57" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Update test cases file for FileOpaeration as new feature #37 has been added
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Update Codes\1212\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Update Codes\1214\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="48" windowWidth="5352" windowHeight="7608" tabRatio="945" firstSheet="5" activeTab="10"/>
+    <workbookView xWindow="480" yWindow="48" windowWidth="5352" windowHeight="7608" tabRatio="945"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -24,16 +24,15 @@
     <sheet name="10.计算文件或文件夹大小" sheetId="17" r:id="rId10"/>
     <sheet name="11.解压缩rar和zip文件" sheetId="19" r:id="rId11"/>
     <sheet name="12.压缩文件或文件夹成zip文件" sheetId="20" r:id="rId12"/>
-    <sheet name="13.压缩文件或文件夹成rar文件" sheetId="21" r:id="rId13"/>
-    <sheet name="14.特殊字符测试" sheetId="15" r:id="rId14"/>
-    <sheet name="15.主界面基本功能检测" sheetId="16" r:id="rId15"/>
+    <sheet name="13.特殊字符测试" sheetId="15" r:id="rId13"/>
+    <sheet name="14.主界面基本功能检测" sheetId="16" r:id="rId14"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="465">
   <si>
     <t>删除文件夹</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -11316,10 +11315,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>在"Please choose :"中输入1-11以外的任何数值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>10. Calculate file or folder size</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -12108,18 +12103,6 @@
     </r>
   </si>
   <si>
-    <t>12.11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>12.12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>12.13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>在"Please choose :"中输入12</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -12699,6 +12682,329 @@
         <scheme val="minor"/>
       </rPr>
       <t>E:\Test123</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示该rar文件不存在的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\配置文件.rar is NOT exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在"Please choose :"中输入13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>进入"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>压缩文件或文件夹成zip文件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"模块，并输出</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Compress file or folder to zip</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>压缩文件或文件夹成zip文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12.Compress file or folder to zip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>再次输入同名的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>再次输入同名的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input file or folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Selenium配置文件\IEDriverServer-old.exe</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示出成功解压到该zip文件夹所在的目录下的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\python经典100例.zip has been decompressed to E:\python经典100例 successfullly!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.能够在对应目录找到该解压后的文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示该zip文件不存在的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\python经典100例.zip is NOT exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.不能在对应目录找到该解压后的文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示出同名解压文件夹已经存在，且不能被覆盖的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\python经典100例 is exists and won't cover!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.不能在对应目录找到该解压后的文件</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -12728,37 +13034,173 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>）</t>
+      <t>）
+3.能够在对应目录找到该解压后的文件</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
       <t>1.能够出现提示输入的信息
-2.显示出成功解压到该zip文件夹所在的目录下的信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\python经典100例.zip has been decompressed to E:\python经典100例 successfullly!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
+2.显示出同名解压文件夹已经存在，且不能被覆盖的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\配置文件 is exists and won't cover!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.不能在对应目录找到该解压后的文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示出非zip和非rar文件无法解压缩的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cannot decompress E:\Test123 as its not the correct format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.不能在对应目录找到该解压后的文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示出成功解压为zip文件夹，且存放所在的目录下的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Selenium配置文件\IEDriverServer-old.exe has been compressed as E:\Selenium配置文件\IEDriverServer-old.zip succeessfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.能够在对应目录找到解压的zip文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示出成功解压为zip文件夹，且存放所在的目录下的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\xfmovies has been compressed as E:\xfmovies.zip succeessfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.能够在对应目录找到解压的zip文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input file or folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\xfmovies</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -12777,139 +13219,217 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>E:\python经典100例.zip is NOT exist!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
+      <t>E:\xfmovies is NOT exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.不能在对应目录找到解压的zip文件</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
       <t>1.能够出现提示输入的信息
-2.显示该rar文件不存在的信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\配置文件.rar is NOT exist!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
+2.显示该zip文件不存在的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Selenium配置文件\IEDriverServer-old.zip is NOT exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.不能在对应目录找到解压的zip文件</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
       <t>1.能够出现提示输入的信息
-2.显示出同名解压文件夹已经存在，且不能被覆盖的信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\配置文件 is exists and won't cover!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
+2.显示出同名zip文件夹已经存在，且不能被覆盖的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\xfmovies.zip is exists and won't cover!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.不能在对应目录找到解压的zip文件</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
       <t>1.能够出现提示输入的信息
-2.显示出同名解压文件夹已经存在，且不能被覆盖的信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\python经典100例 is exists and won't cover!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.能够出现提示输入的信息
-2.显示出非zip和非rar文件无法解压缩的信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cannot decompress E:\Test123 as its not the correct format</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
+2.显示出同名zip文件夹已经存在，且不能被覆盖的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Selenium配置文件\IEDriverServer-old.zip is exists and won't cover!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.不能在对应目录找到解压的zip文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>大于2G以上的文件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>大于2G以上的文件夹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14.12</t>
+  </si>
+  <si>
+    <t>14.13</t>
+  </si>
+  <si>
+    <t>14.14</t>
+  </si>
+  <si>
+    <t>14.15</t>
+  </si>
+  <si>
+    <t>在"Please choose :"中输入1-13以外的任何数值</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -13161,7 +13681,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -13383,6 +13903,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -13785,7 +14308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -13803,14 +14326,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
+      <c r="A1" s="75"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
     </row>
     <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -13842,16 +14365,16 @@
       <c r="A3" s="21">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="79" t="s">
         <v>82</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="76" t="s">
         <v>256</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -13866,12 +14389,12 @@
       <c r="A4" s="21">
         <v>1.2</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
       <c r="D4" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="E4" s="76"/>
+      <c r="E4" s="77"/>
       <c r="F4" s="2" t="s">
         <v>211</v>
       </c>
@@ -13884,12 +14407,12 @@
       <c r="A5" s="21">
         <v>1.3</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
       <c r="D5" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E5" s="76"/>
+      <c r="E5" s="77"/>
       <c r="F5" s="2" t="s">
         <v>213</v>
       </c>
@@ -13902,12 +14425,12 @@
       <c r="A6" s="21">
         <v>1.4</v>
       </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
       <c r="D6" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E6" s="77"/>
+      <c r="E6" s="78"/>
       <c r="F6" s="2" t="s">
         <v>215</v>
       </c>
@@ -13920,8 +14443,8 @@
       <c r="A7" s="21">
         <v>1.5</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
       <c r="D7" s="2" t="s">
         <v>216</v>
       </c>
@@ -13938,8 +14461,8 @@
       <c r="A8" s="25">
         <v>1.6</v>
       </c>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
       <c r="D8" s="19" t="s">
         <v>96</v>
       </c>
@@ -13958,8 +14481,8 @@
       <c r="A9" s="25">
         <v>1.7</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="19" t="s">
         <v>193</v>
       </c>
@@ -13978,8 +14501,8 @@
       <c r="A10" s="52">
         <v>1.8</v>
       </c>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="51" t="s">
         <v>218</v>
       </c>
@@ -13996,8 +14519,8 @@
       <c r="A11" s="57">
         <v>1.9</v>
       </c>
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
+      <c r="B11" s="81"/>
+      <c r="C11" s="81"/>
       <c r="D11" s="51" t="s">
         <v>207</v>
       </c>
@@ -14044,14 +14567,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="86"/>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
+      <c r="A1" s="87"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
     </row>
     <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -14083,16 +14606,16 @@
       <c r="A3" s="21">
         <v>10.1</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="85" t="s">
         <v>179</v>
       </c>
-      <c r="C3" s="84" t="s">
-        <v>323</v>
+      <c r="C3" s="85" t="s">
+        <v>322</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="E3" s="75" t="s">
+        <v>420</v>
+      </c>
+      <c r="E3" s="76" t="s">
         <v>317</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -14107,12 +14630,12 @@
       <c r="A4" s="43">
         <v>10.199999999999999</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
       <c r="D4" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="E4" s="77"/>
+        <v>421</v>
+      </c>
+      <c r="E4" s="78"/>
       <c r="F4" s="2" t="s">
         <v>181</v>
       </c>
@@ -14125,12 +14648,12 @@
       <c r="A5" s="43">
         <v>10.3</v>
       </c>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
       <c r="D5" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="E5" s="75" t="s">
+        <v>422</v>
+      </c>
+      <c r="E5" s="76" t="s">
         <v>318</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -14145,12 +14668,12 @@
       <c r="A6" s="44">
         <v>10.4</v>
       </c>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="6" t="s">
-        <v>427</v>
-      </c>
-      <c r="E6" s="77"/>
+        <v>423</v>
+      </c>
+      <c r="E6" s="78"/>
       <c r="F6" s="2" t="s">
         <v>180</v>
       </c>
@@ -14163,8 +14686,8 @@
       <c r="A7" s="45">
         <v>10.5</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
       <c r="D7" s="19" t="s">
         <v>96</v>
       </c>
@@ -14183,8 +14706,8 @@
       <c r="A8" s="45">
         <v>10.6</v>
       </c>
-      <c r="B8" s="84"/>
-      <c r="C8" s="84"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
       <c r="D8" s="19" t="s">
         <v>193</v>
       </c>
@@ -14217,7 +14740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -14234,14 +14757,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="86"/>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
+      <c r="A1" s="87"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
     </row>
     <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -14269,78 +14792,78 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>11.1</v>
       </c>
-      <c r="B3" s="78" t="s">
-        <v>422</v>
-      </c>
-      <c r="C3" s="78" t="s">
-        <v>423</v>
+      <c r="B3" s="79" t="s">
+        <v>418</v>
+      </c>
+      <c r="C3" s="79" t="s">
+        <v>419</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E3" s="78" t="s">
-        <v>433</v>
+        <v>424</v>
+      </c>
+      <c r="E3" s="79" t="s">
+        <v>429</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
       <c r="A4" s="43">
         <v>11.2</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
       <c r="D4" s="6" t="s">
-        <v>431</v>
-      </c>
-      <c r="E4" s="79"/>
+        <v>427</v>
+      </c>
+      <c r="E4" s="80"/>
       <c r="F4" s="2" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>20</v>
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
       <c r="A5" s="43">
         <v>11.3</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
       <c r="D5" s="6" t="s">
-        <v>434</v>
-      </c>
-      <c r="E5" s="80"/>
+        <v>430</v>
+      </c>
+      <c r="E5" s="81"/>
       <c r="F5" s="2" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
       <c r="A6" s="43">
         <v>11.4</v>
       </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
       <c r="D6" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="E6" s="78" t="s">
-        <v>436</v>
+        <v>425</v>
+      </c>
+      <c r="E6" s="79" t="s">
+        <v>432</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>438</v>
+        <v>446</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>20</v>
@@ -14351,50 +14874,50 @@
       <c r="A7" s="44">
         <v>11.5</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
       <c r="D7" s="6" t="s">
-        <v>430</v>
-      </c>
-      <c r="E7" s="79"/>
+        <v>426</v>
+      </c>
+      <c r="E7" s="80"/>
       <c r="F7" s="2" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>20</v>
       </c>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
       <c r="A8" s="44">
         <v>11.6</v>
       </c>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
       <c r="D8" s="6" t="s">
-        <v>435</v>
-      </c>
-      <c r="E8" s="80"/>
+        <v>431</v>
+      </c>
+      <c r="E8" s="81"/>
       <c r="F8" s="2" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
       <c r="A9" s="44">
         <v>11.7</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="2" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="E9" s="73" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>20</v>
@@ -14405,8 +14928,8 @@
       <c r="A10" s="45">
         <v>11.8</v>
       </c>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="19" t="s">
         <v>96</v>
       </c>
@@ -14425,8 +14948,8 @@
       <c r="A11" s="45">
         <v>11.9</v>
       </c>
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
+      <c r="B11" s="81"/>
+      <c r="C11" s="81"/>
       <c r="D11" s="19" t="s">
         <v>193</v>
       </c>
@@ -14456,31 +14979,262 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="28.77734375" customWidth="1"/>
+    <col min="5" max="5" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.21875" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="87"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+    </row>
+    <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="156" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
+        <v>12.1</v>
+      </c>
+      <c r="B3" s="79" t="s">
+        <v>437</v>
+      </c>
+      <c r="C3" s="79" t="s">
+        <v>438</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="E3" s="79" t="s">
+        <v>442</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="43">
+        <v>12.2</v>
+      </c>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="E4" s="80"/>
+      <c r="F4" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <v>12.3</v>
+      </c>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="E5" s="80"/>
+      <c r="F5" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" ht="156" x14ac:dyDescent="0.25">
+      <c r="A6" s="43">
+        <v>12.4</v>
+      </c>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="E6" s="81"/>
+      <c r="F6" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
+        <v>12.5</v>
+      </c>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="E7" s="79" t="s">
+        <v>451</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="43">
+        <v>12.6</v>
+      </c>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="E8" s="80"/>
+      <c r="F8" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="21">
+        <v>12.7</v>
+      </c>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="E9" s="80"/>
+      <c r="F9" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="43">
+        <v>12.8</v>
+      </c>
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="E10" s="81"/>
+      <c r="F10" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
+        <v>12.9</v>
+      </c>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="20"/>
+    </row>
+    <row r="12" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="74" t="s">
+        <v>333</v>
+      </c>
+      <c r="B12" s="81"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="B3:B12"/>
+    <mergeCell ref="C3:C12"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
@@ -14501,14 +15255,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="86"/>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
+      <c r="A1" s="87"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
     </row>
     <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -14538,12 +15292,12 @@
     </row>
     <row r="3" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
-        <v>11.1</v>
-      </c>
-      <c r="B3" s="78" t="s">
+        <v>13.1</v>
+      </c>
+      <c r="B3" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="79" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -14552,7 +15306,7 @@
       <c r="E3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="78" t="s">
+      <c r="F3" s="79" t="s">
         <v>40</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -14562,17 +15316,17 @@
     </row>
     <row r="4" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
-        <v>11.2</v>
-      </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
+        <v>13.2</v>
+      </c>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
       <c r="D4" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="79"/>
+      <c r="F4" s="80"/>
       <c r="G4" s="2" t="s">
         <v>42</v>
       </c>
@@ -14580,17 +15334,17 @@
     </row>
     <row r="5" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
-        <v>11.3</v>
-      </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
+        <v>13.3</v>
+      </c>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="79"/>
+      <c r="F5" s="80"/>
       <c r="G5" s="2" t="s">
         <v>42</v>
       </c>
@@ -14598,17 +15352,17 @@
     </row>
     <row r="6" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
-        <v>11.4</v>
-      </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
+        <v>13.4</v>
+      </c>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
       <c r="D6" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="79"/>
+      <c r="F6" s="80"/>
       <c r="G6" s="5" t="s">
         <v>42</v>
       </c>
@@ -14616,17 +15370,17 @@
     </row>
     <row r="7" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
-        <v>11.5</v>
-      </c>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
+        <v>13.5</v>
+      </c>
+      <c r="B7" s="81"/>
+      <c r="C7" s="81"/>
       <c r="D7" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="80"/>
+      <c r="F7" s="81"/>
       <c r="G7" s="5" t="s">
         <v>42</v>
       </c>
@@ -14645,9 +15399,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -14666,14 +15420,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="86"/>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
+      <c r="A1" s="87"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
     </row>
     <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
@@ -14703,15 +15457,15 @@
     </row>
     <row r="3" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A3" s="41">
-        <v>12.1</v>
-      </c>
-      <c r="B3" s="84" t="s">
+        <v>14.1</v>
+      </c>
+      <c r="B3" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="85" t="s">
         <v>103</v>
       </c>
-      <c r="D3" s="84" t="s">
+      <c r="D3" s="85" t="s">
         <v>104</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -14727,11 +15481,11 @@
     </row>
     <row r="4" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A4" s="41">
-        <v>12.2</v>
-      </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
+        <v>14.2</v>
+      </c>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
       <c r="E4" s="2" t="s">
         <v>106</v>
       </c>
@@ -14745,16 +15499,16 @@
     </row>
     <row r="5" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A5" s="41">
-        <v>12.3</v>
-      </c>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
+        <v>14.3</v>
+      </c>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
       <c r="E5" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>333</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>20</v>
@@ -14763,13 +15517,13 @@
     </row>
     <row r="6" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A6" s="41">
-        <v>12.4</v>
-      </c>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
+        <v>14.4</v>
+      </c>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
       <c r="E6" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>112</v>
@@ -14781,13 +15535,13 @@
     </row>
     <row r="7" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A7" s="41">
-        <v>12.5</v>
-      </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
+        <v>14.5</v>
+      </c>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
       <c r="E7" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>113</v>
@@ -14799,13 +15553,13 @@
     </row>
     <row r="8" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A8" s="41">
-        <v>12.6</v>
-      </c>
-      <c r="B8" s="84"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
+        <v>14.6</v>
+      </c>
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="85"/>
       <c r="E8" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>114</v>
@@ -14817,13 +15571,13 @@
     </row>
     <row r="9" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A9" s="41">
-        <v>12.7</v>
-      </c>
-      <c r="B9" s="84"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
+        <v>14.7</v>
+      </c>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="85"/>
       <c r="E9" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>115</v>
@@ -14835,13 +15589,13 @@
     </row>
     <row r="10" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A10" s="41">
-        <v>12.8</v>
-      </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
+        <v>14.8</v>
+      </c>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
       <c r="E10" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>116</v>
@@ -14853,16 +15607,16 @@
     </row>
     <row r="11" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A11" s="41">
-        <v>12.9</v>
-      </c>
-      <c r="B11" s="84"/>
-      <c r="C11" s="84"/>
-      <c r="D11" s="84"/>
+        <v>14.9</v>
+      </c>
+      <c r="B11" s="85"/>
+      <c r="C11" s="85"/>
+      <c r="D11" s="85"/>
       <c r="E11" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>98</v>
@@ -14871,13 +15625,13 @@
     </row>
     <row r="12" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A12" s="46" t="s">
-        <v>334</v>
-      </c>
-      <c r="B12" s="84"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
+        <v>458</v>
+      </c>
+      <c r="B12" s="85"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="85"/>
       <c r="E12" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>184</v>
@@ -14889,73 +15643,85 @@
     </row>
     <row r="13" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
+        <v>459</v>
+      </c>
+      <c r="B13" s="85"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>417</v>
-      </c>
-      <c r="B13" s="84"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>421</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A14" s="46" t="s">
-        <v>418</v>
-      </c>
-      <c r="B14" s="84"/>
-      <c r="C14" s="84"/>
-      <c r="D14" s="84"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="5"/>
+        <v>460</v>
+      </c>
+      <c r="B14" s="85"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A15" s="46" t="s">
-        <v>419</v>
-      </c>
-      <c r="B15" s="84"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="5"/>
+        <v>461</v>
+      </c>
+      <c r="B15" s="85"/>
+      <c r="C15" s="85"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
-      <c r="A16" s="41">
-        <v>12.11</v>
-      </c>
-      <c r="B16" s="84"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="84"/>
+    <row r="16" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+      <c r="A16" s="46" t="s">
+        <v>462</v>
+      </c>
+      <c r="B16" s="85"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="85"/>
       <c r="E16" s="2" t="s">
-        <v>420</v>
+        <v>464</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="41">
-        <v>12.12</v>
-      </c>
-      <c r="B17" s="84"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
+      <c r="A17" s="46" t="s">
+        <v>463</v>
+      </c>
+      <c r="B17" s="85"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="85"/>
       <c r="E17" s="2" t="s">
-        <v>322</v>
+        <v>107</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>108</v>
@@ -14964,31 +15730,13 @@
         <v>98</v>
       </c>
       <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="41">
-        <v>12.13</v>
-      </c>
-      <c r="B18" s="84"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="84"/>
-      <c r="E18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="H18" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:B18"/>
-    <mergeCell ref="C3:C18"/>
-    <mergeCell ref="D3:D18"/>
+    <mergeCell ref="B3:B17"/>
+    <mergeCell ref="C3:C17"/>
+    <mergeCell ref="D3:D17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15018,14 +15766,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="81"/>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
+      <c r="A1" s="82"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
     </row>
     <row r="2" spans="1:9" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -15057,20 +15805,20 @@
       <c r="A3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="79" t="s">
         <v>83</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -15081,8 +15829,8 @@
       <c r="A4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
       <c r="D4" s="2" t="s">
         <v>176</v>
       </c>
@@ -15090,7 +15838,7 @@
         <v>263</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>20</v>
@@ -15101,8 +15849,8 @@
       <c r="A5" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
       <c r="D5" s="2" t="s">
         <v>177</v>
       </c>
@@ -15121,8 +15869,8 @@
       <c r="A6" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
       <c r="D6" s="19" t="s">
         <v>96</v>
       </c>
@@ -15141,8 +15889,8 @@
       <c r="A7" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="81"/>
       <c r="D7" s="19" t="s">
         <v>193</v>
       </c>
@@ -15199,10 +15947,10 @@
       <c r="A10" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="78" t="s">
+      <c r="B10" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="78" t="s">
+      <c r="C10" s="79" t="s">
         <v>83</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -15212,7 +15960,7 @@
         <v>268</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>20</v>
@@ -15224,16 +15972,16 @@
       <c r="A11" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="79"/>
-      <c r="C11" s="79"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>403</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>404</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>22</v>
@@ -15245,8 +15993,8 @@
       <c r="A12" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="79"/>
-      <c r="C12" s="79"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="80"/>
       <c r="D12" s="2" t="s">
         <v>178</v>
       </c>
@@ -15266,8 +16014,8 @@
       <c r="A13" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B13" s="79"/>
-      <c r="C13" s="79"/>
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
       <c r="D13" s="19" t="s">
         <v>96</v>
       </c>
@@ -15286,8 +16034,8 @@
       <c r="A14" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
       <c r="D14" s="19" t="s">
         <v>193</v>
       </c>
@@ -15304,7 +16052,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="82"/>
+      <c r="B15" s="83"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -15315,7 +16063,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="82"/>
+      <c r="B16" s="83"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -15326,7 +16074,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="82"/>
+      <c r="B17" s="83"/>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -15337,7 +16085,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="82"/>
+      <c r="B18" s="83"/>
       <c r="C18" s="4"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -15348,7 +16096,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="82"/>
+      <c r="B19" s="83"/>
       <c r="C19" s="4"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -15426,14 +16174,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="83"/>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
+      <c r="A1" s="84"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
     </row>
     <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -15465,20 +16213,20 @@
       <c r="A3" s="21">
         <v>3.1</v>
       </c>
-      <c r="B3" s="84" t="s">
-        <v>406</v>
-      </c>
-      <c r="C3" s="84" t="s">
+      <c r="B3" s="85" t="s">
         <v>405</v>
+      </c>
+      <c r="C3" s="85" t="s">
+        <v>404</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="76" t="s">
         <v>299</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>20</v>
@@ -15489,12 +16237,12 @@
       <c r="A4" s="21">
         <v>3.2</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="76"/>
+      <c r="E4" s="77"/>
       <c r="F4" s="2" t="s">
         <v>142</v>
       </c>
@@ -15507,12 +16255,12 @@
       <c r="A5" s="21">
         <v>3.3</v>
       </c>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
       <c r="D5" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E5" s="77"/>
+      <c r="E5" s="78"/>
       <c r="F5" s="2" t="s">
         <v>75</v>
       </c>
@@ -15525,8 +16273,8 @@
       <c r="A6" s="21">
         <v>3.4</v>
       </c>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="6" t="s">
         <v>139</v>
       </c>
@@ -15534,7 +16282,7 @@
         <v>300</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>20</v>
@@ -15545,8 +16293,8 @@
       <c r="A7" s="21">
         <v>3.5</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
       <c r="D7" s="2" t="s">
         <v>192</v>
       </c>
@@ -15554,7 +16302,7 @@
         <v>301</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -15563,8 +16311,8 @@
       <c r="A8" s="21">
         <v>3.6</v>
       </c>
-      <c r="B8" s="84"/>
-      <c r="C8" s="84"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
       <c r="D8" s="19" t="s">
         <v>96</v>
       </c>
@@ -15583,8 +16331,8 @@
       <c r="A9" s="21">
         <v>3.7</v>
       </c>
-      <c r="B9" s="84"/>
-      <c r="C9" s="84"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
       <c r="D9" s="19" t="s">
         <v>193</v>
       </c>
@@ -15603,8 +16351,8 @@
       <c r="A10" s="21">
         <v>3.8</v>
       </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="84"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="51" t="s">
         <v>232</v>
       </c>
@@ -15695,14 +16443,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A1" s="85"/>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
+      <c r="A1" s="86"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
     </row>
     <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -15734,16 +16482,16 @@
       <c r="A3" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="78" t="s">
-        <v>381</v>
+      <c r="C3" s="79" t="s">
+        <v>380</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="76" t="s">
         <v>273</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -15758,12 +16506,12 @@
       <c r="A4" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
       <c r="D4" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="E4" s="76"/>
+      <c r="E4" s="77"/>
       <c r="F4" s="2" t="s">
         <v>145</v>
       </c>
@@ -15774,14 +16522,14 @@
     </row>
     <row r="5" spans="1:8" ht="78" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
+        <v>381</v>
+      </c>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
       <c r="D5" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="E5" s="76"/>
+      <c r="E5" s="77"/>
       <c r="F5" s="2" t="s">
         <v>71</v>
       </c>
@@ -15792,14 +16540,14 @@
     </row>
     <row r="6" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
+        <v>382</v>
+      </c>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
       <c r="D6" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="76"/>
+      <c r="E6" s="77"/>
       <c r="F6" s="2" t="s">
         <v>146</v>
       </c>
@@ -15810,14 +16558,14 @@
     </row>
     <row r="7" spans="1:8" ht="78" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
+        <v>383</v>
+      </c>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
       <c r="D7" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E7" s="76"/>
+      <c r="E7" s="77"/>
       <c r="F7" s="2" t="s">
         <v>129</v>
       </c>
@@ -15828,14 +16576,14 @@
     </row>
     <row r="8" spans="1:8" ht="140.4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
+        <v>384</v>
+      </c>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
       <c r="D8" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E8" s="76"/>
+      <c r="E8" s="77"/>
       <c r="F8" s="18" t="s">
         <v>147</v>
       </c>
@@ -15846,14 +16594,14 @@
     </row>
     <row r="9" spans="1:8" ht="140.4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
+        <v>385</v>
+      </c>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="E9" s="76"/>
+      <c r="E9" s="77"/>
       <c r="F9" s="18" t="s">
         <v>148</v>
       </c>
@@ -15864,14 +16612,14 @@
     </row>
     <row r="10" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
+        <v>386</v>
+      </c>
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="E10" s="77"/>
+      <c r="E10" s="78"/>
       <c r="F10" s="34" t="s">
         <v>130</v>
       </c>
@@ -15882,10 +16630,10 @@
     </row>
     <row r="11" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="B11" s="79"/>
-      <c r="C11" s="79"/>
+        <v>387</v>
+      </c>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="19" t="s">
         <v>96</v>
       </c>
@@ -15902,10 +16650,10 @@
     </row>
     <row r="12" spans="1:8" s="22" customFormat="1" ht="156" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>389</v>
-      </c>
-      <c r="B12" s="79"/>
-      <c r="C12" s="79"/>
+        <v>388</v>
+      </c>
+      <c r="B12" s="80"/>
+      <c r="C12" s="80"/>
       <c r="D12" s="19" t="s">
         <v>97</v>
       </c>
@@ -15922,10 +16670,10 @@
     </row>
     <row r="13" spans="1:8" s="22" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
-        <v>390</v>
-      </c>
-      <c r="B13" s="79"/>
-      <c r="C13" s="79"/>
+        <v>389</v>
+      </c>
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
       <c r="D13" s="19" t="s">
         <v>202</v>
       </c>
@@ -15942,10 +16690,10 @@
     </row>
     <row r="14" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>391</v>
-      </c>
-      <c r="B14" s="79"/>
-      <c r="C14" s="79"/>
+        <v>390</v>
+      </c>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
       <c r="D14" s="19" t="s">
         <v>249</v>
       </c>
@@ -15962,10 +16710,10 @@
     </row>
     <row r="15" spans="1:8" ht="78" x14ac:dyDescent="0.25">
       <c r="A15" s="62" t="s">
-        <v>392</v>
-      </c>
-      <c r="B15" s="80"/>
-      <c r="C15" s="80"/>
+        <v>391</v>
+      </c>
+      <c r="B15" s="81"/>
+      <c r="C15" s="81"/>
       <c r="D15" s="63" t="s">
         <v>250</v>
       </c>
@@ -16010,16 +16758,16 @@
       <c r="A18" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="B18" s="78" t="s">
+      <c r="B18" s="79" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="78" t="s">
-        <v>381</v>
+      <c r="C18" s="79" t="s">
+        <v>380</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="E18" s="75" t="s">
+      <c r="E18" s="76" t="s">
         <v>278</v>
       </c>
       <c r="F18" s="14" t="s">
@@ -16034,12 +16782,12 @@
       <c r="A19" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B19" s="79"/>
-      <c r="C19" s="79"/>
+      <c r="B19" s="80"/>
+      <c r="C19" s="80"/>
       <c r="D19" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E19" s="76"/>
+      <c r="E19" s="77"/>
       <c r="F19" s="14" t="s">
         <v>70</v>
       </c>
@@ -16050,14 +16798,14 @@
     </row>
     <row r="20" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>393</v>
-      </c>
-      <c r="B20" s="79"/>
-      <c r="C20" s="79"/>
+        <v>392</v>
+      </c>
+      <c r="B20" s="80"/>
+      <c r="C20" s="80"/>
       <c r="D20" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="76"/>
+      <c r="E20" s="77"/>
       <c r="F20" s="14" t="s">
         <v>150</v>
       </c>
@@ -16068,14 +16816,14 @@
     </row>
     <row r="21" spans="1:8" ht="78" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>394</v>
-      </c>
-      <c r="B21" s="79"/>
-      <c r="C21" s="79"/>
+        <v>393</v>
+      </c>
+      <c r="B21" s="80"/>
+      <c r="C21" s="80"/>
       <c r="D21" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="E21" s="76"/>
+      <c r="E21" s="77"/>
       <c r="F21" s="14" t="s">
         <v>69</v>
       </c>
@@ -16086,14 +16834,14 @@
     </row>
     <row r="22" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>395</v>
-      </c>
-      <c r="B22" s="79"/>
-      <c r="C22" s="79"/>
+        <v>394</v>
+      </c>
+      <c r="B22" s="80"/>
+      <c r="C22" s="80"/>
       <c r="D22" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="E22" s="76"/>
+      <c r="E22" s="77"/>
       <c r="F22" s="11" t="s">
         <v>151</v>
       </c>
@@ -16104,14 +16852,14 @@
     </row>
     <row r="23" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>396</v>
-      </c>
-      <c r="B23" s="79"/>
-      <c r="C23" s="79"/>
+        <v>395</v>
+      </c>
+      <c r="B23" s="80"/>
+      <c r="C23" s="80"/>
       <c r="D23" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="E23" s="77"/>
+      <c r="E23" s="78"/>
       <c r="F23" s="34" t="s">
         <v>134</v>
       </c>
@@ -16122,10 +16870,10 @@
     </row>
     <row r="24" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>397</v>
-      </c>
-      <c r="B24" s="79"/>
-      <c r="C24" s="79"/>
+        <v>396</v>
+      </c>
+      <c r="B24" s="80"/>
+      <c r="C24" s="80"/>
       <c r="D24" s="19" t="s">
         <v>80</v>
       </c>
@@ -16142,10 +16890,10 @@
     </row>
     <row r="25" spans="1:8" ht="156" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>398</v>
-      </c>
-      <c r="B25" s="79"/>
-      <c r="C25" s="79"/>
+        <v>397</v>
+      </c>
+      <c r="B25" s="80"/>
+      <c r="C25" s="80"/>
       <c r="D25" s="19" t="s">
         <v>97</v>
       </c>
@@ -16162,10 +16910,10 @@
     </row>
     <row r="26" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>399</v>
-      </c>
-      <c r="B26" s="79"/>
-      <c r="C26" s="79"/>
+        <v>398</v>
+      </c>
+      <c r="B26" s="80"/>
+      <c r="C26" s="80"/>
       <c r="D26" s="19" t="s">
         <v>203</v>
       </c>
@@ -16182,10 +16930,10 @@
     </row>
     <row r="27" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
-        <v>400</v>
-      </c>
-      <c r="B27" s="79"/>
-      <c r="C27" s="79"/>
+        <v>399</v>
+      </c>
+      <c r="B27" s="80"/>
+      <c r="C27" s="80"/>
       <c r="D27" s="19" t="s">
         <v>248</v>
       </c>
@@ -16202,10 +16950,10 @@
     </row>
     <row r="28" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A28" s="62" t="s">
-        <v>401</v>
-      </c>
-      <c r="B28" s="80"/>
-      <c r="C28" s="80"/>
+        <v>400</v>
+      </c>
+      <c r="B28" s="81"/>
+      <c r="C28" s="81"/>
       <c r="D28" s="63" t="s">
         <v>252</v>
       </c>
@@ -16257,14 +17005,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="86"/>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
+      <c r="A1" s="87"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -16294,18 +17042,18 @@
     </row>
     <row r="3" spans="1:8" s="22" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="B3" s="90" t="s">
+        <v>356</v>
+      </c>
+      <c r="B3" s="91" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="90" t="s">
-        <v>356</v>
+      <c r="C3" s="91" t="s">
+        <v>355</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="E3" s="87" t="s">
+      <c r="E3" s="88" t="s">
         <v>282</v>
       </c>
       <c r="F3" s="6" t="s">
@@ -16318,14 +17066,14 @@
     </row>
     <row r="4" spans="1:8" s="22" customFormat="1" ht="78" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>358</v>
-      </c>
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
+        <v>357</v>
+      </c>
+      <c r="B4" s="92"/>
+      <c r="C4" s="92"/>
       <c r="D4" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="E4" s="88"/>
+      <c r="E4" s="89"/>
       <c r="F4" s="6" t="s">
         <v>72</v>
       </c>
@@ -16336,14 +17084,14 @@
     </row>
     <row r="5" spans="1:8" s="22" customFormat="1" ht="124.8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>359</v>
-      </c>
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
+        <v>358</v>
+      </c>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
       <c r="D5" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="88"/>
+      <c r="E5" s="89"/>
       <c r="F5" s="6" t="s">
         <v>153</v>
       </c>
@@ -16354,14 +17102,14 @@
     </row>
     <row r="6" spans="1:8" s="22" customFormat="1" ht="78" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>360</v>
-      </c>
-      <c r="B6" s="91"/>
-      <c r="C6" s="91"/>
+        <v>359</v>
+      </c>
+      <c r="B6" s="92"/>
+      <c r="C6" s="92"/>
       <c r="D6" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="E6" s="88"/>
+      <c r="E6" s="89"/>
       <c r="F6" s="6" t="s">
         <v>72</v>
       </c>
@@ -16372,14 +17120,14 @@
     </row>
     <row r="7" spans="1:8" s="22" customFormat="1" ht="187.2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>361</v>
-      </c>
-      <c r="B7" s="91"/>
-      <c r="C7" s="91"/>
+        <v>360</v>
+      </c>
+      <c r="B7" s="92"/>
+      <c r="C7" s="92"/>
       <c r="D7" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="E7" s="88"/>
+      <c r="E7" s="89"/>
       <c r="F7" s="27" t="s">
         <v>154</v>
       </c>
@@ -16390,14 +17138,14 @@
     </row>
     <row r="8" spans="1:8" s="22" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>362</v>
-      </c>
-      <c r="B8" s="91"/>
-      <c r="C8" s="91"/>
+        <v>361</v>
+      </c>
+      <c r="B8" s="92"/>
+      <c r="C8" s="92"/>
       <c r="D8" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="E8" s="89"/>
+      <c r="E8" s="90"/>
       <c r="F8" s="34" t="s">
         <v>138</v>
       </c>
@@ -16408,10 +17156,10 @@
     </row>
     <row r="9" spans="1:8" s="22" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>363</v>
-      </c>
-      <c r="B9" s="91"/>
-      <c r="C9" s="91"/>
+        <v>362</v>
+      </c>
+      <c r="B9" s="92"/>
+      <c r="C9" s="92"/>
       <c r="D9" s="19" t="s">
         <v>96</v>
       </c>
@@ -16428,10 +17176,10 @@
     </row>
     <row r="10" spans="1:8" s="31" customFormat="1" ht="156" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>364</v>
-      </c>
-      <c r="B10" s="91"/>
-      <c r="C10" s="91"/>
+        <v>363</v>
+      </c>
+      <c r="B10" s="92"/>
+      <c r="C10" s="92"/>
       <c r="D10" s="19" t="s">
         <v>97</v>
       </c>
@@ -16448,10 +17196,10 @@
     </row>
     <row r="11" spans="1:8" s="31" customFormat="1" ht="62.4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="B11" s="91"/>
-      <c r="C11" s="91"/>
+        <v>364</v>
+      </c>
+      <c r="B11" s="92"/>
+      <c r="C11" s="92"/>
       <c r="D11" s="19" t="s">
         <v>204</v>
       </c>
@@ -16468,10 +17216,10 @@
     </row>
     <row r="12" spans="1:8" s="31" customFormat="1" ht="62.4" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>366</v>
-      </c>
-      <c r="B12" s="91"/>
-      <c r="C12" s="91"/>
+        <v>365</v>
+      </c>
+      <c r="B12" s="92"/>
+      <c r="C12" s="92"/>
       <c r="D12" s="19" t="s">
         <v>205</v>
       </c>
@@ -16488,10 +17236,10 @@
     </row>
     <row r="13" spans="1:8" s="31" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A13" s="65" t="s">
-        <v>367</v>
-      </c>
-      <c r="B13" s="92"/>
-      <c r="C13" s="92"/>
+        <v>366</v>
+      </c>
+      <c r="B13" s="93"/>
+      <c r="C13" s="93"/>
       <c r="D13" s="63" t="s">
         <v>253</v>
       </c>
@@ -16543,18 +17291,18 @@
     </row>
     <row r="16" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="B16" s="78" t="s">
+        <v>367</v>
+      </c>
+      <c r="B16" s="79" t="s">
         <v>118</v>
       </c>
-      <c r="C16" s="90" t="s">
-        <v>356</v>
+      <c r="C16" s="91" t="s">
+        <v>355</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E16" s="75" t="s">
+      <c r="E16" s="76" t="s">
         <v>288</v>
       </c>
       <c r="F16" s="2" t="s">
@@ -16567,14 +17315,14 @@
     </row>
     <row r="17" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="B17" s="79"/>
-      <c r="C17" s="91"/>
+        <v>368</v>
+      </c>
+      <c r="B17" s="80"/>
+      <c r="C17" s="92"/>
       <c r="D17" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E17" s="76"/>
+      <c r="E17" s="77"/>
       <c r="F17" s="2" t="s">
         <v>156</v>
       </c>
@@ -16585,14 +17333,14 @@
     </row>
     <row r="18" spans="1:8" ht="78" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="B18" s="79"/>
-      <c r="C18" s="91"/>
+        <v>369</v>
+      </c>
+      <c r="B18" s="80"/>
+      <c r="C18" s="92"/>
       <c r="D18" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E18" s="76"/>
+      <c r="E18" s="77"/>
       <c r="F18" s="2" t="s">
         <v>74</v>
       </c>
@@ -16603,14 +17351,14 @@
     </row>
     <row r="19" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="B19" s="79"/>
-      <c r="C19" s="91"/>
+        <v>370</v>
+      </c>
+      <c r="B19" s="80"/>
+      <c r="C19" s="92"/>
       <c r="D19" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="76"/>
+      <c r="E19" s="77"/>
       <c r="F19" s="2" t="s">
         <v>157</v>
       </c>
@@ -16621,14 +17369,14 @@
     </row>
     <row r="20" spans="1:8" ht="78" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="B20" s="79"/>
-      <c r="C20" s="91"/>
+        <v>371</v>
+      </c>
+      <c r="B20" s="80"/>
+      <c r="C20" s="92"/>
       <c r="D20" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E20" s="76"/>
+      <c r="E20" s="77"/>
       <c r="F20" s="2" t="s">
         <v>73</v>
       </c>
@@ -16639,14 +17387,14 @@
     </row>
     <row r="21" spans="1:8" s="22" customFormat="1" ht="140.4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="B21" s="79"/>
-      <c r="C21" s="91"/>
+        <v>372</v>
+      </c>
+      <c r="B21" s="80"/>
+      <c r="C21" s="92"/>
       <c r="D21" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="E21" s="76"/>
+      <c r="E21" s="77"/>
       <c r="F21" s="11" t="s">
         <v>66</v>
       </c>
@@ -16657,14 +17405,14 @@
     </row>
     <row r="22" spans="1:8" s="22" customFormat="1" ht="140.4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="B22" s="79"/>
-      <c r="C22" s="91"/>
+        <v>373</v>
+      </c>
+      <c r="B22" s="80"/>
+      <c r="C22" s="92"/>
       <c r="D22" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="E22" s="76"/>
+      <c r="E22" s="77"/>
       <c r="F22" s="11" t="s">
         <v>66</v>
       </c>
@@ -16675,14 +17423,14 @@
     </row>
     <row r="23" spans="1:8" s="22" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="B23" s="79"/>
-      <c r="C23" s="91"/>
+        <v>374</v>
+      </c>
+      <c r="B23" s="80"/>
+      <c r="C23" s="92"/>
       <c r="D23" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="E23" s="77"/>
+      <c r="E23" s="78"/>
       <c r="F23" s="34" t="s">
         <v>135</v>
       </c>
@@ -16693,10 +17441,10 @@
     </row>
     <row r="24" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="B24" s="79"/>
-      <c r="C24" s="91"/>
+        <v>375</v>
+      </c>
+      <c r="B24" s="80"/>
+      <c r="C24" s="92"/>
       <c r="D24" s="19" t="s">
         <v>96</v>
       </c>
@@ -16713,10 +17461,10 @@
     </row>
     <row r="25" spans="1:8" ht="156" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
-        <v>377</v>
-      </c>
-      <c r="B25" s="79"/>
-      <c r="C25" s="91"/>
+        <v>376</v>
+      </c>
+      <c r="B25" s="80"/>
+      <c r="C25" s="92"/>
       <c r="D25" s="19" t="s">
         <v>97</v>
       </c>
@@ -16733,10 +17481,10 @@
     </row>
     <row r="26" spans="1:8" ht="62.4" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
-        <v>378</v>
-      </c>
-      <c r="B26" s="79"/>
-      <c r="C26" s="91"/>
+        <v>377</v>
+      </c>
+      <c r="B26" s="80"/>
+      <c r="C26" s="92"/>
       <c r="D26" s="19" t="s">
         <v>206</v>
       </c>
@@ -16753,10 +17501,10 @@
     </row>
     <row r="27" spans="1:8" ht="62.4" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
-        <v>379</v>
-      </c>
-      <c r="B27" s="79"/>
-      <c r="C27" s="91"/>
+        <v>378</v>
+      </c>
+      <c r="B27" s="80"/>
+      <c r="C27" s="92"/>
       <c r="D27" s="19" t="s">
         <v>255</v>
       </c>
@@ -16773,10 +17521,10 @@
     </row>
     <row r="28" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A28" s="62" t="s">
-        <v>380</v>
-      </c>
-      <c r="B28" s="80"/>
-      <c r="C28" s="92"/>
+        <v>379</v>
+      </c>
+      <c r="B28" s="81"/>
+      <c r="C28" s="93"/>
       <c r="D28" s="63" t="s">
         <v>254</v>
       </c>
@@ -16829,14 +17577,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="93"/>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
+      <c r="A1" s="94"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
     </row>
     <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -16868,16 +17616,16 @@
       <c r="A3" s="21">
         <v>6.1</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="78" t="s">
-        <v>355</v>
+      <c r="C3" s="79" t="s">
+        <v>354</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="76" t="s">
         <v>294</v>
       </c>
       <c r="F3" s="14" t="s">
@@ -16892,12 +17640,12 @@
       <c r="A4" s="21">
         <v>6.2</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
       <c r="D4" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="E4" s="76"/>
+      <c r="E4" s="77"/>
       <c r="F4" s="14" t="s">
         <v>224</v>
       </c>
@@ -16910,12 +17658,12 @@
       <c r="A5" s="21">
         <v>6.3</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
       <c r="D5" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="E5" s="76"/>
+      <c r="E5" s="77"/>
       <c r="F5" s="14" t="s">
         <v>226</v>
       </c>
@@ -16928,12 +17676,12 @@
       <c r="A6" s="21">
         <v>6.4</v>
       </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
       <c r="D6" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="E6" s="77"/>
+      <c r="E6" s="78"/>
       <c r="F6" s="14" t="s">
         <v>228</v>
       </c>
@@ -16946,8 +17694,8 @@
       <c r="A7" s="21">
         <v>6.5</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
       <c r="D7" s="14" t="s">
         <v>229</v>
       </c>
@@ -16966,8 +17714,8 @@
       <c r="A8" s="21">
         <v>6.6</v>
       </c>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
       <c r="D8" s="19" t="s">
         <v>96</v>
       </c>
@@ -16986,8 +17734,8 @@
       <c r="A9" s="21">
         <v>6.7</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="19" t="s">
         <v>193</v>
       </c>
@@ -17006,8 +17754,8 @@
       <c r="A10" s="21">
         <v>6.8</v>
       </c>
-      <c r="B10" s="80"/>
-      <c r="C10" s="80"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
       <c r="D10" s="51" t="s">
         <v>219</v>
       </c>
@@ -17058,14 +17806,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="86"/>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
+      <c r="A1" s="87"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
     </row>
     <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -17097,16 +17845,16 @@
       <c r="A3" s="21">
         <v>7.1</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="84" t="s">
-        <v>354</v>
+      <c r="C3" s="85" t="s">
+        <v>353</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="76" t="s">
         <v>299</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -17121,12 +17869,12 @@
       <c r="A4" s="21">
         <v>7.2</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="76"/>
+      <c r="E4" s="77"/>
       <c r="F4" s="2" t="s">
         <v>142</v>
       </c>
@@ -17139,12 +17887,12 @@
       <c r="A5" s="21">
         <v>7.3</v>
       </c>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
       <c r="D5" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E5" s="77"/>
+      <c r="E5" s="78"/>
       <c r="F5" s="2" t="s">
         <v>75</v>
       </c>
@@ -17157,8 +17905,8 @@
       <c r="A6" s="21">
         <v>7.4</v>
       </c>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="6" t="s">
         <v>139</v>
       </c>
@@ -17177,8 +17925,8 @@
       <c r="A7" s="21">
         <v>7.5</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
       <c r="D7" s="2" t="s">
         <v>192</v>
       </c>
@@ -17186,7 +17934,7 @@
         <v>301</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -17195,8 +17943,8 @@
       <c r="A8" s="21">
         <v>7.6</v>
       </c>
-      <c r="B8" s="84"/>
-      <c r="C8" s="84"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
       <c r="D8" s="19" t="s">
         <v>96</v>
       </c>
@@ -17215,8 +17963,8 @@
       <c r="A9" s="21">
         <v>7.7</v>
       </c>
-      <c r="B9" s="84"/>
-      <c r="C9" s="84"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
       <c r="D9" s="19" t="s">
         <v>193</v>
       </c>
@@ -17235,8 +17983,8 @@
       <c r="A10" s="21">
         <v>7.8</v>
       </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="84"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="51" t="s">
         <v>232</v>
       </c>
@@ -17288,14 +18036,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="86"/>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
+      <c r="A1" s="87"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
     </row>
     <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -17325,18 +18073,18 @@
     </row>
     <row r="3" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="B3" s="78" t="s">
+        <v>336</v>
+      </c>
+      <c r="B3" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="78" t="s">
-        <v>336</v>
+      <c r="C3" s="79" t="s">
+        <v>335</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="76" t="s">
         <v>304</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -17349,14 +18097,14 @@
     </row>
     <row r="4" spans="1:8" ht="78" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
+        <v>337</v>
+      </c>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
       <c r="D4" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E4" s="76"/>
+      <c r="E4" s="77"/>
       <c r="F4" s="2" t="s">
         <v>57</v>
       </c>
@@ -17367,14 +18115,14 @@
     </row>
     <row r="5" spans="1:8" ht="78" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
+        <v>338</v>
+      </c>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
       <c r="D5" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E5" s="76"/>
+      <c r="E5" s="77"/>
       <c r="F5" s="2" t="s">
         <v>76</v>
       </c>
@@ -17385,14 +18133,14 @@
     </row>
     <row r="6" spans="1:8" s="22" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
+        <v>339</v>
+      </c>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
       <c r="D6" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="77"/>
+      <c r="E6" s="78"/>
       <c r="F6" s="6" t="s">
         <v>58</v>
       </c>
@@ -17403,10 +18151,10 @@
     </row>
     <row r="7" spans="1:8" s="22" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
+        <v>340</v>
+      </c>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
       <c r="D7" s="2" t="s">
         <v>197</v>
       </c>
@@ -17421,10 +18169,10 @@
     </row>
     <row r="8" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
+        <v>341</v>
+      </c>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
       <c r="D8" s="19" t="s">
         <v>96</v>
       </c>
@@ -17441,10 +18189,10 @@
     </row>
     <row r="9" spans="1:8" ht="62.4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
+        <v>342</v>
+      </c>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="19" t="s">
         <v>193</v>
       </c>
@@ -17461,10 +18209,10 @@
     </row>
     <row r="10" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="B10" s="80"/>
-      <c r="C10" s="80"/>
+        <v>343</v>
+      </c>
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
       <c r="D10" s="51" t="s">
         <v>235</v>
       </c>
@@ -17507,18 +18255,18 @@
     </row>
     <row r="13" spans="1:8" ht="140.4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="B13" s="78" t="s">
+        <v>345</v>
+      </c>
+      <c r="B13" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="78" t="s">
-        <v>345</v>
+      <c r="C13" s="79" t="s">
+        <v>344</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="75" t="s">
+      <c r="E13" s="76" t="s">
         <v>306</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -17531,14 +18279,14 @@
     </row>
     <row r="14" spans="1:8" ht="78" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="B14" s="79"/>
-      <c r="C14" s="79"/>
+        <v>346</v>
+      </c>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
       <c r="D14" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E14" s="76"/>
+      <c r="E14" s="77"/>
       <c r="F14" s="2" t="s">
         <v>99</v>
       </c>
@@ -17549,14 +18297,14 @@
     </row>
     <row r="15" spans="1:8" ht="78" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="B15" s="79"/>
-      <c r="C15" s="79"/>
+        <v>347</v>
+      </c>
+      <c r="B15" s="80"/>
+      <c r="C15" s="80"/>
       <c r="D15" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E15" s="76"/>
+      <c r="E15" s="77"/>
       <c r="F15" s="2" t="s">
         <v>62</v>
       </c>
@@ -17567,14 +18315,14 @@
     </row>
     <row r="16" spans="1:8" s="22" customFormat="1" ht="109.2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="B16" s="79"/>
-      <c r="C16" s="79"/>
+        <v>348</v>
+      </c>
+      <c r="B16" s="80"/>
+      <c r="C16" s="80"/>
       <c r="D16" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="77"/>
+      <c r="E16" s="78"/>
       <c r="F16" s="6" t="s">
         <v>65</v>
       </c>
@@ -17585,10 +18333,10 @@
     </row>
     <row r="17" spans="1:8" s="22" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="B17" s="79"/>
-      <c r="C17" s="79"/>
+        <v>349</v>
+      </c>
+      <c r="B17" s="80"/>
+      <c r="C17" s="80"/>
       <c r="D17" s="2" t="s">
         <v>200</v>
       </c>
@@ -17603,10 +18351,10 @@
     </row>
     <row r="18" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="B18" s="79"/>
-      <c r="C18" s="79"/>
+        <v>350</v>
+      </c>
+      <c r="B18" s="80"/>
+      <c r="C18" s="80"/>
       <c r="D18" s="19" t="s">
         <v>96</v>
       </c>
@@ -17623,10 +18371,10 @@
     </row>
     <row r="19" spans="1:8" ht="62.4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="B19" s="79"/>
-      <c r="C19" s="79"/>
+        <v>351</v>
+      </c>
+      <c r="B19" s="80"/>
+      <c r="C19" s="80"/>
       <c r="D19" s="19" t="s">
         <v>193</v>
       </c>
@@ -17643,10 +18391,10 @@
     </row>
     <row r="20" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="B20" s="80"/>
-      <c r="C20" s="80"/>
+        <v>352</v>
+      </c>
+      <c r="B20" s="81"/>
+      <c r="C20" s="81"/>
       <c r="D20" s="51" t="s">
         <v>238</v>
       </c>
@@ -17697,14 +18445,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="86"/>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
+      <c r="A1" s="87"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
     </row>
     <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -17736,16 +18484,16 @@
       <c r="A3" s="21">
         <v>9.1</v>
       </c>
-      <c r="B3" s="78" t="s">
-        <v>408</v>
-      </c>
-      <c r="C3" s="78" t="s">
+      <c r="B3" s="79" t="s">
         <v>407</v>
+      </c>
+      <c r="C3" s="79" t="s">
+        <v>406</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="76" t="s">
         <v>311</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -17762,12 +18510,12 @@
       <c r="A4" s="21">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
       <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="76"/>
+      <c r="E4" s="77"/>
       <c r="F4" s="2" t="s">
         <v>47</v>
       </c>
@@ -17780,12 +18528,12 @@
       <c r="A5" s="21">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
       <c r="D5" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E5" s="77"/>
+      <c r="E5" s="78"/>
       <c r="F5" s="2" t="s">
         <v>77</v>
       </c>
@@ -17798,16 +18546,16 @@
       <c r="A6" s="21">
         <v>9.4</v>
       </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
       <c r="D6" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E6" s="75" t="s">
+      <c r="E6" s="76" t="s">
         <v>312</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>191</v>
@@ -17818,14 +18566,14 @@
       <c r="A7" s="21">
         <v>9.5</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
       <c r="D7" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="E7" s="76"/>
+      <c r="E7" s="77"/>
       <c r="F7" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>191</v>
@@ -17836,12 +18584,12 @@
       <c r="A8" s="21">
         <v>9.6</v>
       </c>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
       <c r="D8" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E8" s="77"/>
+      <c r="E8" s="78"/>
       <c r="F8" s="2" t="s">
         <v>190</v>
       </c>
@@ -17854,8 +18602,8 @@
       <c r="A9" s="21">
         <v>9.6999999999999993</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="19" t="s">
         <v>96</v>
       </c>
@@ -17874,8 +18622,8 @@
       <c r="A10" s="21">
         <v>9.8000000000000007</v>
       </c>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="19" t="s">
         <v>193</v>
       </c>
@@ -17894,8 +18642,8 @@
       <c r="A11" s="21">
         <v>9.9</v>
       </c>
-      <c r="B11" s="79"/>
-      <c r="C11" s="79"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="51" t="s">
         <v>233</v>
       </c>
@@ -17912,10 +18660,10 @@
     </row>
     <row r="12" spans="1:8" ht="156" x14ac:dyDescent="0.25">
       <c r="A12" s="61" t="s">
-        <v>335</v>
-      </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
+        <v>334</v>
+      </c>
+      <c r="B12" s="81"/>
+      <c r="C12" s="81"/>
       <c r="D12" s="51" t="s">
         <v>234</v>
       </c>

</xml_diff>

<commit_message>
Update test cases file for FileOperation as 'Open file or folder' feature has been added
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="945"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="961"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -19,15 +19,16 @@
     <sheet name="10.计算文件或文件夹大小" sheetId="17" r:id="rId10"/>
     <sheet name="11.解压缩rar和zip文件" sheetId="19" r:id="rId11"/>
     <sheet name="12.压缩文件或文件夹成zip文件" sheetId="20" r:id="rId12"/>
-    <sheet name="13.特殊字符测试" sheetId="15" r:id="rId13"/>
-    <sheet name="14.主界面基本功能检测" sheetId="16" r:id="rId14"/>
+    <sheet name="13.打开文件或文件夹" sheetId="21" r:id="rId13"/>
+    <sheet name="14.特殊字符测试" sheetId="15" r:id="rId14"/>
+    <sheet name="15.主界面基本功能检测" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="477">
   <si>
     <t>删除文件夹</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -13126,26 +13127,6 @@
       <t>路径</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>14.10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>14.11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>14.12</t>
-  </si>
-  <si>
-    <t>14.13</t>
-  </si>
-  <si>
-    <t>14.14</t>
-  </si>
-  <si>
-    <t>14.15</t>
   </si>
   <si>
     <t>在"Please choose :"中输入1-13以外的任何数值</t>
@@ -13551,6 +13532,272 @@
       </rPr>
       <t>)
 2.可以在本地计算机中查到新名称文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打开文件或文件夹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13.Open file or folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在"Please choose :"中输入14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>进入"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>打开文件或文件夹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"模块，并输出</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Open file or folder</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15.12</t>
+  </si>
+  <si>
+    <t>15.13</t>
+  </si>
+  <si>
+    <t>15.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15.14</t>
+  </si>
+  <si>
+    <t>15.15</t>
+  </si>
+  <si>
+    <t>15.16</t>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示出成功解压为zip文件夹，且存放所在的目录下的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Selenium配置文件\IEDriverServer-old.exe has been opened sucessfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.处于已打开的文件依然处于打开状态或者重复打开，不会出现任何报错信息</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示出成功解压为zip文件夹，且存放所在的目录下的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Selenium配置文件\IEDriverServer-old.exe has been opened sucessfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.查看到打开的指定文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示该zip文件不存在的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Selenium配置文件\IEDriverServer-old.zip is NOT exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.不会打开该文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示该zip文件不存在的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\xfmovies is NOT exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.不会打开该文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示出成功解压为zip文件夹，且存放所在的目录下的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\xfmovies has been opened sucessfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.查看到打开的指定文件夹</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示出同名zip文件夹已经存在，且不能被覆盖的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\xfmovies has been opened sucessfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.处于已打开的文件依然处于打开状态或者重复打开，不会出现任何报错信息</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -15324,6 +15571,230 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" customWidth="1"/>
+    <col min="4" max="4" width="28.75" customWidth="1"/>
+    <col min="5" max="5" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.25" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="10.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A1" s="87"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="114" x14ac:dyDescent="0.15">
+      <c r="A3" s="21">
+        <v>13.1</v>
+      </c>
+      <c r="B3" s="79" t="s">
+        <v>460</v>
+      </c>
+      <c r="C3" s="79" t="s">
+        <v>461</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="E3" s="79" t="s">
+        <v>436</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
+      <c r="A4" s="43">
+        <v>13.2</v>
+      </c>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="E4" s="80"/>
+      <c r="F4" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
+      <c r="A5" s="21">
+        <v>13.3</v>
+      </c>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="E5" s="80"/>
+      <c r="F5" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
+      <c r="A6" s="21">
+        <v>13.5</v>
+      </c>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E6" s="79" t="s">
+        <v>445</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+      <c r="A7" s="43">
+        <v>13.6</v>
+      </c>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="E7" s="80"/>
+      <c r="F7" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" ht="114" x14ac:dyDescent="0.15">
+      <c r="A8" s="21">
+        <v>13.7</v>
+      </c>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="E8" s="80"/>
+      <c r="F8" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A9" s="21">
+        <v>13.9</v>
+      </c>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="20"/>
+    </row>
+    <row r="10" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A10" s="74" t="s">
+        <v>459</v>
+      </c>
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="C3:C10"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15380,7 +15851,7 @@
     </row>
     <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A3" s="21">
-        <v>13.1</v>
+        <v>14.1</v>
       </c>
       <c r="B3" s="79" t="s">
         <v>34</v>
@@ -15404,7 +15875,7 @@
     </row>
     <row r="4" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A4" s="21">
-        <v>13.2</v>
+        <v>14.2</v>
       </c>
       <c r="B4" s="80"/>
       <c r="C4" s="80"/>
@@ -15422,7 +15893,7 @@
     </row>
     <row r="5" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A5" s="21">
-        <v>13.3</v>
+        <v>14.3</v>
       </c>
       <c r="B5" s="80"/>
       <c r="C5" s="80"/>
@@ -15440,7 +15911,7 @@
     </row>
     <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="21">
-        <v>13.4</v>
+        <v>14.4</v>
       </c>
       <c r="B6" s="80"/>
       <c r="C6" s="80"/>
@@ -15458,7 +15929,7 @@
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="21">
-        <v>13.5</v>
+        <v>14.5</v>
       </c>
       <c r="B7" s="81"/>
       <c r="C7" s="81"/>
@@ -15487,9 +15958,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -15545,7 +16016,7 @@
     </row>
     <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A3" s="41">
-        <v>14.1</v>
+        <v>15.1</v>
       </c>
       <c r="B3" s="85" t="s">
         <v>102</v>
@@ -15569,7 +16040,7 @@
     </row>
     <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A4" s="41">
-        <v>14.2</v>
+        <v>15.2</v>
       </c>
       <c r="B4" s="85"/>
       <c r="C4" s="85"/>
@@ -15587,7 +16058,7 @@
     </row>
     <row r="5" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A5" s="41">
-        <v>14.3</v>
+        <v>15.3</v>
       </c>
       <c r="B5" s="85"/>
       <c r="C5" s="85"/>
@@ -15605,7 +16076,7 @@
     </row>
     <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A6" s="41">
-        <v>14.4</v>
+        <v>15.4</v>
       </c>
       <c r="B6" s="85"/>
       <c r="C6" s="85"/>
@@ -15623,7 +16094,7 @@
     </row>
     <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A7" s="41">
-        <v>14.5</v>
+        <v>15.5</v>
       </c>
       <c r="B7" s="85"/>
       <c r="C7" s="85"/>
@@ -15641,7 +16112,7 @@
     </row>
     <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A8" s="41">
-        <v>14.6</v>
+        <v>15.6</v>
       </c>
       <c r="B8" s="85"/>
       <c r="C8" s="85"/>
@@ -15659,7 +16130,7 @@
     </row>
     <row r="9" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A9" s="41">
-        <v>14.7</v>
+        <v>15.7</v>
       </c>
       <c r="B9" s="85"/>
       <c r="C9" s="85"/>
@@ -15677,7 +16148,7 @@
     </row>
     <row r="10" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A10" s="41">
-        <v>14.8</v>
+        <v>15.8</v>
       </c>
       <c r="B10" s="85"/>
       <c r="C10" s="85"/>
@@ -15695,7 +16166,7 @@
     </row>
     <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="41">
-        <v>14.9</v>
+        <v>15.9</v>
       </c>
       <c r="B11" s="85"/>
       <c r="C11" s="85"/>
@@ -15713,7 +16184,7 @@
     </row>
     <row r="12" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="46" t="s">
-        <v>452</v>
+        <v>464</v>
       </c>
       <c r="B12" s="85"/>
       <c r="C12" s="85"/>
@@ -15731,7 +16202,7 @@
     </row>
     <row r="13" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A13" s="46" t="s">
-        <v>453</v>
+        <v>467</v>
       </c>
       <c r="B13" s="85"/>
       <c r="C13" s="85"/>
@@ -15749,7 +16220,7 @@
     </row>
     <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A14" s="46" t="s">
-        <v>454</v>
+        <v>465</v>
       </c>
       <c r="B14" s="85"/>
       <c r="C14" s="85"/>
@@ -15767,7 +16238,7 @@
     </row>
     <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A15" s="46" t="s">
-        <v>455</v>
+        <v>466</v>
       </c>
       <c r="B15" s="85"/>
       <c r="C15" s="85"/>
@@ -15776,7 +16247,7 @@
         <v>429</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>141</v>
+        <v>463</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>20</v>
@@ -15785,31 +16256,29 @@
     </row>
     <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A16" s="46" t="s">
-        <v>456</v>
+        <v>468</v>
       </c>
       <c r="B16" s="85"/>
       <c r="C16" s="85"/>
       <c r="D16" s="85"/>
       <c r="E16" s="2" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>98</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A17" s="46" t="s">
-        <v>457</v>
+        <v>469</v>
       </c>
       <c r="B17" s="85"/>
       <c r="C17" s="85"/>
       <c r="D17" s="85"/>
       <c r="E17" s="2" t="s">
-        <v>107</v>
+        <v>452</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>108</v>
@@ -15818,13 +16287,31 @@
         <v>98</v>
       </c>
       <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A18" s="46" t="s">
+        <v>470</v>
+      </c>
+      <c r="B18" s="85"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H18" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:B17"/>
-    <mergeCell ref="C3:C17"/>
-    <mergeCell ref="D3:D17"/>
+    <mergeCell ref="B3:B18"/>
+    <mergeCell ref="C3:C18"/>
+    <mergeCell ref="D3:D18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16311,10 +16798,10 @@
         <v>228</v>
       </c>
       <c r="E3" s="76" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>20</v>
@@ -16370,7 +16857,7 @@
         <v>296</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>20</v>
@@ -17943,10 +18430,10 @@
         <v>228</v>
       </c>
       <c r="E3" s="76" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>20</v>
@@ -18002,7 +18489,7 @@
         <v>296</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>98</v>
@@ -18585,7 +19072,7 @@
         <v>307</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Update the test case file of FileOperation to update function 13
</commit_message>
<xml_diff>
--- a/src/MyItems/Documents/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Documents/Test Cases for FileOperation.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Update codes\1229_new\Afternoon\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="48" windowWidth="5352" windowHeight="7608" tabRatio="961"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="961"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -13470,8 +13465,924 @@
   </si>
   <si>
     <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input folder or file path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:" 输入被复制文件夹的路径，如:D:\Test
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\python经典100例.zip</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.提示“目标路径为文件路径，不能复制到该路径下，请重新输入”（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cannot copy to file path E:\python经典100例.zip please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件夹不应把该复制到指定路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.1.10</t>
+  </si>
+  <si>
+    <t>4.1.11</t>
+  </si>
+  <si>
+    <t>4.1.12</t>
+  </si>
+  <si>
+    <t>4.1.13</t>
+  </si>
+  <si>
+    <t>4.1.14</t>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被复制的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>任何文件夹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的文件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>目标路径
+2.输入被复制文件夹路径和目标文件路径</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input folder or file path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:" 输入被复制文件夹的路径，如:D:\Test\Alonso.txt
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\python经典100例.zip</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.提示“目标路径为文件路径，不能复制到该路径下，请重新输入”（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cannot copy to file path E:\python经典100例.zip please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件不应把该复制到指定路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被复制的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>任何文件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的文件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>目标路径
+2.输入被复制文件夹路径和目标文件路径</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.2.10</t>
+  </si>
+  <si>
+    <t>4.2.11</t>
+  </si>
+  <si>
+    <t>4.2.12</t>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被复制文件的路径和目标路径已经</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的同名</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件，尝试覆盖操作
+2.输入被移动文件路径和目标文件夹路径</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">        </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被移动文件的路径，尝试覆盖操作
+2.被移动文件路径和目标文件路径均输入同一个路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被复制的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>任何文件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的文件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>目标路径
+2.输入被移动文件夹路径和目标文件路径</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示输入需要被移动文件夹或者文件路径时，输入空字符</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.10</t>
+  </si>
+  <si>
+    <t>5.1.11</t>
+  </si>
+  <si>
+    <t>5.1.12</t>
+  </si>
+  <si>
+    <r>
+      <t>1.提示“目标路径为文件路径，不能移动到该路径下，请重新输入”（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cannot move to file path E:\python经典100例.zip please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件不应把该移动到指定路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被复制的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>任何文件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的文件夹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>目标路径
+2.输入被移动文件夹路径和目标文件路径</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input folder or file path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:" 输入被复制文件的路径，如:D:\Test\Alonso.txt
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\python经典100例.zip</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input folder or file path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:" 输入被移动文件夹的路径，如:D:\Test
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:",输入需要移动到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\python经典100例.zip</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.2.10</t>
+  </si>
+  <si>
+    <t>5.2.11</t>
+  </si>
+  <si>
+    <t>5.2.12</t>
+  </si>
+  <si>
+    <t>5.2.13</t>
+  </si>
+  <si>
+    <t>5.2.14</t>
+  </si>
+  <si>
+    <r>
       <t>1.能够出现提示输入的信息
-2.显示出成功解压为zip文件夹，且存放所在的目录下的信息（</t>
+2.显示该文件不存在打开的消息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Selenium配置文件\IEDriverServer-old.zip is NOT exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.不会打开该文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示该文件被成功打开的消息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Selenium配置文件\IEDriverServer-old.exe has been opened sucessfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.查看到打开的指定文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示该文件夹被成功打开的消息（</t>
     </r>
     <r>
       <rPr>
@@ -13502,19 +14413,19 @@
   <si>
     <r>
       <t>1.能够出现提示输入的信息
-2.显示出成功解压为zip文件夹，且存放所在的目录下的信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\Selenium配置文件\IEDriverServer-old.exe has been opened sucessfully!</t>
+2.显示该文件夹被成功打开的消息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\xfmovies has been opened sucessfully!</t>
     </r>
     <r>
       <rPr>
@@ -13526,26 +14437,26 @@
         <scheme val="minor"/>
       </rPr>
       <t>）
-3.查看到打开的指定文件</t>
+3.查看到打开的指定文件夹</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
       <t>1.能够出现提示输入的信息
-2.显示该zip文件不存在的信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\Selenium配置文件\IEDriverServer-old.zip is NOT exist!</t>
+2.显示该文件夹不存在的消息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\xfmovies is NOT exist!</t>
     </r>
     <r>
       <rPr>
@@ -13564,69 +14475,7 @@
   <si>
     <r>
       <t>1.能够出现提示输入的信息
-2.显示该zip文件不存在的信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\xfmovies is NOT exist!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-3.不会打开该文件</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.能够出现提示输入的信息
-2.显示出成功解压为zip文件夹，且存放所在的目录下的信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\xfmovies has been opened sucessfully!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-3.查看到打开的指定文件夹</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.能够出现提示输入的信息
-2.显示出同名zip文件夹已经存在，且不能被覆盖的信息（</t>
+2.显示该文件被成功打开的消息（</t>
     </r>
     <r>
       <rPr>
@@ -13653,866 +14502,12 @@
 3.处于已打开的文件依然处于打开状态或者重复打开，不会出现任何报错信息</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input folder or file path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:" 输入被复制文件夹的路径，如:D:\Test
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input target folder path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:",输入需要复制到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\python经典100例.zip</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.提示“目标路径为文件路径，不能复制到该路径下，请重新输入”（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cannot copy to file path E:\python经典100例.zip please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件夹不应把该复制到指定路径</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.1.10</t>
-  </si>
-  <si>
-    <t>4.1.11</t>
-  </si>
-  <si>
-    <t>4.1.12</t>
-  </si>
-  <si>
-    <t>4.1.13</t>
-  </si>
-  <si>
-    <t>4.1.14</t>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>需要被复制的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>任何文件夹</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的路径和</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的文件</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>目标路径
-2.输入被复制文件夹路径和目标文件路径</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input folder or file path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:" 输入被复制文件夹的路径，如:D:\Test\Alonso.txt
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input target folder path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:",输入需要复制到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\python经典100例.zip</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.提示“目标路径为文件路径，不能复制到该路径下，请重新输入”（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cannot copy to file path E:\python经典100例.zip please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件不应把该复制到指定路径</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>需要被复制的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>任何文件</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的路径和</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的文件</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>目标路径
-2.输入被复制文件夹路径和目标文件路径</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.2.10</t>
-  </si>
-  <si>
-    <t>4.2.11</t>
-  </si>
-  <si>
-    <t>4.2.12</t>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>需要被复制文件的路径和目标路径已经</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的同名</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件，尝试覆盖操作
-2.输入被移动文件路径和目标文件夹路径</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">        </t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>需要被移动文件的路径，尝试覆盖操作
-2.被移动文件路径和目标文件路径均输入同一个路径</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>需要被复制的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>任何文件</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的路径和</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的文件</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>目标路径
-2.输入被移动文件夹路径和目标文件路径</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>提示输入需要被移动文件夹或者文件路径时，输入空字符</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.1.10</t>
-  </si>
-  <si>
-    <t>5.1.11</t>
-  </si>
-  <si>
-    <t>5.1.12</t>
-  </si>
-  <si>
-    <r>
-      <t>1.提示“目标路径为文件路径，不能移动到该路径下，请重新输入”（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cannot move to file path E:\python经典100例.zip please input again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件不应把该移动到指定路径</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>需要被复制的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>任何文件</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的路径和</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的文件夹</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>目标路径
-2.输入被移动文件夹路径和目标文件路径</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input folder or file path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:" 输入被复制文件的路径，如:D:\Test\Alonso.txt
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input target folder path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:",输入需要复制到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\python经典100例.zip</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input folder or file path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:" 输入被移动文件夹的路径，如:D:\Test
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input target folder path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:",输入需要移动到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\python经典100例.zip</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.2.10</t>
-  </si>
-  <si>
-    <t>5.2.11</t>
-  </si>
-  <si>
-    <t>5.2.12</t>
-  </si>
-  <si>
-    <t>5.2.13</t>
-  </si>
-  <si>
-    <t>5.2.14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -15101,7 +15096,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -15134,26 +15129,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -15186,23 +15164,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -15385,20 +15346,20 @@
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="53" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="53" customWidth="1"/>
-    <col min="3" max="3" width="23.88671875" style="53" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" style="53" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.88671875" style="53" customWidth="1"/>
-    <col min="6" max="6" width="41.6640625" style="53" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="53" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" style="53" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.875" style="53" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.375" style="53" customWidth="1"/>
+    <col min="3" max="3" width="23.875" style="53" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.625" style="53" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.875" style="53" customWidth="1"/>
+    <col min="6" max="6" width="41.625" style="53" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="53" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.375" style="53" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A1" s="74"/>
       <c r="B1" s="74"/>
       <c r="C1" s="74"/>
@@ -15408,7 +15369,7 @@
       <c r="G1" s="74"/>
       <c r="H1" s="74"/>
     </row>
-    <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -15434,7 +15395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="21">
         <v>1.1000000000000001</v>
       </c>
@@ -15458,7 +15419,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A4" s="21">
         <v>1.2</v>
       </c>
@@ -15476,7 +15437,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A5" s="21">
         <v>1.3</v>
       </c>
@@ -15494,7 +15455,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="21">
         <v>1.4</v>
       </c>
@@ -15512,7 +15473,7 @@
       </c>
       <c r="H6" s="54"/>
     </row>
-    <row r="7" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A7" s="21">
         <v>1.5</v>
       </c>
@@ -15530,7 +15491,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="54"/>
     </row>
-    <row r="8" spans="1:8" s="55" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="55" customFormat="1" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A8" s="25">
         <v>1.6</v>
       </c>
@@ -15550,7 +15511,7 @@
       </c>
       <c r="H8" s="20"/>
     </row>
-    <row r="9" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A9" s="25">
         <v>1.7</v>
       </c>
@@ -15570,7 +15531,7 @@
       </c>
       <c r="H9" s="20"/>
     </row>
-    <row r="10" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A10" s="52">
         <v>1.8</v>
       </c>
@@ -15588,7 +15549,7 @@
       <c r="G10" s="56"/>
       <c r="H10" s="56"/>
     </row>
-    <row r="11" spans="1:8" ht="156" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A11" s="57">
         <v>1.9</v>
       </c>
@@ -15627,19 +15588,19 @@
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="28.77734375" customWidth="1"/>
-    <col min="5" max="5" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" customWidth="1"/>
+    <col min="4" max="4" width="28.75" customWidth="1"/>
+    <col min="5" max="5" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.25" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A1" s="86"/>
       <c r="B1" s="86"/>
       <c r="C1" s="86"/>
@@ -15649,7 +15610,7 @@
       <c r="G1" s="86"/>
       <c r="H1" s="86"/>
     </row>
-    <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -15675,7 +15636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A3" s="21">
         <v>10.1</v>
       </c>
@@ -15699,7 +15660,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A4" s="43">
         <v>10.199999999999999</v>
       </c>
@@ -15717,7 +15678,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A5" s="43">
         <v>10.3</v>
       </c>
@@ -15737,7 +15698,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A6" s="44">
         <v>10.4</v>
       </c>
@@ -15755,7 +15716,7 @@
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A7" s="45">
         <v>10.5</v>
       </c>
@@ -15775,7 +15736,7 @@
       </c>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A8" s="45">
         <v>10.6</v>
       </c>
@@ -15817,19 +15778,19 @@
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="28.77734375" customWidth="1"/>
-    <col min="5" max="5" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" customWidth="1"/>
+    <col min="4" max="4" width="28.75" customWidth="1"/>
+    <col min="5" max="5" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.25" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A1" s="86"/>
       <c r="B1" s="86"/>
       <c r="C1" s="86"/>
@@ -15839,7 +15800,7 @@
       <c r="G1" s="86"/>
       <c r="H1" s="86"/>
     </row>
-    <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -15865,7 +15826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A3" s="21">
         <v>11.1</v>
       </c>
@@ -15889,7 +15850,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A4" s="43">
         <v>11.2</v>
       </c>
@@ -15907,7 +15868,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A5" s="43">
         <v>11.3</v>
       </c>
@@ -15923,7 +15884,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A6" s="43">
         <v>11.4</v>
       </c>
@@ -15943,7 +15904,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A7" s="44">
         <v>11.5</v>
       </c>
@@ -15961,7 +15922,7 @@
       </c>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A8" s="44">
         <v>11.6</v>
       </c>
@@ -15977,7 +15938,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A9" s="44">
         <v>11.7</v>
       </c>
@@ -15997,7 +15958,7 @@
       </c>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A10" s="45">
         <v>11.8</v>
       </c>
@@ -16017,7 +15978,7 @@
       </c>
       <c r="H10" s="20"/>
     </row>
-    <row r="11" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="45">
         <v>11.9</v>
       </c>
@@ -16058,19 +16019,19 @@
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="28.77734375" customWidth="1"/>
-    <col min="5" max="5" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" customWidth="1"/>
+    <col min="4" max="4" width="28.75" customWidth="1"/>
+    <col min="5" max="5" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.25" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A1" s="86"/>
       <c r="B1" s="86"/>
       <c r="C1" s="86"/>
@@ -16080,7 +16041,7 @@
       <c r="G1" s="86"/>
       <c r="H1" s="86"/>
     </row>
-    <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -16106,7 +16067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="156" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A3" s="21">
         <v>12.1</v>
       </c>
@@ -16130,7 +16091,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A4" s="43">
         <v>12.2</v>
       </c>
@@ -16148,7 +16109,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A5" s="21">
         <v>12.3</v>
       </c>
@@ -16164,7 +16125,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="156" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A6" s="43">
         <v>12.4</v>
       </c>
@@ -16180,7 +16141,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A7" s="21">
         <v>12.5</v>
       </c>
@@ -16200,7 +16161,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A8" s="43">
         <v>12.6</v>
       </c>
@@ -16218,7 +16179,7 @@
       </c>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A9" s="21">
         <v>12.7</v>
       </c>
@@ -16236,7 +16197,7 @@
       </c>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A10" s="43">
         <v>12.8</v>
       </c>
@@ -16254,7 +16215,7 @@
       </c>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A11" s="21">
         <v>12.9</v>
       </c>
@@ -16274,7 +16235,7 @@
       </c>
       <c r="H11" s="20"/>
     </row>
-    <row r="12" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="72" t="s">
         <v>327</v>
       </c>
@@ -16315,19 +16276,19 @@
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="28.77734375" customWidth="1"/>
-    <col min="5" max="5" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" customWidth="1"/>
+    <col min="4" max="4" width="28.75" customWidth="1"/>
+    <col min="5" max="5" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.25" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A1" s="86"/>
       <c r="B1" s="86"/>
       <c r="C1" s="86"/>
@@ -16337,7 +16298,7 @@
       <c r="G1" s="86"/>
       <c r="H1" s="86"/>
     </row>
-    <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -16363,7 +16324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="21">
         <v>13.1</v>
       </c>
@@ -16380,14 +16341,14 @@
         <v>422</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>458</v>
+        <v>488</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A4" s="43">
         <v>13.2</v>
       </c>
@@ -16398,14 +16359,14 @@
       </c>
       <c r="E4" s="79"/>
       <c r="F4" s="2" t="s">
-        <v>459</v>
+        <v>487</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>20</v>
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="140.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A5" s="21">
         <v>13.3</v>
       </c>
@@ -16416,12 +16377,12 @@
       </c>
       <c r="E5" s="79"/>
       <c r="F5" s="2" t="s">
-        <v>457</v>
+        <v>489</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A6" s="21">
         <v>13.5</v>
       </c>
@@ -16434,14 +16395,14 @@
         <v>431</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>461</v>
+        <v>490</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A7" s="43">
         <v>13.6</v>
       </c>
@@ -16452,14 +16413,14 @@
       </c>
       <c r="E7" s="79"/>
       <c r="F7" s="2" t="s">
-        <v>460</v>
+        <v>491</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>20</v>
       </c>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A8" s="21">
         <v>13.7</v>
       </c>
@@ -16470,14 +16431,14 @@
       </c>
       <c r="E8" s="79"/>
       <c r="F8" s="2" t="s">
-        <v>462</v>
+        <v>492</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>20</v>
       </c>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A9" s="21">
         <v>13.9</v>
       </c>
@@ -16497,7 +16458,7 @@
       </c>
       <c r="H9" s="20"/>
     </row>
-    <row r="10" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A10" s="72" t="s">
         <v>445</v>
       </c>
@@ -16539,19 +16500,19 @@
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37" customWidth="1"/>
     <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A1" s="86"/>
       <c r="B1" s="86"/>
       <c r="C1" s="86"/>
@@ -16561,7 +16522,7 @@
       <c r="G1" s="86"/>
       <c r="H1" s="86"/>
     </row>
-    <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -16587,7 +16548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A3" s="21">
         <v>14.1</v>
       </c>
@@ -16611,7 +16572,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A4" s="21">
         <v>14.2</v>
       </c>
@@ -16629,7 +16590,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A5" s="21">
         <v>14.3</v>
       </c>
@@ -16647,7 +16608,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="21">
         <v>14.4</v>
       </c>
@@ -16665,7 +16626,7 @@
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="21">
         <v>14.5</v>
       </c>
@@ -16704,19 +16665,19 @@
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="13.875" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.875" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="28.33203125" customWidth="1"/>
-    <col min="5" max="5" width="31.77734375" customWidth="1"/>
-    <col min="6" max="6" width="31.109375" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="28.375" customWidth="1"/>
+    <col min="5" max="5" width="31.75" customWidth="1"/>
+    <col min="6" max="6" width="31.125" customWidth="1"/>
+    <col min="7" max="7" width="10.625" customWidth="1"/>
+    <col min="8" max="8" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A1" s="86"/>
       <c r="B1" s="86"/>
       <c r="C1" s="86"/>
@@ -16726,7 +16687,7 @@
       <c r="G1" s="86"/>
       <c r="H1" s="86"/>
     </row>
-    <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="40" t="s">
         <v>19</v>
       </c>
@@ -16752,7 +16713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A3" s="41">
         <v>15.1</v>
       </c>
@@ -16776,7 +16737,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A4" s="41">
         <v>15.2</v>
       </c>
@@ -16794,7 +16755,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A5" s="41">
         <v>15.3</v>
       </c>
@@ -16812,7 +16773,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A6" s="41">
         <v>15.4</v>
       </c>
@@ -16830,7 +16791,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A7" s="41">
         <v>15.5</v>
       </c>
@@ -16848,7 +16809,7 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A8" s="41">
         <v>15.6</v>
       </c>
@@ -16866,7 +16827,7 @@
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A9" s="41">
         <v>15.7</v>
       </c>
@@ -16884,7 +16845,7 @@
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A10" s="41">
         <v>15.8</v>
       </c>
@@ -16902,7 +16863,7 @@
       </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="41">
         <v>15.9</v>
       </c>
@@ -16920,7 +16881,7 @@
       </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="46" t="s">
         <v>450</v>
       </c>
@@ -16938,7 +16899,7 @@
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A13" s="46" t="s">
         <v>453</v>
       </c>
@@ -16956,7 +16917,7 @@
       </c>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A14" s="46" t="s">
         <v>451</v>
       </c>
@@ -16974,7 +16935,7 @@
       </c>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A15" s="46" t="s">
         <v>452</v>
       </c>
@@ -16992,7 +16953,7 @@
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A16" s="46" t="s">
         <v>454</v>
       </c>
@@ -17008,7 +16969,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A17" s="46" t="s">
         <v>455</v>
       </c>
@@ -17026,7 +16987,7 @@
       </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A18" s="46" t="s">
         <v>456</v>
       </c>
@@ -17065,20 +17026,20 @@
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="36.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="36.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17.45" x14ac:dyDescent="0.25">
       <c r="A1" s="81"/>
       <c r="B1" s="81"/>
       <c r="C1" s="81"/>
@@ -17088,7 +17049,7 @@
       <c r="G1" s="81"/>
       <c r="H1" s="81"/>
     </row>
-    <row r="2" spans="1:9" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -17114,7 +17075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="218.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="171" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>85</v>
       </c>
@@ -17138,7 +17099,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="202.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="171" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>86</v>
       </c>
@@ -17158,7 +17119,7 @@
       </c>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="1:9" ht="78" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>87</v>
       </c>
@@ -17178,7 +17139,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A6" s="19" t="s">
         <v>92</v>
       </c>
@@ -17198,7 +17159,7 @@
       </c>
       <c r="H6" s="20"/>
     </row>
-    <row r="7" spans="1:9" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="57" x14ac:dyDescent="0.15">
       <c r="A7" s="25" t="s">
         <v>189</v>
       </c>
@@ -17218,7 +17179,7 @@
       </c>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -17229,7 +17190,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -17256,7 +17217,7 @@
       </c>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="202.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="171" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>88</v>
       </c>
@@ -17281,7 +17242,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="218.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="171" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>89</v>
       </c>
@@ -17302,7 +17263,7 @@
       <c r="H11" s="13"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="78" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>90</v>
       </c>
@@ -17323,7 +17284,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" s="22" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="22" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A13" s="19" t="s">
         <v>91</v>
       </c>
@@ -17343,7 +17304,7 @@
       </c>
       <c r="H13" s="20"/>
     </row>
-    <row r="14" spans="1:9" s="22" customFormat="1" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="22" customFormat="1" ht="57" x14ac:dyDescent="0.15">
       <c r="A14" s="25" t="s">
         <v>191</v>
       </c>
@@ -17363,7 +17324,7 @@
       </c>
       <c r="H14" s="20"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="82"/>
       <c r="C15" s="4"/>
@@ -17374,7 +17335,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="82"/>
       <c r="C16" s="4"/>
@@ -17385,7 +17346,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="82"/>
       <c r="C17" s="4"/>
@@ -17396,7 +17357,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="82"/>
       <c r="C18" s="4"/>
@@ -17407,7 +17368,7 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="82"/>
       <c r="C19" s="4"/>
@@ -17418,7 +17379,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -17429,7 +17390,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -17440,7 +17401,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="10"/>
       <c r="D22" s="3"/>
@@ -17473,20 +17434,20 @@
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="68" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="68" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="68" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.875" style="68" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.625" style="68" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" style="68" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" style="68" customWidth="1"/>
-    <col min="5" max="5" width="26.77734375" style="68" customWidth="1"/>
+    <col min="5" max="5" width="26.75" style="68" customWidth="1"/>
     <col min="6" max="6" width="38" style="68" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="68" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" style="68" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="68" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="68" customWidth="1"/>
     <col min="9" max="16384" width="9" style="68"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A1" s="83"/>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
@@ -17496,7 +17457,7 @@
       <c r="G1" s="83"/>
       <c r="H1" s="83"/>
     </row>
-    <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -17522,7 +17483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="356.25" x14ac:dyDescent="0.15">
       <c r="A3" s="21">
         <v>3.1</v>
       </c>
@@ -17546,7 +17507,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="21">
         <v>3.2</v>
       </c>
@@ -17564,7 +17525,7 @@
       </c>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="1:8" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A5" s="21">
         <v>3.3</v>
       </c>
@@ -17582,7 +17543,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="327.75" x14ac:dyDescent="0.15">
       <c r="A6" s="21">
         <v>3.4</v>
       </c>
@@ -17602,7 +17563,7 @@
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A7" s="21">
         <v>3.5</v>
       </c>
@@ -17620,7 +17581,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" s="70" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="70" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A8" s="21">
         <v>3.6</v>
       </c>
@@ -17640,7 +17601,7 @@
       </c>
       <c r="H8" s="20"/>
     </row>
-    <row r="9" spans="1:8" s="70" customFormat="1" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="70" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A9" s="21">
         <v>3.7</v>
       </c>
@@ -17660,7 +17621,7 @@
       </c>
       <c r="H9" s="20"/>
     </row>
-    <row r="10" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A10" s="21">
         <v>3.8</v>
       </c>
@@ -17680,7 +17641,7 @@
       </c>
       <c r="H10" s="56"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -17690,7 +17651,7 @@
       <c r="G11" s="9"/>
       <c r="H11" s="66"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -17700,7 +17661,7 @@
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -17710,7 +17671,7 @@
       <c r="G13" s="67"/>
       <c r="H13" s="67"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -17720,7 +17681,7 @@
       <c r="G14" s="67"/>
       <c r="H14" s="67"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B17" s="69"/>
     </row>
   </sheetData>
@@ -17744,15 +17705,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="52.21875" customWidth="1"/>
+    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="52.25" customWidth="1"/>
     <col min="6" max="6" width="42" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.109375" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
@@ -17765,7 +17726,7 @@
       <c r="G1" s="85"/>
       <c r="H1" s="85"/>
     </row>
-    <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -17791,7 +17752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="156" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>123</v>
       </c>
@@ -17815,7 +17776,7 @@
       </c>
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="1:8" ht="156" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>124</v>
       </c>
@@ -17833,7 +17794,7 @@
       </c>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>369</v>
       </c>
@@ -17851,7 +17812,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>370</v>
       </c>
@@ -17869,7 +17830,7 @@
       </c>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>371</v>
       </c>
@@ -17887,7 +17848,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="140.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>372</v>
       </c>
@@ -17905,7 +17866,7 @@
       </c>
       <c r="H8" s="15"/>
     </row>
-    <row r="9" spans="1:8" ht="140.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>373</v>
       </c>
@@ -17923,7 +17884,7 @@
       </c>
       <c r="H9" s="15"/>
     </row>
-    <row r="10" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>374</v>
       </c>
@@ -17941,29 +17902,29 @@
       </c>
       <c r="H10" s="35"/>
     </row>
-    <row r="11" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>375</v>
       </c>
       <c r="B11" s="79"/>
       <c r="C11" s="79"/>
       <c r="D11" s="33" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="E11" s="73" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="F11" s="34" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="G11" s="35" t="s">
         <v>20</v>
       </c>
       <c r="H11" s="35"/>
     </row>
-    <row r="12" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="B12" s="79"/>
       <c r="C12" s="79"/>
@@ -17981,9 +17942,9 @@
       </c>
       <c r="H12" s="20"/>
     </row>
-    <row r="13" spans="1:8" s="22" customFormat="1" ht="156" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="22" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="B13" s="79"/>
       <c r="C13" s="79"/>
@@ -18001,9 +17962,9 @@
       </c>
       <c r="H13" s="24"/>
     </row>
-    <row r="14" spans="1:8" s="22" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="22" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="B14" s="79"/>
       <c r="C14" s="79"/>
@@ -18021,9 +17982,9 @@
       </c>
       <c r="H14" s="20"/>
     </row>
-    <row r="15" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="B15" s="79"/>
       <c r="C15" s="79"/>
@@ -18041,9 +18002,9 @@
       </c>
       <c r="H15" s="20"/>
     </row>
-    <row r="16" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="B16" s="80"/>
       <c r="C16" s="80"/>
@@ -18061,7 +18022,7 @@
       </c>
       <c r="H16" s="63"/>
     </row>
-    <row r="18" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -18087,7 +18048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="156" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A19" s="14" t="s">
         <v>125</v>
       </c>
@@ -18111,7 +18072,7 @@
       </c>
       <c r="H19" s="14"/>
     </row>
-    <row r="20" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A20" s="14" t="s">
         <v>126</v>
       </c>
@@ -18129,7 +18090,7 @@
       </c>
       <c r="H20" s="14"/>
     </row>
-    <row r="21" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A21" s="14" t="s">
         <v>376</v>
       </c>
@@ -18147,7 +18108,7 @@
       </c>
       <c r="H21" s="14"/>
     </row>
-    <row r="22" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A22" s="14" t="s">
         <v>377</v>
       </c>
@@ -18165,7 +18126,7 @@
       </c>
       <c r="H22" s="14"/>
     </row>
-    <row r="23" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A23" s="14" t="s">
         <v>378</v>
       </c>
@@ -18183,7 +18144,7 @@
       </c>
       <c r="H23" s="16"/>
     </row>
-    <row r="24" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A24" s="14" t="s">
         <v>379</v>
       </c>
@@ -18201,27 +18162,27 @@
       </c>
       <c r="H24" s="35"/>
     </row>
-    <row r="25" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A25" s="14" t="s">
         <v>380</v>
       </c>
       <c r="B25" s="79"/>
       <c r="C25" s="79"/>
       <c r="D25" s="33" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="E25" s="73" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="G25" s="35" t="s">
         <v>20</v>
       </c>
       <c r="H25" s="35"/>
     </row>
-    <row r="26" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A26" s="14" t="s">
         <v>381</v>
       </c>
@@ -18241,7 +18202,7 @@
       </c>
       <c r="H26" s="20"/>
     </row>
-    <row r="27" spans="1:8" ht="156" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A27" s="14" t="s">
         <v>382</v>
       </c>
@@ -18261,9 +18222,9 @@
       </c>
       <c r="H27" s="20"/>
     </row>
-    <row r="28" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A28" s="14" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="B28" s="79"/>
       <c r="C28" s="79"/>
@@ -18281,9 +18242,9 @@
       </c>
       <c r="H28" s="20"/>
     </row>
-    <row r="29" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A29" s="14" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="B29" s="79"/>
       <c r="C29" s="79"/>
@@ -18301,9 +18262,9 @@
       </c>
       <c r="H29" s="20"/>
     </row>
-    <row r="30" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A30" s="14" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="B30" s="80"/>
       <c r="C30" s="80"/>
@@ -18345,19 +18306,19 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.44140625" customWidth="1"/>
-    <col min="5" max="5" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5" customWidth="1"/>
+    <col min="5" max="5" width="59.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A1" s="86"/>
       <c r="B1" s="86"/>
       <c r="C1" s="86"/>
@@ -18367,7 +18328,7 @@
       <c r="G1" s="86"/>
       <c r="H1" s="86"/>
     </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -18393,7 +18354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="22" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="22" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>350</v>
       </c>
@@ -18417,7 +18378,7 @@
       </c>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" s="22" customFormat="1" ht="78" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>351</v>
       </c>
@@ -18435,7 +18396,7 @@
       </c>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" s="22" customFormat="1" ht="124.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="22" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>352</v>
       </c>
@@ -18453,7 +18414,7 @@
       </c>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" s="22" customFormat="1" ht="78" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
         <v>353</v>
       </c>
@@ -18471,14 +18432,14 @@
       </c>
       <c r="H6" s="23"/>
     </row>
-    <row r="7" spans="1:8" s="22" customFormat="1" ht="187.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="22" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
         <v>354</v>
       </c>
       <c r="B7" s="91"/>
       <c r="C7" s="91"/>
       <c r="D7" s="27" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="E7" s="88"/>
       <c r="F7" s="27" t="s">
@@ -18489,14 +18450,14 @@
       </c>
       <c r="H7" s="29"/>
     </row>
-    <row r="8" spans="1:8" s="22" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>355</v>
       </c>
       <c r="B8" s="91"/>
       <c r="C8" s="91"/>
       <c r="D8" s="33" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="E8" s="89"/>
       <c r="F8" s="34" t="s">
@@ -18507,34 +18468,34 @@
       </c>
       <c r="H8" s="37"/>
     </row>
-    <row r="9" spans="1:8" s="22" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
         <v>356</v>
       </c>
       <c r="B9" s="91"/>
       <c r="C9" s="91"/>
       <c r="D9" s="33" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="E9" s="73" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="G9" s="35" t="s">
         <v>20</v>
       </c>
       <c r="H9" s="35"/>
     </row>
-    <row r="10" spans="1:8" s="22" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
         <v>357</v>
       </c>
       <c r="B10" s="91"/>
       <c r="C10" s="91"/>
       <c r="D10" s="19" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>278</v>
@@ -18547,7 +18508,7 @@
       </c>
       <c r="H10" s="20"/>
     </row>
-    <row r="11" spans="1:8" s="31" customFormat="1" ht="156" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="31" customFormat="1" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
         <v>358</v>
       </c>
@@ -18567,9 +18528,9 @@
       </c>
       <c r="H11" s="24"/>
     </row>
-    <row r="12" spans="1:8" s="31" customFormat="1" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="31" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="B12" s="91"/>
       <c r="C12" s="91"/>
@@ -18587,9 +18548,9 @@
       </c>
       <c r="H12" s="20"/>
     </row>
-    <row r="13" spans="1:8" s="31" customFormat="1" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="31" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="B13" s="91"/>
       <c r="C13" s="91"/>
@@ -18607,9 +18568,9 @@
       </c>
       <c r="H13" s="20"/>
     </row>
-    <row r="14" spans="1:8" s="31" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="31" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="B14" s="92"/>
       <c r="C14" s="92"/>
@@ -18627,7 +18588,7 @@
       </c>
       <c r="H14" s="64"/>
     </row>
-    <row r="15" spans="1:8" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="31" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -18636,7 +18597,7 @@
       <c r="F15" s="9"/>
       <c r="H15" s="32"/>
     </row>
-    <row r="16" spans="1:8" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="31" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -18662,7 +18623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>359</v>
       </c>
@@ -18686,7 +18647,7 @@
       </c>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>360</v>
       </c>
@@ -18704,7 +18665,7 @@
       </c>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>361</v>
       </c>
@@ -18722,7 +18683,7 @@
       </c>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>362</v>
       </c>
@@ -18740,7 +18701,7 @@
       </c>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>363</v>
       </c>
@@ -18758,7 +18719,7 @@
       </c>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:8" s="22" customFormat="1" ht="140.4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="22" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>364</v>
       </c>
@@ -18776,7 +18737,7 @@
       </c>
       <c r="H22" s="16"/>
     </row>
-    <row r="23" spans="1:8" s="22" customFormat="1" ht="140.4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="22" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>365</v>
       </c>
@@ -18794,7 +18755,7 @@
       </c>
       <c r="H23" s="16"/>
     </row>
-    <row r="24" spans="1:8" s="22" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>366</v>
       </c>
@@ -18812,29 +18773,29 @@
       </c>
       <c r="H24" s="39"/>
     </row>
-    <row r="25" spans="1:8" s="22" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>367</v>
       </c>
       <c r="B25" s="79"/>
       <c r="C25" s="91"/>
       <c r="D25" s="33" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="E25" s="73" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="G25" s="35" t="s">
         <v>20</v>
       </c>
       <c r="H25" s="35"/>
     </row>
-    <row r="26" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="B26" s="79"/>
       <c r="C26" s="91"/>
@@ -18852,9 +18813,9 @@
       </c>
       <c r="H26" s="20"/>
     </row>
-    <row r="27" spans="1:8" ht="156" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="B27" s="79"/>
       <c r="C27" s="91"/>
@@ -18872,9 +18833,9 @@
       </c>
       <c r="H27" s="20"/>
     </row>
-    <row r="28" spans="1:8" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="B28" s="79"/>
       <c r="C28" s="91"/>
@@ -18892,9 +18853,9 @@
       </c>
       <c r="H28" s="20"/>
     </row>
-    <row r="29" spans="1:8" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="B29" s="79"/>
       <c r="C29" s="91"/>
@@ -18912,9 +18873,9 @@
       </c>
       <c r="H29" s="20"/>
     </row>
-    <row r="30" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="B30" s="80"/>
       <c r="C30" s="92"/>
@@ -18956,20 +18917,20 @@
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="58" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="58" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.88671875" style="58" customWidth="1"/>
-    <col min="5" max="5" width="34.21875" style="58" customWidth="1"/>
+    <col min="1" max="1" width="13.875" style="58" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.125" style="58" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" style="58" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.875" style="58" customWidth="1"/>
+    <col min="5" max="5" width="34.25" style="58" customWidth="1"/>
     <col min="6" max="6" width="34" style="58" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.88671875" style="58" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="58" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.875" style="58" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A1" s="93"/>
       <c r="B1" s="93"/>
       <c r="C1" s="93"/>
@@ -18979,7 +18940,7 @@
       <c r="G1" s="93"/>
       <c r="H1" s="93"/>
     </row>
-    <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>19</v>
       </c>
@@ -19005,7 +18966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A3" s="21">
         <v>6.1</v>
       </c>
@@ -19029,7 +18990,7 @@
       </c>
       <c r="H3" s="59"/>
     </row>
-    <row r="4" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A4" s="21">
         <v>6.2</v>
       </c>
@@ -19047,7 +19008,7 @@
       </c>
       <c r="H4" s="59"/>
     </row>
-    <row r="5" spans="1:8" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A5" s="21">
         <v>6.3</v>
       </c>
@@ -19065,7 +19026,7 @@
       </c>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="21">
         <v>6.4</v>
       </c>
@@ -19083,7 +19044,7 @@
       </c>
       <c r="H6" s="59"/>
     </row>
-    <row r="7" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A7" s="21">
         <v>6.5</v>
       </c>
@@ -19103,7 +19064,7 @@
       </c>
       <c r="H7" s="59"/>
     </row>
-    <row r="8" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A8" s="21">
         <v>6.6</v>
       </c>
@@ -19123,7 +19084,7 @@
       </c>
       <c r="H8" s="20"/>
     </row>
-    <row r="9" spans="1:8" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A9" s="21">
         <v>6.7</v>
       </c>
@@ -19143,7 +19104,7 @@
       </c>
       <c r="H9" s="20"/>
     </row>
-    <row r="10" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A10" s="21">
         <v>6.8</v>
       </c>
@@ -19163,7 +19124,7 @@
       </c>
       <c r="H10" s="56"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="60"/>
     </row>
   </sheetData>
@@ -19187,18 +19148,18 @@
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1"/>
-    <col min="5" max="5" width="30.109375" customWidth="1"/>
-    <col min="6" max="6" width="31.109375" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.375" customWidth="1"/>
+    <col min="5" max="5" width="30.125" customWidth="1"/>
+    <col min="6" max="6" width="31.125" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A1" s="86"/>
       <c r="B1" s="86"/>
       <c r="C1" s="86"/>
@@ -19208,7 +19169,7 @@
       <c r="G1" s="86"/>
       <c r="H1" s="86"/>
     </row>
-    <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -19234,7 +19195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="280.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="242.25" x14ac:dyDescent="0.15">
       <c r="A3" s="21">
         <v>7.1</v>
       </c>
@@ -19258,7 +19219,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="21">
         <v>7.2</v>
       </c>
@@ -19276,7 +19237,7 @@
       </c>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A5" s="21">
         <v>7.3</v>
       </c>
@@ -19294,7 +19255,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="171.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A6" s="21">
         <v>7.4</v>
       </c>
@@ -19314,7 +19275,7 @@
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A7" s="21">
         <v>7.5</v>
       </c>
@@ -19332,7 +19293,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A8" s="21">
         <v>7.6</v>
       </c>
@@ -19352,7 +19313,7 @@
       </c>
       <c r="H8" s="20"/>
     </row>
-    <row r="9" spans="1:8" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A9" s="21">
         <v>7.7</v>
       </c>
@@ -19372,7 +19333,7 @@
       </c>
       <c r="H9" s="20"/>
     </row>
-    <row r="10" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A10" s="21">
         <v>7.8</v>
       </c>
@@ -19392,7 +19353,7 @@
       </c>
       <c r="H10" s="56"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B12" s="8"/>
     </row>
   </sheetData>
@@ -19416,19 +19377,19 @@
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="30.88671875" customWidth="1"/>
-    <col min="5" max="5" width="35.33203125" customWidth="1"/>
-    <col min="6" max="6" width="30.77734375" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" customWidth="1"/>
+    <col min="4" max="4" width="30.875" customWidth="1"/>
+    <col min="5" max="5" width="35.375" customWidth="1"/>
+    <col min="6" max="6" width="30.75" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A1" s="86"/>
       <c r="B1" s="86"/>
       <c r="C1" s="86"/>
@@ -19438,7 +19399,7 @@
       <c r="G1" s="86"/>
       <c r="H1" s="86"/>
     </row>
-    <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -19464,7 +19425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>330</v>
       </c>
@@ -19488,7 +19449,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>331</v>
       </c>
@@ -19506,7 +19467,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>332</v>
       </c>
@@ -19524,7 +19485,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" s="22" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>333</v>
       </c>
@@ -19542,7 +19503,7 @@
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" s="22" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>334</v>
       </c>
@@ -19560,7 +19521,7 @@
       </c>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>335</v>
       </c>
@@ -19580,7 +19541,7 @@
       </c>
       <c r="H8" s="20"/>
     </row>
-    <row r="9" spans="1:8" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>336</v>
       </c>
@@ -19600,7 +19561,7 @@
       </c>
       <c r="H9" s="20"/>
     </row>
-    <row r="10" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>337</v>
       </c>
@@ -19620,7 +19581,7 @@
       </c>
       <c r="H10" s="56"/>
     </row>
-    <row r="12" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -19646,7 +19607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="140.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>339</v>
       </c>
@@ -19670,7 +19631,7 @@
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>340</v>
       </c>
@@ -19688,7 +19649,7 @@
       </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>341</v>
       </c>
@@ -19706,7 +19667,7 @@
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" s="22" customFormat="1" ht="109.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="22" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>342</v>
       </c>
@@ -19724,7 +19685,7 @@
       </c>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" s="22" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="22" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>343</v>
       </c>
@@ -19742,7 +19703,7 @@
       </c>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>344</v>
       </c>
@@ -19762,7 +19723,7 @@
       </c>
       <c r="H18" s="20"/>
     </row>
-    <row r="19" spans="1:8" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>345</v>
       </c>
@@ -19782,7 +19743,7 @@
       </c>
       <c r="H19" s="20"/>
     </row>
-    <row r="20" spans="1:8" ht="109.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>346</v>
       </c>
@@ -19826,18 +19787,18 @@
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="40.21875" customWidth="1"/>
-    <col min="6" max="6" width="48.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="40.25" customWidth="1"/>
+    <col min="6" max="6" width="48.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A1" s="86"/>
       <c r="B1" s="86"/>
       <c r="C1" s="86"/>
@@ -19847,7 +19808,7 @@
       <c r="G1" s="86"/>
       <c r="H1" s="86"/>
     </row>
-    <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -19873,7 +19834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="343.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="242.25" x14ac:dyDescent="0.15">
       <c r="A3" s="21">
         <v>9.1</v>
       </c>
@@ -19899,7 +19860,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A4" s="21">
         <v>9.1999999999999993</v>
       </c>
@@ -19917,7 +19878,7 @@
       </c>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="1:8" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A5" s="21">
         <v>9.3000000000000007</v>
       </c>
@@ -19935,7 +19896,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="124.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A6" s="21">
         <v>9.4</v>
       </c>
@@ -19955,7 +19916,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A7" s="21">
         <v>9.5</v>
       </c>
@@ -19973,7 +19934,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A8" s="21">
         <v>9.6</v>
       </c>
@@ -19991,7 +19952,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A9" s="21">
         <v>9.6999999999999993</v>
       </c>
@@ -20011,7 +19972,7 @@
       </c>
       <c r="H9" s="20"/>
     </row>
-    <row r="10" spans="1:8" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A10" s="21">
         <v>9.8000000000000007</v>
       </c>
@@ -20031,7 +19992,7 @@
       </c>
       <c r="H10" s="20"/>
     </row>
-    <row r="11" spans="1:8" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A11" s="21">
         <v>9.9</v>
       </c>
@@ -20051,7 +20012,7 @@
       </c>
       <c r="H11" s="57"/>
     </row>
-    <row r="12" spans="1:8" ht="156" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A12" s="61" t="s">
         <v>328</v>
       </c>

</xml_diff>